<commit_message>
Auto update insta products
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>productDescription</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -471,21 +476,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pdi</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1223</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1223</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1223</v>
-      </c>
-      <c r="F2" t="n">
-        <v>123</v>
-      </c>
+          <t>크리스마스트리 미니트리 풀세트 전구포함 초록트리 트윙클 크리스탈 45cm</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://naver.me/GhS2Sjwk</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221031_127/1667199162521wbDVQ_JPEG/68335061228336326_657608575.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>미니 크리스마스트리 세트</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>작고 아담한 45cm 트리로 공간을 환하게 꾸며보세요. 전구 포함으로 손쉬운 크리스마스 준비를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
All-in-one: update products & pages
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,12 +486,912 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>반짝이는 미니 크리스마스트리</t>
+          <t>미니 크리스마스 트리 세트</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>작은 공간에도 완벽한 45cm 미니트리로 따뜻한 연말 분위기를 만끽하세요.</t>
+          <t>작고 귀여운 45cm 트리로 공간을 환하게 밝혀보세요. 전구 포함으로 바로 완성 가능한 풀세트입니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>크리스마스트리 나무 장식 전구 풀세트 미니트리 카민로즈 60cm</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://naver.me/FGEWBxqd</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241120_247/1732090908328AggYN_JPEG/568915876437276_1930833792.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>크리스마스 미니 트리 조명</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>아늑한 연말 분위기, 작고 예쁜 미니 트리로 집안을 따뜻하게 꾸며보세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>크리스마스트리 나무 전구일체형 전나무 올레디 짠짠짠트리 150cm</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://naver.me/FSSdB72e</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250926_28/1758871462021fy9WH_JPEG/9234680545723543_992110204.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>150cm 전구 일체형 크리스마스트리</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>설치 걱정 없이 완성되는 전구 일체형 트리로, 따뜻한 연말 분위기를 쉽게 연출하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>레토 크리스마스 오르골 스노우볼 무드등 트리 인테리어조명 선물</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://naver.me/5r3XqzYE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251110_233/1762753004020JnvvV_JPEG/45185075123977079_605772484.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>크리스마스 오르골 무드등</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>따뜻한 빛과 감미로운 멜로디로 포근한 크리스마스 분위기를 선사합니다. 특별한 선물로도 완벽해요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>벽장식 고급 크리스마스 가랜드 대형 장식 그린전나무 가랜드 270cm 현관 꾸미기</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://naver.me/GtJkWRHz</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250905_228/1757038877436WuX2m_JPEG/40849809432601330_1125731568.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>대형 크리스마스 전나무 가랜드</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>현관이나 벽을 화사하게 꾸며주는 270cm 대형 전나무 가랜드로 크리스마스 분위기를 완성하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LED 야광 머리띠 고양이 생일 파티 할로윈 캐릭터 동물 크리스마스 이벤트 G-04</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgBmHkgp</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221101_78/1667285988930nBDR6_JPEG/68421822725526886_379458607.jpg</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LED 고양이 야광 머리띠</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>파티와 이벤트 분위기를 살리는 LED 고양이 머리띠로 특별한 순간을 빛내보세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>움직이는 기차 크리스마스 오르골 크리스마스장식 선물 크리스마스소품 트레인눈사람</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gsoun2FX</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251111_297/1762827045499vAUQa_JPEG/17525346596007412_1805044427.jpg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>움직이는 크리스마스 오르골</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>반짝이는 조명과 움직임으로 크리스마스 분위기를 더해요. 소중한 이에게 특별한 선물을 선사하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>고급 양모 양털 화이트 크리스마스 인테리어 트리 덮개 스커트 담요 매트 가리개 60cm</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://naver.me/5noaB4SW</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240927_22/17274228566063Nu4n_JPEG/61555714704941476_342412971.jpg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>포근한 크리스마스 트리 스커트</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>차가운 바닥에 포근함을 더해주는 양모 트리 스커트로 따뜻한 연말 분위기를 완성하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>카플 AAWireless 2 무선 안드로이드 오토 동글 전용앱 제공</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://naver.me/xfYHRkxl</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241213_8/17340703644297BxWp_JPEG/17881205318910450_409354498.jpg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>무선 안드로이드 오토 동글</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>복잡한 케이블 없이 편리한 무선 연결! 드라이브 중 스마트 기능을 쉽고 빠르게 사용하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>샤오미 미밴드 10 스마트 밴드 워치 웨어러블 심박수 만보기 운동 시계 스포츠 러닝 런닝</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://naver.me/G3PAhXKA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250905_186/1757064393149bD6th_JPEG/90817591629460387_2040145490.jpg</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>심박수 측정 스마트 밴드</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>운동 중 심박수를 정확히 체크하며 건강 관리를 쉽고 편리하게 도와줍니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>삼성 정품 갤럭시 스마트 태그2 위치추적기 원격 UWB 분실방지 어린이 미아방지 트래커</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://naver.me/FgTKvSOj</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241202_29/17331027876933cNNl_JPEG/19868530163881398_1602592050.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>실시간 위치추적 스마트 태그</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>소중한 아이와 물건을 안전하게 지키세요. 정확한 위치 확인으로 분실 걱정을 덜어줍니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>올인원 삼각대 블루투스 셀카봉 SEL-CT1300M</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://naver.me/xquYo5v6</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250228_131/17407235862945oMRT_JPEG/87097046226135825_1266053080.jpg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>간편 조절 올인원 삼각대</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>흔들림 없는 촬영과 자유로운 각도 조절로 소중한 순간을 완벽하게 담아보세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>샤오미 레드미 워치 5 액티브 만보기 러닝 런닝 운동 스포츠 시계</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://naver.me/GOhZQzzp</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250908_43/1757298331836lMKkK_JPEG/91306051896156888_898425836.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>운동 최적화 스마트워치</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>러닝과 일상 운동을 효과적으로 기록해 건강 관리에 도움을 줍니다. 활동량 측정으로 꾸준한 운동 습관을 만들어보세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>아이뮤즈 안드로이드 태블릿PC, 뮤패드 K11 LTE [RAM 8GB/저장공간 128GB]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://naver.me/5UT4Grri</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240927_39/1727400379472DQTUT_JPEG/15699937494177277_361597048.jpg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>강력한 LTE 태블릿PC</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>빠른 속도와 넉넉한 저장 공간으로 일상과 업무를 스마트하게 해결하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1+1 살림백서 차량용 방향제 디퓨저 80ml 포레스트가든 고급 자동차 차량 명품</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://naver.me/F5aRqMqk</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240819_68/1724027723542VVf1H_JPEG/51365116327154854_1852510496.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>차량용 포레스트가든 방향제</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>차 안 공기 냄새에 고민인가요? 포레스트가든 향기로 쾌적하고 상쾌한 드라이빙을 즐기세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>방풍 비닐 대형 맞춤 두꺼운 창문 우풍차단 현관 자석 베란다 커튼 40x10cm</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://naver.me/5zXwI6Tw</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230925_287/1695632594321Cmm6C_JPEG/15567567921752873_555173247.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>두꺼운 창문 우풍 차단 커튼</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>찬 바람과 외부 먼지를 막아 냉기 걱정을 덜어줍니다. 맞춤 크기로 완벽한 밀착 효과를 경험하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[단독] 세면대 워터탭 아기 비데 회전 수전 신생아 스윙글1개+필터3세트</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fc5kpSw8</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_107/1720410690591NRdag_JPEG/1103900859598527_1402585696.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>아기용 회전 비데 수전</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>신생아 세면대에 딱 맞는 부드러운 회전 수전으로 청결과 편리함을 동시에 해결하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>방풍 비닐 대형 맞춤 두꺼운 창문 우풍차단 현관 자석 베란다 커튼 40x10cm</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://naver.me/5zXwI6Tw</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230925_287/1695632594321Cmm6C_JPEG/15567567921752873_555173247.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>맞춤형 두꺼운 창문 우풍차단</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>찬바람과 외부 먼지를 효과적으로 막아내는 우풍차단 커튼으로 따뜻한 공간을 유지하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>바툼 욕실 온풍기 4.0 벽걸이 전기 가정용 화장실 온풍기 욕실난방기</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://naver.me/FFa7JX5k</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251023_115/1761211850133FRxx9_PNG/15387102926594746_1605516923.png</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>벽걸이 욕실 온풍기</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>차가운 욕실 공기 걱정 끝! 빠른 난방으로 따뜻한 공간을 만들어 드려요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>에어메이드 가열식 신생아 아기 살균 자동세척 더 위대한 가습기 2.0 AMH-4502</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://naver.me/57QgYU2c</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250924_28/1758676576537EYoku_JPEG/6546070264973758_920198057.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>신생아용 자동 살균 가습기</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>아기 건강 걱정되시나요? 자동 살균으로 청결하고 안전한 가습기로 안심하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>풀라스 프리미엄 니트 세탁소 업소용 보풀제거기</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://naver.me/xI1Vl7rX</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251107_236/1762499531292mAaJn_JPEG/35033975560962307_906682600.jpeg</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>업소용 보풀제거기</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>니트 보풀 고민, 풀라스 보풀제거기로 깔끔하게 해결하세요. 손쉬운 사용으로 옷감 손상 걱정 없이 새 옷처럼 관리됩니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>케어팟 저온 가열식 대용량 완벽살균 스텐 큐브 가습기 X50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://naver.me/x3HIR7ri</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250123_218/1737609793942smSh5_JPEG/73945063421327_269656625.jpg</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>저온 완벽살균 대용량 가습기</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>건조한 실내, 세균 걱정 없이 촉촉하게! 저온 가열로 안심하고 쓸 수 있는 대용량 가습기입니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>블라우풍트 ENC 노이즈캔슬링 오픈형 블루투스 이어폰 오픈픽 BLP-OE383</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://naver.me/GxLQTGqt</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250627_293/1751006736835cb2VB_JPEG/5579795974650774_1714364793.jpg</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>노이즈캔슬링 오픈형 이어폰</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>소음에 시달리는 일상, 편안한 오픈형 디자인으로 자유로운 착용감까지 경험하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>에디르 스텐 초음파 가습기 탁상용 사무실 가습기 세척편한 미니 가습기</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://naver.me/F4Lng487</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_61/1761008802600sm4Cz_JPEG/95141641731442454_589146379.jpg</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>탁상용 미니 초음파 가습기</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>건조한 사무실 공기, 간편한 세척으로 쾌적하게 관리하세요. 작은 크기로 어디서나 신선한 습도를 유지합니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>따수미 패브릭 난방텐트 S-PE폴 침대 방한 수면 돔 텐트 슈퍼싱글, 핑크</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://naver.me/GPlsfmYw</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241118_171/1731895960486HOpWb_JPEG/323422604722331_495017488.jpg</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>포근한 침대 난방텐트</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>추운 겨울, 따수미 난방텐트로 침대 속을 따뜻하게 감싸세요. 편안한 수면 환경을 제공합니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>빈슨메시프 포그닝 난방 텐트 실내 침대 방한 방풍 보온 겨울 수면텐트 싱글, 스너그그레이</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://naver.me/F0ADRhsp</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240925_43/1727247121467EsFej_JPEG/61379945672017850_902973394.jpg</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>겨울용 보온 난방 텐트</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>춥고 바람 부는 겨울에도 따뜻하게 감싸주는 보온 난방 텐트로 포근한 수면을 경험해 보세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>나이키 버로우 털 슬리퍼 플리스 패딩 겨울 방한 캠핑 방한화</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://naver.me/58jzSoV0</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251125_58/1764060075073JQf9t_JPEG/18587057830696921_1446136759.jpg</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 패딩 슬리퍼</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>차가운 겨울 발을 포근하게 감싸주는 패딩 슬리퍼로 집 안팎 어디서나 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>보아털후드집업 방상내피 방한 겨울작업잠바 돕바 겨울외투 빅사이즈</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1mxdnwk</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250305_129/1741140926671AmyOJ_JPEG/75273732410163524_139688753.jpg</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>포근한 보아털 후드집업</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>차가운 겨울 바람도 걱정 없는 따뜻한 보아털과 방한 내피로 포근함을 선사합니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>귀도리 방한 겨울 털 이어머프 양털 귀돌이 귀덮개 퍼 아이보리 이어워머 목도리 귀마개</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://naver.me/GXgIo933</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241222_133/17348056359229qYSC_JPEG/70852511689562404_401854286.jpg</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 털 귀도리</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>찬 바람에 얼어붙는 귀를 포근하게 감싸주는 양털 귀덮이로 올겨울도 따뜻하게 보내세요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>스마트폰터치장갑 방한장갑 겨울 기모 털 니트</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://naver.me/5pqCnp8A</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251118_192/1763454741284rRVOV_PNG/60932875818579484_1409168096.png</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>스마트 터치 방한 니트장갑</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 스마트폰 사용에 불편함 없음, 따뜻한 기모로 손끝까지 보호해줘요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>경량 패딩 목도리 머플러 방한 스카프 워머</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://naver.me/xMnmvTIB</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251031_18/17618851287512l7Wq_JPEG/87516762761071598_1836635782.jpg</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>경량 패딩 방한 머플러</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 가볍고 따뜻한 패딩 머플러로 목을 편안하게 감싸세요.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-13 20:19)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -2,31 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="645" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
       <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +56,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +81,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +446,11 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -481,7 +500,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>relatedNos</t>
+          <t>category</t>
         </is>
       </c>
     </row>
@@ -514,10 +533,26 @@
           <t>작은 공간도 환하게 채우는 미니 트리, 전구 포함 세트로 바로 꾸밀 수 있어요.</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>크리스마스트리 미니트리 45cm 전구포함 풀세트 추천</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>작은 공간을 화사하게 꾸며주는 45cm 미니 크리스마스트리 풀세트로, 전구 포함해 바로 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>크리스마스트리,미니트리,45cm,전구포함,풀세트,트윙클,크리스탈,초록트리,작은트리,홈데코</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>크리스마스/인테리어</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -548,10 +583,26 @@
           <t>작은 공간도 화사하게, 미니 트리와 전구 세트로 크리스마스 분위기를 완성하세요.</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>크리스마스트리 나무 장식 전구 풀세트 미니트리 60cm 추천</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>작은 공간에 딱 맞는 60cm 미니 크리스마스트리와 전구 세트로 따뜻한 연말 분위기를 연출하세요.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>크리스마스트리,미니트리,전구세트,나무장식,60cm,연말장식,크리스마스장식</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>크리스마스/인테리어</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -582,10 +633,26 @@
           <t>크리스마스 분위기를 완벽하게! 전구가 일체형으로 편리하게 빛나는 전나무 트리로 집안을 환하게 밝혀보세요.</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>크리스마스트리 150cm 전구일체형 전나무 트리 추천</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>전구가 일체형으로 설치가 편리한 150cm 전나무 크리스마스트리로 집안을 따뜻하고 화사하게 장식해보세요.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>크리스마스트리,전나무트리,전구일체형,150cm트리,크리스마스장식,인테리어트리</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>크리스마스/트리</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -616,10 +683,26 @@
           <t>따뜻한 분위기와 아름다운 멜로디로 연말 감성을 채워보세요. 소중한 이에게 특별한 선물로 추천합니다.</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>레토 크리스마스 오르골 스노우볼 무드등 추천, 연말 선물용</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>따뜻한 조명과 멜로디가 어우러진 크리스마스 스노우볼로 연말 분위기를 더욱 특별하게 연출하세요. 소중한 사람에게 선물하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>크리스마스오르골,스노우볼,무드등,연말선물,인테리어조명,트리장식,감성조명</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>크리스마스/인테리어</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -650,10 +733,26 @@
           <t>현관이나 벽을 화사하게 꾸미고 싶은데 고민된다면, 풍성한 전나무 가랜드로 따뜻한 연말 분위기를 완성하세요.</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>고급 크리스마스 가랜드 270cm 대형 전나무 벽장식 추천</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>풍성한 그린 전나무 가랜드로 현관과 벽을 화사하게 꾸미기에 적합한 크리스마스 장식입니다.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>크리스마스 가랜드,전나무 가랜드,벽장식,현관 꾸미기,대형 장식,연말 장식</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>크리스마스/인테리어</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -684,10 +783,26 @@
           <t>파티 분위기를 특별하게 밝혀줄 LED 고양이 머리띠로 즐거운 이벤트를 완성하세요.</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LED 야광 고양이 머리띠 파티 이벤트 추천</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>LED 빛나는 고양이 머리띠로 생일, 할로윈, 크리스마스 파티를 더욱 특별하게 연출하세요.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>LED머리띠,고양이머리띠,파티용품,생일파티,할로윈소품,크리스마스이벤트,야광아이템</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>파티/이벤트</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -718,10 +833,26 @@
           <t>따뜻한 크리스마스 분위기 연출, 감성 가득한 기차 오르골로 특별한 선물을 준비하세요.</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>움직이는 기차 크리스마스 오르골 추천 특별한 선물용</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>감성 가득한 움직이는 기차 오르골로 따뜻한 크리스마스 분위기를 연출하며 특별한 선물로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>크리스마스오르골,기차장식,크리스마스선물,크리스마스소품,눈사람장식,감성인테리어</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>크리스마스/장식</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -752,10 +883,26 @@
           <t>차가운 겨울, 크리스마스 트리에 포근함을 더해보세요. 부드러운 양모가 따뜻한 분위기를 완성합니다.</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>고급 양모 양털 화이트 크리스마스 트리 스커트 추천</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>포근한 양모 소재로 겨울철 크리스마스 트리에 따뜻함을 더하는 60cm 스커트입니다. 인테리어와 실용성 모두 갖춘 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>크리스마스트리스커트,양모트리스커트,화이트트리스커트,겨울인테리어,트리덮개,트리스커트매트,크리스마스장식</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>크리스마스/인테리어</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -786,10 +933,26 @@
           <t>복잡한 선 걱정 없이 무선으로 편리한 안드로이드 오토를 즐기세요. 차량 내 스마트 연결을 간편하게 도와드립니다.</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>카플 AAWireless 2 무선 안드로이드 오토 동글 구매 추천</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>무선으로 안드로이드 오토를 간편하게 연결해주는 카플 AAWireless 2 동글로 차량 내 스마트한 주행 환경을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>카플, AAWireless 2, 무선 동글, 안드로이드 오토, 차량 연결, 스마트카, 무선 미러링, 자동차 액세서리</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>자동차/스마트기기</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -820,10 +983,26 @@
           <t>운동 중 심박수를 정확히 측정하여 건강 관리를 도와줍니다. 러닝과 스포츠에 최적화된 스마트 워치로 활동을 더 즐겁게!</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>샤오미 미밴드 10 스마트 밴드 심박수 측정 추천</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>정확한 심박수 측정과 만보기 기능으로 운동과 러닝 시 건강 관리를 돕는 스마트 워치입니다.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>샤오미, 미밴드10, 스마트밴드, 심박수측정, 만보기, 운동시계, 스포츠워치, 러닝워치, 웨어러블</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>스포츠/웨어러블</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -854,10 +1033,26 @@
           <t>아이와 귀중한 물건을 잃어버릴 걱정 없이 안전하게 지키세요. 간편한 원격 관리로 안심을 선사합니다.</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>삼성 갤럭시 스마트 태그2 위치추적기 원격 분실방지 추천</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>아이와 귀중품을 안전하게 지키는 삼성 갤럭시 스마트 태그2, 원격 위치추적과 UWB 기술로 분실 걱정 없이 사용하세요.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>삼성 스마트 태그,갤럭시 태그2,위치추적기,UWB 분실방지,어린이 미아방지,트래커,원격 관리,위치 확인</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>위치추적/안전</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -888,10 +1083,26 @@
           <t>흔들림 없는 완벽한 셀카를 원하세요? 올인원 삼각대가 스마트한 촬영을 도와드립니다.</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>올인원 삼각대 블루투스 셀카봉 SEL-CT1300M 추천</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>흔들림 없는 완벽한 셀카 촬영을 위한 올인원 삼각대 블루투스 셀카봉으로 스마트한 촬영 환경을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>삼각대,셀카봉,블루투스 셀카봉,셀카 촬영,휴대용 삼각대,올인원 셀카봉,SEL-CT1300M</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>카메라/액세서리</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -922,10 +1133,26 @@
           <t>러닝과 운동 시 실시간 활동을 기록해 목표 달성에 도움을 줍니다. 건강한 라이프스타일을 시작하세요.</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>샤오미 레드미 워치 5 액티브 만보기 추천 스포츠 시계</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>러닝과 운동 중 실시간 활동 데이터를 기록해 목표 달성을 지원하는 샤오미 레드미 워치 5 액티브, 건강한 라이프스타일에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>샤오미,레드미 워치,스포츠 시계,만보기,운동 기록,러닝 시계,헬스케어,액티브워치</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>스포츠/웨어러블</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -956,10 +1183,26 @@
           <t>빠르고 넉넉한 저장공간으로 일상과 업무 모두 완벽하게! 가성비 좋은 태블릿이 필요할 때 추천합니다.</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>아이뮤즈 뮤패드 K11 LTE 태블릿PC RAM 8GB 128GB 추천</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>빠르고 넉넉한 저장공간을 갖춘 아이뮤즈 뮤패드 K11 LTE는 일상과 업무용 태블릿으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>아이뮤즈, 뮤패드 K11, 태블릿PC, LTE, RAM 8GB, 저장공간 128GB, 가성비 태블릿, 업무용 태블릿</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>가전/태블릿</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -990,10 +1233,26 @@
           <t>차 안의 답답한 냄새를 산뜻한 숲 향기로 채워보세요. 1+1으로 더욱 실속 있는 선택!</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1+1 살림백서 차량용 방향제 80ml 포레스트가든 추천</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>차량 내 답답한 냄새를 상쾌한 포레스트가든 향기로 채워주며 1+1 구성으로 경제적인 차량용 방향제입니다.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>차량용방향제,디퓨저,포레스트가든,자동차향수,차량냄새제거,1+1방향제,살림백서</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>자동차/방향제</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1024,10 +1283,26 @@
           <t>추운 날씨, 틈새 바람 때문에 고민이라면 두꺼운 비닐 커튼으로 따뜻함을 지켜보세요.</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>방풍 비닐 대형 두꺼운 창문 커튼 우풍차단 추천</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>두꺼운 대형 비닐 커튼으로 창문과 현관 틈새 바람을 효과적으로 차단해 추위로부터 실내를 따뜻하게 보호합니다.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>방풍커튼,비닐커튼,우풍차단,대형커튼,창문커튼,두꺼운비닐,현관커튼,베란다커튼,맞춤커튼</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>홈인테리어/방풍</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1058,10 +1333,26 @@
           <t>신생아의 민감한 피부를 위한 부드러운 세정, 회전 기능으로 편리함까지 더했어요.</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>[단독] 세면대 워터탭 아기 비데 회전 수전 추천</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>신생아 피부에 부드러운 세정과 편리한 회전 기능을 갖춘 아기 비데 워터탭, 필터 3세트 포함으로 위생적입니다.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>아기비데,세면대수전,워터탭,신생아용비데,회전수전,필터포함,스윙글워터탭</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>유아용품/욕실</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1092,10 +1383,26 @@
           <t>찬 바람과 외부 소음을 막아주는 두꺼운 맞춤 비닐로 겨울철 실내 온도를 지켜보세요.</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>방풍 비닐 대형 맞춤 창문 우풍차단 커튼 할인 추천</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>두꺼운 맞춤 비닐로 겨울철 우풍과 소음을 효과적으로 차단하여 실내 온도를 유지하는 방풍 커튼입니다.</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>방풍비닐,맞춤커튼,우풍차단,대형비닐,창문보온,현관커튼,베란다커튼,소음차단,두꺼운비닐</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>홈인테리어,방풍용품</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1126,10 +1433,26 @@
           <t>추운 욕실에서 빠르게 따뜻함을 즐기세요. 편리한 벽걸이형으로 공간 활용도 만점입니다.</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>바툼 욕실 온풍기 4.0 벽걸이형 가정용 욕실난방기 추천</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>추운 욕실에서 빠르게 따뜻함을 제공하는 벽걸이형 온풍기로 공간 활용이 뛰어나며 안전하게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>욕실온풍기,벽걸이온풍기,욕실난방기,전기온풍기,가정용온풍기,화장실난방기,빠른난방</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>욕실/가전</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1160,10 +1483,26 @@
           <t>아기 방 안 건조함과 세균 걱정 없이 건강한 습도를 유지해 주세요.</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>에어메이드 가열식 신생아 아기 가습기 2.0 추천</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>신생아 방에 적합한 에어메이드 가열식 가습기로 건강한 습도 조절과 자동 세척 기능을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>에어메이드,가습기,신생아,아기용,가열식,살균,자동세척,건강습도,AMH-4502</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>가전,육아</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1194,10 +1533,26 @@
           <t>니트 보풀 고민 끝! 프리미엄 보풀 제거기로 깔끔한 옷 상태를 유지하세요.</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>풀라스 프리미엄 니트 세탁소 업소용 보풀제거기 추천</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>니트 보풀 걱정 없이 깔끔한 의류 관리가 가능한 프리미엄 보풀 제거기입니다. 세탁소 및 개인용으로 적합한 고성능 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>보풀제거기,니트보풀제거,세탁소용,업소용보풀제거기,의류관리,프리미엄보풀제거기</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>세탁용품</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1228,10 +1583,26 @@
           <t>건조한 실내, 세균 걱정 없이 촉촉한 공기를 원한다면 저온 가열로 완벽 살균되는 대용량 가습기로 건강한 생활을 누리세요.</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>케어팟 X50 대용량 저온 가열식 스텐 큐브 가습기 추천</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>저온 가열로 완벽 살균되어 위생적인 대용량 가습기로 건조한 실내 공기를 촉촉하게 유지해줍니다. 건강한 생활에 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>가습기,저온가열식,대용량,살균가습기,스텐가습기,케어팟,실내가습,건강생활,큐브가습기</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>가전,생활가전</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1262,10 +1633,26 @@
           <t>소음 걱정 없이 선명한 음악을 즐기고 싶다면, ENC 기술로 깨끗한 음질을 경험해 보세요.</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>블라우풍트 ENC 노이즈캔슬링 블루투스 이어폰 추천</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ENC 노이즈캔슬링 기술로 소음 걱정 없이 선명한 음악 감상, 오픈형 블루투스 이어폰으로 편안한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>블루투스 이어폰, 노이즈캔슬링, ENC, 오픈형 이어폰, 블라우풍트, 무선 이어폰, 음악감상</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>가전/이어폰</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1296,10 +1683,26 @@
           <t>작고 조용한 가습기로 사무실 공기 건조함을 해결하세요. 간편 세척으로 편리함까지 챙겼습니다.</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>에디르 스텐 초음파 가습기 미니 탁상용 사무실 추천</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>조용하고 작은 초음파 가습기로 사무실 공기 건조함을 효과적으로 개선하며, 간편한 세척으로 관리가 쉽습니다.</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>에디르,스텐,초음파가습기,탁상용가습기,미니가습기,사무실가습기,조용한가습기,간편세척</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>가전/가습기</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1330,10 +1733,26 @@
           <t>추운 겨울, 따뜻한 공간이 필요할 때 완벽한 난방 텐트로 쾌적한 수면 환경을 제공합니다.</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>따수미 패브릭 난방텐트 S-PE폴 슈퍼싱글 핑크 추천</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하게 사용하는 난방 텐트로 쾌적한 수면 공간을 만들어 줍니다. 슈퍼싱글 침대에 딱 맞는 사이즈입니다.</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>난방텐트,패브릭텐트,겨울텐트,수면돔,방한텐트,슈퍼싱글,핑크텐트,침대텐트</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>침구/생활</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1364,10 +1783,26 @@
           <t>추운 날씨에도 따뜻하게 지낼 수 있는 보온 텐트로, 편안한 수면 환경을 만들어 드립니다.</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>빈슨메시프 포그닝 난방 텐트 싱글 보온텐트 추천</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하고 포근한 수면 환경을 제공하는 보온 난방 텐트로 실내 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>난방텐트,보온텐트,겨울텐트,수면텐트,실내용텐트,방한텐트,방풍텐트,싱글텐트</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>텐트/침실용품</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1398,10 +1833,26 @@
           <t>차가운 발끝 걱정 끝! 따뜻한 플리스와 패딩으로 겨울 내내 포근함을 느껴보세요.</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>나이키 버로우 털 슬리퍼 겨울 방한 캠핑 추천</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>따뜻한 플리스와 패딩으로 겨울철 발을 포근하게 보호하는 나이키 버로우 털 슬리퍼입니다. 캠핑이나 일상 방한화로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>나이키 슬리퍼,겨울 방한화,털 슬리퍼,캠핑 슬리퍼,패딩 슬리퍼,플리스 슬리퍼,발 보온</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>방한용품/슬리퍼</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1432,10 +1883,26 @@
           <t>추운 겨울 야외 작업에도 든든한 보아털 후드집업으로 따뜻함을 유지하세요.</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>보아털후드집업 방한 겨울작업잠바 추천</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>추운 겨울 야외에서도 따뜻한 보아털 후드집업, 빅사이즈로 편안한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>보아털,후드집업,방한,겨울작업잠바,빅사이즈,겨울외투,돕바,야외작업</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>겨울/작업복</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1466,10 +1933,26 @@
           <t>차가운 바람에 귀가 시려울 때, 부드러운 양털 귀도리가 따뜻함을 선사합니다.</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>귀도리 방한 겨울 털 이어머프 아이보리 추천</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>부드러운 양털 소재로 제작된 방한 이어머프로 겨울철 차가운 바람으로부터 귀를 따뜻하게 보호합니다.</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>귀도리, 겨울이어머프, 털이어머프, 방한귀덮개, 양털귀돌이, 아이보리이어워머, 귀마개, 목도리형이어머프</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>방한용품/액세서리</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1500,10 +1983,26 @@
           <t>추운 겨울에도 손 시림 걱정 없이 스마트폰 터치가 가능해요. 따뜻한 기모로 포근한 착용감을 선사합니다.</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>스마트폰터치장갑 겨울 기모 털 니트 방한장갑 추천</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 손 시림 없이 스마트폰 터치가 가능하며, 부드러운 기모로 따뜻한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>스마트폰터치장갑,방한장갑,기모장갑,겨울장갑,니트장갑,털장갑,손시림방지,터치장갑</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>패션/겨울용품</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1534,10 +2033,26 @@
           <t>차가운 바람에도 따뜻함을 잃지 마세요. 가볍고 포근한 목도리로 겨울철 필수 아이템입니다.</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>경량 패딩 목도리 머플러 방한 스카프 추천</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>가벼우면서도 따뜻한 경량 패딩 목도리로 겨울철 추위를 효과적으로 막아줍니다. 야외활동에 적합한 포근한 방한 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>경량패딩,목도리,방한스카프,겨울머플러,워머,겨울패션,따뜻한목도리,방한용품</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>겨울용품</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1568,10 +2083,26 @@
           <t>번거로운 변기 청소, 이 스틱 하나로 간편하게 해결하세요. 청결과 상쾌함을 동시에 느껴보세요.</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>New 닥터퓨리 변기세정제 스틱+청소포 12개입 간편청소 추천</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>New 닥터퓨리 변기세정제 스틱과 청소포 12개입으로 번거로운 변기 청소를 간편하게! 청결과 상쾌함을 동시에 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>변기세정제, 변기클리너, 청소스틱, 청소포, 간편청소, 닥터퓨리, 위생용품</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>생활/청소</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1602,10 +2133,26 @@
           <t>개업·승진·재물·합격 등 행운을 바라는 당신의 소원에 힘을 더해 드려요.</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>행운의부 소원부적 황금 소원 거북이 추천 - 개업·승진·재물·합격 행운</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>개업, 승진, 재물, 합격 등 다양한 소원에 맞춘 황금 소원 거북이 부적으로 행운을 더해드립니다. 새해 및 중요한 순간 선물용으로 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>행운부적,황금거북이,개업선물,승진부적,재물운,합격부적,새해선물,소원부적,삼재방지,행운기원</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>부적/행운</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1636,10 +2183,26 @@
           <t>귀여운 짱구와 함께하는 새해! 일정을 한눈에 관리하며 특별한 연말을 완성해보세요.</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025년 짱구 벽걸이 달력 추천 연말 선물용 오렌지 캐릭터 굿즈</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>귀여운 짱구 캐릭터가 돋보이는 2025년 벽걸이 달력으로 새해 일정을 쉽게 관리하고 연말 선물로 제격입니다.</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>짱구 달력,2025년 달력,벽걸이 달력,연말 선물,캐릭터 굿즈,오렌지 달력,일정관리,새해 달력</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>달력/캐릭터</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1670,10 +2233,26 @@
           <t>소중한 분께 전통의 의미를 담은 미니 복주머니로 새해 행운을 전해보세요.</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>데이로이 미니 복주머니 전통 복조리 새해 복주머니 추천</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>전통 복조리 디자인의 미니 복주머니로 새해 행운을 전하고 외국인 선물로도 좋은 명절용 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>데이로이,미니 복주머니,전통 복조리,새해 복주머니,명절 선물,외국인 기념품,행운 주머니</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1704,10 +2283,26 @@
           <t>소중한 마음을 전하는 작은 카드, 한 장으로 따뜻한 인사를 완성해 보세요.</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>메리크리스마스카드 8cm 30개입 A,B형 선택 구매 추천</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>소중한 마음을 전하는 미니 크리스마스카드로 새해 인사와 감사를 전하기에 적합한 8cm 사이즈 30개입 상품입니다.</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>크리스마스카드,미니카드,성탄카드,새해카드,감사카드,인사카드,메리크리스마스,카드세트</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>크리스마스/감사</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1738,10 +2333,26 @@
           <t>새 출발을 축하하는 황금빗자루로 액운을 쓸어내고 행운을 담아보세요.</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>돈쓸어담는 황금빗자루 각인제작 액막이 추천</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>액막이와 행운을 담는 황금빗자루로 신혼집들이, 개업, 이사 선물로 적합한 맞춤 각인 상품입니다.</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>황금빗자루,액막이,신혼집들이선물,개업선물,이사선물,각인제작,행운,재물운</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>선물/행운</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1772,10 +2383,26 @@
           <t>새해 시작에 행운을 더해줄 용띠 맞춤 키링으로 특별한 기운을 느껴보세요.</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2024 갑진년 용의 해 신년 행운 푸른 용 용띠키링 추천</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024년 용의 해를 기념하는 맞춤 용띠 키링으로 새해 행운과 특별한 기운을 더하세요. 선물용으로도 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2024용띠키링,갑진년키링,신년행운키링,푸른용키링,용띠선물,행운키링</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>신년/키링</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1806,10 +2433,26 @@
           <t>새해 시작을 깔끔하게! 2026년 한눈에 확인하고 계획 세우세요.</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2026년 달력 벽걸이 캘린더 추천 - 계획 세우기 최적</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2026년 한눈에 확인 가능한 벽걸이 달력으로 새해 계획을 쉽게 세울 수 있습니다. 깔끔한 디자인으로 가정과 사무실에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2026년 달력,벽걸이 달력,캘린더,새해 달력,계획 달력,은행 달력,카렌다</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>달력/캘린더</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-14 14:07)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="645" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -444,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -2454,6 +2454,506 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>시리어스 근적외선 LED 패치 손목 찜질 보호대 발목 온열 무선</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://naver.me/FaO246ab</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240222_219/17085750709655ncrM_PNG/109710850683113521_113151619.png</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>근적외선 온열 손목 발목 패치</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>손목과 발목 통증, 찜질 효과로 완화하세요. 무선으로 편리하게 온열을 경험할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>시리어스 근적외선 LED 패치 손목 발목 온열 찜질 추천</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>손목과 발목 통증 완화를 위한 무선 온열 패치로, 근적외선 LED로 찜질 효과를 제공합니다. 휴대가 편리해 언제 어디서나 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>근적외선,LED패치,손목찜질,발목보호대,무선온열,통증완화,온열찜질,휴대용보호대</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>건강/보호대</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>잠온 원적외선 온열찜질기 찜질팩 전기핫팩 찜질기 황토 돌 생리통 허리 배 복부 무릎 베이지</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://naver.me/x2cuEvqX</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241001_156/17277613467390Hbp7_JPEG/12946312524396113_1597810359.jpg</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>원적외선 온열찜질팩</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>생리통과 허리 통증에 따뜻한 온열 찜질로 편안함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>잠온 원적외선 온열찜질기 찜질팩 추천 - 생리통 허리 통증 완화</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>잠온 원적외선 온열찜질기로 생리통과 허리 통증을 부드럽게 완화하세요. 베이지 색상의 따뜻한 찜질팩으로 복부와 무릎에도 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>잠온,원적외선,온열찜질기,찜질팩,전기핫팩,생리통,허리통증,복부찜질,무릎보호,베이지</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>건강/찜질</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>수족냉증 찜질기 전기찜질매트 오르홈 한일의료기 온열찜질기 발 생리통 허리 어깨 배 무릎</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://naver.me/GJ5uln6d</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250417_257/1744897828204fFu0v_JPEG/24836975015592192_1794947346.jpg</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>수족냉증 전기 찜질기</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>차가운 손발과 반복되는 통증으로 힘든 당신을 위해, 따뜻한 온열 찜질로 편안함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>수족냉증 찜질기 전기찜질매트 오르홈 온열찜질 추천</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>차가운 손발과 반복되는 통증 개선에 효과적인 전기찜질기입니다. 발, 생리통, 허리, 어깨, 무릎까지 편안한 온열 찜질을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>수족냉증,찜질기,전기찜질매트,온열찜질,발찜질,생리통완화,허리찜질,어깨통증,무릎찜질</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>건강/의료</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>수쌤네가게 전기 온열찜질기 참숯 맥반석 황토 천연옥 찜질매트 전기 찜질팩 다용도밴드</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://naver.me/GmtOHcxj</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240711_52/1720677458765m9s2r_JPEG/67734424059655192_560233155.jpg</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>참숯 천연온열 찜질매트</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>뭉친 근육과 냉기에 지친 당신을 위한 천연옥 온열찜질기로 편안한 휴식을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>수쌤네가게 전기 온열찜질기 참숯 맥반석 추천</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>천연옥과 맥반석이 포함된 전기 찜질기로 근육 이완과 냉기 해소에 효과적이며 다용도로 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>수쌤네가게, 전기찜질기, 온열찜질기, 참숯찜질매트, 맥반석, 천연옥, 찜질팩, 다용도밴드</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>건강,생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>온쉼 전기 배 찜질기 온열기 온찜질기 허리 찜질 매트 통증 570-1500</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://naver.me/xTsu8KZs</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251107_156/1762483628133tWdKq_PNG/2153083109898866_468317951.png</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>허리 통증 완화 온찜질기</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>끊임없는 허리 통증, 온쉼 전기 찜질기로 따뜻하게 케어하세요. 집에서도 간편한 온열 치료로 편안함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>온쉼 전기 배 찜질기 허리 통증 완화에 추천</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>온쉼 전기 배 찜질기는 집에서 간편하게 사용하는 온열기로 허리 통증 완화에 도움을 줍니다. 편안한 찜질 효과로 꾸준한 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>온쉼,전기찜질기,허리찜질기,온열기,통증완화,찜질매트,허리케어</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>건강/찜질기</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>홍여진 온몸애 찜질박사 찜질기 1세트 진동 허리찜질 무선 전기 온열찜질기</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://naver.me/57QYsUkv</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250121_114/1737445433275q2GUg_JPEG/28789299582442606_257377433.jpg</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>무선 진동 허리 온열찜질기</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>끊임없는 허리 통증, 온열과 진동으로 따뜻하게 케어하세요. 무선으로 편리한 찜질이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>홍여진 온몸애 찜질박사 찜질기 1세트 무선 진동 허리찜질 추천</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>무선 방식으로 편리한 사용이 가능하며, 온열과 진동 기능으로 허리 통증 완화를 돕는 찜질기입니다.</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>홍여진, 찜질박사, 온열찜질기, 진동찜질기, 무선찜질기, 허리찜질, 통증완화, 건강관리</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>건강/찜질기</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>[프로덕트피알] 180도 회전 고속충전케이블 C TO C 컬러 케이블 PD 100W 꼬임방지 초고속충전기 1.5m</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://naver.me/xwwlTXfV</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251030_218/1761799191348GWYAz_JPEG/86060415742267370_2017281185.jpg</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>180도 회전 고속충전케이블</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>꼬임 걱정 없이 빠르게 충전하세요. 100W 고속 충전으로 편리함을 더합니다.</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>[프로덕트피알] 180도 회전 고속충전케이블 C TO C 100W 추천</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>100W 고속 충전 지원과 180도 회전 기능으로 꼬임 걱정 없이 빠르게 충전할 수 있는 C to C 충전 케이블입니다.</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>고속충전케이블,C TO C 케이블,100W 충전,180도 회전,꼬임방지,초고속충전기,1.5m 케이블,PD 충전</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>가전/충전기</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>네고 아이폰 16 e 14 13 프로 강화유리 액정보호필름 지문방지 0.29 2매</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://naver.me/50JEVyQx</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251127_254/17642296510689kTSc_JPEG/98362475850349616_23478345.jpg</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>지문방지 강화유리 2매</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>아이폰 화면을 깨끗하게 지켜주는 지문방지 강화유리, 2매 세트로 든든한 보호를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>네고 아이폰 16 e 14 13 프로 강화유리 액정보호필름 추천</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>지문방지 기능이 탁월한 아이폰용 강화유리 액정보호필름 2매 세트로 깨끗한 화면을 오래도록 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>아이폰강화유리, 액정보호필름, 지문방지, 아이폰16, 아이폰14, 아이폰13프로, 강화유리, 2매세트</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>스마트폰/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>갤럭시 S25 울트라 지문인식 강화유리 액정보호필름 지문방지 방탄 풀점착 1366번 2매</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://naver.me/FvQrXM3k</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251127_152/1764226473564zRp5P_JPEG/24270640699557810_332792624.jpg</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>지문방지 강화유리 필름 2매</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>지문과 스크래치 걱정 없이 선명한 화면을 유지하세요. 강력한 방탄 소재로 안심 보호를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>갤럭시 S25 울트라 방탄 지문인식 강화유리 액정보호필름 추천</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>갤럭시 S25 울트라용 지문방지 강화유리 필름으로 선명한 화면과 강력한 방탄 보호를 제공합니다. 지문과 스크래치 걱정 없이 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>갤럭시S25울트라, 강화유리, 액정보호필름, 지문방지, 방탄, 풀점착, 스크래치방지</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>모바일/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>메이튼 무선 안드로이드 오토 프로 X 유튜브 동글 연결</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://naver.me/52cnsfDa</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250114_41/1736853688384NGjTO_JPEG/60809513204200545_1121298826.jpg</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>무선 안드로이드 오토 연결</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>차량에서 간편히 유튜브와 안드로이드 오토를 무선으로 즐기고 싶은 분들에게 완벽한 솔루션입니다.</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>메이튼 무선 안드로이드 오토 프로 X 유튜브 동글 추천</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>차량에서 유튜브와 안드로이드 오토를 무선으로 간편하게 연결해주는 메이튼 무선 안드로이드 오토 프로 X 동글로 안전하고 편리한 드라이빙을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>메이튼,무선안드로이드오토,유튜브동글,차량연결,드라이브,안드로이드오토동글,무선미디어,차량용동글</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>자동차/모바일</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-15 03:30)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -2,41 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="맑은 고딕"/>
-      <charset val="129"/>
-      <family val="3"/>
       <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="맑은 고딕"/>
-      <charset val="129"/>
-      <family val="3"/>
-      <sz val="8"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,19 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -81,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -444,13 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2951,6 +2932,806 @@
       <c r="J50" t="inlineStr">
         <is>
           <t>자동차/모바일</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>휴고스 미니 컴팩트 PTC 전기온풍기 소형 히터 캠핑 사무실 발난로</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://naver.me/xbjdAyGm</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250926_101/17588598135561I8SR_JPEG/92992735688983672_1838852221.jpg</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>미니 전기온풍기 발난로</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>작고 강력한 온풍기로 사무실과 캠핑장에서 따뜻함을 빠르게 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>휴고스 미니 컴팩트 PTC 전기온풍기 추천</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>작고 강력한 휴고스 미니 전기온풍기로 사무실과 캠핑 등 다양한 공간을 빠르게 따뜻하게 해 줍니다.</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>휴고스,미니온풍기,컴팩트히터,PTC히터,전기온풍기,소형히터,발난로,캠핑히터,사무실히터</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>가전/히터</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>르젠 감성 동파방지 무타공 1초발열 절전형 순간발열 PTC 욕실용히터 온풍기 LZH-B770D</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://naver.me/5eZBUv8s</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251126_137/1764118554399jnJnU_JPEG/25455801497886398_1776636856.jpg</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>절전형 욕실용 순간발열 히터</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>추운 욕실도 빠르게 따뜻하게, 전기세 걱정 없이 절전형 발열 기술로 쾌적함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>르젠 감성 동파방지 욕실용 히터 LZH-B770D 절전형 구매</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>추운 욕실을 빠르게 따뜻하게 만드는 절전형 PTC 순간발열 욕실용 온풍기로 실용적이고 경제적입니다.</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>르젠,동파방지,욕실히터,절전형,순간발열,PTC히터,온풍기,욕실온풍기</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>가전,욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>쿠오레 불멍 전기 가습 히터 가정용 거실 사무실 온풍기 벽난로 인테리어 CH-LH20B</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://naver.me/55PhraLO</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251205_157/1764921072519h2VVN_PNG/99053885603308557_650950176.png</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>거실용 전기 가습 히터</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>추운 겨울, 따뜻한 온기와 촉촉한 습기로 쾌적한 공간을 만들어 보세요.</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>쿠오레 불멍 전기 가습 히터 CH-LH20B 온풍기 추천</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>쿠오레 불멍 가습 히터는 거실과 사무실에 따뜻한 온기와 촉촉한 습기를 제공합니다. 겨울철 쾌적한 실내 환경에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>쿠오레,전기히터,가습히터,온풍기,벽난로,거실히터,사무실히터,겨울가전</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>가정용 욕실 온풍기 화장실 벽걸이 난방기 PTC 히터 2255WF</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQiXMG1Y</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251010_8/17600522426622O3Ko_JPEG/45896581643329479_1789907410.jpg</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>욕실 벽걸이 온풍기</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>추운 욕실도 걱정 끝, 빠르게 따뜻한 온기로 쾌적한 공간을 만들어드립니다.</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>가정용 욕실 온풍기 PTC 히터 2255WF 추천 및 할인</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>추운 욕실에 적합한 벽걸이형 온풍기로 빠르게 따뜻한 공간을 제공합니다. 쾌적한 욕실 환경을 원하는 가정에 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>욕실온풍기,가정용온풍기,벽걸이난방기,PTC히터,화장실난방,욕실난방기,온풍기추천</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>가전/난방기</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>가정용온풍기 저소음 PTC히터 스탠드 난방기 사무실온풍기 2550</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://naver.me/5L7ZHXqX</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251103_37/1762124882953bmRwM_JPEG/78350197805646922_647395038.jpg</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>저소음 가정용 온풍기</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 조용하고 빠른 온기로 따뜻함을 느껴보세요. 사무실과 가정 어디서나 편안한 난방을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>가정용온풍기 2550 저소음 PTC히터 난방기 추천</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>가정과 사무실에서 사용할 수 있는 저소음 PTC 스탠드 온풍기로 빠르게 따뜻함을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>가정용온풍기,저소음히터,PTC히터,스탠드난방기,사무실온풍기,효율난방기</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>가전/난방기</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>이나프 무선 청소기 MV1 차량용 미니 핸디 소형 원룸 청소기</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://naver.me/5UTCEAyE</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251202_14/1764633907026ALdah_JPEG/2418911230288605_1249188675.jpg</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>차량용 초경량 무선청소기</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>좁은 공간도 깔끔하게! 차량과 원룸 청소 고민을 한 번에 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>이나프 무선 차량용 미니 청소기 MV1 추천</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>좁은 공간과 차량, 원룸 청소에 최적화된 무선 핸디 청소기로 간편하게 청소하세요.</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>이나프,무선청소기,차량용청소기,미니청소기,핸디청소기,원룸청소기,소형청소기</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>드리미 V10s 무선청소기 핸디스틱형 진공청소기 140AW 3자기 흡입 모드 국내 A/S</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://naver.me/xhlqzLoH</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250812_259/17549936621890965E_PNG/81486967999075804_618541934.png</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>강력 무선 진공청소기</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>가벼운 무선으로 집안 구석구석 깔끔하게! 흡입력 걱정 없이 편리한 청소를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>드리미 V10s 무선청소기 핸디 스틱형 추천 및 할인</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>가벼운 무선 청소기로 집안 구석구석 손쉽게 청소하세요. 140AW 강력 흡입력에 3가지 자기 흡입 모드로 효율적입니다.</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>드리미,무선청소기,핸디스틱,진공청소기,강력흡입,가벼운청소기,국내용A/S,140AW</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>청소기/가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>몬스타기어 클래식104 멤브레인 보글보글 사무용 저소음 키보드 투명 실리콘 키스킨 세트</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://naver.me/FOZj95EJ</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240215_292/17079859121505xnDj_JPEG/109121739972719035_130031986.jpg</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>저소음 사무용 멤브레인 키보드</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>조용한 업무 환경을 원한다면 저소음 멤브레인 키보드가 제격입니다. 투명 실리콘 키스킨으로 깨끗함까지 챙겨보세요.</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>몬스타기어 클래식104 저소음 멤브레인 키보드 추천</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>사무용으로 적합한 저소음 멤브레인 키보드와 투명 실리콘 키스킨 세트로 조용하고 깔끔한 업무 환경을 만들어줍니다.</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>몬스타기어,저소음키보드,멤브레인키보드,사무용키보드,투명키스킨,키스킨세트,실리콘키스킨,조용한키보드</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>사무용,키보드</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>가츠 클래식104 보글보글 5세대 멤브레인 저소음 풀윤활 게이밍 사무용 유선 키보드</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://naver.me/58jUNQIy</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240215_292/17079859121505xnDj_JPEG/109121739972719035_130031986.jpg</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>저소음 멤브레인 게이밍 키보드</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>소음 걱정 없이 게임과 업무에 집중하세요. 부드러운 타건감과 풀윤활 기능이 손끝부터 편안함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>가츠 클래식104 멤브레인 저소음 키보드 추천</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>저소음 멤브레인과 풀윤활 기능으로 부드럽고 편안한 타건감을 제공하는 게이밍 및 사무용 유선 키보드입니다.</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>가츠,클래식104,멤브레인 키보드,저소음 키보드,게이밍 키보드,사무용 키보드,유선 키보드,풀윤활 키보드</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>키보드/컴퓨터</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>몬스타기어 X108 보글보글 5세대 멤브레인 사무용 저소음 풀윤활 키보드 리퍼 리퍼비시</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQiveUCS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241129_297/17328483143964YXbe_JPEG/14921095412492371_319647656.jpg</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>사무용 저소음 멤브레인 키보드</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>조용한 타건감으로 업무 집중을 도와주는 5세대 멤브레인 키보드입니다.</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>몬스타기어 X108 보글보글 5세대 멤브레인 키보드 추천</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>저소음 타입의 5세대 멤브레인 키보드로 사무용에 적합하며, 조용한 타건감이 업무 집중을 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>몬스타기어, 멤브레인 키보드, 사무용 키보드, 저소음 키보드, 풀윤활, 리퍼비시 키보드, X108</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>사무용/키보드</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>호무로 그래피트 알러지프리 극세사 자가발열 겨울 패드 SS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://naver.me/xnrHIZY3</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241217_285/1734421817729xsGjl_JPEG/68554763848718013_580686861.jpg</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>알러지 방지 자가발열 패드</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없는 알러지프리 자가발열 패드로 따뜻한 겨울을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>호무로 그래피트 알러지프리 자가발열 겨울 패드 SS 추천</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 알러지프리 자가발열 극세사 패드로 따뜻하고 편안한 겨울을 보내세요.</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>호무로,그래피트,알러지프리,자가발열,겨울패드,극세사,민감피부,따뜻한침구</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>침구/겨울</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>호이데코 코지 단모 러그 [워셔블] - 50x100</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fhf1qzbE</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250324_277/1742798947884NpXGU_JPEG/76931733998516137_1175007394.jpg</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>포근한 코지 단모 러그</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>차가운 바닥 걱정 없이 따뜻한 공간을 만들어줄 워셔블 러그입니다.</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>호이데코 코지 단모 러그 50x100 워셔블 러그 추천</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>차가운 바닥을 따뜻하게 보호하는 워셔블 러그로 실내 공간을 아늑하게 만들어줍니다. 세탁이 쉬워 청결하게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>러그,단모러그,워셔블러그,따뜻한러그,호이데코,실내용러그,러그추천</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>인테리어/러그</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>원목 침대 프레임 매트리스 깔판 저상형 침대 받침대 소나무 2단 접이식 깔판 미니싱글</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://naver.me/5CF3SNoV</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220215_148/1644907248123CQ5MB_JPEG/46043136798435759_475255463.jpg</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>저상형 원목 침대 프레임</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>견고한 소나무 2단 접이식 디자인으로 공간 활용을 극대화하고 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>원목 소나무 2단 접이식 저상형 침대 프레임 미니싱글 추천</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>견고한 소나무 소재의 2단 접이식 원목 침대 프레임으로 공간 활용과 쾌적한 잠자리를 모두 만족시키는 미니싱글 침대 받침대입니다.</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>원목침대,소나무침대,저상형침대,접이식침대,미니싱글침대,침대프레임,침대받침대</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>가구/침대</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>모노 러그 거실 카페트 먼지없는 사계절 단모 대형 온감 워셔블 아트 100x150</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://naver.me/FMT4y2f2</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250103_186/1735853909606RTMwG_JPEG/16485232410076329_319247054.jpg</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>사계절 먼지없는 대형 러그</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>먼지 걱정 없이 쾌적한 거실을 만들어주는 사계절용 대형 러그로 집안을 따뜻하고 아늑하게 꾸며보세요.</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>모노 러그 거실용 대형 사계절 먼지없는 단모 카페트 추천</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>먼지 없는 사계절용 대형 러그로 쾌적하고 따뜻한 거실 인테리어에 적합하며 세탁도 간편한 워셔블 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>모노러그,거실러그,사계절러그,대형카페트,먼지없는러그,단모러그,워셔블러그,온감러그,아트러그</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>거실/인테리어</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>사계절 이불 포근한 차렵 겨울이불 알러지케어 에코 옥수수솜 단품 S</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://naver.me/FK0uYd8y</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240911_232/1726043960560guMeS_JPEG/29600834309618471_1085720924.jpg</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>사계절 포근 차렵이불</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 사계절 내내 포근하게 감싸주는 옥수수솜 이불로 쾌적한 잠자리를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>사계절 이불 포근한 차렵 겨울이불 알러지케어 추천</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 에코 옥수수솜으로 사계절 내내 포근하게 사용할 수 있는 차렵 이불입니다.</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>사계절이불,차렵이불,알러지케어,옥수수솜이불,포근한이불,겨울이불,에코이불,단품이불,S사이즈</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>핸드폰 사진인화 액자 사진인쇄 사진출력 웨딩 제작 만들기 미니 9x9cm</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://naver.me/FjCSRZ3S</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241114_112/1731563190364xHlO5_JPEG/59945680989044442_289981561.jpg</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>미니 사진인화 액자</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>소중한 추억을 작고 귀여운 액자에! 특별한 순간을 간편하게 간직해보세요.</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>핸드폰 사진인화 미니 액자 9x9cm 제작 추천</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>작고 귀여운 9x9cm 미니 액자에 핸드폰 사진을 인화하여 웨딩 등 특별한 순간을 간편하게 간직할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>핸드폰 사진인화, 미니 액자, 사진출력, 웨딩 사진, 사진인쇄, 소형 액자, 추억 보관</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>사진인화/액자</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-15 22:43)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3735,6 +3735,3756 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>살래오 건조기 시트 플로럴머스크향 캡형 8g 80매입 + 개별형 40매입</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://naver.me/xnrITAjt</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250328_253/1743121462246rfuUQ_JPEG/61424769197033037_1526317481.jpg</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>플로럴머스크 향 건조기 시트</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>옷감에 은은한 플로럴머스크 향을 남겨 건조 후에도 상쾌함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>살래오 건조기 시트 플로럴머스크향 120매입 추천</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>은은한 플로럴머스크 향기로 옷을 상쾌하게 해주는 살래오 건조기 시트 120매입 세트입니다. 건조 후 향기 유지에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>살래오,건조기시트,플로럴머스크,향기시트,세탁템,옷향기,살균,캡형,개별형</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>생활/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>순수백과 정전기 방지 섬유탈취제 스프레이 500ml 리필</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://naver.me/ximpGpdS</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240828_260/1724808244818kj5Hj_JPEG/11573987308316661_1421396589.jpg</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>정전기 방지 섬유탈취 스프레이</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>정전기로 불편한 옷과 섬유에 쾌적한 향과 함께 깔끔한 탈취 효과를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>순수백과 정전기 방지 섬유탈취제 스프레이 500ml 리필 추천</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>정전기 방지와 효과적인 탈취로 옷과 섬유를 상쾌하게 관리하는 500ml 리필 스프레이입니다. 쾌적한 향을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>섬유탈취제,정전기방지,섬유스프레이,탈취스프레이,순수백과,섬유관리,리필스프레이</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>생활/섬유관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>온다숲 아토피등록 숲속향 섬유탈취제 섬유향수 드레스퍼퓸 이불 룸스프레이 500ml</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://naver.me/FQyojobx</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251030_282/1761825280364f9kuy_JPEG/37443357836240633_930884562.jpg</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>아토피 안심 숲속 섬유탈취제</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>예민한 피부도 안심, 아토피 등록된 자연 숲향이 옷과 이불을 산뜻하게 케어합니다.</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>온다숲 아토피등록 숲속향 섬유탈취제 500ml 추천</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>아토피 등록된 자연 숲향으로 예민한 피부도 안심하고 사용할 수 있는 섬유 탈취제. 이불과 옷을 산뜻하게 케어합니다.</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>온다숲,아토피등록,섬유탈취제,섬유향수,드레스퍼퓸,이불탈취제,룸스프레이,자연숲향,피부안심,산뜻케어</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>생활용품/탈취제</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>룩브라이트 건조기섬유유연제시트 에어드레서시트 정전기방지 80매+80매</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://naver.me/GiamEoLi</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241014_36/1728866744552aIxAc_JPEG/1187824708625186_2024542167.jpg</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>정전기방지 섬유유연 시트</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>건조기 사용 시 섬유 정전기와 냄새 고민을 한 번에 해결해주는 80매+80매 대용량 시트입니다.</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>룩브라이트 건조기섬유유연제시트 160매 정전기방지 추천</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>건조기 사용 시 섬유 정전기와 냄새를 한 번에 케어하는 룩브라이트 건조기 섬유유연제 시트 160매 대용량 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>룩브라이트,건조기,섬유유연제시트,정전기방지,냄새제거,대용량,에어드레서시트,섬유관리</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>[1개] 부케가르니 딥 퍼퓸 섬유향수 500ml 향 4</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://naver.me/GoiQyQgy</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241227_291/1735267098307v5esX_JPEG/69399965435267895_706526868.jpg</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>풍부한 향기 섬유퍼퓸 500ml</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>옷과 섬유에 오래가는 깊은 향기로 일상의 불쾌한 냄새를 없애보세요.</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>부케가르니 딥 퍼퓸 섬유향수 500ml 향 4 추천</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>부케가르니 딥 퍼퓸 섬유향수는 옷과 섬유에 오래 지속되는 깊은 향기로 불쾌한 냄새 제거에 효과적입니다.</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>섬유향수,부케가르니,퍼퓸,옷향수,냄새제거,딥퍼퓸,향수500ml</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>생활용품/향수</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>메르헨트 올데이 필로우미스트 200ml, 1개 히노키우드 룸스프레이 섬유탈취제 릴렉싱</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://naver.me/F6n8th6F</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250218_35/1739866293168RG9mD_JPEG/10240714289409294_678013523.jpg</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>편안한 히노키우드 섬유탈취</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>누적된 생활 냄새 걱정 끝, 편안한 히노키 향으로 공간을 상쾌하게 탈취하세요.</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>메르헨트 올데이 필로우미스트 200ml 히노키우드 룸스프레이 추천</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>생활 냄새 걱정을 덜어주는 히노키우드 향의 메르헨트 필로우미스트로 공간과 섬유를 상쾌하게 탈취하세요.</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>필로우미스트,히노키우드,룸스프레이,섬유탈취제,릴렉싱,탈취,향기,집안냄새,공간탈취</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>생활용품/탈취제</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1+1 쉼표365 섬유탈취제 500ml 시그니처솝 정전기방지 섬유향수 룸스프레이 드레스퍼퓸</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://naver.me/IxKJEJ4h</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250220_67/17400376567304KNo1_JPEG/1374903834185697_1360148376.jpg</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>섬유탈취 정전기방지 스프레이</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>옷과 공간에 숨어있는 냄새와 정전기 고민, 한 번에 해결해보세요. 상쾌한 향기로 매일 새로워집니다.</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>1+1 쉼표365 섬유탈취제 500ml - 정전기방지와 상쾌한 향 추천</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>쉼표365 섬유탈취제로 옷과 공간의 냄새와 정전기 걱정을 동시에 해결하세요. 상쾌한 시그니처솝 향이 매일 쾌적함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>섬유탈취제,정전기방지,섬유향수,룸스프레이,드레스퍼퓸,쉼표365,섬유탈취,향기,옷냄새</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>생활용품/탈취제</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1+1 뭉클 남이섬의 숲 홈앤패션 스프레이 500ml 섬유향수 룸스프레이 드레스퍼퓸</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://naver.me/5W9252bR</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250618_58/1750178367060QwHwh_JPEG/84311177206072835_767011752.jpg</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>남이섬 숲 향기 스프레이</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>집안 가득 청량한 숲 향기로 불쾌한 냄새를 깨끗하게 제거해보세요.</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>1+1 뭉클 남이섬 숲 홈앤패션 스프레이 500ml 추천</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>청량한 숲 향기로 집안 냄새를 깨끗하게 제거하는 섬유향수 및 룸스프레이로 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>홈앤패션,섬유향수,룸스프레이,숲향,드레스퍼퓸,냄새제거,남이섬,청량향</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>홈/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1+1 몽때리 섬유향수 100ml 드레스 퍼퓸 정전기 방지 편백수</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://naver.me/G9peVefT</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240307_75/1709814614975dYEaL_PNG/110950398666514794_1394363799.png</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>정전기 방지 섬유향수</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>옷에 남는 불쾌한 냄새와 정전기 걱정 이제 그만! 산뜻한 편백수 향으로 기분까지 상쾌해집니다.</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>1+1 몽때리 섬유향수 100ml 드레스 퍼퓸 추천</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>불쾌한 냄새와 정전기 걱정을 줄여주는 몽때리 섬유향수로 산뜻한 편백수 향을 경험하세요. 옷에 상쾌함과 쾌적함을 더해줍니다.</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>섬유향수,정전기방지,드레스퍼퓸,편백수향,옷냄새제거,몽때리,사계절향수</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>패션/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>폴리보이 더스트스탑 티슈 3팩/ 정전기 먼지 방지 유리 가구 세정 다목적 청소티슈</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://naver.me/FLedRplq</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250912_132/1757642106885ShHmG_JPEG/40241676691363361_1403346838.jpg</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>정전기 먼지 방지 티슈</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>정전기로 인한 먼지 걱정 끝! 유리부터 가구까지 깨끗하게 닦아주는 다목적 청소티슈입니다.</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>폴리보이 더스트스탑 티슈 3팩 정전기 먼지 방지 청소 추천</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>정전기 발생 없이 유리, 가구 등 다양한 표면의 먼지를 효과적으로 제거하는 다목적 청소티슈입니다.</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>폴리보이,더스트스탑,청소티슈,정전기방지,먼지제거,유리세정,가구청소,다목적티슈</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>샤프란아우라드라이 건조기시트지40매 건조기정전기 종이섬유유연제</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://naver.me/IFG7r5bx</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221008_139/1665185538143D3z07_JPEG/66321436851106191_989421741.jpg</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>정전기 완화 건조기시트</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>건조기 사용 시 정전기로 불편했던 옷들이 산뜻하고 부드럽게 변해요. 종이섬유 유연제로 쉽고 깔끔한 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>샤프란아우라드라이 건조기시트지 40매 정전기 방지 추천</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>샤프란아우라드라이 건조기시트지는 건조기 사용 시 옷의 정전기를 줄여 산뜻하고 부드럽게 관리해줍니다.</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>샤프란아우라드라이,건조기시트지,정전기방지,종이섬유유연제,의류관리,섬유유연제</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>디부스 섬유향수 섬유탈취제 룸스프레이 100ml 드레스퍼퓸 은은한 발향 확실한 탈취</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://naver.me/5kxWto6g</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251102_252/1762042299251ec72r_PNG/112726781272483736_456122528.png</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>은은한 향의 섬유탈취제</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>옷과 공간의 불쾌한 냄새 걱정 끝! 은은하게 퍼지는 향기로 상쾌함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>디부스 섬유향수 100ml 은은한 발향 섬유탈취제 추천</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>옷과 공간의 불쾌한 냄새를 확실히 탈취하고 은은한 향기로 상쾌함을 더해줍니다. 섬유용 룸스프레이로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>디부스,섬유향수,섬유탈취제,룸스프레이,드레스퍼퓸,탈취,은은한향,발향,옷냄새제거,공간탈취</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>생활/섬유</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>[1+1] 생활살균연구소 건조기시트 드라이시트 40매 시트형 섬유유연제 개별포장 건조시트</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://naver.me/5qcXvEuD</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230809_134/1691540378801lQ1rD_JPEG/6466066909268907_1508108061.jpg</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>건조기용 섬유유연 시트</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>건조기 사용 시 옷감 손상을 막고 은은한 향기로 산뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>[1+1] 생활살균연구소 건조기시트 40매 할인 구매 추천</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>옷감 손상 방지와 은은한 향기를 동시에 제공하는 건조기용 드라이시트, 산뜻한 세탁 완성을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>건조기시트,섬유유연제,드라이시트,건조기용품,옷감보호,향기유지,생활살균</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>생활/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>휴고스 미니 컴팩트 PTC 전기온풍기 소형 히터 캠핑 사무실 발난로</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://naver.me/xbjdAyGm</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250926_101/17588598135561I8SR_JPEG/92992735688983672_1838852221.jpg</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>미니 컴팩트 전기온풍기</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>작고 강력한 발난로로 캠핑과 사무실 어디서든 따뜻함을 누려보세요.</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>휴고스 미니 컴팩트 PTC 전기온풍기 소형 히터 추천</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>캠핑과 사무실에서 간편하게 사용할 수 있는 소형 전기온풍기로 강력한 발열 효과를 제공합니다. 휴대가 용이해 따뜻한 환경을 유지하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>휴고스,미니전기온풍기,소형히터,캠핑히터,사무실난로,발난로,컴팩트온풍기,PTC히터</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>히터/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>쿠오레 가정용 욕실 화장실 무타공 온풍기 미니 PTC 세라믹 벽걸이 CH-B20W</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQivlvk9</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251010_184/1760059711022nEzNw_JPEG/73948568830118888_840016024.jpeg</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>무타공 벽걸이 온풍기</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>작은 공간도 따뜻하게, 무타공 설치로 간편한 욕실 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>쿠오레 욕실 무타공 온풍기 CH-B20W 추천 구매</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>작은 욕실 공간에도 간편하게 설치 가능한 쿠오레 PTC 세라믹 무타공 온풍기입니다. 빠른 온열로 쾌적한 욕실 환경을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>쿠오레,욕실온풍기,무타공온풍기,PTC세라믹,벽걸이온풍기,미니온풍기,욕실필수템</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>욕실/가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>TOB-7200 미니온풍기 캠핑히터 소형 PTC난로 사무실용</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://naver.me/5L7ZvZZN</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241202_70/1733122808748vbSXv_JPEG/26545841558217460_2192638.jpg</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>소형 미니 PTC 온풍기</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>작고 강력한 미니 온풍기로 캠핑과 사무실 따뜻하게! 추위 걱정 끝.</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>TOB-7200 미니온풍기 캠핑히터 소형 PTC난로 추천</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>작고 강력한 TOB-7200 미니온풍기로 캠핑과 사무실에서 간편하게 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>TOB-7200,미니온풍기,캠핑히터,PTC난로,소형히터,사무실난방,휴대용히터</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>가전,캠핑용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>보아르 모노라운드 AI 자동온도조절 회전 미니 전기 온풍기 세라믹PTC 탁상용 소형 원룸</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://naver.me/5EnFUVLa</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_250/176101138713378rfx_JPEG/46855726101281466_607494156.jpg</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>자동온도 조절 미니 온풍기</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>작고 강력한 온풍기로 쾌적한 온도 유지, 원룸 겨울 난방 걱정을 덜어드립니다.</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>보아르 모노라운드 AI 자동 온도조절 미니 전기 온풍기 추천</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>작고 강력한 세라믹 PTC 온풍기로 원룸 겨울 난방에 적합하며 탁상용으로 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>보아르,모노라운드,AI 자동온도조절,전기 온풍기,미니 온풍기,세라믹 PTC,원룸 난방,소형 온풍기,탁상용 전기히터</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>가전,생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>한일 온풍기 가정용 미니온풍기 욕실 캠핑 ptc히터 화장실 101</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://naver.me/5TQGodCV</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241227_224/1735264497349MGdRK_JPEG/69397345137799142_1209129089.jpg</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>가정용 미니 온풍기</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>추운 겨울, 집안 곳곳을 따뜻하게 데워줄 소형 온풍기입니다. 욕실부터 캠핑까지 다양하게 활용해보세요.</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>한일 미니온풍기 가정용 캠핑용 PTC히터 추천</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>한일 온풍기 101은 욕실, 캠핑 등 다양한 공간에서 효율적으로 사용 가능한 소형 히터입니다. 겨울철 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>한일온풍기,미니온풍기,가정용히터,캠핑히터,욕실온풍기,PTC히터,소형히터</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>가전/난방기기</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>가정용 욕실온풍기 화장실 온풍기 벽걸이 PTC히터 난방기 미니</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://naver.me/xoQhHcos</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251031_110/1761871422847GxtEP_JPEG/96004238904642610_1849221746.jpg</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>벽걸이 욕실용 온풍기</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>추운 욕실에서 빠르게 따뜻함을 느껴보세요. 공간 절약형 벽걸이 디자인으로 편리합니다.</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>가정용 욕실온풍기 벽걸이 PTC히터 난방기 추천</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>작고 효율적인 벽걸이형 욕실 온풍기로 추운 공간을 빠르게 따뜻하게 해주는 미니 난방기입니다.</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>욕실온풍기,벽걸이난방기,PTC히터,미니온풍기,욕실난방기,가정용온풍기</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>욕실,난방기</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>캐로스 PTC 미니 전기 온풍기 캠핑용 탁상용 사무실 원룸 욕실 난로 휴대용 난방기</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://naver.me/x6xdzdO9</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231122_205/17006442735358UVI2_JPEG/27471538730268592_407255665.jpg</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>미니 전기 온풍기</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>작고 강력한 온풍기로 캠핑부터 사무실까지 따뜻함을 간편하게 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>캐로스 PTC 미니 전기 온풍기 캠핑 및 사무실 추천</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>작고 강력한 캐로스 PTC 미니 전기 온풍기로 캠핑, 사무실, 원룸 등 다양한 공간에서 간편하게 따뜻함을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>캐로스,PTC 전기 온풍기,미니 온풍기,캠핑 난로,사무실 난로,휴대용 난방기,탁상용 난방기,원룸 난방기</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>가전,난방기</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>TOB-3600 미니온풍기 캠핑히터 소형 PTC난로 사무실용</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://naver.me/FZ8pBpmY</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241213_271/17340729588974CSfE_JPEG/68205810008144267_847727751.jpg</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>작고 강력한 미니온풍기</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>작은 공간도 빠르게 따뜻하게! 캠핑이나 사무실에서 간편하게 사용할 수 있어요.</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>TOB-3600 미니온풍기 캠핑히터 소형 PTC난로 추천</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>작은 공간을 빠르게 난방하는 TOB-3600 미니온풍기 캠핑히터로 캠핑과 사무실 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>미니온풍기,캠핑히터,소형난로,PTC난로,사무실난방,캠핑난방,휴대용히터</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>난방/캠핑</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>한양 발따숨 발난로 풋워머 전기히터 난방기 온열기 온풍기 책상 미니 사무실 가정용 캠핑용</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://naver.me/FDGOnUen</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251023_30/17611863220449PIKt_JPEG/4817768874306344_1252633182.jpg</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>포근한 발난로 풋워머</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>차가운 발을 따뜻하게 감싸주는 전기 히터로 겨울철 사무실과 캠핑에 꼭 필요한 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>한양 발따숨 풋워머 전기히터 추천 겨울 캠핑용 온열기</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>차가운 발을 따뜻하게 감싸주는 한양 발따숨 풋워머로 사무실, 가정, 캠핑 시 편안한 온기를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>한양,발따숨,풋워머,전기히터,발난로,온열기,온풍기,사무실난방,캠핑용난로,미니히터</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>가전,난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>가정용 미니 온풍기 소형 히터 휴대용 욕실 온풍기 화장실 1등급</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://naver.me/IGZ5JnUH</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251201_19/1764579727733KQzPz_JPEG/3205252973815909_1193997662.jpg</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>소형 미니 욕실 온풍기</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>작고 강력한 온풍기로 추운 욕실도 따뜻하게! 휴대도 간편해 어디서나 사용 가능해요.</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>가정용 미니 온풍기 소형 히터 휴대용 욕실용 추천</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>작고 강력한 1등급 미니 온풍기로 추운 욕실 공간을 빠르게 따뜻하게 해줍니다. 휴대가 간편해 다양한 장소에서 사용하기 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>미니 온풍기,소형 히터,휴대용 온풍기,욕실 히터,1등급 전기히터,가정용 온풍기,화장실 히터</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>가전/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>디큐브 PTC 미니 탁상용 온풍기 사무실 난방기 소형 손히터 실내</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://naver.me/FJIDbJkx</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251104_292/1762226206882p6ln7_JPEG/96359042005279985_1074419712.jpg</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>미니 탁상용 온풍기</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>작고 강력한 온기로 사무실과 실내를 따뜻하게, 겨울철 손이 시린 고민을 해결해 드립니다.</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>디큐브 PTC 미니 탁상용 온풍기 사무실 난방기 추천</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>작고 강력한 온기로 사무실과 실내 공간을 따뜻하게 유지하는 소형 탁상용 온풍기입니다. 겨울철 손 시림 걱정 없이 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>디큐브, PTC 온풍기, 탁상용 난방기, 소형 온풍기, 사무실 난방기, 손히터, 실내 난방, 겨울 난방기</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>가전,난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>사무실 가정용난방기 미니 PTC 전기온풍기</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://naver.me/5pqWuWWw</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231025_108/1698202063400zRvPf_JPEG/2835304278113756_1620964874.jpg</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>작고 강력한 미니 전기온풍기</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>작은 공간도 빠르게 따뜻하게! 사무실과 가정 어디서나 쉽고 안전한 난방 솔루션입니다.</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>사무실 가정용 미니 PTC 전기온풍기 추천</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>작고 강력한 PTC 전기온풍기로 사무실과 가정에서 빠르게 따뜻함을 제공합니다. 안전하고 간편한 난방 솔루션입니다.</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>전기온풍기,사무실난방기,가정용온풍기,PTC히터,미니난방기,안전난방기,소형온풍기</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>툴콘 팬히터 미니 온풍기 캠핑 전기 PTC 히터 MF-3050</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://naver.me/5lfjajQS</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240108_246/1704724022690ygBjI_PNG/105859802328367597_1623935834.png</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>미니 캠핑 온풍기</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>작고 강력한 온풍기로 캠핑장에서도 따뜻함을 유지하세요. 추운 날씨 걱정 없이 쾌적한 시간을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>툴콘 팬히터 미니 온풍기 캠핑 전기 PTC 히터 MF-3050 추천</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>작고 강력한 툴콘 미니 팬히터로 캠핑 시 따뜻한 온기를 유지하세요. 추운 날씨에도 쾌적한 환경을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>툴콘, 팬히터, 미니 온풍기, 캠핑 히터, 전기 히터, PTC 히터, MF-3050, 휴대용 온풍기</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>캠핑/히터</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>한경희 온풍기 가정용 PTC 히터 사무실 전기 캠핑 미니 소형 거실 저전력 업소용</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://naver.me/FaOjJ66D</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_254/1761007498496dnsh6_JPEG/15970512795213284_1634109809.jpg</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>저전력 미니 온풍기</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>작고 강력한 온기로 사무실과 캠핑도 따뜻하게, 전기 요금 걱정 없이 쾌적한 겨울을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>한경희 온풍기 PTC 히터 미니 소형 가정용 추천</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>작고 강력한 PTC 온풍기로 가정, 사무실, 캠핑에 적합하며 저전력으로 경제적인 난방 솔루션을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>한경희,온풍기,PTC히터,미니히터,가정용난방,사무실히터,소형전기히터,캠핑히터,저전력히터</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>가전/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>르젠 감성 동파방지 무타공 1초발열 절전형 순간발열 PTC 욕실용히터 온풍기 LZH-B770D</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://naver.me/5eZBUv8s</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251126_137/1764118554399jnJnU_JPEG/25455801497886398_1776636856.jpg</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>빠른 동파방지 욕실히터</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>추운 욕실도 순식간에 따뜻하게, 동파 걱정 없이 쾌적한 공간을 만들어드립니다.</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>르젠 감성 동파방지 무타공 욕실용히터 LZH-B770D 추천</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>추운 욕실을 빠르게 따뜻하게 해주는 절전형 PTC 온풍기로 동파 걱정 없이 쾌적한 공간 조성에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>르젠,욕실히터,동파방지,무타공,순간발열,절전형,PTC온풍기,욕실온풍기</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>욕실가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PTC 가열 3초 욕실 화장실 난방기 사무실 가정 강력한 난방 온풍기</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://naver.me/FgT9s9ah</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251105_282/17623332771174bz2l_JPEG/86594501515085315_16038143.jpg</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>초고속 욕실 온풍기</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>춥고 습한 욕실을 3초 만에 따뜻하게! 빠른 난방으로 쾌적한 공간을 만들어 드려요.</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>PTC 가열 3초 욕실 난방기 강력 온풍기 추천</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>3초 만에 빠르게 난방하여 욕실과 사무실을 따뜻하게 만드는 PTC 가열 온풍기입니다. 겨울철 쾌적한 공간 조성에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>PTC 난방기,욕실 난방기,온풍기,사무실 난방기,가정용 온풍기,빠른 난방,강력 온풍기,3초 난방</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>가전/난방용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>[2세대] 루민 무선 미니 청소기 에어건 핸디 소형 진공 머리카락 원룸 저렴한</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://naver.me/xCtUB0ym</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230912_86/1694496757540QUxuB_JPEG/7751985366111485_1481667594.jpg</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>소형 무선 미니 청소기</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>원룸 생활의 작은 고민, 무선 미니 청소기로 간편하게 해결하세요. 머리카락부터 먼지까지 깔끔하게 청소됩니다.</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>[2세대] 루민 무선 미니 청소기 추천 - 소형 핸디 진공청소기 할인</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>원룸 생활에 최적화된 무선 미니 청소기로 머리카락과 먼지를 손쉽게 제거할 수 있는 소형 진공기입니다.</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>무선청소기,미니청소기,핸디청소기,소형진공기,원룸청소,루민청소기,에어건,머리카락제거</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>블랙앤데커 코끼리코 핸디 스틱 그라인더 청소기 TPD1420BK</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://naver.me/58jUNQXN</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221005_210/1664956365440B88Pv_JPEG/66092193269045779_909170808.jpg</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>핸디 스틱 청소기</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>좁은 공간도 깨끗하게! 가벼워 편리한 스틱 청소기로 집안 구석구석 먼지를 쉽게 제거하세요.</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>블랙앤데커 코끼리코 핸디 스틱 그라인더 청소기 추천</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>가벼운 무게와 강력한 흡입력으로 좁은 공간의 먼지까지 꼼꼼하게 청소할 수 있는 스틱 청소기입니다.</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>블랙앤데커, 스틱청소기, 핸디청소기, 무선청소기, 청소기추천, 코끼리코청소기, 가벼운청소기</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>자일렉 BLDC 고출력 미니청소기 소형 핸디 청소기 원룸 차량용 4in1 올인원</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://naver.me/FvQwEfOv</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250218_243/1739841488947dpj8H_PNG/73974332091220034_1339792375.png</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>고출력 소형 핸디 청소기</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>작고 강력한 미니청소기로 원룸과 차량도 깨끗하게! 간편한 올인원 청소 솔루션을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>자일렉 BLDC 고출력 미니청소기 원룸 차량용 추천</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>작고 강력한 BLDC 미니청소기로 원룸과 차량 청소에 적합한 4in1 올인원 핸디 청소기입니다.</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>미니청소기,핸디청소기,원룸청소기,차량용청소기,자일렉청소기,BLDC모터,소형청소기,고출력청소기,올인원청소기</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>보만 4in1 차량 가정용 핸디형 가벼운 미니 무선 청소기 VC7210PL</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://naver.me/GmtObR4y</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241125_80/1732522154340KA090_JPEG/13134125435106616_24684644.jpg</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>가벼운 무선 핸디 청소기</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>차량과 가정 모두 깔끔하게! 가벼운 무선 청소기로 손쉽게 먼지를 제거해 보세요.</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>보만 4in1 차량 가정용 핸디형 무선 청소기 VC7210PL 추천</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>가볍고 무선인 보만 VC7210PL 청소기로 차량과 가정에서 손쉽게 먼지 제거가 가능합니다. 휴대가 간편해 다양한 공간에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>보만,무선청소기,핸디형청소기,차량청소기,가정용청소기,미니청소기,가벼운청소기</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2025년형 아이룸 무선청소기 OG-20 PLUS</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://naver.me/FHVHlKGr</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251112_282/1762915819395aVIp3_JPEG/9677362383449819_1060615033.jpg</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>강력 무선 청소기</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>집안 구석구석 먼지 걱정 끝! 강력한 흡입력으로 깨끗한 공간을 만드세요.</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>2025년형 아이룸 무선청소기 OG-20 PLUS 추천 청소기</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>강력한 흡입력으로 집안 구석까지 깨끗하게 청소하는 2025년형 아이룸 OG-20 PLUS 무선청소기입니다.</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>아이룸,무선청소기,OG-20 PLUS,2025년형,청소기,강력흡입,집안청소</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>슬라운드 인네이처 핀포인트 부드러운 고밀도 순면 모달 사계절 겨울 차렵 이불 SS</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEi3M8Od</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_208/175799509030656Y8Q_JPEG/52109313228365997_126477467.jpg</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>부드러운 고밀도 순면 이불</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>포근한 겨울밤을 위한 부드럽고 고밀도 순면 모달 이불로 사계절 내내 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>슬라운드 인네이처 핀포인트 부드러운 순면 모달 이불 SS 추천</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>고밀도 순면 모달 소재로 사계절 사용 가능한 슬라운드 인네이처 차렵 이불로 포근한 겨울밤을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>슬라운드,인네이처,핀포인트,고밀도,순면,모달,사계절,차렵이불,겨울이불,부드러운</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>슬라운드 인네이처 호라이즌 고밀도 순면 사계절 겨울 차렵 이불 SS</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbLpF9N</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_252/1757994877006AM1yl_JPEG/12652225893820308_1698887882.jpg</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>고밀도 순면 겨울 차렵이불</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>차가운 겨울밤에도 포근한 온기를 선사하는 고밀도 순면 이불로 편안한 잠자리를 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>슬라운드 인네이처 호라이즌 고밀도 순면 사계절 이불 추천</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>고밀도 순면 소재로 사계절 사용 가능한 슬라운드 인네이처 호라이즌 이불은 겨울철에도 포근하고 편안한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>순면 이불, 사계절 이불, 겨울 이불, 고밀도 이불, 슬라운드, 차렵 이불, 침구</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>오가닉 순면 줄누비 여름이불 겸 패드 워싱피그먼트 스프레드 5색상</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://naver.me/GcKyHmOI</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210910_166/163124253864689f3O_JPEG/32378437318720780_1435251976.jpg</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>여름용 순면 줄누비 이불패드</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>더운 여름에도 시원하고 쾌적한 잠자리를 원한다면, 오가닉 순면 줄누비 이불패드가 답입니다.</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>오가닉 순면 줄누비 여름이불 겸 패드 추천 시원한 잠자리</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>오가닉 순면으로 만든 줄누비 여름이불 겸 패드로 시원하고 쾌적한 여름 잠자리를 제공합니다. 다섯 가지 색상으로 다양한 선택이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>오가닉 순면,여름이불,줄누비 이불,패드,워싱피그먼트,여름 침구,시원한 이불,쾌적한 잠자리</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>침구/여름이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>솔리드 에어워싱 시어서커 순면 프릴 시원한 차렵 침구 여름 이불 SS</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://naver.me/GBvBeREq</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230510_18/16837094446781FSnv_JPEG/751925091355024_598702691.JPG</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>시원한 프릴 순면 차렵이불</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>여름 밤의 무더위, 시원한 순면 시어서커 차렵이불로 쾌적하게 보내세요. 부드러운 프릴 디자인이 포근함을 더해줍니다.</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>솔리드 에어워싱 시어서커 순면 프릴 차렵 침구 SS 추천</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>여름 무더위에도 시원한 시어서커 순면 차렵 이불로 쾌적한 숙면을 도와줍니다. 프릴 디자인이 부드러운 감성을 더합니다.</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>시어서커 이불, 순면 차렵이불, 여름침구, 프릴 침구, 시원한 여름이불, 솔리드 이불, 에어워싱 침구</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>침구/여름</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>순면 고밀도 60수 워싱 먼지없는 이불 빈티지 사계절 호텔 차렵이불</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://naver.me/GA8AIKpy</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_28/1761297031185wXJn3_JPEG/8058574132902256_812954801.jpg</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>고밀도 순면 사계절 이불</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>먼지 걱정 없는 고밀도 순면으로 사계절 내내 쾌적하고 포근한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>순면 고밀도 60수 워싱 이불 사계절용 먼지없는 추천</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>고밀도 순면 60수 원단으로 제작되어 먼지 걱정 없이 사계절 쾌적한 숙면을 도와주는 차렵이불입니다.</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>순면이불,고밀도이불,워싱이불,사계절이불,먼지없는이불,차렵이불,호텔이불,포근한이불,빈티지이불</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>침구류/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>구름 호텔식침구 봄 가을 겨울이불 라지킹 순면차렵이불</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://naver.me/GT6HDFoI</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210209_247/1612851300616fVXp6_JPEG/13987143316315094_1801057338.jpg</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>순면 호텔식 대형 침구</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>봄부터 겨울까지 쾌적하게, 구름처럼 부드러운 순면 침구로 편안한 잠자리를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>구름 호텔식침구 라지킹 순면차렵이불 봄가을겨울 추천</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>구름처럼 부드러운 순면 소재로 봄부터 겨울까지 쾌적한 잠자리를 제공하는 라지킹 침구입니다. 다양한 계절 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>호텔식침구,순면이불,라지킹이불,봄이불,가을이불,겨울이불,차렵이불,부드러운침구,계절이불</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>오가닉 순면 누빔 매트리스커버 피그먼트 몽제 침대커버 기본 S</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://naver.me/F5aYBEUy</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230913_106/1694595919454hh5BQ_JPEG/1943649633606211_1211085774.jpg</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>오가닉 순면 누빔 매트리스커버</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심, 부드러운 순면 누빔으로 쾌적한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>오가닉 순면 누빔 매트리스커버 피그먼트 몽제 S 추천</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없는 부드러운 순면 누빔 매트리스 커버로 쾌적한 숙면 환경을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>오가닉,순면,매트리스커버,누빔,피그먼트,몽제,침대커버,민감피부,쾌적한잠자리,S사이즈</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>침구/매트리스</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>드로잉데이지 60수 아사 순면 부드러운 알러지케어 사계절 꽃 이불 차렵이불 SS</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://naver.me/5sGYVOZm</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240905_102/1725514233002048Gp_JPEG/5646655849153914_1239178399.jpg</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>부드러운 알러지케어 차렵이불</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심! 60수 아사 순면으로 사계절 쾌적하게 사용하세요.</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>드로잉데이지 60수 아사 순면 사계절 차렵이불 SS 추천</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심할 수 있는 60수 아사 순면 소재로 사계절 쾌적하게 사용할 수 있는 부드러운 알러지케어 차렵이불입니다.</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>차렵이불,순면이불,알러지케어,사계절이불,60수아사,부드러운이불,민감피부이불,꽃무늬이불,침구</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>모달 순면 피그먼트 침대고정패드 SS 데이라인 화이트</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://naver.me/FMTyDWe0</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240430_136/1714463131069Nwr4c_JPEG/115599029779804127_584000935.jpg</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>순면 침대 고정패드 SS</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>침대 매트리스를 깔끔하게 보호하며, 모달 순면 소재로 부드럽고 편안한 잠자리를 완성합니다.</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>모달 순면 피그먼트 침대고정패드 SS 데이라인 화이트 추천</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>모달 순면 소재로 부드럽고 편안하며, 침대 매트리스를 깔끔하게 보호하는 침대고정패드입니다.</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>모달 순면,침대고정패드,피그먼트,매트리스 보호,침실용,데이라인,화이트,SS사이즈</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>모제무드 오가닉 순면 무형광 피그먼트 광목 차렵이불 스퀘어 XS</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://naver.me/GzimLpvM</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230117_46/1673947550549BPGD4_JPEG/1250234417820745_730898238.jpg</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>순면 무형광 광목 차렵이불</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심, 무형광 천연 순면으로 쾌적한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>모제무드 오가닉 순면 무형광 피그먼트 광목 차렵이불 XS 추천</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심할 수 있는 무형광 천연 순면 소재의 차렵이불로 쾌적한 잠자리를 제공합니다. 스퀘어 XS 사이즈로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>모제무드, 오가닉 순면, 무형광 이불, 피그먼트 광목, 차렵이불, 민감피부, 쾌적한 잠자리, 스퀘어 XS</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>고밀도 60수 순면패드 고정밴드 알러지케어 밴드형 순면 침대패드 SS</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://naver.me/5owH7PG3</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250814_254/1755170801704EYGJ5_PNG/17720886776347289_915532796.png</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>알러지케어 순면 침대패드</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심, 고밀도 순면으로 쾌적한 잠자리를 만들어 드려요.</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>고밀도 60수 순면패드 알러지케어 SS 추천</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>민감한 피부에 적합한 고밀도 60수 순면패드로 쾌적하고 건강한 잠자리를 제공합니다. 알러지 케어 기능 포함하여 안심 사용이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>순면패드,고밀도,알러지케어,침대패드,순면,고정밴드,SS사이즈,민감피부</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>침구/패드</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>레오나 알러지케어 순면 모달100 안감 극세사 겨울 차렵이불</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://naver.me/Giam7Por</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231109_233/1699490151283bSjk2_JPEG/901308147676003_1016478622.jpg</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>알러지 케어 극세사 차렵이불</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심! 부드러운 극세사와 순면 모달로 편안한 겨울 숙면을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>레오나 알러지케어 순면 모달 극세사 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 부드러운 극세사와 순면 모달 안감의 겨울용 차렵이불로 따뜻하고 편안한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>레오나, 알러지케어, 순면 모달, 극세사 이불, 겨울 차렵이불, 민감 피부, 따뜻한 이불, 숙면용 이불</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>침구/겨울이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>순면 침대패드 고정밴드 매트리스패드 사계절 패드ss 차콜</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://naver.me/5gYGnEZQ</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250520_118/1747730232962zOWUf_JPEG/59023343976195288_1169140559.jpg</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>순면 사계절 침대패드 고정밴드</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>꿈 같은 착용감으로 매트리스를 깔끔하게 고정하세요. 사계절 내내 쾌적한 잠자리를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>순면 침대패드 고정밴드 SS 차콜 사계절 매트리스패드 추천</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>순면 소재로 사계절 쾌적한 잠자리를 제공하며, 고정밴드로 매트리스를 깔끔하게 고정해 사용 편리성을 높였습니다.</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>순면 침대패드,매트리스패드,고정밴드,사계절 패드,차콜 색상,침대 용품,잠자리 쾌적,매트리스 보호</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>침구류</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>리틀홈즈 극세사 알러지케어 이불 먼지없는 사계절 차렵이불 슈퍼싱글</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://naver.me/xNne53P1</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251119_120/17635290619387l0Gd_JPEG/97661947341788366_2104797548.jpg</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>극세사 알러지케어 차렵이불</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심, 먼지없는 알러지케어 이불로 사계절 쾌적한 잠자리를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>리틀홈즈 극세사 알러지케어 사계절 차렵이불 슈퍼싱글 추천</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>민감한 피부에 적합한 리틀홈즈 알러지케어 이불로 먼지 걱정 없이 사계절 내내 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>리틀홈즈,극세사이불,알러지케어,사계절이불,차렵이불,슈퍼싱글,먼지없는이불</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>겨울 극세사 차렵 이불 두꺼운 순면 간절기 모엘 양털 / 레드오렌지, SS(슈퍼싱글)</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://naver.me/Giam7P4d</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251126_118/1764084072258qsICX_JPEG/98216933390319302_1801939407.jpg</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>포근한 겨울 극세사 이불</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>차가운 겨울밤도 따뜻하게 감싸주는 두꺼운 극세사 이불로 포근한 숙면을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>겨울 극세사 차렵 이불 두꺼운 순면 모엘 양털 SS 추천</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>두꺼운 극세사와 순면 소재로 제작된 겨울용 차렵 이불로 따뜻한 숙면을 도와줍니다. 슈퍼싱글 사이즈, 레드오렌지 색상으로 공간을 포근하게 연출합니다.</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>겨울이불,극세사이불,차렵이불,두꺼운이불,순면이불,모엘양털,간절기이불,슈퍼싱글이불,레드오렌지</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>슈크림 리버시블 극세사 겨울 차렵이불 SS</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://naver.me/GRuwn7TO</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250123_139/1737609485505tS9hb_JPEG/71742319589317703_1477621541.jpg</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>포근한 극세사 겨울 차렵이불</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻함을 유지하고 싶은 당신을 위한 슈크림 극세사 이불로 포근하게 감싸보세요.</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>슈크림 리버시블 극세사 겨울 차렵이불 SS 추천 보온</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하게 유지되는 슈크림 리버시블 극세사 차렵이불로 포근한 수면 환경을 제공합니다. 부드럽고 가벼워 아이부터 어른까지 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>슈크림,리버시블,극세사,겨울이불,차렵이불,SS,보온,부드러운,포근한</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>침구/겨울</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>구름 프릴 극세사이불 알러지케어 겨울이불</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://naver.me/FjCRGLWR</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20191219_70/1576723570164TFjCr_JPEG/14083404705701201_136165078.jpg</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>극세사 알러지케어 겨울이불</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 포근한 겨울밤을 보내세요. 부드러운 극세사로 따뜻함을 더했습니다.</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>구름 프릴 극세사이불 알러지케어 겨울이불 추천</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 부드러운 극세사로 따뜻한 겨울밤을 선사하는 구름 프릴 극세사이불입니다.</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>극세사이불,알러지케어,겨울이불,포근한이불,부드러운이불,따뜻한이불</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>침구/겨울이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>[에이트룸]두꺼운 프리미엄 라셀 10미리 겨울 극세사 이불 SS</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://naver.me/GQST7sUx</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_117/1729730875700XO6Vm_JPEG/4292809809694254_738112778.jpg</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>두꺼운 겨울 극세사 이불 SS</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 포근하고 따뜻하게 감싸주는 두꺼운 프리미엄 극세사 이불로 편안한 잠자리를 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>[에이트룸]두꺼운 프리미엄 라셀 10미리 극세사 이불 SS 추천</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>두꺼운 10미리 라셀 극세사 이불로 겨울철 포근하고 따뜻한 잠자리를 완성하세요. SS 사이즈로 가벼우면서도 따뜻합니다.</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>에이트룸,극세사이불,겨울이불,프리미엄이불,라셀이불,두꺼운이불,포근한이불,따뜻한이불,SS이불</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>나라데코 프리미엄 라셀 10mm 극세사 두꺼운 겨울 이불 SS</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://naver.me/5eZBlExH</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251017_64/1760667443556tHjV6_JPEG/15630457844667724_1835896413.jpg</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>두꺼운 겨울용 극세사 이불</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>찬 바람에도 포근하게 감싸주는 두께감으로 겨울 추위를 걱정 없이 보내세요.</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>나라데코 프리미엄 라셀 10mm 극세사 이불 SS 겨울용 추천</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>10mm 두꺼운 극세사로 찬 겨울철에도 포근하게 감싸주는 나라데코 프리미엄 라셀 SS 이불입니다. 겨울철 따뜻함을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>나라데코,프리미엄이불,극세사이불,겨울이불,두꺼운이불,SS사이즈,포근한이불,라셀이불</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>침구/겨울이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>모달 극세사 양면 차렵침구 [샤네르] 그레이 S Q K</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://naver.me/xF20EJM1</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250115_248/1736930718659t5Ts9_JPEG/5836482478815944_2016286452.jpg</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>포근한 극세사 양면 차렵침구</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>차가운 밤에도 포근하게 감싸주는 극세사 침구로 편안한 잠자리를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>모달 극세사 양면 차렵침구 샤네르 그레이 S Q K 추천</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>포근하고 부드러운 모달 극세사 양면 차렵침구로 쾌적한 숙면을 도와주는 제품입니다. S, Q, K 사이즈로 다양한 침대에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>모달,극세사,차렵침구,양면침구,포근한침구,샤네르,그레이,침실용,숙면</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>모닝 알러지케어 양면 모달100%+5mm극세사 차렵이불 단품</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://naver.me/xnrIplwe</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251030_17/1761798600202eu1cj_PNG/95931502335176377_229563500.png</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>알러지케어 극세사 차렵이불</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심! 모달 100%와 5mm 극세사로 알러지 걱정 없이 포근한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>모닝 알러지케어 양면 모달100%+5mm극세사 차렵이불 단품 추천</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>민감한 피부에 적합한 모달 100%와 5mm 극세사로 알러지 걱정 없는 포근하고 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>모달이불,알러지케어,극세사이불,차렵이불,민감피부침구,포근한이불,단품이불</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>침구류/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>오넬로이 이불 알러지케어 먼지없는 옥수수솜 고밀도 극세사 차렵이불 헬렌 단품S</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>https://naver.me/xrC3nB3A</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240705_281/1720160469669MhltI_JPEG/27472072485622616_123521233.jpg</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>알러지 케어 고밀도 차렵이불</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심, 먼지 없는 옥수수솜으로 쾌적한 잠자리를 만들어 드립니다.</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>오넬로이 먼지없는 옥수수솜 차렵이불 헬렌 단품S 추천</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심할 수 있는 고밀도 극세사와 알러지케어 옥수수솜으로 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>오넬로이,차렵이불,알러지케어,옥수수솜,극세사,고밀도,먼지없는,단품S,헬렌,침구</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>마운트뷰 5kg지탱 아이패드 거치대 갤럭시탭 침대 책상 태블릿 거치대 암 스탠드 휴대용</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://naver.me/xfYB8Uz2</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251028_218/1761635573332TPhUc_JPEG/22972820427662292_1735986674.jpg</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>안정적인 태블릿 거치대</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>침대나 책상 어디서든 태블릿을 편리하게 지탱해 편안한 사용감을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>마운트뷰 5kg지탱 아이패드 거치대 추천 – 갤럭시탭 태블릿 스탠드</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>침대와 책상 어디서나 아이패드와 갤럭시탭을 편안하게 거치할 수 있는 5kg 지탱 태블릿 스탠드로 안정적인 사용이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>아이패드거치대,갤럭시탭거치대,태블릿스탠드,휴대용거치대,책상거치대,침대거치대,태블릿암스탠드</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>가전,액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>태블릿 거치대 회전 아이패드 거치대 스탠드 갤럭시탭</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://naver.me/FIN4yFyl</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240802_290/1722584085893a5tfd_JPEG/72153580499058306_1569605756.jpg</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>360도 회전 태블릿 스탠드</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>편리한 각도 조절로 장시간 사용해도 편안한 태블릿 거치대를 만나보세요.</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>태블릿 거치대 회전 아이패드 거치대 추천</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>편리한 각도 조절로 장시간 사용에도 편안한 태블릿 거치대입니다. 아이패드와 갤럭시탭 등 다양한 기기에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>태블릿거치대, 아이패드거치대, 갤럭시탭거치대, 회전스탠드, 태블릿스탠드, 각도조절, 휴대용거치대</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>모바일/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>[헬로아이즈 베이비] [2매입 / 30개]  아이 전용 눈에쓰는 아이패드 민감성 눈가케어 눈꺼풀세정제</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://naver.me/xpBedcvL</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220810_256/16600969994904yxox_JPEG/61232842192818482_374559131.jpg</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>민감 눈가 케어 세정제</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>아기 눈가 민감함에 걱정되시나요? 부드럽게 깨끗이 케어해주세요.</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>헬로아이즈 베이비 아이 전용 눈가케어 2매입 30개 추천</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>민감한 아기 눈가를 부드럽게 세정해주는 헬로아이즈 베이비 눈꺼풀 세정제입니다. 안전한 성분으로 아기 눈 건강 케어에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>아기눈세정제,아이눈가케어,민감성눈,눈꺼풀세정제,베이비아이패드,어린이눈관리</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>베이비/눈케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>[4세대초고속충전 내장형] 태블릿거치대 아이패드거치대 침대 갤럭시탭 패드</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://naver.me/FytdEgUe</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240528_297/1716828371876lhd1d_JPEG/44131055719890088_1611120325.jpg</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>초고속 내장형 태블릿거치대</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>침대나 책상에서 편하게 태블릿을 사용하세요. 빠른 충전으로 스마트한 휴식을 지원합니다.</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>[4세대초고속충전] 태블릿 아이패드 거치대 추천, 편리한 사용</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>침대와 책상에서 편하게 태블릿을 거치하고 4세대 초고속 충전으로 스마트한 휴식을 지원하는 아이패드 및 갤럭시탭 거치대입니다.</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>태블릿거치대,아이패드거치대,갤럭시탭거치대,초고속충전,침대거치대,패드거치대,스마트폰충전,편리한사용</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>가전/태블릿악세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>아이폰 정품 충전기 애플 어댑터 아이패드 애플워치 충전기 20W C타입 아이폰17 프로 용</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://naver.me/IFG7XRX2</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241209_220/1733729439112rpTSv_JPEG/67862205549994262_265236565.jpg</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>아이폰 20W 고속 충전기</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>느린 충전 불편함 이제 그만! 아이폰17 프로에 딱 맞는 고속 충전기로 빠르고 안정적인 충전을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>아이폰17 프로 정품 20W C타입 고속 충전기 추천</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>아이폰17 프로에 최적화된 20W C타입 충전기로 빠르고 안정적인 고속 충전을 지원합니다. 애플 기기 사용자에게 적합한 충전 솔루션입니다.</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>아이폰충전기,애플어댑터,아이폰17프로충전기,고속충전,20W충전기,C타입충전기,아이패드충전기,애플워치충전기</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>모바일/충전기</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>링크로 아이패드 키보드 케이스 매직키보드 구조독 호환 한국어 블랙, 아이패드 프로 27.9cm(11인치) 2세대</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://naver.me/5AgSX7ZT</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251125_243/1764053339175K5tia_PNG/98186200264269890_268568663.png</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>아이패드 완벽 키보드 케이스</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>아이패드 작업 효율을 높여주는 매직키보드 호환 케이스로 편리한 타이핑 환경을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>링크로 아이패드 키보드 케이스 매직키보드 호환 추천</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>아이패드 프로 11인치 2세대에 적합한 매직키보드 호환 키보드 케이스로 편리한 타이핑과 작업 효율을 높여줍니다.</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>아이패드키보드, 매직키보드호환, 키보드케이스, 아이패드프로11인치, 작업효율, 블랙키보드케이스, 한국어자판</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>키보드케이스/아이패드액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>아이패드 애플펜슬 호환 스타일러스 태블릿 터치펜 짭플펜슬</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://naver.me/5wNMVojW</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250609_65/1749430377164HAoI3_JPEG/3968340776911262_864412302.jpg</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>정밀 터치 아이패드펜</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>아이패드 터치감이 아쉽다면 이 스타일러스펜으로 자연스러운 필기와 드로잉을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>아이패드 애플펜슬 호환 스타일러스펜 추천 자연스러운 필기감</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>아이패드용 호환 스타일러스펜으로 부드러운 터치감과 정확한 드로잉을 제공합니다. 자연스러운 필기 경험을 원하는 사용자에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>아이패드펜, 스타일러스펜, 애플펜슬호환, 터치펜, 태블릿펜, 드로잉펜, 필기용펜</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>모바일액세서리/스타일러스</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>벨킨 30W USB C타입 PD 3.1 PPS 초소형 고속 충전기 WCA008kr 갤럭시 S25 아이폰 아이패드 호환</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://naver.me/GbAPIJXI</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241115_212/1731664362965DqSWb_JPEG/23008229280465252_885609012.jpg</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>초소형 30W 고속 충전기</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>빠른 충전이 필요할 때, 벨킨 초소형 고속 충전기로 간편하게 스마트 기기를 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>벨킨 30W USB C타입 PD 3.1 PPS 고속 충전기 추천</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>벨킨의 초소형 30W USB C PD 3.1 PPS 충전기로 갤럭시 S25, 아이폰, 아이패드 등 다양한 스마트 기기를 빠르게 충전할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>벨킨,30W,USB C,PD 3.1,PPS,고속 충전기,갤럭시 S25,아이폰,아이패드,초소형</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>충전기/모바일</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>니케 아이패드 마그네틱 거치대 태블릿 자석 아이패드 프로 12.9 Magsnap Basic</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://naver.me/xKtiXdX6</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240715_103/1721007004895r2xND_JPEG/28307891772250064_1409646026.jpg</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>아이패드 자석 거치대</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>아이패드를 안정적으로 고정해 편리함을 더하세요. 깔끔한 마그네틱 디자인으로 공간 활용까지 완벽합니다.</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>니케 아이패드 마그네틱 거치대 프로 12.9 추천</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>아이패드 프로 12.9를 안정적으로 고정하는 마그네틱 거치대로 편리하고 깔끔한 공간 활용이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>아이패드 거치대, 마그네틱 거치대, 태블릿 거치대, 아이패드 프로, 12.9인치, 자석 거치대, 니케, Magsnap Basic</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>가전/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>애플 아이패드 6세대 태블릿 태블릿PC Wi-Fi 32G 실버</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://naver.me/ID3ZDWIv</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250722_146/1753149727575zsFTb_JPEG/16394499398033248_1106340227.jpg</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>고성능 6세대 태블릿</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>빠른 Wi-Fi 연결과 넉넉한 저장 공간으로 학습과 엔터테인먼트 모두 완벽하게 즐기세요.</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>애플 아이패드 6세대 Wi-Fi 32G 태블릿PC 추천</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>신속한 Wi-Fi 연결과 32GB 저장 공간으로 학습과 엔터테인먼트에 적합한 애플 아이패드 6세대 태블릿입니다.</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>아이패드, 애플 태블릿, 6세대, Wi-Fi 태블릿, 32GB 저장, 학습용 태블릿, 엔터테인먼트, 실버</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>태블릿/IT</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>알파플랜 휴대용 태블릿 거치대 접이식 패드 스탠드 ATH01 실버, 아이패드 갤럭시탭</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://naver.me/5gYGnEIB</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241113_87/1731480215521SNrb9_JPEG/37319514330793189_1686103487.jpg</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>휴대용 태블릿 스탠드</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>어디서나 편하게 태블릿을 사용하고 싶다면 접이식 휴대용 스탠드가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>알파플랜 휴대용 태블릿 거치대 ATH01 접이식 스탠드 추천</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>간편한 접이식 디자인으로 아이패드, 갤럭시탭 등 다양한 태블릿에 잘 맞는 휴대용 스탠드입니다. 어디서나 편리하게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>알파플랜, 태블릿거치대, 휴대용스탠드, 접이식스탠드, 아이패드거치대, 갤럭시탭스탠드, 태블릿액세서리</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>가전/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>usb led 북 라이트 램프 조명 미니 휴대용 독서등 전등 자석 바 30cm</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://naver.me/FeNWscHG</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230419_94/1681884503040QTrDJ_JPEG/3201840042424628_516535581.jpg</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>휴대용 USB LED 독서등</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>어두운 환경에서도 편안한 독서를 원하세요? 작고 가벼운 USB LED 독서등으로 언제 어디서나 밝게 빛나세요.</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>USB LED 북 라이트 30cm 미니 독서등 추천</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>휴대하기 좋은 USB LED 북 라이트로 어두운 곳에서도 편안한 독서를 즐기세요. 작고 가벼워 이동 시 사용하기 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>USB LED 북 라이트, 미니 독서등, 휴대용 조명, 자석 독서등, 30cm LED 램프</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>조명/독서</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>[ALLDOCUBE] 올도큐브 iPlay60 mini LTE 태블릿 글로벌버전 4+64GB</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://naver.me/FlcvrUNT</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250616_62/1750074869252QYx4S_JPEG/5283040351640274_1480884964.jpg</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>휴대용 LTE 태블릿</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>언제 어디서나 끊김 없는 인터넷! 올도큐브 iPlay60 mini LTE로 스마트한 일상을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>ALLDOCUBE 올도큐브 iPlay60 mini LTE 4+64GB 태블릿 추천</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>글로벌 버전 올도큐브 iPlay60 mini LTE 태블릿으로 언제 어디서나 끊김 없는 인터넷과 스마트한 일상을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>ALLDOCUBE,올도큐브,iPlay60 mini,LTE,태블릿,글로벌버전,4GB RAM,64GB 저장용량,스마트 태블릿</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>태블릿/모바일</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>아이프라브 기내용 캐리어 여행용 미니 기내반입 승무원 튼튼한 경량 솔리도 48cm(20인치)</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1mYmvJK</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250102_294/173579257732373olX_JPEG/3269987339317163_1002742303.jpg</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>튼튼한 경량 기내용 캐리어</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>작고 가벼워 기내 반입이 편리해요. 여행 중 짐 걱정 없이 자유롭게 이동하세요.</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>아이프라브 기내용 캐리어 20인치 경량 여행용 추천</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>작고 가벼운 20인치 아이프라브 기내용 캐리어로 기내 반입이 간편하며 튼튼한 내구성으로 여행에 최적화된 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>아이프라브, 기내용 캐리어, 20인치 캐리어, 경량 캐리어, 여행용 캐리어, 미니 캐리어, 기내반입 캐리어, 튼튼한 캐리어</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>여행용품/캐리어</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>이어맥 미니 도킹형 C타입 고속충전 보조배터리 10000mAh 22.5W</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://naver.me/G1mgaR0C</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250605_82/17491116704832iLkU_JPEG/3649634084587338_866734813.jpg</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>고속충전 10000mAh 보조배터리</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>충전 걱정 없이 빠르게! 22.5W 고속충전으로 언제 어디서나 스마트 기기를 완벽하게 지원합니다.</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>이어맥 미니 도킹형 C타입 보조배터리 10000mAh 고속충전 추천</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>컴팩트한 미니 도킹형 보조배터리로 22.5W 고속충전을 지원해 스마트기기를 빠르게 충전할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>이어맥, 미니 도킹형, C타입, 고속충전, 보조배터리, 10000mAh, 휴대용 충전기, 스마트기기 충전</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>생폰 풀커버 초슬림 변색없는 PC 하드 케이스 투명, 아이폰13 미니</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://naver.me/xGFuvMMA</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250207_91/17389001708738VYcB_JPEG/152449015504096_1637978841.jpg</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>초슬림 변색없는 투명 케이스</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>폰 변색 걱정 없이 깔끔하게 보호하세요. 아이폰13 미니에 꼭 맞는 초슬림 디자인입니다.</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>아이폰13 미니 생폰 풀커버 초슬림 변색없는 케이스 추천</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>변색 걱정 없는 투명 PC 하드 케이스로 아이폰13 미니를 깔끔하게 보호하는 초슬림 디자인입니다.</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>아이폰13미니, 투명케이스, 변색없는케이스, 초슬림케이스, PC하드케이스, 폰보호케이스</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>스마트폰케이스</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>솔리드 에어건 무선 미니 초강력 송풍기 차량용 세차 캠핑 컴퓨터 청소 하이퍼건 S-A168</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://naver.me/G1mgaRZN</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251203_133/176475124896739PeF_JPEG/34042243091498135_1474572477.jpg</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>무선 미니 초강력 송풍기</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>차량, 캠핑, 컴퓨터 구석구석 먼지 걱정을 덜어주는 강력한 무선 송풍기입니다.</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>솔리드 에어건 무선 미니 송풍기 S-A168 추천</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>차량, 캠핑, 컴퓨터 청소에 적합한 무선 초강력 송풍기로 구석구석 먼지를 간편하게 제거할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>무선 송풍기, 차량 청소, 캠핑용 송풍기, 컴퓨터 청소, 미니 송풍기</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>자동차/청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>아이패드미니 6 7 태블릿 이북리더기 7인치 뮤패드K8 8인치 7세대 y700 4세대</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://naver.me/FK0YjPXg</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240429_104/1714368129334p5Agk_JPEG/63165662567918790_816637243.jpeg</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>휴대용 7~8인치 태블릿</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>작고 가벼운 태블릿으로 언제 어디서나 편리하게 독서와 작업을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>아이패드미니 6·뮤패드K8 태블릿 추천 할인 구매</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>작고 가벼운 7~8인치 태블릿으로 독서와 작업에 적합한 아이패드미니 6, 뮤패드K8, y700 4세대 태블릿을 만나보세요.</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>아이패드미니6,뮤패드K8,태블릿,이북리더기,7인치태블릿,8인치태블릿,가벼운태블릿,휴대용태블릿</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>태블릿/전자기기</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>코끼리 10000mAh 보조배터리 미니 슬림 대용량 고속 동시충전 C타입 LCD 잔량표시</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://naver.me/5sGYVODM</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251214_160/1765694096390dudJh_JPEG/2693364385595039_372171932.jpg</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>미니 슬림 대용량 보조배터리</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>언제 어디서나 부족한 배터리 걱정 끝! 슬림한 디자인에 대용량으로 빠르게 충전하세요.</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>코끼리 10000mAh 보조배터리 슬림 대용량 고속 충전 추천</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>슬림한 디자인과 대용량 10000mAh로 언제 어디서나 빠르게 충전 가능한 보조배터리입니다. LCD 잔량표시와 동시충전 지원으로 편리함을 더했습니다.</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>보조배터리, 10000mAh, 슬림 보조배터리, 고속 충전, C타입, LCD 잔량표시, 대용량 배터리, 휴대용 충전기</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>전자/액세서리</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-17 15:07)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7485,6 +7485,1756 @@
         </is>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>타이머 기능 덕분에 편리한 미니 에그 쿠커 활용기</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://naver.me/GoiIShEC</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240807_160/17229930313398cj6A_JPEG/3437894163784505_1887435591.jpg</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>간편 타이머 미니 에그쿠커</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>타이머 기능으로 완벽한 삶은 달걀 완성, 바쁜 아침에도 간편하게 건강을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>타이머 기능 미니 에그 쿠커 추천, 간편한 건강 아침 준비</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>타이머 기능으로 정확한 삶은 달걀 조리가 가능해 바쁜 아침에도 간편하고 건강하게 식사를 준비할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>미니 에그 쿠커, 타이머 기능, 삶은 달걀, 아침 조리, 간편 요리</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>주방용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>전자파 걱정 없는 순면 전기요로 따뜻한 출퇴근길</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://naver.me/5zXwFgkw</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_94/17612936816819wczP_JPEG/10963655798824589_1654747919.jpg</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>전자파 없는 순면 전기요</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길 전자파 걱정 없이 따뜻함을 느껴보세요. 순면 소재로 안심하고 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>전자파 걱정 없는 순면 전기요 추천, 따뜻한 출퇴근길 필수품</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길에도 전자파 걱정 없이 사용할 수 있는 순면 전기요로 안전하고 따뜻한 온기를 제공합니다. 피부에 자극 없이 안심 사용 가능.</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>순면 전기요,전자파 걱정 없는 전기요,출퇴근길 전기요,따뜻한 전기요,안심 전기요,전기요 추천</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>생활용품/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>핸디 타입 무선청소기, 원룸 생활에 딱 맞아요</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://naver.me/FOZGnzzF</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251014_194/1760426785807aD6yQ_JPEG/15389800108980484_977986873.jpg</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>컴팩트 무선 청소기</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>원룸 청소가 번거롭다면 가볍고 효율적인 무선 청소기로 손쉽게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>핸디 타입 무선청소기 원룸 생활 추천 가볍고 효율적인 청소기</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>원룸 청소에 적합한 가볍고 효율적인 핸디 타입 무선청소기로 손쉬운 청소를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>무선청소기,핸디청소기,원룸청소,가벼운청소기,효율적청소</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>가전,청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기로 집에서도 손쉬운 헤어 관리</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://naver.me/5asn2WWK</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250908_225/1757299713109uaQek_JPEG/72189419974616713_1624091115.jpg</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>전문가급 헤어 드라이기</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>집에서도 쉽게 전문가 손질같은 완벽한 스타일을 완성해보세요.</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기 집에서도 손쉬운 헤어 관리 추천</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>집에서 전문가 수준의 헤어 스타일을 간편하게 완성할 수 있는 드라이기입니다. 다양한 모드로 맞춤형 스타일링 가능해 누구나 쉽게 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기,헤어 드라이기,헤어 스타일링,집에서 손질,헤어 관리,간편 스타일링</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>뷰티,헤어</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>진동클렌저로 모공 속 피지를 깨끗하게 제거해요</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://naver.me/5xaSEcc2</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250909_257/1757404766913PtOm0_JPEG/91537561911410856_252064605.jpg</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>모공 속 피지 진동클렌저</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>끈적이는 피지와 모공 고민, 진동클렌저로 깨끗하게 해결하세요. 맑고 촉촉한 피부를 경험할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>진동클렌저로 모공 속 피지 깨끗하게 제거 추천</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>진동클렌저로 끈적이는 피지와 모공 고민을 깨끗하게 해결해 맑고 촉촉한 피부를 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>진동클렌저,모공관리,피지제거,클렌징,촉촉한피부</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>뷰티/스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>오픈형 무선 이어폰으로 운동할 때도 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://naver.me/xNnJHfXc</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250909_101/1757398735157HS66s_JPEG/12983763141442581_725538606.jpg</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>운동용 오픈형 무선 이어폰</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>운동 중 이어폰 불편함으로 스트레스 받나요? 가벼운 착용감으로 자유로운 운동을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>운동용 오픈형 무선 이어폰 추천 가벼운 착용감</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>가벼운 착용감과 오픈형 디자인으로 운동 시 편안함을 제공합니다. 자유로운 움직임을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>오픈형 이어폰,무선 이어폰,운동 이어폰,가벼운 착용감,편안한 이어폰,스포츠 이어폰</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>운동/이어폰</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>가정용 한경희 온풍기로 쾌적한 거실 휴식시간 보내기</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://naver.me/FaOjJ66D</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_254/1761007498496dnsh6_JPEG/15970512795213284_1634109809.jpg</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>쾌적한 거실 온풍기</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻한 거실 만들기, 온풍기로 편안한 휴식시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>가정용 한경희 온풍기 추천 쾌적한 거실 휴식용</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>한경희 가정용 온풍기로 추운 날씨에도 따뜻하고 쾌적한 거실 환경을 만들어 편안한 휴식을 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>한경희,온풍기,가정용,거실난방,쾌적한휴식,난방기,겨울가전</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>업소용 보플제거기로 세탁소 업무가 훨씬 편해졌어요</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://naver.me/GuDIv1cF</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251104_8/17622387332964InOy_JPEG/80542040246152147_1111200455.jpg</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>효율적인 보풀 제거기</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>보풀 걱정으로 스트레스 받나요? 강력한 업소용 보풀제거기로 깔끔한 세탁을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>업소용 보풀제거기 추천, 세탁 업무 편리하게 해결</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>강력한 업소용 보풀제거기로 보풀 걱정을 줄이고 세탁소 업무 효율을 높여보세요. 깔끔한 세탁 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>업소용 보풀제거기, 세탁소, 보풀 제거, 세탁 업무, 깔끔한 세탁</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>세탁/업소용</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>유리 바스켓 적용한 자일렉 에어프라이어 사용 후기</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://naver.me/xmBFYZZD</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241023_47/17296726911493Kemw_JPEG/63805540692189067_363561276.jpg</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>유리 바스켓 에어프라이어</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>기름 튀김 걱정 없이 건강하게 요리하세요. 깔끔한 유리 바스켓으로 사용 후기도 만족스럽습니다.</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>자일렉 에어프라이어 유리 바스켓 추천 사용 후기</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>기름 튀김 걱정 없이 건강한 요리가 가능한 자일렉 에어프라이어, 깔끔한 유리 바스켓으로 손쉬운 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>자일렉,에어프라이어,유리바스켓,건강요리,기름튀김없음,간편세척,사용후기</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>주방가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>통화품질이 뛰어난 노이즈캔슬링 이어폰 추천</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://naver.me/xGFpUhhn</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250314_292/1741928217371ISvfp_JPEG/21601617717735680_1089888875.jpg</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>고음질 노이즈캔슬링 이어폰</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>통화 중 잡음에 불편함을 느끼나요? 선명한 음질로 통화 품질을 높여드립니다.</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>통화품질 뛰어난 노이즈캔슬링 이어폰 추천, 깨끗한 통화 지원</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>잡음 없는 선명한 음질로 통화 품질을 개선하는 노이즈캔슬링 이어폰입니다. 전화 통화가 많은 분들께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>노이즈캔슬링,이어폰,통화품질,선명한음질,무선이어폰,통화용이어폰</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>이어폰/통화</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>UV 살균 기능으로 더 깨끗하게 사용하는 가습기</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://naver.me/5eZazQnC</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241127_57/1732696869552Gk6Dp_JPEG/80530609348265639_334682759.jpg</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>UV 살균 청정 가습기</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>공기 중 세균 걱정 없이 깨끗한 가습 효과로 건강한 실내 환경을 만들어 드립니다.</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>UV 살균 기능 가습기 추천 - 깨끗한 실내 공기 보장</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>UV 살균 가습기로 세균 걱정 없이 건강한 실내 습도 유지에 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>UV 가습기,살균 가습기,깨끗한 가습기,실내 공기 정화,건강 가습기</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>가전/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>세척충전스테이션으로 편리한 면도기 관리법</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://naver.me/GvfamyQs</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_129/1761008594736w1MKX_JPEG/2821988536529357_1099031453.jpg</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>편리한 면도기 세척 관리</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>면도기 청소가 번거로우신가요? 세척충전스테이션으로 깨끗하고 간편한 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>세척충전스테이션 면도기 관리 추천, 깨끗하고 간편한 사용법</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>세척충전스테이션으로 면도기 청소를 쉽고 간편하게! 깨끗한 면도기 관리로 쾌적한 사용이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>면도기, 세척충전스테이션, 면도기 청소, 간편 관리, 충전스테이션, 위생 면도기, 전기 면도기</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>갤럭시와 잘 맞는 삼성 C타입 이어폰으로 통화 품질 향상</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://naver.me/IM4oFTHO</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251121_17/1763705179898fAyPu_JPEG/36305044011059490_1675749816.jpg</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>고음질 C타입 이어폰</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>통화 음질 걱정 끝! 갤럭시에 최적화된 선명한 사운드로 더 깨끗하게 대화하세요.</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>갤럭시 최적화 삼성 C타입 이어폰 통화품질 향상 추천</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>갤럭시에 최적화된 삼성 C타입 이어폰으로 선명한 통화 음질을 경험하세요. 깨끗한 대화에 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>삼성, C타입 이어폰, 갤럭시, 통화품질, 선명한 사운드, 통화 이어폰</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>이어폰/스마트폰</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>갤럭시와 찰떡궁합, 삼성 유선 이어폰 통화 품질 분석</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://naver.me/FOZGnz7b</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251121_296/1763705295822b5R1Q_JPEG/97838273029276458_63080566.jpg</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>선명한 통화 이어폰</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>통화 품질 걱정 끝! 삼성과 찰떡궁합으로 선명한 음질을 경험해 보세요.</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>갤럭시와 찰떡궁합 삼성 유선 이어폰 통화 품질 추천</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>삼성 갤럭시와 완벽 호환되는 유선 이어폰으로 선명한 통화 품질을 제공합니다. 통화 걱정 없이 안정적인 음질 경험에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>삼성 이어폰,갤럭시 이어폰,유선 이어폰,통화 품질,선명한 음질,스마트폰 액세서리</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>이어폰/통화</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>매일 사용하는 음식물 분쇄기의 효율적인 관리 팁</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://naver.me/xZjaOG6x</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250915_136/1757903299681pyzSt_JPEG/92036119800923973_115446622.jpg</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>음식물 분쇄기 관리법</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>분쇄기 냄새와 막힘 걱정 끝! 쉽고 효과적인 관리로 매일 깨끗하게 사용하세요.</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>음식물 분쇄기 효율적 관리 팁 추천</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>분쇄기 냄새와 막힘 걱정 없이 쉽고 효과적으로 관리하는 방법을 소개합니다. 매일 깨끗하게 음식물 분쇄기를 사용하세요.</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>음식물분쇄기,분쇄기관리,냄새제거,막힘해결,주방청소,효율적관리,분쇄기청소팁</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>주방가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>자동 먼지비움 기능으로 손쉬운 청소 유지법</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://naver.me/FSSdholg</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250602_291/1748845630464MuNgs_JPEG/14774569327017779_696507649.jpg</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>자동 먼지비움 청소편리</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>먼지 걱정 없이 자동 청소로 깔끔한 공간을 유지하세요. 청소 스트레스가 확 줄어듭니다.</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>자동 먼지비움 기능 청소기 추천으로 손쉬운 청소 유지</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>자동 먼지비움 기능으로 별도의 청소 걱정 없이 깔끔한 공간을 쉽게 유지할 수 있는 청소기입니다.</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>자동 먼지비움, 청소기, 손쉬운 청소, 자동 청소, 먼지 제거, 깔끔한 공간</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>가전,청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>게이밍 마이크 탑재한 삼성 이어폰으로 실시간 통화도 문제없어요</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Ag5IHHl</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241007_2/1728291647685oJN7z_JPEG/7867011550772335_1134175854.jpg</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>게이밍 마이크 내장 이어폰</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>실시간 통화 음질 걱정 끝, 게이밍 마이크로 선명한 대화 경험을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>게이밍 마이크 탑재 삼성 이어폰 실시간 통화 추천</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>삼성 이어폰에 내장된 게이밍 마이크로 선명한 실시간 통화가 가능하며, 게임과 통화 모두에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>삼성 이어폰, 게이밍 마이크, 실시간 통화, 선명한 음질, 게임용 이어폰</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>이어폰/음향</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>휘핑기로 완성하는 부드러운 머랭 만들기 팁</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://naver.me/FTM7kqt8</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240626_204/1719388630466HOqrL_JPEG/13326978595111809_552915840.jpg</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>부드러운 머랭 완성법</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>휘핑이 어려운 분들을 위한 부드럽고 완벽한 머랭 만들기 비법을 알려드립니다.</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>휘핑기로 완성하는 부드러운 머랭 만들기 팁 추천</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>휘핑이 어려운 분들을 위해 부드럽고 완벽한 머랭 만드는 방법을 쉽고 자세히 안내합니다. 홈베이킹에 적합한 팁입니다.</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>휘핑기,머랭 만들기,부드러운 머랭,편리한 휘핑,홈베이킹 팁</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>베이킹/팁</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>소닉케어 칫솔모와 함께 건강한 플라그 제거 방법 소개</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://naver.me/5W9NBHdG</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_251/1729729172042XJGxa_JPEG/80079447986312376_865681665.jpg</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>효과적인 플라그 제거 칫솔모</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>플라그 걱정 끝! 전문 칫솔모로 깨끗한 구강 건강을 지켜보세요.</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>소닉케어 칫솔모 추천 플라그 제거로 건강한 구강 관리</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>소닉케어 칫솔모로 플라그를 효율적으로 제거해 구강 건강을 유지하세요. 전문 칫솔모로 매일 깨끗한 입안을 경험할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>소닉케어, 칫솔모, 플라그 제거, 구강 건강, 치아 관리, 전동칫솔모, 구강 위생</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>구강관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편리한 전문가용 드라이기의 성능</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://naver.me/GA8o6BaL</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250908_169/1757299716989mDdif_JPEG/91432514122095419_248458711.jpg</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>출퇴근용 전문가 드라이기</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 빠르고 완벽한 스타일링을 원한다면 이 전문가용 드라이기가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>출퇴근길 전문가용 드라이기 추천 빠른 스타일링</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 빠르고 완벽한 헤어 스타일을 도와주는 전문가용 드라이기입니다. 휴대가 간편하고 강력한 성능을 자랑합니다.</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기,출퇴근 드라이기,빠른 스타일링,휴대용 드라이기,헤어드라이기,헤어 스타일링</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>뷰티/헤어</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>운동 후 위생을 지키는 유토렉스 칫솔소독기 경험기</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://naver.me/xv6Ablw3</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220603_278/1654242393068KaSP4_JPEG/100367_1.jpg</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 소독</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 위생 걱정 없이 깨끗하게 관리하세요. 유토렉스가 세균 걱정을 싹 해결해 드립니다.</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>유토렉스 칫솔소독기 운동 후 위생 관리 추천</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔을 깨끗하게 소독해 세균 걱정을 줄여주는 유토렉스 칫솔소독기입니다. 위생적인 칫솔 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>유토렉스,칫솔소독기,운동후,위생관리,세균제거,칫솔청결,구강위생</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>위생/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>벽걸이 난방기 설치로 화장실 공간 활용도가 높아졌어요</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQiXMG1Y</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251010_8/17600522426622O3Ko_JPEG/45896581643329479_1789907410.jpg</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>공간 절약 벽걸이 난방기</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>좁은 화장실도 따뜻하게! 벽걸이 난방기로 공간을 효율적으로 활용하세요.</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>벽걸이 난방기 추천 화장실 공간 활용도 높이는 난방기</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>좁은 화장실 공간에도 적합한 벽걸이 난방기로 따뜻하고 효율적인 공간 활용을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>벽걸이 난방기, 화장실 난방, 공간 절약 난방기, 화장실 온열기, 난방기 설치</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>가전,난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>핸디형이라 구석구석 청소하기 좋은 제트클린 청소기</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://naver.me/xBMOVFL0</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250722_44/1753166690459tuWWz_JPEG/10792431535091475_322105301.jpg</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>구석구석 핸디 청소기</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>좁은 틈새도 완벽 청소! 가벼운 핸디형으로 집안 구석구석 깔끔하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>핸디형 제트클린 청소기 추천 - 구석구석 완벽 청소</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>가벼운 핸디형 제트클린 청소기로 좁은 틈새와 구석구석을 손쉽게 청소하세요. 효율적인 집안 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>핸디형 청소기, 제트클린, 구석구석 청소, 좁은 틈새 청소, 가벼운 청소기, 집안 청소, 휴대용 청소기</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>가전/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>30분 타이머 기능으로 바쁜 출퇴근 시간에도 딱 좋은 계란찜기</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://naver.me/x0Xu5xVy</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250103_212/1735867649427NkgGm_JPEG/3345059427219219_981906763.jpg</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>빠른 계란찜 타이머</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>30분 타이머로 바쁜 아침에도 간편하게 맛있는 계란찜을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>30분 타이머 계란찜기 추천 바쁜 아침 간편 조리</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>30분 타이머 기능으로 바쁜 아침에도 손쉽게 맛있는 계란찜을 완성할 수 있는 주방용품입니다. 간편하고 빠른 조리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>계란찜기,30분 타이머,간편 조리,아침 식사,주방용품,빠른 조리</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>주방/조리도구</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 신경 쓰이는 공기, 엘지 필터 교체법</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://naver.me/GnRL3fYk</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251126_146/1764146601329s6TLs_JPEG/98279486731776721_430917020.jpg</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>깨끗한 출퇴근 공기</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>출퇴근길 미세먼지 고민, 간편한 필터 교체로 신선한 공기를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>출퇴근길 미세먼지 걱정, 엘지 필터 교체법 추천</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>출퇴근길 미세먼지 걱정을 덜어주는 엘지 공기청정기 필터 간편 교체법으로 항상 신선한 공기 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>엘지, 필터교체, 공기청정기, 미세먼지, 출퇴근, 공기관리, 간편교체</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>광파오븐 기능 덕분에 다양한 요리를 간편하게 즐겨요</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://naver.me/GwSBZlnv</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250613_109/1749776542952XhLzh_PNG/25969217060873863_778861537.png</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>광파오븐으로 간편요리</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>광파오븐으로 다양한 요리를 빠르고 쉽게 완성하세요. 시간과 노력은 줄이고 맛은 그대로 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>광파오븐 추천 다양한 요리 간편하게 완성하기</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>광파오븐으로 빠르고 쉽게 다양한 요리를 완성할 수 있어 바쁜 주방에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>광파오븐, 오븐, 간편 요리, 주방가전, 빠른 조리</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>소형 믹서기로 집에서 신선한 이유식 만들기</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://naver.me/FivQmpRx</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250721_294/1753071024274nhjnm_JPEG/85888288164255087_1766249390.jpg</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>신선한 이유식 믹서기</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>아이 먹거리 걱정 끝! 집에서 간편하게 신선한 이유식을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>소형 믹서기로 신선한 이유식 쉽게 만들기 추천</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>집에서 간편하게 신선한 이유식을 만들 수 있는 소형 믹서기입니다. 아이 먹거리 걱정 없이 안심하고 사용하세요.</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>소형믹서기,이유식만들기,신선이유식,아기식품,가정용믹서기,간편조리</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>가전,육아</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 든든한 한경희 EMF 전자파 차단 매트</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://naver.me/Ig4XKxdo</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250926_85/1758865300828Jo6p2_PNG/92998286853013450_986561594.png</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>전자파 차단 매트</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>출퇴근길 전자파 걱정 없이 편안함을 느껴보세요. 안전한 환경으로 건강을 지켜드립니다.</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>한경희 EMF 전자파 차단 매트 출퇴근길 사용 추천</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>출퇴근길 전자파 걱정 없이 편안함을 제공하는 한경희 EMF 전자파 차단 매트로 건강을 지켜보세요.</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>한경희,전자파차단,EMF,출퇴근,건강매트,전자파매트,안전매트,전자기장차단</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>건강/전자파</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기 유닉스로 집에서도 미용실 퀄리티 완성</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://naver.me/5EnD91gg</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210114_197/1610590677722Uxibj_GIF/11726505515146192_1001555163.gif</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>프로급 전문가용 드라이기</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>집에서도 미용실 퀄리티 드라이! 전문가용 드라이기로 완벽한 스타일을 손쉽게 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기 유닉스 추천 집에서도 미용실 퀄리티 완성</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기로 집에서도 미용실처럼 깔끔하고 완벽한 헤어 스타일을 손쉽게 완성하세요. 강력한 바람과 열 조절 기능으로 다양한 모발에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>전문가용 드라이기,유닉스 드라이기,미용실 드라이기,헤어 스타일링,열 조절,강력 바람,홈뷰티,헤어드라이기 추천</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>뷰티/헤어</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편한 1인용 미니 탄소매트</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gq9Ky0F6</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250925_114/1758790386549g7scf_JPEG/92923277644308481_127228875.jpg</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>간편 1인용 미니 탄소매트</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 끝! 작고 가벼운 미니 탄소매트로 따뜻하게 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>출퇴근길 1인용 미니 탄소매트 추천 - 간편하고 따뜻한 보온</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>작고 가벼운 1인용 미니 탄소매트로 출퇴근길 추위 걱정을 해결하세요. 간편하게 휴대하며 따뜻함을 유지할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>미니 탄소매트, 1인용, 출퇴근 보온, 휴대용 전기매트, 간편 보온제품</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>겨울용품/보온</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>SkinIQ 5000 전기면도기로 출퇴근 시간 절약하기</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://naver.me/xKt3WzaZ</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250519_220/1747620963208lhAzd_JPEG/335275296955581_177994795.jpg</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>빠른 출퇴근 전기면도기</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>바쁜 아침, 빠르고 깔끔한 면도로 출퇴근 시간을 아껴보세요. 간편한 사용감이 매일의 고민을 덜어줍니다.</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>SkinIQ 5000 전기면도기 빠른 출퇴근 시간 절약 추천</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>SkinIQ 5000 전기면도기는 빠르고 깔끔한 면도로 바쁜 아침 출퇴근 시간을 효율적으로 절약해 줍니다. 매일 손쉬운 사용이 가능해 남성에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>SkinIQ 5000,전기면도기,빠른면도,출퇴근시간절약,남성면도기,간편사용</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>전자제품/뷰티</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>통세척 기능으로 간편한 무선 미니 가습기 관리법</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://naver.me/GNRNx0Dr</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250912_16/17576628467019zJLj_JPEG/30509653938332270_1915257772.jpg</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>간편 통세척 무선 미니가습기</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>번거로운 가습기 관리, 통세척 기능으로 손쉽게 해결하세요. 깨끗한 공기, 건강한 공간을 만들어 드립니다.</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>무선 미니 가습기 통세척 기능으로 간편한 관리 추천</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>번거로운 가습기 청소를 통세척 기능으로 간편하게 해결해 깨끗하고 건강한 실내 공기를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>무선 가습기, 미니 가습기, 통세척, 간편 청소, 건강한 공기, 실내 가습</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에서 편안히 쉴 때 탄소매트의 장점</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://naver.me/GUmXBPeK</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251017_141/1760685911672nIYxq_JPEG/43592577268620098_1266794736.jpg</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>출퇴근 후 탄소매트 휴식</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후 집에서 편안한 휴식을 원한다면 탄소매트가 최적입니다. 따뜻함과 편안함을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식용 탄소매트 추천</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후 집에서 따뜻하고 편안하게 쉴 수 있는 탄소매트로 최적의 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>탄소매트,출퇴근,휴식,따뜻함,편안함,집에서,온열매트</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>생활/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>한일 분쇄기로 신선한 재료를 빠르게 준비하는 법</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://naver.me/FDG8Faf5</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250729_210/1753762941591YKnGr_JPEG/71089873122816051_983044129.jpg</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>신선 재료 빠른 분쇄</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>시간 부족에 지친 당신을 위한 효율적인 분쇄기로 신선함을 한층 높여보세요.</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>한일 분쇄기 추천 신선한 재료 빠른 준비법</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>한일 분쇄기로 신선한 재료를 빠르고 효율적으로 준비하세요. 바쁜 일상 속 시간 절약과 신선함 유지에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>한일 분쇄기, 신선 재료 분쇄, 주방 가전, 빠른 요리 준비, 효율적인 분쇄기</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>주방/가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 손쉬운 자동건조 가습기 추천</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://naver.me/GlG0alE9</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251123_37/1763894038444Lruib_JPEG/26358189530507976_416506867.jpg</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>자동건조 가습기로 쾌적한 출퇴근</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>출퇴근길 습도 걱정 끝! 자동건조 기능으로 항상 신선하고 쾌적한 공기를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>출퇴근길 자동건조 가습기 추천, 쾌적한 실내 습도 관리</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>자동건조 기능으로 출퇴근길 습도 걱정 없이 신선하고 쾌적한 공기를 제공하는 가습기입니다.</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>자동건조가습기,가습기추천,출퇴근용가습기,실내습도관리,쾌적한공기</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-18 17:47)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J176"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9235,6 +9235,2106 @@
         </is>
       </c>
     </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>모달 소재 차렵 이불로 사계절 편안한 잠자리</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEi3M8Od</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_208/175799509030656Y8Q_JPEG/52109313228365997_126477467.jpg</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>사계절 모달 차렵이불</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>사계절 내내 부드럽고 포근한 잠자리를 원한다면, 모달 소재 차렵이불이 최적입니다.</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>모달 소재 차렵 이불 추천 사계절 편안한 잠자리</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>모달 소재 차렵 이불은 사계절 사용 가능하며 부드럽고 포근한 잠자리를 제공합니다. 언제나 쾌적한 수면 환경을 원하시는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>모달 이불,차렵 이불,사계절 이불,부드러운 이불,포근한 이불,수면용품,침구,편안한 잠자리</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 편안한 밤을 위한 이불 선택법</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>https://naver.me/52c8uo1a</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240911_232/1726043960560guMeS_JPEG/29600834309618471_1085720924.jpg</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>알러지 걱정 걷는 편안한 이불</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>알레르기 때문에 밤마다 불편하셨나요? 알러지 걱정 없이 안심하고 사용할 수 있는 이불로 편안한 밤을 선물하세요.</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 이불 추천으로 편안한 밤 보내기</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>알레르기 걱정 없이 사용할 수 있는 안전한 이불로 편안한 잠자리를 제공합니다. 민감한 피부와 알러지 환자에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>알러지이불,편안한밤,알레르기없는이불,안심이불,민감피부이불,천연소재이불</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>침구류/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>알러지케어 기능 덕분에 민감한 피부에도 안심되는 겨울이불</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>https://naver.me/5qcXFAFt</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250910_115/1757468588009XrfE3_JPEG/91221786477578799_1593638652.jpg</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>민감피부 겨울 알러지케어 이불</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없는 알러지케어 기능으로 겨울철 포근하고 건강한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>알러지케어 기능 겨울이불 추천 - 민감 피부 안심 보온</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심할 수 있는 알러지케어 기능으로 겨울철 건강하고 포근한 잠자리를 제공합니다. 알러지 걱정을 덜어내세요.</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>알러지케어,겨울이불,민감피부,보온이불,포근한이불,건강한잠자리,알레르기방지</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>사계절 내내 쾌적하게 사용하는 슬라운드 차렵이불</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>https://naver.me/GXgb9R97</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251127_107/1764222480446B4rPl_JPEG/26688527148770218_205193700.jpg</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>사계절 쾌적 차렵이불</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>여름엔 시원하고 겨울엔 따뜻한, 사계절 내내 편안한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>사계절 내내 쾌적한 슬라운드 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>여름에는 시원하고 겨울에는 따뜻하게 사용할 수 있는 사계절용 차렵이불로 편안한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>사계절이불,차렵이불,슬라운드,여름이불,겨울이불,쾌적한이불,잠자리용품</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>침구류</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>광폭 차렵이불, 침실 공간을 넉넉하게 채워줍니다</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>https://naver.me/F5aYiF3G</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230317_167/1679044645362MRyCv_JPEG/80180425077348583_716125085.jpg</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>넉넉한 광폭 차렵이불</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>좁은 침실도 넉넉하게 감싸는 광폭 차렵이불로 편안한 잠자리를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>광폭 차렵이불 추천, 넉넉한 침실 공간 채우기</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>좁은 침실도 편안하게 감싸주는 광폭 차렵이불로 쾌적한 잠자리를 완성하세요. 공간 활용과 편안함 모두 만족합니다.</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>광폭 차렵이불, 침실이불, 넉넉한 이불, 편안한 잠자리, 침실용 이불</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>침실/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>겨울에도 포근한 알러지케어 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbL9vQM</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_142/1757995168717hCMgv_JPEG/33959842846349089_1400039922.jpg</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>알러지케어 포근 차렵이불</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>알레르기 걱정 없이 겨울 내내 따뜻하고 포근한 잠자리를 경험하세요. 건강한 숙면을 위한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>겨울 알러지케어 차렵이불 추천, 포근한 숙면 보장</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>알레르기 걱정 없이 겨울 내내 따뜻하고 포근한 차렵이불로 건강한 숙면을 누리세요. 민감한 피부에도 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>알러지케어,차렵이불,겨울이불,포근한이불,건강한숙면,민감피부,따뜻한이불</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>침구/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>가벼운 겨울 차렵이불, 출퇴근 후 빠른 정리 가능해요</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>https://naver.me/FZ8pEFpz</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_278/1729777109554SVeU8_JPEG/63910046238836952_1908061046.jpg</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>가벼운 겨울 차렵이불</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>출퇴근 후 빠른 정리로 번거로움 없이 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>가벼운 겨울 차렵이불, 빠른 정리로 따뜻함 유지 추천</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 정리 가능한 가벼운 겨울 차렵이불로 따뜻함을 유지하세요. 번거로움 없이 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>겨울이불,가벼운차렵이불,빠른정리이불,출퇴근이불,따뜻한이불</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>침구/겨울</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>사계절 내내 포근하게, 슬라운드 차렵이불 사용 후기</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>https://naver.me/xzlDYvqh</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250822_214/1755854732139IUmrd_JPEG/10553347128737707_323621417.jpg</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>사계절 포근 차렵이불</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>한여름 빼고 내내 사용 가능한 포근한 차렵이불로 쾌적한 잠자리를 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>사계절 내내 포근한 슬라운드 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>한여름을 제외한 사계절 내내 사용할 수 있는 슬라운드 차렵이불로 쾌적하고 따뜻한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>차렵이불, 사계절이불, 슬라운드차렵이불, 포근한이불, 침구류, 여름빼고, 따뜻한이불</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>침구류/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>쾌적한 잠자리를 위한 먼지 없는 알러지케어 이불 추천</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>https://naver.me/IGZ58G8l</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_222/1765257061500feGAD_JPEG/4103320608295234_79141880.jpg</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 쾌적 이불</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>알러지 때문에 잠자리가 불편한 분들을 위해 먼지 걱정 없이 편안한 숙면을 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>알러지케어 이불 추천으로 쾌적한 잠자리 할인 구매</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 먼지 제거 기능으로 편안한 숙면을 지원하는 이불, 알러지 민감한 분들에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>알러지케어 이불, 먼지 없는 이불, 알러지 이불 추천, 숙면 이불, 알러지 방지 이불</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>침구/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>사계절용 차렵이불, 출퇴근 후 휴식에 딱 맞는 선택</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fr0PXVPM</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250930_249/1759207590143C5DiP_JPEG/84407682824540725_1652315039.jpg</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>사계절용 차렵이불</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>바쁜 하루 끝, 편안한 휴식을 꿈꾸는 당신을 위한 사계절용 차렵이불입니다.</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>사계절용 차렵이불, 출퇴근 후 휴식 추천</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>바쁜 하루 끝 편안한 휴식을 위한 사계절용 차렵이불로, 사계절 내내 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>사계절이불, 차렵이불, 휴식용이불, 편안한이불, 출퇴근휴식</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>침구류</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 쁘리엘르 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>https://naver.me/GVEIFWF9</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_254/1765257460490tPrDp_JPEG/14849012182256771_1707393930.jpg</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>알러지 걱정 차렵이불</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심! 알러지 걱정 없이 포근한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 쁘리엘르 차렵이불 추천, 민감피부용</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 쁘리엘르 차렵이불로 알러지 걱정 없이 포근하고 편안한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>알러지 차렵이불, 민감피부 이불, 쁘리엘르 이불, 포근한 이불, 피부 안전 이불</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>따뜻한 극세사 차렵이불, 겨울철 숙면에 딱 좋아요</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>https://naver.me/GRuwn7TO</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250123_139/1737609485505tS9hb_JPEG/71742319589317703_1477621541.jpg</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>따뜻한 극세사 차렵이불</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 포근하게 감싸줘 숙면을 도와주는 극세사 이불입니다.</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>따뜻한 극세사 차렵이불 겨울철 숙면 추천</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>포근한 극세사 소재로 겨울철에도 따뜻하게 감싸주어 숙면을 돕는 차렵이불입니다.</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>극세사이불,차렵이불,겨울이불,숙면이불,따뜻한이불,포근한이불</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>침구/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>포근한 프리미엄 라셀 소재로 편안한 취침 시간</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>https://naver.me/GQST7sUx</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_117/1729730875700XO6Vm_JPEG/4292809809694254_738112778.jpg</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>포근한 취침 라셀 소재</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>편안함을 원하는 당신께, 부드러운 라셀 소재로 포근한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>포근한 프리미엄 라셀 소재 침구 추천, 편안한 취침 시간</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>부드러운 프리미엄 라셀 소재로 만들어져 포근하고 쾌적한 잠자리를 제공합니다. 편안함을 중시하는 분들께 적합한 침구입니다.</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>프리미엄 라셀,부드러운 침구,포근한 잠자리,편안한 취침,라셀 침구,침실용품</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>침구/취침</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>발열솜 이불이 있어 출퇴근 뒤에도 포근함 가득</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ZSHUfHC</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250123_199/1737609259416NGAA1_JPEG/71742111548610353_2127045042.jpg</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>포근한 발열 이불</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>출퇴근 후에도 따뜻함이 필요하다면 발열솜 이불로 하루의 피로를 녹여보세요.</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>발열솜 이불 추천 출퇴근 후 포근함 유지</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로를 덜어주는 발열솜 이불로 따뜻하고 포근한 휴식 시간을 즐기세요. 부드러운 소재로 편안한 보온 효과를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>발열솜 이불, 따뜻한 이불, 출퇴근 이불, 포근한 침구, 보온 이불</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>침구류</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>포근한 겨울밤, 자가발열 차렵이불로 숙면하기</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>https://naver.me/5noNdPt9</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251205_84/1764918271242C1mz4_JPEG/20127329116115111_1000961943.jpg</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>자가발열 차렵이불</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>추운 겨울 밤, 따뜻한 자가발열 이불로 포근한 숙면을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>포근한 겨울밤 자가발열 차렵이불 추천, 따뜻한 숙면</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>추운 겨울 밤에도 자가발열 차렵이불로 따뜻하고 포근한 숙면을 도와줍니다. 겨울철 보온용 이불로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>자가발열이불,차렵이불,겨울이불,숙면용이불,보온이불,포근한이불</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>침구/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식, 알러지케어 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fr0XwlQm</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251016_253/1760625306110ClalQ_PNG/6582379853053281_316157583.png</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>알러지케어 차렵이불</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>출퇴근 후에도 편안한 휴식을 원한다면, 알러지 걱정 없이 쾌적한 잠자리를 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>알러지케어 차렵이불 추천, 출퇴근 후 편안한 휴식</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 쾌적한 잠자리를 제공하는 차렵이불로 출퇴근 후 편안한 휴식을 누리세요.</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>알러지케어, 차렵이불, 편안한휴식, 출퇴근, 쾌적한잠자리, 알러지방지, 침구, 편안한이불</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>침구/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 사용할 수 있는 광목천 차렵 이불</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>https://naver.me/IGZ5UT5h</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231026_241/1698250996229Ijfxc_JPEG/6624675081102509_1550560026.jpg</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 광목 이불</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심할 수 있는 광목천 소재로 쾌적한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 광목천 차렵 이불 추천</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 광목천 소재로 쾌적한 잠자리를 제공합니다. 알러지 걱정 없이 편안한 수면을 원하시는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>광목천,차렵이불,알러지 걱정없음,민감피부,쾌적한잠자리,수면용이불,친환경이불</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>봄가을에 적합한 신혼이불, 차렵이불 선택법</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>https://naver.me/GVEIFWUQ</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240820_89/1724117020596p7nQH_PNG/5617374440941956_676684482.png</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>봄가을 신혼 차렵이불</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>봄가을 쾌적한 수면을 위한 신혼 차렵이불, 가벼우면서도 보온성을 갖춰 편안한 잠자리를 완성합니다.</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>봄가을 신혼이불 추천, 쾌적한 차렵이불 선택법 안내</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>봄가을 사용하기 좋은 가벼운 신혼 차렵이불로 쾌적하고 따뜻한 수면 환경을 만들어 드립니다. 적절한 보온성과 편안함이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>봄이불, 가을이불, 신혼이불, 차렵이불, 가벼운이불, 보온이불, 쾌적수면</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>가볍고 포근한 화이트 차렵이불, 출퇴근 후 휴식에 딱</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>https://naver.me/FBactDtZ</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251130_258/1764505001260vJDud_JPEG/97981552288066931_1605419542.jpg</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>가볍고 포근한 차렵이불</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 가벼운 이불로 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>가볍고 포근한 화이트 차렵이불 추천, 출퇴근 휴식용</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 가벼운 화이트 차렵이불로 편안한 휴식을 취해보세요.</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>차렵이불,화이트이불,가벼운이불,포근한이불,휴식이불,출퇴근용이불,편안한이불</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>무봉제 디자인 덕분에 더욱 깔끔한 침실 인테리어</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>https://naver.me/xxFs8yvL</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250604_295/1749020097542vVfUy_JPEG/3558061139718052_222822425.jpg</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>무봉제 깔끔 인테리어</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>침실을 더욱 깔끔하고 세련되게 꾸미고 싶다면 무봉제 디자인이 답입니다. 깔끔한 공간을 완성해보세요.</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>무봉제 디자인으로 깔끔한 침실 인테리어 추천</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>무봉제 디자인으로 침실을 더욱 깔끔하고 세련되게 꾸밀 수 있습니다. 깔끔한 공간 연출에 최적입니다.</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>무봉제 디자인,침실 인테리어,깔끔한 침실,세련된 인테리어,침실 꾸미기</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>인테리어,침실</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 안심할 수 있는 차렵이불</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>https://naver.me/FwjIdAEU</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240116_287/17053984983886iOue_JPEG/106534394125122912_313496207.jpg</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>알러지 걱정 차렵이불</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>알러지로 잠 못 드는 밤, 안심하고 사용할 수 있는 부드러운 차렵이불로 편안한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 부드러운 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>알러지로부터 안전한 부드러운 차렵이불로 쾌적한 잠자리를 제공합니다. 안심하고 사용할 수 있어 민감한 피부에도 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>차렵이불,알러지안심,부드러운이불,침구추천,민감피부이불</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>침구/차렵이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 편안한 극세사 차렵이불 경험</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fm3WexRX</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_97/175799185907703OMi_PNG/92124802135700834_1225614008.png</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>알러지 걱정 극세사 이불</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>알러지로 잠 못 드는 밤, 부드러운 극세사 차렵이불로 편안함을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없는 편안한 극세사 차렵이불 추천</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>알러지 걱정 없이 부드러운 극세사 소재로 만든 차렵이불로 쾌적한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>알러지차렵이불,극세사이불,부드러운담요,편안한침구,알러지걱정없음</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>어린이 겨울 차렵이불로 따뜻한 잠자리를 완성해보세요</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>https://naver.me/FSS4ZOhJ</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200706_136/1594024985631qdu4n_JPEG/31384820160166898_1243809867.jpg</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>어린이용 포근한 겨울이불</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>추운 겨울, 아이가 편안하게 잘 수 있는 따뜻한 차렵이불로 포근한 잠자리를 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>어린이 겨울 차렵이불 추천 따뜻한 잠자리 완성</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>추운 겨울 아이를 위한 부드럽고 포근한 어린이 차렵이불로 따뜻한 잠자리를 제공합니다. 편안한 수면에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>어린이차렵이불,겨울이불,따뜻한이불,아이이불,포근한이불,차렵이불</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>침구/어린이</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>운동 중에도 간편하게 사용하는 미니 손난로 추천</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>https://naver.me/GXgb9q8Q</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250707_145/1751854954885zbz5C_JPEG/65234936738071491_289386213.jpg</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>운동용 휴대용 미니 손난로</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>추운 운동 중에도 손 시림 걱정 없이 간편하게 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>운동 중 사용하기 좋은 미니 손난로 추천</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>추운 날씨 운동 시 손 시림 걱정 없이 간편하게 따뜻함을 유지할 수 있는 미니 손난로로 편리한 사용을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>미니 손난로,운동 손난로,간편 손난로,손 시림 방지,겨울 운동용,휴대용 손난로,따뜻한 손난로</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>운동/손난로</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>200</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편하게 사용하는 대용량 손난로 추천</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>https://naver.me/GZ6vws5Q</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251117_9/1763337523631LPQ03_JPEG/97470479880981327_2004125488.jpg</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>대용량 간편 손난로</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위에 손 시림 걱정 끝! 간편하게 따뜻함을 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>출퇴근길 대용량 손난로 추천, 간편 따뜻함 구매</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 없이 간편하게 사용하는 대용량 손난로로 손 시림을 방지하세요. 휴대하기 좋아 실용적입니다.</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>대용량 손난로, 출퇴근 손난로, 휴대용 손난로, 겨울 손난로, 손 시림 방지</t>
+        </is>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>출퇴근길 필수템, 대용량 캠핑용 핫팩 추천해요</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>https://naver.me/FivXYOlb</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250929_55/1759109368089XhBFU_JPEG/13712456235637845_2133307008.jpg</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>대용량 캠핑 핫팩</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길과 캠핑 시 따뜻함이 부족할 때, 든든한 대용량 핫팩으로 온기를 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>대용량 캠핑용 핫팩 추천 출퇴근길 필수템 온기 구매</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>출퇴근길과 캠핑 시 빠르고 오래가는 대용량 핫팩으로 따뜻함을 유지하세요. 휴대가 간편해 언제 어디서나 온기 충전이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>대용량 핫팩,캠핑 핫팩,출퇴근 핫팩,휴대용 핫팩,따뜻한 핫팩,장시간 핫팩</t>
+        </is>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>아웃도어/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>휴대용 손난로로 출퇴근길 찬 공기 걱정 끝</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>https://naver.me/IFG7vIep</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240904_199/1725436051315swllD_JPEG/59568845718397480_120727303.jpg</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>따뜻한 휴대용 손난로</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길 손 시리면 걱정 마세요. 간편한 휴대용 손난로가 따뜻함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>휴대용 손난로 추천 출퇴근길 찬 공기 걱정 끝</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길 손이 시릴 때 간편하게 사용하는 휴대용 손난로로 따뜻함을 유지하세요. 손쉬운 휴대와 강력한 보온 효과가 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>휴대용 손난로, 출퇴근, 손난로 추천, 따뜻한 손, 겨울 손난로, 휴대 손난로, 손 보온, 손난로 인기</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>휴대가 간편한 국산 핫팩으로 겨울철 통화도 걱정 없어</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>https://naver.me/FfB2TAKV</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241102_105/17305435473046z2dq_JPEG/57244789377628186_272484039.jpg</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>휴대용 국산 핫팩</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻함을 간편하게! 손쉽게 휴대해 언제 어디서나 포근한 온기를 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>국산 휴대용 핫팩 추천 겨울철 따뜻한 온기 유지</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>국산 핫팩으로 겨울철에도 손쉽게 휴대하며 따뜻함을 유지하세요. 언제 어디서나 편리하게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>국산핫팩,휴대용핫팩,겨울핫팩,손난로,온열제품,따뜻한핫팩</t>
+        </is>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>생활/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>대용량 손난로로 겨울 캠핑 중에도 따뜻함 유지하기</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>https://naver.me/58jUo398</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251117_67/1763337517556w5T2x_JPEG/97470290698554335_33348729.jpg</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>대용량 손난로로 따뜻함 유지</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>겨울 캠핑 중 손 시려운 걱정 끝! 대용량 손난로로 오랜 시간 따뜻함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>대용량 손난로 겨울 캠핑용 추천 따뜻함 유지</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>겨울 캠핑 중 손 시림 걱정 없이 대용량 손난로로 오랜 시간 따뜻함을 유지하세요. 활동적인 야외 활동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>대용량 손난로,겨울 캠핑,손난로 추천,야외용 손난로,따뜻한 손난로</t>
+        </is>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>캠핑/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>운동할 때 손이 시릴 때 유용한 흔드는 손난로 사용기</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>https://naver.me/5v3hg4Dg</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241129_113/1732874710871u4Uxq_PNG/14627704007522448_1159510423.png</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>운동용 간편 손난로</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>운동 중 차가운 손 때문에 고민이라면 흔드는 손난로로 따뜻함을 즉시 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>운동할 때 손 시림 해결 손난로 추천</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>운동 중 차가운 손을 따뜻하게 해주는 흔드는 손난로로 즉시 온기를 제공합니다. 야외 운동 시 활용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>운동손난로, 흔드는손난로, 손 시림, 온열용품, 겨울운동용품</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>운동/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>장시간 통화 중에도 도움 되는 군용 핫팩 활용법</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>https://naver.me/xrC3RcEw</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230915_214/1694744744893VGIXY_JPEG/qPeTy_101672_1.jpg</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>장시간 통화 핫팩 효과</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>오랜 통화로 지친 손과 귀를 따뜻하게 보호해주는 군용 핫팩으로 휴식을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>군용 핫팩 추천 장시간 통화 시 손과 귀 보호</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>오랜 통화로 지친 손과 귀를 따뜻하게 감싸주는 군용 핫팩으로 편안한 휴식을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>군용 핫팩,통화용 핫팩,손 보온,귀 보호,장시간 통화,휴대용 핫팩</t>
+        </is>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>생활용품/보온</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>운동 후 지친 발을 위한 효과적인 발바닥 찜질법</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>https://naver.me/xVGbvAJ3</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251014_240/17604268931424yQN6_PNG/1534056879279578_1372272855.png</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>운동 후 깔끔한 발 찜질</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>운동 후 피로한 발을 따뜻하게 감싸 편안함을 선사합니다. 지친 발을 위한 최적의 찜질법을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>운동 후 지친 발을 위한 효과적인 발바닥 찜질법 추천</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>운동 후 피로한 발을 따뜻하게 감싸 편안함을 제공합니다. 지친 발을 위한 최적의 찜질법으로 회복을 돕습니다.</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>발바닥 찜질,운동 후 피로,발 피로 회복,발 찜질법,발 건강,찜질 방법,피로 해소</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>건강/운동</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>출퇴근길 군용 발핫팩으로 발 시림 걱정 끝</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>https://naver.me/GIG2N81P</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241107_37/17309578911281fN6F_JPEG/11039862864888223_1714174626.jpg</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>군용 발핫팩 발 시림 완화</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>출퇴근길 발 시림 때문에 고생이신가요? 군용 발핫팩으로 따뜻하게 보호하세요.</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>출퇴근길 군용 발핫팩 추천, 발 시림 걱정 없는 따뜻함</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>출퇴근길에 발 시림을 방지해 주는 군용 발핫팩으로 따뜻하게 보호하세요. 간편하고 효율적인 보온 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>군용 발핫팩, 발 시림, 출퇴근 필수품, 보온팩, 발난로, 따뜻한 발, 겨울용 핫팩</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>겨울용품/보온</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>출퇴근길 손난로로 안성맞춤인 마이핫 보온대</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>https://naver.me/5IiAjTxX</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251204_8/1764831829118IVwwO_JPEG/40449861600698043_759671641.jpg</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>출퇴근 손난로 보온대</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길 손 시림 걱정 끝, 따뜻함을 오래 유지해줘요.</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>출퇴근손난로 마이핫 보온대 추천, 따뜻함 오래 유지</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길 손 시림 걱정을 덜어주는 마이핫 보온대로 따뜻함을 오래 유지해 줍니다. 간편하게 사용하는 핸드워머로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>손난로,출퇴근용손난로,마이핫보온대,핸드워머,손시림방지,겨울용품,보온대</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>210</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>캠핑 갈 때 꼭 챙기는 빈슨메시프 핫팩 사용 후기</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>https://naver.me/FFaJ1SVB</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240904_154/1725436084517BuLMG_JPEG/50636177212765312_2366622.jpg</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>캠핑 필수 온열 핫팩</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>찬 바람에도 든든한 온기, 캠핑 갈 때 꼭 챙기세요. 손끝까지 따뜻함이 지속돼 외출 걱정 끝!</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>빈슨메시프 핫팩 추천 캠핑 필수 아이템 따뜻한 온기</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>캠핑 시 찬 바람에도 따뜻함을 유지해 손끝까지 온기를 제공합니다. 야외 활동 시 사용하기 좋은 핫팩입니다.</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>빈슨메시프,핫팩,캠핑핫팩,야외활동,겨울용핫팩,따뜻한핫팩</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>캠핑/아웃도어</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>211</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>출퇴근길 주머니에 쏙 들어가는 파우치형 온열 핫팩</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>https://naver.me/F5aYiCuv</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250226_180/1740536657945QYqq2_PNG/88205482742050578_906395635.png</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>포켓형 온열 핫팩</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>출퇴근길 손시림 걱정 끝! 작고 간편한 파우치형 핫팩으로 따뜻함을 언제나 지켜주세요.</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>출퇴근길 파우치형 온열 핫팩 추천, 간편한 손난로 보온용</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>작고 휴대하기 편한 파우치형 온열 핫팩으로 출퇴근길 손 시림 걱정을 덜어줍니다. 언제 어디서나 따뜻함을 유지하는 실용적인 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>온열핫팩,파우치핫팩,손난로,휴대용핫팩,출퇴근핫팩,손시림해결,온열용품,따뜻한핫팩</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>보온/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>212</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>출퇴근길 손쉽게 사용하는 파스형 발 핫팩의 장점</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>https://naver.me/5UTCkrX2</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221214_275/16709941871296Ryag_JPEG/72130029840632643_1519990334.jpg</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>파스형 휴대용 발 핫팩</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>출퇴근길 발 시림 걱정 끝! 간편하게 붙여 따뜻함을 오래 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>출퇴근길 파스형 발 핫팩 추천, 간편하고 오래가는 따뜻함</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>출퇴근길 발 시림 걱정을 덜어주는 파스형 핫팩으로 간편하게 부착해 오랜 시간 따뜻함을 유지합니다.</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>파스형 핫팩,발 핫팩,출퇴근길 핫팩,손쉬운 발 난방,발 시림 방지</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>생활용품/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>213</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>곰팡이 걱정 없는 은박시트 단열재로 집안 환경 개선하기</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>https://naver.me/x7jRNB7Z</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241210_293/1733791440704O9g4J_JPEG/10278816946853881_1592604604.jpg</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>곰팡이 걱정 없는 단열 시트</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>집안 습기로 인한 곰팡이 고민, 은박시트 단열재로 간편하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>곰팡이 걱정 없는 은박시트 단열재 추천</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>집안 습기로 인한 곰팡이 걱정을 줄여 주는 은박시트 단열재로 쾌적한 환경을 만드세요. 설치가 간편해 누구나 쉽게 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>은박시트,단열재,곰팡이방지,습기제거,집안환경개선</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>단열/건축</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>214</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>운동 중 땀 식히기 좋은 열반사단열재 활용법</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ixE3pQ8</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241210_291/1733790916573hh0uD_JPEG/67923710971649565_1280005041.jpg</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>운동 중 쾌적 열차단</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>운동할 때 땀으로 불편한 순간, 열반사단열재로 시원하고 쾌적한 운동 환경을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>운동 중 땀 식히기 좋은 열반사단열재 활용법 추천</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>운동 시 땀으로 인한 불편함을 해결하는 열반사단열재 활용법으로 시원하고 쾌적한 운동 환경을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>운동, 땀 식히기, 열반사단열재, 쾌적한 운동, 운동 환경, 단열재 활용법</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>운동/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>215</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>자석형 창문단열재로 간편하게 결로 걱정 줄이기</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>https://naver.me/FwjIdSD2</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251009_167/1760003271376UYYwL_JPEG/94136110502229900_1378805760.jpg</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>간편 자석 창문단열</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>결로 때문에 창문 관리가 어려우신가요? 자석형 창문단열재로 간편하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>자석형 창문단열재로 결로 걱정 없이 간편하게 추천</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>자석형 창문단열재로 결로 문제를 쉽고 빠르게 해결하세요. 간편한 설치로 창문 단열과 관리에 효과적입니다.</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>자석형 단열재, 창문 단열, 결로 방지, 간편 설치, 창문 관리</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>단열재/창문</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>216</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>습기제거 테이프로 겨울철 창문 관리하는 법</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>https://naver.me/5noNdXKj</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241014_286/1728897382404b5RyF_JPEG/_______resize.jpg</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>겨울철 창문 습기 제거</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>겨울철 창문에 습기와 결로 고민, 간편한 습기제거 테이프로 쾌적한 실내 환경을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>습기제거 테이프로 겨울철 창문 결로 관리법 추천</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>겨울철 창문의 습기와 결로를 간편하게 제거하는 습기제거 테이프로 쾌적한 실내 환경을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>습기제거,결로제거,겨울철,창문관리,실내습기,창문결로,습기방지,테이프</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>생활/홈케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>217</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>창틀에 붙이는 결로방지 테이프로 쉽게 습기 차단</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>https://naver.me/F0AFhtCA</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241014_76/1728898652571Qs0d8_JPEG/_______resize.jpg</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>창문 결로방지 테이프</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>창틀에 쉽게 붙여 겨울철 습기와 결로 걱정을 덜어줍니다. 쾌적한 실내 환경을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>창틀 결로방지 테이프 습기 차단으로 겨울철 추천</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>창틀에 손쉽게 부착하여 겨울철 습기 및 결로를 효과적으로 방지하는 결로방지 테이프입니다. 쾌적한 실내 환경을 유지할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>결로방지,습기차단,창틀테이프,겨울철,실내환경,간편부착,홈케어</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>생활용품/홈케어</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-18 23:59)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J218"/>
+  <dimension ref="A1:J281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11335,6 +11335,3156 @@
         </is>
       </c>
     </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>218</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에 돌아오면 프리미엄 디퓨저 향기로 힐링하세요</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>https://naver.me/FvQcQgcV</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20211201_51/1638326637809V8OEo_JPEG/39462417266224864_538693973.jpg</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>집에서 누리는 프리미엄 향기</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 당신, 프리미엄 디퓨저로 집안 가득 힐링하세요. 편안한 휴식을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>프리미엄 디퓨저 추천 출퇴근 후 집에서 힐링 향기</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸과 마음에 프리미엄 디퓨저가 집안 가득 편안한 휴식을 선사합니다. 집에서 간편하게 힐링하세요.</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>프리미엄 디퓨저,집향기,힐링,출퇴근 피로 해소,휴식,홈디퓨저</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>생활/디퓨저</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>219</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>한우 구이용 소고기로 특별한 추석 식탁 완성하기</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>https://naver.me/ximfmufy</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_42/1736592727976wb9iD_JPEG/20754741779743894_1724877240.jpg</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>한우 구이용 소고기</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>추석에 가족과 함께 즐기는 신선한 한우 구이, 풍성한 명절 식탁을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>한우 구이용 소고기 추천, 추석 명절 특선 구매</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>추석 명절에 가족과 함께 즐기는 신선한 한우 구이용 소고기로 풍성한 식탁을 완성해보세요.</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>한우,구이용 소고기,추석,명절,신선한 소고기,가족 식사,특별한 추석,고기 추천</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>추석/한우</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>220</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>소중한 이에게 선물하기 좋은 부사 사과 선물세트</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>https://naver.me/F0ADR9rv</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250923_107/1758611281469EifQt_JPEG/105576549245608435_1653005778.jpg</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>신선한 부사 사과 세트</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>달콤하고 신선한 부사 사과로 소중한 사람에게 감동을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>부사 사과 선물세트 - 소중한 이에게 추천하는 신선한 과일 선물</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>달콤하고 신선한 부사 사과 선물세트로 소중한 사람에게 감동과 건강을 선물하세요. 가족, 친구 모두에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>부사사과,사과선물,과일선물,신선한사과,건강선물,사과세트,선물추천</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>선물/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>221</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>프리미엄 향기 디퓨저로 출퇴근 후 편안한 휴식 공간 만들기</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>https://naver.me/GhS2Su2p</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210728_100/1627438660062I82Nr_JPEG/28574555065200849_1033190179.jpg</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>편안한 휴식 향기 디퓨저</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>긴 하루 끝, 집에서 편안한 향기로 휴식하세요. 스트레스 완화에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>프리미엄 향기 디퓨저 추천, 편안한 휴식 공간 만들기</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>긴 하루 끝, 집에서 편안한 향기로 스트레스 완화에 도움을 주는 프리미엄 향기 디퓨저입니다. 출퇴근 후 휴식에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>프리미엄 디퓨저,향기 디퓨저,휴식용 디퓨저,스트레스 완화,집안 향기,아로마 디퓨저</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>홈데코/휴식</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>222</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>화려한우 선물세트로 특별한 날 소고기 맛보기</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>https://naver.me/FbqLqnLN</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_211/1720395611635zPhvg_JPEG/31289291941500558_1720856556.jpg</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>특별한 날 소고기 선물세트</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>소중한 분께 고품질 소고기로 감동을 전하세요. 특별한 날 더욱 빛나는 맛을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>화려한우 선물세트 추천, 특별한 날 고품질 소고기 맛보기</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>소중한 분께 고품질 화려한우 선물세트로 특별한 날 감동을 전하세요. 신선하고 맛있는 소고기를 경험할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>화려한우,소고기선물세트,고품질소고기,특별한날선물,한우선물,스페셜소고기</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>선물/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>223</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>명절 분위기를 살리는 1등급 한우 선물 세트 경험기</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>https://naver.me/5kxyxfyT</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250106_117/1736152797355nDvwq_JPEG/70285738497904845_1046362743.jpg</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>명절 선물 고민 끝! 1등급 한우로 가족과 특별한 순간을 더욱 풍성하게 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>명절 분위기 살리는 1등급 한우 선물 세트 추천</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>명절 선물 고민 없이 1등급 한우 선물 세트로 가족과 특별한 시간을 풍성하게 만드세요. 고품질 한우로 만족도 높은 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>한우선물,명절선물,1등급한우,한우세트,가족선물,명절한우</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>224</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>특별한 날, 나주배 가정용 선물세트가 딱이에요</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>https://naver.me/GFC3lKoz</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241021_54/1729494740638q5jTY_JPEG/33922805930090691_106919601.jpg</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>달콤한 나주배 선물세트</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>특별한 날 사랑을 전하는 달콤한 나주배 선물세트로 소중한 마음을 전해보세요.</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>특별한 날 나주배 가정용 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>달콤한 나주배 선물세트로 소중한 사람에게 감사와 사랑을 전하세요. 신선하고 품질 좋은 나주배가 가정용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>나주배, 선물세트, 가정용, 특별한날, 과일선물, 달콤한배</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>과일/선물세트</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>225</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>선물하기 좋은 투뿔 한우로 마음 전하세요</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>https://naver.me/xYvtvstC</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220812_57/1660267565596YR2l3_JPEG/61403411288097468_1297543586.jpg</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>프리미엄 투뿔 한우</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>질 좋은 한우로 소중한 사람의 마음을 따뜻하게 전해보세요. 특별한 날 완벽한 선물입니다.</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물 추천으로 마음을 전하세요</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>질 좋은 투뿔 한우로 소중한 분께 따뜻한 마음을 전할 수 있는 특별한 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>투뿔한우,한우선물,선물추천,고기선물,명절선물,특별한선물</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>선물/한우</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>226</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에서 편안함을 주는 프리미엄 방향제</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>https://naver.me/GhS2Su2c</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251125_228/1764033050998Krkqr_JPEG/111077114676320754_2120972026.jpg</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>프리미엄 집안 방향제</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후 집안에 편안한 향기로 피로를 풀어보세요. 집이 더 아늑해집니다.</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>프리미엄 방향제 추천 출퇴근 후 집안 편안함 선사</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에서 편안한 향기로 피로를 풀어주는 프리미엄 방향제입니다. 집안을 아늑하게 만들어 휴식 공간으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>방향제,프리미엄방향제,집안향기,편안한향기,출퇴근휴식,아늑한집</t>
+        </is>
+      </c>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>생활용품/방향제</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>227</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>테리파머 호텔수건, 휴대하기 좋은 고중량 타월</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>https://naver.me/FHVJVgJh</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250806_112/1754458992115A96LK_JPEG/88591808224616767_510704394.jpg</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>고중량 휴대용 호텔수건</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>부드럽고 흡수력 뛰어난 고중량 수건으로 언제 어디서나 쾌적함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>테리파머 호텔수건 고중량 타월 휴대용 추천</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>부드럽고 흡수력이 뛰어난 테리파머 호텔수건으로 여행이나 일상에서 언제나 쾌적함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>테리파머, 호텔수건, 고중량 수건, 휴대용 타월, 흡수력 좋은 수건, 부드러운 타월, 여행 필수품</t>
+        </is>
+      </c>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>생활/타월</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>228</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간단하게 구워 먹는 1등급 한우 설로인</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>https://naver.me/53141Kio</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250516_70/1747376499101pjWBR_JPEG/1893456200039790_1666635204.jpg</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>간단 구이용 1등급 한우 설로인</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 당신을 위한 간편한 고기 한 끼, 신선한 1등급 한우 설로인으로 특별한 맛을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>1등급 한우 설로인 간편구이 추천 출퇴근후 특별한 한끼</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>신선한 1등급 한우 설로인으로 출퇴근 후 간단히 구워 먹는 특별한 한 끼로 적합합니다. 빠르고 간편한 고기 요리를 원하시는 분께 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>한우,설로인,1등급,간편구이,출퇴근,한끼,신선한고기,간단요리</t>
+        </is>
+      </c>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>한우/정육</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>229</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집들이 선물로 좋은 인덕션 보호 매트 리뷰</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>https://naver.me/xdjbjF9o</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_37/1729695870151ua7tA_JPEG/63828717943776536_1877807330.jpg</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>인덕션 보호 매트</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집들이 선물로 딱! 인덕션 손상 걱정 없이 깔끔히 보호하세요.</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집들이 선물 추천 인덕션 보호 매트 구매 가이드</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>출퇴근 후에도 사용하기 좋은 인덕션 보호 매트로 손상 걱정 없이 깔끔하게 보호하세요. 집들이 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>인덕션 보호 매트, 집들이 선물, 주방용품, 인덕션 손상 방지, 출퇴근 후 추천</t>
+        </is>
+      </c>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>주방용품/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>230</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>차량용 방향제로 쾌적한 운전환경 만드는 방법</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>https://naver.me/GZ6P6uvM</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_24/17580292196727cOac_JPEG/2153769576746312_644773946.jpg</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>차량용 방향제로 쾌적한 운전</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>차 안 냄새 때문에 고민이라면 차량용 방향제로 산뜻하고 쾌적한 드라이빙 환경을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>차량용 방향제로 쾌적한 운전환경 만드는 방법 추천</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>차 안 냄새 제거에 효과적인 차량용 방향제로 산뜻하고 쾌적한 드라이빙 환경을 제공합니다. 운전 중 기분 좋은 향을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>차량용 방향제, 자동차 방향제, 차 냄새 제거, 쾌적한 운전, 드라이빙 향기</t>
+        </is>
+      </c>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>자동차/용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>231</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>가정용으로 딱 좋은 신선한 제주 감귤 선물세트 이야기</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>https://naver.me/FSSLS746</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241015_121/1728951908188Quisj_JPEG/4569934656639774_889067550.jpg</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>신선한 제주 감귤 선물세트</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>가정에서 신선한 제주 감귤의 향긋함을 즐기고 싶은 분께 완벽한 선물세트입니다.</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>가정용 신선한 제주 감귤 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>신선한 제주 감귤의 향긋함을 가정에서 즐길 수 있는 완벽한 선물세트로 가족과 함께 건강한 과일을 만나보세요.</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>제주감귤,감귤선물세트,가정용감귤,신선과일,제주특산품,과일선물</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>가정용/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>232</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>가정용으로 최적, 손질된 특대 보리굴비 사용 후기</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>https://naver.me/xGFgFPuf</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250929_156/1759130671305Ce5GI_JPEG/9686162952224733_763763689.jpg</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>특대 보리굴비 가정용</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>가정에서도 신선한 특대 보리굴비를 손쉽게 즐기고 싶은 분들께 추천합니다. 간편한 손질로 맛있는 식사를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>가정용 손질된 특대 보리굴비 추천 및 사용 후기</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>가정에서도 신선한 특대 보리굴비를 간편하게 즐길 수 있어 손쉬운 조리와 맛있는 식사를 원하시는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>보리굴비,특대 보리굴비,가정용,손질된 보리굴비,신선 보리굴비,간편 보리굴비,보리굴비 추천</t>
+        </is>
+      </c>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>수산물/가정식</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>특별한 날 선물용으로 좋은 목 어깨 마사지기 세트</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgBhBk03</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250909_282/1757385344744eBi2u_JPEG/41196276736117817_1155900437.jpg</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>목 어깨 집중 마사지기</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>피로한 목과 어깨를 효과적으로 풀어주는 마사지기로 특별한 날 소중한 분께 선물해 보세요.</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>목 어깨 마사지기 세트 추천 - 특별한 날 선물용</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>피로한 목과 어깨를 부드럽게 풀어주는 마사지기 세트로, 특별한 날 소중한 분께 안성맞춤인 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>목 마사지기, 어깨 마사지기, 선물 추천, 피로 해소, 마사지기 세트, 건강관리, 특별한 선물</t>
+        </is>
+      </c>
+      <c r="J234" t="inlineStr">
+        <is>
+          <t>건강/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>휴대가 간편한 비비랩 석류 콜라겐 젤리로 피부 관리하세요</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>https://naver.me/GsoDo2yV</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250227_91/1740643292312ceErl_PNG/7942574432690952_2021446082.png</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>피부 탄력 석류 콜라겐 젤리</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>피부 탄력이 고민이라면 휴대가 간편한 콜라겐 젤리로 건강한 피부를 챙겨보세요.</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>휴대가 간편한 비비랩 석류 콜라겐 젤리 피부관리 추천</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>피부 탄력 개선에 도움을 주는 비비랩 석류 콜라겐 젤리로 언제 어디서나 간편하게 피부 건강을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>비비랩,콜라겐젤리,석류,피부관리,피부탄력,휴대용젤리,건강보조식품</t>
+        </is>
+      </c>
+      <c r="J235" t="inlineStr">
+        <is>
+          <t>건강/뷰티</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>235</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>가정용으로 부담 없는 상주곶감 실속형 세트</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>https://naver.me/FYqNqyYd</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210117_141/1610868427042A3eIW_JPEG/12004254839536204_1995603776.JPG</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>가정용 부담 없는 상주곶감 세트</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>맛과 건강 둘 다 챙기고 싶은 당신을 위한 실속형 상주곶감 세트로 가족의 특별한 시간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>가정용 상주곶감 실속형 세트 추천 - 맛과 건강 챙기기</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>가정용 부담 없는 상주곶감 세트로 건강과 맛을 동시에 경험하세요. 가족 모두가 즐길 수 있는 실속형 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>상주곶감, 실속형 세트, 가정용 곶감, 건강 간식, 가족 선물, 곶감 추천</t>
+        </is>
+      </c>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>간식/가공식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>설날을 빛내는 프리미엄 한우 선물세트, 건강한 먹거리 선택</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>https://naver.me/5qc1cjXM</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221118_146/1668748995088DI8je_JPEG/69884778792702594_1294477324.jpg</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>설날 가족과 함께하는 특별한 식탁, 신선한 한우로 건강한 맛을 선물하세요.</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 선물세트 설날 추천, 건강한 먹거리</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>설날 가족과 함께 즐기는 신선한 한우 선물세트로 건강하고 맛있는 식탁을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>한우,설날선물,프리미엄,한우선물세트,건강먹거리,명절선물,가족식사,신선한고기</t>
+        </is>
+      </c>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>명절/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>237</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>휴대가 편한 풀리지 마사지기와 압박밴드 세트</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>https://naver.me/xqupuaTI</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251106_73/1762426159970pl56a_JPEG/39405885082356032_1343819192.jpg</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>풀림 마사지와 압박 세트</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>피로 풀리는 마사지와 편안한 압박 밴드로 하루 종일 쌓인 긴장을 완화하세요.</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>휴대가 편한 마사지기와 압박밴드 세트 추천</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>피로 회복과 긴장 완화에 좋은 휴대용 마사지기와 압박밴드 세트로 하루 종일 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>마사지기,압박밴드,휴대용마사지기,피로회복,긴장완화,헬스케어,셀프마사지</t>
+        </is>
+      </c>
+      <c r="J238" t="inlineStr">
+        <is>
+          <t>헬스케어/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>출퇴근 후 테리파머 호텔수건으로 상쾌하게 마무리하는 습관</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>https://naver.me/GcKTKryS</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250718_86/1752802109994HW7ql_JPEG/6569793910599683_581695595.jpg</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>상쾌한 출퇴근 호텔수건</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>출퇴근 후 느껴지는 찝찝함, 테리파머 호텔수건으로 깔끔하고 상쾌하게 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>테리파머 호텔수건으로 출퇴근 후 상쾌한 마무리 추천</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>출퇴근 후 찝찝함을 깔끔하게 해결하는 테리파머 호텔수건으로 상쾌한 기분을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>테리파머, 호텔수건, 출퇴근, 상쾌함, 세안수건, 욕실용품</t>
+        </is>
+      </c>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>239</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>집들이 선물로 좋은 실용적인 실리콘 방수 매트</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>https://naver.me/FPUpU5xE</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250303_165/17409353469363HG3l_PNG/75068133018318390_447142848.png</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>실용적인 실리콘 방수 매트</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>집들이 선물 고민 끝! 튼튼한 실리콘 매트로 물기 걱정 없이 깔끔한 공간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>집들이 선물 추천 실용적인 실리콘 방수 매트 구매</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>튼튼한 실리콘으로 제작되어 물기 걱정 없이 깔끔한 공간을 유지하는 실용적인 방수 매트입니다. 집들이 선물로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>집들이선물,실리콘매트,방수매트,실용적인매트,주방매트,청소용매트,생활용품</t>
+        </is>
+      </c>
+      <c r="J240" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>240</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>선물용으로 좋은 투뿔한우 숙성로스 세트의 특별함</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>https://naver.me/5EnMnZF5</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250228_208/1740694115536Xhl34_JPEG/47249825932196547_1421438944.jpg</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>투뿔한우 숙성로스 세트</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>특별한 날, 선물용으로 딱 좋아요. 깊고 풍부한 맛이 선물 받는 이의 마음까지 채웁니다.</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>투뿔한우 숙성로스 세트 선물용 추천, 깊은 맛과 품격</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>특별한 날 선물용으로 적합한 투뿔한우 숙성로스 세트로 깊고 풍부한 맛을 경험하세요. 고급스러운 선물로 좋은 선택입니다.</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>투뿔한우, 숙성로스, 한우선물세트, 고급선물, 특별한선물</t>
+        </is>
+      </c>
+      <c r="J241" t="inlineStr">
+        <is>
+          <t>선물/한우</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>241</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>운동 후 휴대하기 좋은 종아리 마사지기와 파우치 세트</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>https://naver.me/GtJaJR2D</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251123_277/1763867145455BxI1U_JPEG/98000006591361451_808832460.jpg</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>운동 후 종아리 마사지기</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>종아리 뭉침과 피로, 휴대용 마사지기로 간편하게 풀어보세요. 운동 후 회복에 딱 맞는 세트입니다.</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>종아리 마사지기 휴대용 세트 추천 운동 후 회복에 적합</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>운동 후 종아리 뭉침과 피로를 간편하게 풀어주는 휴대용 마사지기와 파우치 세트로 빠른 회복을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>종아리 마사지기,휴대용 마사지기,운동 회복,피로 해소,운동용품,파우치 세트</t>
+        </is>
+      </c>
+      <c r="J242" t="inlineStr">
+        <is>
+          <t>운동/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>242</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>셀프로 꾸미는 웨딩 이벤트, 프로포즈 세트 추천</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>https://naver.me/F6nCnThy</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251120_208/1763618884681ULgUc_JPEG/36218748679401752_873071273.jpg</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>셀프 웨딩 이벤트 세트</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>특별한 날, 직접 꾸미는 프로포즈 세트로 소중한 추억을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>셀프로 꾸미는 웨딩 이벤트 프로포즈 세트 추천</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>특별한 날에 직접 꾸미는 프로포즈 세트로 소중한 추억을 만들어보세요. 쉽고 예쁘게 연출할 수 있어 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>웨딩,프로포즈,이벤트세트,셀프꾸미기,웨딩소품,기념일선물,웨딩장식</t>
+        </is>
+      </c>
+      <c r="J243" t="inlineStr">
+        <is>
+          <t>웨딩/이벤트</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>243</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에 들어오면 느껴지는 프리미엄 향기</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>https://naver.me/5DD9DtdO</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20211201_273/1638326913209frdiO_JPEG/39462692920875105_1944749285.jpg</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>프리미엄 집 향기</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>집에 들어설 때마다 기분 좋은 향기로 스트레스를 날려보세요. 일상의 피로를 향기로 풀어드립니다.</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>프리미엄 향기 추천 집에 들어올 때 기분 좋은 향기</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>출퇴근 후 집에 들어오면 느껴지는 기분 좋은 프리미엄 향기로 스트레스를 해소하고 일상의 피로를 풀어 드립니다.</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>프리미엄향기,집들이향기,스트레스해소,기분전환,일상피로,향기추천,홈프래그런스</t>
+        </is>
+      </c>
+      <c r="J244" t="inlineStr">
+        <is>
+          <t>홈/향기</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>출퇴근 후 든든하게 즐기는 제주 은갈치 한 끼</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>https://naver.me/xS1U1alj</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240707_120/1720361510287YTKPs_JPEG/45550784175869416_1618187137.jpg</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>출퇴근 든든 제주 은갈치</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길, 든든한 한 끼로 제주 은갈치의 신선한 맛과 영양을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>제주 은갈치 한 끼 추천 출퇴근 식사 간편함까지</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길 신선한 제주 은갈치로 간편하고 든든한 한 끼를 즐겨보세요. 건강한 영양 공급에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>제주은갈치,출퇴근식사,간편식,신선한생선,건강식,든든한한끼,영양가높은</t>
+        </is>
+      </c>
+      <c r="J245" t="inlineStr">
+        <is>
+          <t>식사,간편식</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>운동 후 쾌적함을 더하는 헤트라스 멀티스프레이의 매력</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gf0g0sFC</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240819_215/1724028625827QKMJv_JPEG/51366018629681554_114961488.jpg</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>운동 후 쾌적 멀티스프레이</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>운동 후 땀과 냄새 고민, 이 멀티스프레이로 상쾌하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>헤트라스 멀티스프레이 운동 후 쾌적함 추천</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>운동 후 땀과 냄새 고민을 해소하는 헤트라스 멀티스프레이로 상쾌함을 유지하세요. 간편한 사용으로 청결함을 더해줍니다.</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>헤트라스,멀티스프레이,운동후,땀냄새제거,상쾌함,청결,스프레이</t>
+        </is>
+      </c>
+      <c r="J246" t="inlineStr">
+        <is>
+          <t>운동/케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>코코도르 디퓨저와 함께하는 출퇴근길 기분 전환</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>https://naver.me/5v3l3HeK</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251125_236/1764033029067XtTz5_JPEG/98165985294962410_1659825631.jpg</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>기분 전환 출퇴근 디퓨저</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>매일 반복되는 출퇴근길, 향기로 상쾌함을 더해보세요. 스트레스 완화와 기분 전환에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>코코도르 디퓨저 출퇴근길 기분 전환 추천</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>출퇴근길 스트레스 완화와 기분 전환에 좋은 코코도르 디퓨저로 상쾌한 향기를 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>코코도르,디퓨저,출퇴근길,기분전환,스트레스완화,향기</t>
+        </is>
+      </c>
+      <c r="J247" t="inlineStr">
+        <is>
+          <t>생활용품/향기</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>오설록 프리미엄 티로 출퇴근길에 여유 즐기기</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>https://naver.me/xJGJGBkA</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241128_71/1732759947054xNyqa_JPEG/57100975860821426_132371176.jpg</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>출퇴근길 여유 티</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>바쁜 일상 속 잠깐의 휴식, 오설록 프리미엄 티로 여유를 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>오설록 프리미엄 티 출퇴근길 여유 추천</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>출퇴근길 바쁜 일상에 오설록 프리미엄 티 한잔으로 편안한 휴식을 선사합니다. 깊은 향과 부드러운 맛이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>오설록,프리미엄 티,출퇴근 휴식,편안한 차,녹차,허브티,티 추천</t>
+        </is>
+      </c>
+      <c r="J248" t="inlineStr">
+        <is>
+          <t>차/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>소중한 분께 마음을 전하는 선물세트 구성 소개</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>https://naver.me/F4LVLMKH</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_289/1761286613913xMUuo_PNG/826630703187061_982343861.png</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>마음 전하는 선물세트</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 마음을 전하고 싶을 때 완벽한 선물세트로 특별한 감동을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>소중한 분께 마음 전달 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 감동을 전하는 완벽한 선물세트로 특별한 순간을 만드세요. 다양한 구성으로 마음을 담았습니다.</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>선물세트, 마음전달, 특별한선물, 감동선물, 선물추천</t>
+        </is>
+      </c>
+      <c r="J249" t="inlineStr">
+        <is>
+          <t>선물/기프트</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 신선한 향기를 선사하는 차량용 디퓨저 추천</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>https://naver.me/565z56TM</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251022_97/1761126654332d2Mfb_PNG/14721566477662320_862374576.png</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>차량용 신선한 향기 디퓨저</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량 냄새 걱정 끝! 신선한 향기로 쾌적한 드라이브를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량용 디퓨저 추천으로 신선한 향기 유지하기</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량 냄새 걱정 없이 신선한 향기로 쾌적한 드라이브를 즐길 수 있는 차량용 디퓨저를 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>차량용 디퓨저, 출퇴근길, 자동차 향기, 차량 냄새 제거, 쾌적한 드라이브</t>
+        </is>
+      </c>
+      <c r="J250" t="inlineStr">
+        <is>
+          <t>자동차/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량용 주차번호판으로 깔끔한 주차 관리</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>https://naver.me/GplplT8E</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240225_58/1708862149411AdL44_JPEG/109997929127275299_1320203773.jpg</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>깔끔한 차량 주차번호판</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>출퇴근길 주차 번호판으로 불편한 주차 문제를 간편하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량용 주차번호판 추천으로 깔끔한 주차 관리</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량용 주차번호판으로 주차 시 불편함을 줄이고 간편한 번호 표시가 가능합니다. 깔끔한 차량 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>출퇴근길,차량용,주차번호판,주차관리,번호표시,편리한주차,차량번호판</t>
+        </is>
+      </c>
+      <c r="J251" t="inlineStr">
+        <is>
+          <t>차량용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>출퇴근길에 도움이 되는 차량용 주차번호판</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>https://naver.me/FMTOTgzE</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230921_136/1695287392134I8gfQ_JPEG/13590823949101061_5970963.jpg</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>차량용 주차번호판</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>출퇴근길 주차 걱정 끝! 쉽게 번호를 노출해 안전한 주차를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>출퇴근길 차량용 주차번호판 안전한 주차 추천</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>출퇴근길 주차 걱정을 덜어주는 차량용 주차번호판으로, 번호 노출이 쉽고 빠른 소통이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>차량용 주차번호판, 출퇴근 주차, 번호판 노출, 안전 주차, 차량용 액세서리</t>
+        </is>
+      </c>
+      <c r="J252" t="inlineStr">
+        <is>
+          <t>자동차/주차용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>신선한 사골 우족으로 만든 든든한 보신 선물</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>https://naver.me/IxKrKqe2</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250421_175/17452185383971cXO4_JPEG/79351377525417490_494538899.jpg</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>든든한 보신 사골 우족</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>하루 피로를 풀고 건강을 챙기고 싶을 때, 신선한 사골 우족으로 만든 보신 선물이 든든한 힘이 되어 드립니다.</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>신선한 사골 우족으로 만든 든든한 보신 선물 추천</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>피로 회복과 건강 증진에 좋은 신선한 사골 우족 보신 선물로 몸과 마음을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>사골,우족,보신,건강선물,피로회복,영양식,선물추천</t>
+        </is>
+      </c>
+      <c r="J253" t="inlineStr">
+        <is>
+          <t>건강/보신</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>253</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>출퇴근길 간편한 신라명과 쿠키 선물 추천</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>https://naver.me/GHY2YqqY</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251204_6/1764836214376dGgMR_JPEG/19799228671751237_330483933.jpg</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>출퇴근 간편 쿠키 선물</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>출퇴근길 달콤한 즐거움, 간편한 신라명과 쿠키로 소중한 사람에게 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>출퇴근길 간편한 신라명과 쿠키 선물 추천</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>출퇴근길 달콤한 즐거움을 선사하는 신라명과 쿠키, 간편하게 소중한 사람에게 마음을 전할 수 있는 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>신라명과,쿠키,출퇴근선물,간편선물,달콤한간식,선물추천</t>
+        </is>
+      </c>
+      <c r="J254" t="inlineStr">
+        <is>
+          <t>선물,간식</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>254</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>선물로도 좋은 완도 활 전복 1kg 세트 추천</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>https://naver.me/FqZsZttE</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220706_107/1657095880555Sog8w_JPEG/58231660258829903_2018731965.jpg</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>신선한 완도 활 전복 1kg</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>바다의 신선함을 집에서도! 영양 가득 전복으로 건강한 식탁을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>완도 활 전복 1kg 세트 추천 선물용 신선한 해산물</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>신선한 완도 활 전복 1kg 세트로 건강한 식탁을 완성하세요. 선물용으로도 좋은 고품질 해산물 세트입니다.</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>완도전복,활전복,전복세트,해산물선물,건강식품,고급식재료,전복구매</t>
+        </is>
+      </c>
+      <c r="J255" t="inlineStr">
+        <is>
+          <t>해산물/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>255</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 구워 먹는 2kg LA갈비 선물 세트</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>https://naver.me/5b0U0ssc</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_59/1720403498896AbObJ_PNG/945707466979107_665950170.png</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>간편 구이용 2kg LA갈비</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 즐기는 2kg LA갈비로 맛있는 한 끼 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>간편하게 구워 먹는 2kg LA갈비 선물 세트 추천</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 즐기는 2kg LA갈비로 맛있는 한 끼를 완성할 수 있는 선물 세트입니다.</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>LA갈비,간편요리,선물세트,2kg,출퇴근식사,구이용고기,한끼식사</t>
+        </is>
+      </c>
+      <c r="J256" t="inlineStr">
+        <is>
+          <t>식품/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>256</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>개업할 때 좋은 소 코뚜레 명태 선물 추천</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>https://naver.me/xqupuaa2</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250604_156/17490030933634tbde_JPEG/156093852876024_921553735.jpg</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>행운 부르는 소 코뚜레</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>개업 선물 고민된다면, 행운과 번창을 기원하는 소 코뚜레 명태가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>개업 선물 추천 소 코뚜레 명태로 행운과 번창 기원</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>개업할 때 좋은 선물로 행운과 번창을 상징하는 소 코뚜레 명태를 추천합니다. 실용적이고 의미 있는 개업 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>개업선물,소코뚜레명태,행운선물,번창기원,사업선물</t>
+        </is>
+      </c>
+      <c r="J257" t="inlineStr">
+        <is>
+          <t>개업/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>257</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>중소형 거실화분꽃으로 집들이 선물 고민 끝</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>https://naver.me/GkUtU33l</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251203_151/1764743405790srsX8_JPEG/19187787603237652_1746713524.jpeg</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>중소형 거실화분</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>집들이 선물 고민 없이 집안 분위기를 싱그럽게 바꾸세요.</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>중소형 거실화분꽃으로 집들이 선물 추천</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>중소형 거실화분꽃으로 집안 분위기를 싱그럽게 바꾸는 집들이 선물입니다. 실내 공간을 화사하게 연출하는 데 효과적입니다.</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>거실화분,중소형화분,집들이선물,실내식물,화분꽃</t>
+        </is>
+      </c>
+      <c r="J258" t="inlineStr">
+        <is>
+          <t>인테리어</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>258</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>추석 명절 부모님께 고당도 선물세트로 감사 전하기</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>https://naver.me/5dAzA44z</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250212_285/1739319122995oAYkc_JPEG/73451991724315923_628767981.jpg</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>고당도 추석 선물세트</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>추석 명절, 부모님께 건강과 달콤함을 선물하세요. 감사한 마음을 고당도 과일로 전해드립니다.</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>추석 명절 고당도 선물세트 추천, 부모님께 감사 전하기</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>건강과 달콤함을 담은 고당도 과일 선물세트로 추석 부모님께 감사의 마음을 전하세요. 신선하고 품질 좋은 상품입니다.</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>추석선물,고당도과일,부모님선물,명절선물세트,감사선물,과일선물,건강선물,달콤한과일</t>
+        </is>
+      </c>
+      <c r="J259" t="inlineStr">
+        <is>
+          <t>명절/선물세트</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>259</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>헤트라스 퍼퓸 디퓨저 선물세트로 소중한 이에게 향기 선물</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>https://naver.me/xktCtnnn</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251002_224/17593836868990YM5I_JPEG/32203741045507315_579286885.jpg</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>고급 향기 디퓨저 세트</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 특별한 향기를 전하세요. 집안 가득 은은한 향기로 감동을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>헤트라스 퍼퓸 디퓨저 선물세트 추천 - 특별한 향기 선물</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 은은한 향기를 전하는 헤트라스 퍼퓸 디퓨저 선물세트입니다. 집안 분위기를 고급스럽게 연출할 수 있어 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>헤트라스, 퍼퓸디퓨저, 선물세트, 향기선물, 집들이선물, 인테리어소품, 은은한향기</t>
+        </is>
+      </c>
+      <c r="J260" t="inlineStr">
+        <is>
+          <t>선물/디퓨저</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>260</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>포레스트가든 아로마 디퓨저로 화장실도 상쾌하게 관리</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlb2bDDA</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230807_69/1691390100180DOleE_JPEG/5693001996794982_1645672374.jpg</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>화장실 상쾌 아로마 디퓨저</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>화장실 냄새로 고민이라면, 포레스트가든 아로마 디퓨저가 공간을 깔끔하고 쾌적하게 만들어줍니다.</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>포레스트가든 아로마 디퓨저 화장실 상쾌한 공간 관리 추천</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>화장실 냄새 고민 해결, 포레스트가든 아로마 디퓨저로 공간을 깔끔하고 쾌적하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>아로마디퓨저, 화장실향기, 냄새제거, 공간관리, 포레스트가든, 상쾌한향, 실내방향제</t>
+        </is>
+      </c>
+      <c r="J261" t="inlineStr">
+        <is>
+          <t>생활/방향제</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>261</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>실내 인테리어 포인트, 헤트라스 디퓨저 활용법</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gf0g0ssz</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241206_50/1733474425691X5smX_PNG/57951645646410034_462888095.png</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>실내 공간 향기로 채우기</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>답답한 실내 공기, 헤트라스 디퓨저로 상쾌하고 쾌적한 분위기를 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>헤트라스 디퓨저 추천, 실내 인테리어 공기 개선 아이템</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>헤트라스 디퓨저로 실내 공기를 상쾌하게 해 쾌적한 분위기를 조성하세요. 인테리어 포인트로도 활용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>헤트라스,디퓨저,실내공기,인테리어,공기정화,향기,실내디퓨저</t>
+        </is>
+      </c>
+      <c r="J262" t="inlineStr">
+        <is>
+          <t>실내공기,인테리어</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>262</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>선물용으로 좋은 영광 법성포 보리굴비 세트 추천</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://naver.me/FK0g0vvw</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251021_19/1761021843473fQTJf_JPEG/95154682582289943_1177925349.jpg</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>신선한 영광 보리굴비 세트</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>소중한 분들께 건강한 바다의 선물, 영광 법성포 보리굴비로 특별한 감동을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>영광 법성포 보리굴비 세트 추천 건강한 바다 선물</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>영광 법성포 보리굴비 세트로 소중한 분들께 건강하고 특별한 바다 선물을 전해 보세요. 고품질 굴비로 감동을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>영광법성포,보리굴비,선물세트,건강선물,바다선물,굴비세트,특별선물,영양식품</t>
+        </is>
+      </c>
+      <c r="J263" t="inlineStr">
+        <is>
+          <t>선물/수산물</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>263</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>소중한 이에게 전하는 제주 감귤 선물 이야기</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>https://naver.me/IM4Y4GAn</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230801_140/1690849790225XnvEA_JPEG/37815045024725445_1206822907.jpg</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>신선한 제주 감귤 선물</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>향긋한 제주 감귤로 소중한 이의 마음을 따뜻하게 전하세요. 건강함 가득한 자연의 선물입니다.</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>제주 감귤 선물 추천 소중한 이에게 따뜻한 마음 전하기</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>향긋한 제주 감귤로 건강과 사랑을 전하세요. 자연의 신선함이 가득한 특별한 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>제주감귤,감귤선물,제주과일,건강선물,자연선물,감귤추천,과일선물</t>
+        </is>
+      </c>
+      <c r="J264" t="inlineStr">
+        <is>
+          <t>선물/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>264</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>소중한 분께 전하는 상주 곶감 선물의 의미</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>https://naver.me/5AgYgpGu</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231216_209/1702730111585XsSia_JPEG/103865946393950032_1606861176.JPG</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>정성 담은 곶감 선물</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>소중한 분께 마음을 전하는 최고의 선택, 건강과 감사의 의미를 담아 선물하세요.</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>상주 곶감 선물 추천 소중한 마음 전하는 건강한 선택</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>상주 곶감으로 건강과 감사의 마음을 전하세요. 소중한 분께 전하는 최고의 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>상주 곶감, 곶감 선물, 건강 선물, 감사 선물, 명절 선물</t>
+        </is>
+      </c>
+      <c r="J265" t="inlineStr">
+        <is>
+          <t>선물/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>265</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>설 추석 맞이 건강 선물, 도라지정과의 특별함</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgBhBk8R</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20161017_165/asqw4381_1476673278687okTzW_JPEG/1016960326905260_-1313122428.jpg</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>도라지정과 건강선물</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>소중한 분들의 건강을 위한 전통 도라지정과로 설과 추석 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>설 추석 건강 선물 도라지정과 추천, 전통의 맛과 영양</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>소중한 분들의 건강을 위한 전통 도라지정과로 설과 추석에 마음을 전하세요. 맛과 영양을 모두 갖춘 건강 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>설선물,추석선물,건강선물,도라지정과,전통과자,한과,도라지,명절선물</t>
+        </is>
+      </c>
+      <c r="J266" t="inlineStr">
+        <is>
+          <t>건강선물/명절</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>266</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>일상과 여행 기록, 바인딩 포토북 한 권에 담다</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gj7q7XgV</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_17/17612819740748L4L1_PNG/8043516925763501_866553750.png</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>추억을 담는 포토북</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>일상과 여행의 소중한 순간을 한 권에 간직하세요. 감성 가득한 추억 정리에 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>일상과 여행 기록 바인딩 포토북 추천</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>감성 가득한 일상과 여행 추억을 한 권에 담아 소중하게 간직할 수 있는 바인딩 포토북입니다.</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>포토북,바인딩,추억정리,일상기록,여행기록,감성포토북,사진앨범</t>
+        </is>
+      </c>
+      <c r="J267" t="inlineStr">
+        <is>
+          <t>사진,포토북</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>267</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>특별한 날 선물하기 좋은 한우 선물세트 이야기</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>https://naver.me/xJGJGBd7</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251105_169/1762302985687lcE7L_JPEG/80606292631494242_399949605.jpg</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>특별한 한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 최고의 한우를 선물하세요. 특별한 날, 맛과 감동을 함께 전할 완벽한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>특별한 날 선물하기 좋은 한우 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>소중한 사람에게 선물하기 좋은 고품질 한우 선물세트로 특별한 날 더욱 뜻깊게 만들 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>한우, 선물세트, 특별한날, 고품질, 선물추천, 맛있는한우, 명절선물</t>
+        </is>
+      </c>
+      <c r="J268" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>268</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>명절 맞아 해림참바다 영광굴비 선물세트 추천합니다</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://naver.me/GvfhfTt3</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250808_168/1754645515587rDG6y_JPEG/3974324699920575_1958689333.jpg</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>신선한 영광굴비 선물세트</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>명절 고민 끝! 신선하고 맛있는 영광굴비로 감사의 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>명절 맞아 해림참바다 영광굴비 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>신선하고 맛있는 해림참바다 영광굴비 선물세트로 명절 감사의 마음을 전하세요. 가족과 지인에게 적합한 고품질 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>영광굴비,선물세트,명절선물,해림참바다,신선굴비,가족선물,감사선물</t>
+        </is>
+      </c>
+      <c r="J269" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>269</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>환갑·팔순 선물로 좋은 어버이날 용돈박스</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>https://naver.me/59U0UoQU</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250724_160/17533348830746WMM0_JPEG/1363668099070063_1904840391.jpg</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>특별한 어버이날 용돈박스</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>환갑·팔순 부모님의 마음을 따뜻하게 전하는 특별한 용돈박스로 감사의 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>환갑·팔순 선물 어버이날 용돈박스 추천</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>환갑·팔순을 맞은 부모님께 감사의 마음을 전하는 특별한 용돈박스로, 따뜻한 선물로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>용돈박스,환갑선물,팔순선물,어버이날선물,부모님선물,특별선물,감사의선물</t>
+        </is>
+      </c>
+      <c r="J270" t="inlineStr">
+        <is>
+          <t>선물/용돈박스</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>270</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>설날 가족 모임에 좋은 제주 갈치 선물 아이디어</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://naver.me/FFaWaM6Y</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250421_200/1745214772362Wcobd_JPEG/79347611477271628_684403218.jpg</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>제주 갈치 인기 선물</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>가족 모임에 꼭 맞는 신선한 제주 갈치로 따뜻한 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>설날 맞이 제주 갈치 선물 추천, 가족 모임에 최적</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>신선한 제주 갈치로 설날 가족 모임에 따뜻한 마음을 전할 수 있는 선물입니다. 풍부한 맛과 건강한 영양을 함께 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>제주 갈치, 설날 선물, 가족 모임, 신선한 생선, 갈치 선물, 건강한 식품, 명절 선물</t>
+        </is>
+      </c>
+      <c r="J271" t="inlineStr">
+        <is>
+          <t>설날/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>271</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>특별한 날을 빛내줄 신선한 한우 소고기 구이용 추천</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>https://naver.me/I5yVyaqn</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240312_254/1710212835119HOzJF_JPEG/111348668915722225_289730806.jpg</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>신선한 한우 소고기 구이</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>특별한 날, 신선한 한우로 풍미 가득한 고기 구이를 즐겨보세요. 소중한 순간을 더 빛나게 할 최고의 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>특별한 날 신선한 한우 소고기 구이용 추천</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>특별한 날에 어울리는 신선한 한우 소고기로 풍미 가득한 구이를 즐기세요. 소중한 순간을 더욱 빛내줄 최고의 선택입니다.</t>
+        </is>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>한우,소고기,구이용,신선한한우,특별한날,고기추천,풍미가득,한우구이</t>
+        </is>
+      </c>
+      <c r="J272" t="inlineStr">
+        <is>
+          <t>한우/육류</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>272</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 좋은 상주곶감 간편 간식 추천</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://naver.me/5NMiM58i</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240201_71/1706799527656JkDib_JPEG/107935423383841497_424352679.jpg</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>출퇴근용 간편 곶감</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에 달콤한 상주곶감으로 간편하게 건강 간식을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>출퇴근길 간편 건강 간식 상주곶감 추천</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 간편하게 즐길 수 있는 달콤한 상주곶감으로 건강 간식을 만나보세요.</t>
+        </is>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>상주곶감,간편간식,출퇴근간식,건강간식,달콤한곶감</t>
+        </is>
+      </c>
+      <c r="J273" t="inlineStr">
+        <is>
+          <t>간식/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>273</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>특별한 날 소중한 분께 전하는 은갈치 선물세트 이야기</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>https://naver.me/xTsXs6FF</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240619_294/1718776505340fcqun_JPEG/69625100302755188_424853057.jpg</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>은갈치 선물세트</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>특별한 날, 소중한 분께 건강한 맛을 전하세요. 신선한 은갈치로 마음을 듬뿍 전할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>소중한 분께 추천하는 은갈치 선물세트, 특별한 날 건강한 선택</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>신선한 은갈치로 구성된 건강한 선물세트로 특별한 날 소중한 분께 마음을 전하세요. 품질 좋은 은갈치가 담겨 있어 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>은갈치,선물세트,특별한날,건강선물,신선한생선,맛있는선물,추석선물,명절선물</t>
+        </is>
+      </c>
+      <c r="J274" t="inlineStr">
+        <is>
+          <t>선물/생선</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>274</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>시들지 않는 꽃선물로 감동을 전하는 방법</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://naver.me/FXkAkGNC</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251114_117/1763083769458fGTFu_PNG/17610752234411039_213839983.png</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>영원히 피는 꽃선물</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>소중한 마음을 오래 간직하고 싶을 때, 시들지 않는 꽃으로 특별한 감동을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>시들지 않는 꽃선물로 특별한 감동 전달법 추천</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>오래가는 시들지 않는 꽃으로 소중한 마음을 전하세요. 선물용으로 적합하며 감동을 오래 간직할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>시들지않는꽃,꽃선물,감동선물,오래가는꽃,특별한선물</t>
+        </is>
+      </c>
+      <c r="J275" t="inlineStr">
+        <is>
+          <t>선물/플라워</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>275</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 간편하게 즐기는 사무실 간식 추천</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>https://naver.me/5cqPqu79</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241027_167/17300084441337CsDl_JPEG/9583807967875334_684801100.jpg</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>출퇴근 간편 사무실 간식</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>출퇴근길 허기질 때 간편하게 즐길 수 있는 건강한 사무실 간식으로 힘차게 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>출퇴근길 사무실 간식 추천 건강한 간편 간식 구매</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>출퇴근길 허기짐에 딱 맞는 건강한 사무실 간식으로 간편하게 에너지를 충전하세요. 가볍고 휴대하기 좋아 직장인에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>사무실간식,출퇴근간식,건강간식,간편간식,직장인간식,에너지충전,간식추천,휴대간식</t>
+        </is>
+      </c>
+      <c r="J276" t="inlineStr">
+        <is>
+          <t>간식/직장인</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>276</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>출퇴근길 기분 전환, 인테리어소품 겸 디퓨저 활용법</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://naver.me/xYvtvsLC</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240912_143/17261025803106Co1f_PNG/5255032472855693_1702886427.png</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>기분 전환 인테리어 디퓨저</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>출퇴근길 답답함을 달래주는 향기로 공간을 채우고 기분까지 살려보세요.</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>출퇴근길 기분 전환 디퓨저 추천, 인테리어소품 활용법</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>출퇴근길 답답함을 향기로 달래고 공간을 아름답게 꾸며 기분 전환에 도움을 주는 디퓨저와 인테리어소품입니다.</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>기분전환,출퇴근,디퓨저,인테리어소품,향기,공간꾸미기,스트레스해소</t>
+        </is>
+      </c>
+      <c r="J277" t="inlineStr">
+        <is>
+          <t>인테리어/디퓨저</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>277</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>선물하기 좋은 헤트라스 헤리티지 퍼퓸 디퓨저 세트</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>https://naver.me/GuDVDwcX</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251002_80/1759385250502q9nh9_JPEG/3629225027718737_1556012021.jpg</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>향기 가득한 디퓨저 세트</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>집안 분위기를 한층 고급스럽게, 선물용으로도 완벽한 향기 디퓨저 세트입니다.</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>헤트라스 헤리티지 퍼퓸 디퓨저 세트 추천 선물용</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>고급스러운 향기로 집안을 풍성하게 채우는 헤트라스 헤리티지 퍼퓸 디퓨저 세트, 특별한 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>헤트라스,헤리티지,퍼퓸 디퓨저,향기 디퓨저,선물세트,홈데코,집안향기,선물추천</t>
+        </is>
+      </c>
+      <c r="J278" t="inlineStr">
+        <is>
+          <t>홈데코/향기</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>278</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>집들이 선물로 좋은 원목 냄비 받침 3P 세트 추천</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>https://naver.me/FOZQZode</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250424_104/1745476070233MXH8N_JPEG/21094120677097932_77795164.jpg</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>원목 냄비 받침 3P 세트</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>집들이 선물로 딱 좋은 자연스러운 원목 냄비 받침, 주방을 더욱 따뜻하게 만들어줍니다.</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>원목 냄비 받침 3P 세트 집들이 선물 추천</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>자연스러운 원목 소재로 제작된 냄비 받침 3P 세트로 집들이 선물에 적합하며 주방 분위기를 따뜻하게 연출합니다.</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>원목 냄비 받침,주방 소품,집들이 선물,내츄럴 디자인,주방 인테리어</t>
+        </is>
+      </c>
+      <c r="J279" t="inlineStr">
+        <is>
+          <t>주방용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>279</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>풍경종 소리로 집 현관을 특별하게 꾸며보는 방법</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>https://naver.me/5W9f9Qkb</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241023_102/1729665284852U4qv5_JPEG/1283422668477570_1966309825.jpeg</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>집 현관 풍경종 소리</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>현관이 밋밋해 고민이라면, 풍경종 소리로 따뜻한 분위기를 연출해보세요.</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>풍경종 소리로 집 현관 특별하게 꾸미기 추천</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>밋밋한 현관에 따뜻하고 특별한 분위기를 더하는 풍경종 소리 활용법을 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>풍경종,현관꾸미기,인테리어소품,집꾸미기,따뜻한분위기,소리소품</t>
+        </is>
+      </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>인테리어/소품</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>280</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 간편하게 챙기는 제주 황금향 감귤 간식</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>https://naver.me/FTMAMwiS</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250917_56/17580846546721Vfdi_JPEG/92217502379813458_1893330567.jpg</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>상큼한 제주 황금향 감귤</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>출퇴근 길 간편하게 즐기는 신선한 제주 황금향으로 기분 좋은 상쾌함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>출퇴근 간편 간식 제주 황금향 감귤 추천</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 간편하게 즐기는 신선한 제주 황금향 감귤로 상쾌하고 건강한 간식을 만나보세요.</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>제주 황금향, 감귤, 출퇴근 간식, 간편 간식, 신선한 감귤</t>
+        </is>
+      </c>
+      <c r="J281" t="inlineStr">
+        <is>
+          <t>과일/간식</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-20 15:38)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J281"/>
+  <dimension ref="A1:J353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14485,6 +14485,3606 @@
         </is>
       </c>
     </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>281</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>출퇴근 길 편안하면서도 스타일리시한 시스루 원피스</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>https://naver.me/GoiQNNXh</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221022_298/1666405773541U56Bc_PNG/27366687458624600_666301208.png</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>편안함 가득 시스루 원피스</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>출퇴근길 불편함 없이 스타일과 편안함을 동시에 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>출퇴근길 편안한 시스루 원피스 추천 스타일리시한 디자인</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편안함과 스타일을 동시에 느낄 수 있는 시스루 원피스입니다. 활동성이 좋고 세련된 디자인으로 일상에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>시스루원피스,출퇴근패션,편안한원피스,스타일리시원피스,여성원피스,데일리룩,오피스룩</t>
+        </is>
+      </c>
+      <c r="J282" t="inlineStr">
+        <is>
+          <t>패션/원피스</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>282</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>데이트룩으로 좋은 화려한 스팽글 투피스 스타일링</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>https://naver.me/5cqzaa01</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231207_36/1701959542961H9NHL_JPEG/103095385670931699_1094303005.jpg</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>화려한 스팽글 투피스</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>특별한 날, 빛나는 스팽글 투피스로 데이트룩 고민을 해결하세요. 자신감 넘치는 스타일을 완성해드립니다.</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>데이트룩 추천 스팽글 투피스 스타일링으로 빛나는 변신</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>특별한 날을 위한 화려한 스팽글 투피스로 데이트룩 고민을 해결하고 자신감 있는 스타일을 완성해보세요.</t>
+        </is>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>데이트룩,스팽글,투피스,여성패션,특별한날,스타일링,화려한,자신감</t>
+        </is>
+      </c>
+      <c r="J283" t="inlineStr">
+        <is>
+          <t>패션/여성의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>오피스와 하객룩 모두 어울리는 세련된 원피스 스타일</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>https://naver.me/GScW441U</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250819_89/1755594346204fgDPX_JPEG/5205878707051219_199464500.jpg</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>세련된 오피스 하객 원피스</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>오피스와 하객룩 고민 끝! 어디서든 돋보이는 세련된 원피스로 자신감을 채우세요.</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>오피스와 하객룩에 어울리는 세련된 원피스 추천</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>오피스와 하객룩 모두에 적합한 세련된 원피스로 다양한 자리에서 자신감을 높여줍니다. 깔끔한 디자인과 편안한 착용감이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>세련된원피스,오피스룩,하객룩,원피스스타일,여성의류,비즈니스룩,격식있는복장</t>
+        </is>
+      </c>
+      <c r="J284" t="inlineStr">
+        <is>
+          <t>패션/원피스</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>284</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>출퇴근길 멋스러운 양모 앙고라 롱코트 스타일링</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>https://naver.me/GT6H5523</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241113_23/1731492364457MNvbg_JPEG/62214893347739704_1279954382.jpg</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>포근한 멋스러운 롱코트</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 없이 스타일 살릴 수 있는 따뜻한 양모 앙고라 코트입니다.</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>출퇴근길 멋스러운 양모 앙고라 롱코트 추천</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 없이 따뜻하고 세련된 스타일을 완성하는 양모 앙고라 롱코트입니다.</t>
+        </is>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>양모코트,앙고라코트,롱코트,출퇴근코트,겨울코트,따뜻한코트,스타일코트</t>
+        </is>
+      </c>
+      <c r="J285" t="inlineStr">
+        <is>
+          <t>패션/코트</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>285</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>낮은 기온에도 포근한 울 모직코트 착용 후기</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>https://naver.me/546f99nl</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240123_118/17060183772802pWEl_JPEG/107154275980801762_816289207.jpg</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>포근한 울 모직코트</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻하고 부드러운 울 코트로 겨울 걱정을 덜어보세요.</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>포근한 울 모직코트 추천, 추운 겨울 따뜻하게 착용하기</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하고 부드러운 울 모직코트로 실용적이고 편안한 착용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>울코트,모직코트,겨울코트,따뜻한코트,겨울패션,포근한코트,겨울외투</t>
+        </is>
+      </c>
+      <c r="J286" t="inlineStr">
+        <is>
+          <t>패션/겨울의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>286</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>쉽게 관리 가능한 에센셜 워셔블 외투 활용법</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>https://naver.me/GFCjqqbv</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241120_240/1732063438849rFdqW_JPEG/66196296815786153_559259082.jpg</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>간편 세탁 가능 외투</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>복잡한 관리 없이도 언제나 깔끔한 외투, 손쉬운 세탁으로 부담 없이 즐기세요.</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>에센셜 워셔블 외투 쉽게 관리하는 방법 추천</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>복잡한 관리 없이 깔끔한 에센셜 워셔블 외투, 손쉬운 세탁으로 언제나 부담 없이 스타일을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>에센셜 외투, 워셔블 외투, 손쉬운 관리, 세탁 간편, 깔끔한 외투, 실용 외투</t>
+        </is>
+      </c>
+      <c r="J287" t="inlineStr">
+        <is>
+          <t>패션/관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>287</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>운동복 관리에 좋은 천연 양모 건조볼 사용 후기</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>https://naver.me/FXkz44s5</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250602_50/1748843008139CtDg3_JPEG/29474330971534938_208476195.JPG</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>천연 양모 건조볼</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>운동복 건조 후 뭉침 걱정 끝! 천연 양모 볼로 부드럽고 깔끔하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>천연 양모 건조볼 추천 운동복 관리 뭉침 걱정 해소</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>운동복 건조 후에도 뭉침 걱정 없이 부드럽고 깔끔한 관리가 가능한 천연 양모 건조볼 사용 후기입니다.</t>
+        </is>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>천연 양모 건조볼, 운동복 관리, 건조볼 추천, 뭉침 방지, 세탁용품</t>
+        </is>
+      </c>
+      <c r="J288" t="inlineStr">
+        <is>
+          <t>세탁용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>288</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>야외 운동 시에도 편안한 울 후드 롱코트</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>https://naver.me/xpBebbUV</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_217/1736568921740E9slN_JPEG/70701851881003883_1437439229.jpg</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>야외 운동용 울 후드 코트</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>야외 운동할 때도 따뜻함과 편안함이 필요하신가요? 부드러운 울 소재로 쾌적하게 착용해보세요.</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>울 후드 롱코트 야외 운동용 편안한 코트 추천</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>야외 운동 시 따뜻하고 편안한 울 후드 롱코트로 부드러운 착용감을 경험하세요. 활동성 높은 디자인으로 운동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>울코트,후드롱코트,야외운동,편안한코트,따뜻한코트,운동복,겨울코트</t>
+        </is>
+      </c>
+      <c r="J289" t="inlineStr">
+        <is>
+          <t>패션/아우터</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>289</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>멋스러운 오버핏 숏코트, 일상 휴대하기 좋아요</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>https://naver.me/5kxWvvJj</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241030_44/17302795386066dQNt_JPEG/12904910477484864_2038136892.jpg</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>멋스러운 오버핏 숏코트</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>편안하면서 스타일리시한 오버핏 숏코트로 일상 어디서나 멋을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>멋스러운 오버핏 숏코트 추천, 편안한 일상 스타일 완성</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>편안하면서도 스타일리시한 오버핏 숏코트로 일상 어디서나 멋스러운 룩을 연출하세요. 가볍고 휴대하기 좋아 다양한 상황에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>오버핏,숏코트,여성코트,일상코디,편안한아우터,간절기코트,캐주얼룩</t>
+        </is>
+      </c>
+      <c r="J290" t="inlineStr">
+        <is>
+          <t>패션/아우터</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>290</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>편안한 착용감의 여성 양모 베스트 추천</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>https://naver.me/xTsu44Mw</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240227_113/1709043113608aCfFm_JPEG/36345797483766546_699751601.jpg</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>여성 양모 베스트</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>추운 계절에도 따뜻하고 편안한 착용감을 찾는 당신께 꼭 맞는 여성 양모 베스트입니다.</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>여성 양모 베스트 추천, 따뜻하고 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하게 입을 수 있는 여성용 양모 베스트로 편안한 착용감을 제공합니다. 데일리웨어로 적합한 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>여성베스트,양모베스트,겨울패션,따뜻한옷,편안한착용감,겨울의류</t>
+        </is>
+      </c>
+      <c r="J291" t="inlineStr">
+        <is>
+          <t>패션/겨울의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>291</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>출퇴근 시간 활용, 양모펠트 인형 만들기 즐기기</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>https://naver.me/GagB119v</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220613_159/1655083727851QEAw1_JPEG/56219623313791722_471242747.jpg</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>출퇴근 시간 양모펠트 인형</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>출퇴근 시간을 알차게 보내고 싶다면 양모펠트 인형 만들기 키트가 딱입니다. 집중하며 힐링할 수 있어요.</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>출퇴근 시간 활용 양모펠트 인형 만들기 키트 추천</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>출퇴근 시간을 활용해 집중력과 힐링을 동시에 경험할 수 있는 양모펠트 인형 만들기 키트로 즐거운 취미 생활을 시작해보세요.</t>
+        </is>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>양모펠트,인형만들기,출퇴근시간,취미키트,힐링활동,집중력향상,핸드메이드</t>
+        </is>
+      </c>
+      <c r="J292" t="inlineStr">
+        <is>
+          <t>취미/공예</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>292</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식 공간에 어울리는 대형 러그 선택법</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgB0ggmo</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20191126_70/1574757705631ueQFD_JPEG/12121094169725709_1882013177.jpg</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>편안한 대형 러그</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 발을 감싸주는 대형 러그로 집 안 휴식 공간을 포근하게 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식 공간에 어울리는 대형 러그 추천</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>지친 발을 부드럽게 감싸주는 대형 러그로 집 안 휴식 공간을 포근하게 꾸며보세요. 편안한 휴식에 적합한 러그 선택법을 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>대형러그,휴식공간,출퇴근후,집안꾸미기,포근한러그,러그선택법,발편안러그</t>
+        </is>
+      </c>
+      <c r="J293" t="inlineStr">
+        <is>
+          <t>홈데코/러그</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>293</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 좋은 슬라운드 부드러운 차렵 이불</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>https://naver.me/xv6piiXc</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_208/175799509030656Y8Q_JPEG/52109313228365997_126477467.jpg</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>부드러운 차렵 이불</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 포근하게 감싸주는 부드러운 차렵 이불로 편안한 휴식을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 좋은 슬라운드 부드러운 차렵 이불 추천</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>지친 출퇴근 후 편안한 휴식을 위한 슬라운드 부드러운 차렵 이불입니다. 포근한 감촉으로 편안한 잠자리를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>슬라운드,차렵이불,부드러운이불,출퇴근휴식,포근한이불,편안한잠자리</t>
+        </is>
+      </c>
+      <c r="J294" t="inlineStr">
+        <is>
+          <t>침구류</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>294</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>사계절 사용하는 고밀도 순면 이불의 매력</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>https://naver.me/FE3oQQRp</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_252/1757994877006AM1yl_JPEG/12652225893820308_1698887882.jpg</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>사계절용 고밀도 순면 이불</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>변덕스러운 날씨에도 깊은 숙면을 선사하는 고밀도 순면 이불로 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>사계절 고밀도 순면 이불 추천으로 깊은 숙면</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>변덕스러운 날씨에도 쾌적한 사용이 가능한 고밀도 순면 이불로 사계절 내내 편안함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>고밀도,순면,이불,사계절,쾌적,숙면,침구,면이불,편안함</t>
+        </is>
+      </c>
+      <c r="J295" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>295</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 좋은 포근한 차렵 이불 추천</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>https://naver.me/FK0uYd8y</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240911_232/1726043960560guMeS_JPEG/29600834309618471_1085720924.jpg</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>포근한 출퇴근 휴식 차렵이불</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>하루의 피로를 부드럽게 감싸주는 차렵이불로 출퇴근 후 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>포근한 차렵 이불 추천 출퇴근 후 휴식용 편안한 선택</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>부드러운 촉감과 보온성으로 출퇴근 후 피로를 풀어주는 차렵 이불입니다. 집에서 편안한 휴식을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>차렵이불,출퇴근휴식,포근한이불,편안한이불,보온이불,침구류</t>
+        </is>
+      </c>
+      <c r="J296" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>296</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 딱 좋은 사계절 침구</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>https://naver.me/IxKJ44li</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250910_115/1757468588009XrfE3_JPEG/91221786477578799_1593638652.jpg</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>사계절 쾌적 침구</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 포근하게 감싸주는 사계절 침구로 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 좋은 사계절 침구 추천</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 포근하게 감싸주는 사계절 침구로 사계절 내내 편안한 휴식을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>사계절침구,출퇴근휴식,포근한이불,편안한숙면,침구추천</t>
+        </is>
+      </c>
+      <c r="J297" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>297</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>일상에 편안함을 더하는 사계절용 알러지 차렵이불 소개</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>https://naver.me/x5m3aaJJ</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250916_142/1757995168717hCMgv_JPEG/33959842846349089_1400039922.jpg</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>사계절 알러지 차렵이불</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>알레르기 걱정 없이 사계절 내내 쾌적한 잠자리를 선사합니다. 포근한 편안함으로 건강한 수면을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>사계절용 알러지 차렵이불 추천, 편안한 건강 수면 아이템</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>알레르기 걱정 없는 사계절용 차렵이불로 쾌적하고 포근한 잠자리를 제공합니다. 건강한 수면에 적합한 알러지 차단 기능이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>차렵이불,사계절이불,알러지차단,편안한수면,건강이불</t>
+        </is>
+      </c>
+      <c r="J298" t="inlineStr">
+        <is>
+          <t>침구/이불</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>298</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로를 녹여주는 광폭 차렵이불 사용기</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>https://naver.me/xrC3rrYn</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230317_167/1679044645362MRyCv_JPEG/80180425077348583_716125085.jpg</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>피로완화 광폭 차렵이불</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 광폭 차렵이불로 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>광폭 차렵이불 추천 출퇴근 후 피로 회복용</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 포근하게 감싸주는 광폭 차렵이불로 편안한 휴식을 제공합니다. 넓은 폭으로 쾌적한 수면 환경을 완성합니다.</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>차렵이불,광폭이불,출퇴근 피로회복,수면용이불,편안한휴식,포근한이불</t>
+        </is>
+      </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>299</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>겨울철에도 따뜻하게, 저소음 차렵이불의 매력</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://naver.me/G4G9DDBq</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_254/1765257460490tPrDp_JPEG/14849012182256771_1707393930.jpg</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>저소음 겨울 차렵이불</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>추운 겨울, 저소음 차렵이불로 포근함과 편안한 숙면을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>저소음 차렵이불 추천 겨울철 따뜻한 숙면용</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>추운 겨울철에도 포근하고 편안한 숙면을 돕는 저소음 차렵이불로 따뜻하게 지내세요.</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>차렵이불,저소음이불,겨울이불,따뜻한이불,숙면,포근한이불,겨울침구</t>
+        </is>
+      </c>
+      <c r="J300" t="inlineStr">
+        <is>
+          <t>침구/겨울</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>300</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>양면 사용 가능한 리버시블 이불로 실용성 더하기</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>https://naver.me/FXkz44Vr</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250123_139/1737609485505tS9hb_JPEG/71742319589317703_1477621541.jpg</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>양면 사용 리버시블 이불</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>한 번 구매로 두 가지 스타일을 즐기세요. 실용적인 리버시블 이불로 쾌적한 잠자리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>리버시블 이불 추천, 양면 사용 가능한 실용 이불 구매</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>양면 사용 가능한 리버시블 이불로 다양한 스타일과 쾌적한 잠자리를 경험하세요. 실용적인 디자인으로 부담 없이 활용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>리버시블 이불, 양면 이불, 실용 이불, 쾌적한 잠자리, 침구, 이불 추천</t>
+        </is>
+      </c>
+      <c r="J301" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>301</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>포근함과 보온성 갖춘 10미리 두꺼운 이불 추천</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://naver.me/Ig4abxe4</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_117/1729730875700XO6Vm_JPEG/4292809809694254_738112778.jpg</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>10mm 두꺼운 포근 이불</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>추운 겨울, 따뜻함이 부족해 고민이라면 10mm 두꺼운 이불로 포근한 보온을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>포근함과 보온성 갖춘 10미리 두꺼운 이불 추천</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>10mm 두꺼운 이불로 추운 겨울에도 포근하고 따뜻하게 보온을 유지해줍니다. 겨울철 실내 온도 걱정하는 분들께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>두꺼운이불,보온이불,겨울이불,10mm이불,포근한이불,겨울침구,따뜻한이불</t>
+        </is>
+      </c>
+      <c r="J302" t="inlineStr">
+        <is>
+          <t>침구,겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>302</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>운동 후 몸을 녹여주는 초미니 탄소매트의 휴대성 체험기</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://naver.me/GScW4jjZ</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230224_47/1677208459679HURaE_JPEG/78344358387767877_812693386.jpg</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>초미니 탄소매트 휴대용</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>운동 후 뭉친 몸을 간편하게 녹여주는 초소형 탄소매트로 언제 어디서나 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>초미니 탄소매트 휴대용 운동 후 피로회복 추천</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>초소형 탄소매트로 운동 후 뭉친 몸을 간편히 녹여주며, 휴대성이 뛰어나 언제 어디서나 편안함을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>초미니 탄소매트, 휴대용 탄소매트, 운동 후 피로회복, 미니 탄소매트, 휴대성 좋은 매트</t>
+        </is>
+      </c>
+      <c r="J303" t="inlineStr">
+        <is>
+          <t>건강,운동</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>303</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>작지만 강한 카본 전기매트, 운동 후 휴식에 딱!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://naver.me/5h1yMWOT</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230316_229/1678952552361X90Cs_JPEG/80088380187467301_1225847098.jpg</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>강력한 카본 전기매트</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>운동 후 빠른 회복이 필요할 때, 작지만 강한 전기매트가 따뜻한 휴식을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>작지만 강한 카본 전기매트 추천, 운동 후 휴식용</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>운동 후 빠른 회복을 돕는 작고 강한 카본 전기매트로 따뜻하고 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>카본 전기매트, 운동 회복, 전기매트 추천, 휴식용 전기매트, 따뜻한 매트</t>
+        </is>
+      </c>
+      <c r="J304" t="inlineStr">
+        <is>
+          <t>건강/운동</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>304</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>작고 가벼운 탄소매트로 집에서 편안한 휴식</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://naver.me/5QiWzXc6</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221018_280/1666073786298nj1y9_JPEG/67209632011537380_1372275144.jpg</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>가벼운 휴식용 탄소매트</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>작고 가벼워 어디서나 편안한 휴식을 원한다면, 이 탄소매트가 딱 맞아요.</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>작고 가벼운 탄소매트 추천, 집에서 편안한 휴식용</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>작고 가벼운 탄소매트로 집안 어디서나 편안하게 휴식할 수 있습니다. 휴대하기 좋아 실용적인 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>탄소매트,휴식용매트,편안한매트,가벼운매트,작은매트,휴대용매트,집에서휴식</t>
+        </is>
+      </c>
+      <c r="J305" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>305</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>출퇴근 후 디지털조절기 전기매트로 피로 풀기</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://naver.me/5IiRrvHw</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240925_212/1727254124351YMWjp_JPEG/9857966854853689_490126031.jpg</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>출퇴근 피로 해소 매트</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>긴 하루 끝에 지친 몸을 부드럽게 감싸주는 전기매트로 피로를 풀어보세요.</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>디지털조절기 전기매트로 출퇴근 후 피로 풀기 추천</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 쌓인 피로를 전기매트로 부드럽게 풀어보세요. 디지털온도 조절로 편리하게 사용 가능해 누구에게나 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>전기매트,디지털조절기,피로회복,출퇴근,온열매트,휴식용매트</t>
+        </is>
+      </c>
+      <c r="J306" t="inlineStr">
+        <is>
+          <t>건강/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>306</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>캠핑과 차박에 안성맞춤인 원적외선 탄소매트 경험</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://naver.me/GNREZufn</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251205_19/1764924150410MscWt_PNG/99056963482005284_1178200909.png</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>원적외선 탄소매트 차박용</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>추운 야외에서도 따뜻하게, 캠핑과 차박 시 편안한 온기를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>캠핑과 차박에 추천하는 원적외선 탄소매트 따뜻함 경험</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>추운 야외에서도 원적외선 탄소매트로 따뜻함을 유지해 캠핑과 차박 시 쾌적한 온기를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>캠핑매트,차박용품,원적외선매트,탄소매트,야외난방,온열매트,야외캠핑</t>
+        </is>
+      </c>
+      <c r="J307" t="inlineStr">
+        <is>
+          <t>캠핑/차박</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>307</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 완벽한 그래핀 탄소매트 경험기</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://naver.me/xcATfc2e</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231006_177/1696559913168UUDgU_JPEG/24149332146199387_659731680.jpg</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>출퇴근 피로 풀어주는 그래핀 탄소매트</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>하루 종일 쌓인 피로, 그래핀 탄소매트로 간편하게 풀어보세요. 편안한 휴식이 필요할 때 완벽한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>그래핀 탄소매트 추천 출퇴근 후 휴식용 피로해소</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>하루 종일 쌓인 피로를 그래핀 탄소매트로 간편하게 풀어주는 휴식 아이템으로, 편안한 휴식을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>그래핀매트,탄소매트,휴식용매트,피로해소,출퇴근후휴식</t>
+        </is>
+      </c>
+      <c r="J308" t="inlineStr">
+        <is>
+          <t>생활/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>308</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>온열매트 활용해 출퇴근길 피로를 풀어보세요</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://naver.me/GmtOyLkY</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251107_40/17625045722139Cosw_JPEG/38966483355708767_964972807.jpg</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>출퇴근 필수 온열매트</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>장시간 출퇴근으로 쌓인 피로를 효과적으로 풀어주는 온열매트로 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>출퇴근길 피로 해소 온열매트 추천</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>장시간 출퇴근으로 쌓인 피로를 효과적으로 풀어주는 온열매트로 편안한 휴식을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>온열매트,출퇴근,피로해소,휴식용품,편안한매트</t>
+        </is>
+      </c>
+      <c r="J309" t="inlineStr">
+        <is>
+          <t>건강/휴식</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>309</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>집 안 어디서나 편안한 전기매트 사용법</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://naver.me/Ig4bPpp1</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241009_149/1728467847015JboeA_JPEG/20231110_111111111111111111111111111111_resize_%281%29.jpg20231110_11111111111111111.jpg</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>편안한 전기매트 사용법</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>추운 겨울, 집 안 어디서나 따뜻함을 누리세요. 쉽고 안전한 전기매트 사용법으로 편안함을 더해드립니다.</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>전기매트 사용법 추천, 집 안 어디서나 따뜻하게</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 집 안 어디서나 안전하고 편안하게 사용할 수 있는 전기매트 사용법을 소개합니다. 따뜻함과 안전을 동시에 누려보세요.</t>
+        </is>
+      </c>
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>전기매트,전기매트사용법,겨울난방,안전전기매트,따뜻한집,추위해소,실내난방</t>
+        </is>
+      </c>
+      <c r="J310" t="inlineStr">
+        <is>
+          <t>가전,난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>310</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>출퇴근 후 몸을 녹이는 전자파안심 온열매트</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://naver.me/FivXhyyF</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241115_214/1731653266695igo51_JPEG/65786133783255137_33714900.jpg</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>전자파안심 온열매트</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 피로와 찬 기운을 부드럽게 녹여주는 안전한 온열매트로 편안한 휴식을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로 완화 전자파안심 온열매트 추천</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>출퇴근 후 몸을 녹여주는 전자파 안심 온열매트로 안전하고 편안한 휴식을 도와줍니다. 피로 회복용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>온열매트,전자파안심,피로회복,출퇴근,휴식용 온열매트,안전온열매트,온열기</t>
+        </is>
+      </c>
+      <c r="J311" t="inlineStr">
+        <is>
+          <t>생활건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>311</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>무선 기능이 더해진 칫솔살균기로 집에서도 편리하게</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://naver.me/GXgyNvf5</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240607_62/1717732473373LHsbf_JPEG/118868362084806925_835522525.jpg</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>무선 칫솔 살균기로 깨끗함</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>매일 칫솔 위생 걱정 끝! 무선 기능으로 어디서나 간편하게 살균하세요.</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>무선 칫솔살균기 추천 무선 기능으로 간편한 위생 관리</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>무선 기능이 추가된 칫솔살균기로 집 안 어디서나 간편하게 칫솔을 위생적으로 관리할 수 있습니다. 깔끔한 생활을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>무선 칫솔살균기,칫솔 살균,위생 관리,무선 살균기,휴대용 살균기</t>
+        </is>
+      </c>
+      <c r="J312" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>312</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>가정용 칫솔살균기로 출퇴근 준비 간편하게</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ixbynOX</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250825_252/1756116747080U0FMA_PNG/90249594828132937_947993757.png</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>간편 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>바쁜 아침, 칫솔 위생 걱정 끝! 간편하게 살균해 건강한 미소를 지켜요.</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>가정용 칫솔살균기 건강 관리 추천</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>바쁜 아침에도 간편하게 칫솔을 살균해 깨끗한 위생을 유지할 수 있는 가정용 칫솔살균기입니다.</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>칫솔살균기,가정용,칫솔위생,살균,건강관리,아침준비,간편사용</t>
+        </is>
+      </c>
+      <c r="J313" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>313</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>가정용 UV 클린 살균기로 가족 건강 지키는 방법</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://naver.me/5zXPjCg3</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200928_113/1601280646866W2cMM_JPEG/38644035392221448_703944714.jpg</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>가정용 UV 살균기로 청결 유지</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>가족 건강 걱정되시나요? 강력한 UV 살균기로 집안의 세균을 깨끗하게 제거하세요.</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>가정용 UV 클린 살균기 추천으로 가족 건강 지키기</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>강력한 UV 살균기로 집안의 세균을 효과적으로 제거해 가족 건강을 지키는 데 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>UV살균기,가정용살균기,세균제거,가족건강,클린살균기,안전살균</t>
+        </is>
+      </c>
+      <c r="J314" t="inlineStr">
+        <is>
+          <t>가전,건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>314</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>가정용 무선 칫솔살균기로 매일 간편한 소독 경험</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1m6RSEN</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250428_197/1745842026991HCg5N_JPEG/435394937129072_1403241097.jpg</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>간편 무선 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>매일 사용하는 칫솔, 깨끗하게 관리하기 어려우셨나요? 무선 살균기로 안심 위생을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>가정용 무선 칫솔살균기 추천, 간편한 위생 관리</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>매일 사용하는 칫솔을 간편하고 깨끗하게 관리할 수 있는 무선 칫솔살균기로 위생을 지키세요.</t>
+        </is>
+      </c>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>칫솔살균기,무선살균기,가정용위생,칫솔관리,위생제품</t>
+        </is>
+      </c>
+      <c r="J315" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>315</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>운동 후 휴대하기 좋은 무선 칫솔 살균기의 실용성</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://naver.me/GwSOFgP2</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250418_77/1744935369534r4f5s_JPEG/79068291458232168_1118201276.jpg</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>휴대용 무선 칫솔 살균기</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 위생 걱정 끝! 언제 어디서나 간편하게 살균하세요.</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>운동 후 휴대용 무선 칫솔 살균기 추천 및 구매 가이드</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 위생 걱정을 덜어주는 휴대용 무선 칫솔 살균기로 언제 어디서나 간편하게 살균하세요.</t>
+        </is>
+      </c>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>무선 칫솔 살균기, 휴대용 칫솔 살균, 운동 후 위생, 간편 칫솔 살균, 휴대 칫솔 관리</t>
+        </is>
+      </c>
+      <c r="J316" t="inlineStr">
+        <is>
+          <t>위생/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>316</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>운동 후에도 안심! 휴대용 UV 자외선 살균기로 위생 챙기기</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlb7QzPo</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200516_65/1589610452982hBQiX_JPEG/26971995611326808_911477727.jpg</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>휴대용 UV 자외선 살균기</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>운동 후 장비나 소지품 위생 걱정 없이 언제 어디서나 깨끗하게 살균하세요.</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>운동 후에도 안심! 휴대용 UV 자외선 살균기 추천</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>운동 장비와 소지품을 언제 어디서나 깨끗하게 살균할 수 있는 휴대용 UV 자외선 살균기로 위생을 간편하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>휴대용 자외선 살균기,UV 살균기,운동 위생,휴대용 살균기,소지품 살균</t>
+        </is>
+      </c>
+      <c r="J317" t="inlineStr">
+        <is>
+          <t>위생/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>317</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>사무실 책상 위에서 활용하는 국산 휴대용 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://naver.me/x9zEK1bl</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240602_272/1717329537583jg1Yi_JPEG/118465426289368526_2014121092.jpg</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>사무실 책상 위에서도 간편하게 칫솔을 깨끗하게 살균하세요. 위생 걱정 끝!</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>국산 휴대용 칫솔살균기 사무실 책상 위 추천</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>사무실 책상 위에서 간편하게 사용 가능한 국산 휴대용 칫솔살균기로 위생 관리를 손쉽게 하세요.</t>
+        </is>
+      </c>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기,사무실용 칫솔살균기,국산 칫솔살균기,책상 위 칫솔살균기,칫솔 위생관리</t>
+        </is>
+      </c>
+      <c r="J318" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>318</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>사무실 책상 위 놓기 좋은 휴대용 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://naver.me/IGZtvWlw</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240525_102/1716621585936YHWRf_JPEG/43924269791980974_1551691435.jpg</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>책상용 휴대 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>사무실에서 위생 걱정 끝! 언제 어디서나 깨끗한 칫솔로 안심하세요.</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>사무실 책상용 휴대용 칫솔살균기 추천으로 위생 관리</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>사무실 책상 위에 놓기 좋은 휴대용 칫솔살균기로 언제 어디서나 깨끗하고 위생적인 칫솔 사용을 돕습니다.</t>
+        </is>
+      </c>
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기, 사무실 칫솔살균기, 칫솔 위생, 책상용 칫솔살균기, 휴대 칫솔 살균기, 위생용품, 칫솔관리</t>
+        </is>
+      </c>
+      <c r="J319" t="inlineStr">
+        <is>
+          <t>사무실/위생용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>319</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>운동 후에도 깨끗하게, 프리미엄 전신형 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://naver.me/5pqveTXR</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210120_292/1611124227378rYXdT_JPEG/12260007070287175_146801771.jpg</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>운동 후 전신 칫솔살균</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>운동 후에도 깨끗한 칫솔 관리가 필요하신가요? 프리미엄 전신형 살균기로 위생을 지키세요.</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>프리미엄 전신형 칫솔살균기 추천 운동 후 깨끗한 관리</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 위생을 효과적으로 지키는 프리미엄 전신형 칫솔살균기입니다. 깔끔하고 안전한 칫솔 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>칫솔살균기, 전신형살균기, 칫솔위생, 운동후칫솔관리, 프리미엄살균기</t>
+        </is>
+      </c>
+      <c r="J320" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>320</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>휴대용 UVC 살균기로 스마트폰까지 간편하게 소독하는 방법</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://naver.me/GwSOFgC9</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220425_158/1650849295608muLtE_JPEG/51985129427617274_1703398111.jpg</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>스마트폰 휴대용 살균기</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>스마트폰과 소지품 위생, 번거로운 청소가 어려웠다면 휴대용 UVC 살균기로 간편하게 살균해보세요.</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>휴대용 UVC 살균기 스마트폰 소독 추천 및 간편 사용법</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>휴대용 UVC 살균기로 스마트폰과 소지품을 간편하게 살균하여 위생을 유지할 수 있습니다. 집이나 외출 시 간편한 위생 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I321" t="inlineStr">
+        <is>
+          <t>휴대용 살균기,UVC 살균기,스마트폰 소독,휴대용 위생기기,간편 살균,소지품 살균</t>
+        </is>
+      </c>
+      <c r="J321" t="inlineStr">
+        <is>
+          <t>생활용품/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>321</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편한 유선 칫솔살균기 활용법</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://naver.me/GWivZGHh</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240222_6/1708566974183fFMze_JPEG/2681110025750080_289345845.jpg</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>간편 유선 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 청결한 칫솔 관리가 고민이라면 간편한 유선 칫솔살균기를 만나보세요.</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>출퇴근길 유선 칫솔살균기 추천으로 간편한 칫솔관리</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 청결한 칫솔 관리가 가능한 유선 칫솔살균기로 간편하고 위생적으로 사용하세요.</t>
+        </is>
+      </c>
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>유선 칫솔살균기,칫솔살균,칫솔관리,위생용품,출퇴근용,간편사용,칫솔소독</t>
+        </is>
+      </c>
+      <c r="J322" t="inlineStr">
+        <is>
+          <t>생활용품/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>322</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>온열 열판 기능이 더해진 무선 칫솔 살균기의 효과적인 사용법</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlb7QzX1</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250722_160/1753160564405vPf8N_JPEG/1030058150967789_1562127427.jpg</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>무선 온열 칫솔 살균기</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>칫솔 세균 걱정 끝! 온열 기능으로 깨끗하고 위생적인 칫솔 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>온열 열판 무선 칫솔 살균기 사용법 추천</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>온열 기능이 더해진 무선 칫솔 살균기로 세균 걱정 없이 위생적인 칫솔 관리를 할 수 있습니다. 간편하고 효과적인 사용법을 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I323" t="inlineStr">
+        <is>
+          <t>칫솔 살균기,무선 칫솔 살균,온열 칫솔 소독,위생 칫솔 관리,칫솔 세균 제거,무선 살균기,칫솔 위생,온열 기능 칫솔</t>
+        </is>
+      </c>
+      <c r="J323" t="inlineStr">
+        <is>
+          <t>위생/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>323</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>주방 공간 효율 높이는 자외선 살균 보관함</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://naver.me/x9zEK1SQ</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250124_119/1737685227026KEsPP_JPEG/51065208881595295_1774086517.jpg</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>자외선 살균 보관함</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>주방 위생과 공간 고민을 한번에 해결해주는 자외선 살균 보관함으로 신선함을 오래 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>주방 공간 효율 자외선 살균 보관함 추천</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>주방 위생과 공간 활용에 좋은 자외선 살균 보관함으로 식품 신선도 유지에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I324" t="inlineStr">
+        <is>
+          <t>자외선살균,주방보관함,위생보관,공간활용,식품신선,살균보관함</t>
+        </is>
+      </c>
+      <c r="J324" t="inlineStr">
+        <is>
+          <t>주방용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>324</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>휴대용 UV 살균기로 골프 필드 위생까지 챙기기</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://naver.me/F6nhqFvA</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250328_6/1743125566782ffnla_PNG/33896427682498019_973408185.png</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>휴대용 UV 살균기</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>골프 필드에서도 깨끗한 위생 관리가 필요하신가요? 휴대용 UV 살균기로 간편하게 세균 걱정 없이 안전하게 사용하세요.</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>휴대용 UV 살균기 골프 위생 관리 추천</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>골프 필드에서도 청결한 위생을 유지할 수 있는 휴대용 UV 살균기로 간편하고 안전하게 사용하세요.</t>
+        </is>
+      </c>
+      <c r="I325" t="inlineStr">
+        <is>
+          <t>휴대용 UV 살균기,골프 위생,세균 제거,안전 살균,간편 살균</t>
+        </is>
+      </c>
+      <c r="J325" t="inlineStr">
+        <is>
+          <t>골프/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>325</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 간편하게 휴대 가능한 프롬비 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ZSbGwp2</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251201_51/1764578577506CqQS9_PNG/111543845316792026_1951245759.png</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편하게 칫솔을 깨끗하게 관리하세요. 언제 어디서나 위생적인 구강케어를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>프롬비 칫솔살균기 출퇴근 시 휴대용 위생관리 추천</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편하게 휴대 가능한 프롬비 칫솔살균기로 언제 어디서나 구강 위생을 효과적으로 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I326" t="inlineStr">
+        <is>
+          <t>프롬비,칫솔살균기,휴대용,출퇴근,구강위생,위생관리,휴대칫솔살균기</t>
+        </is>
+      </c>
+      <c r="J326" t="inlineStr">
+        <is>
+          <t>건강/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>326</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>출퇴근 가방에 쏙 들어가는 휴대용 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://naver.me/565TeQE0</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230615_256/16868031990834uu8P_JPEG/62090092658678_321636576.jpg</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>출퇴근 중 칫솔 걱정 끝! 간편한 휴대로 언제 어디서나 깨끗한 칫솔 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>출퇴근 가방에 쏙 휴대용 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>출퇴근 중에도 간편하게 휴대 가능한 칫솔살균기로 언제 어디서나 깨끗한 칫솔 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I327" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔살균기, 출퇴근 칫솔 관리, 간편 칫솔살균, 휴대 칫솔살균기, 깨끗한 칫솔</t>
+        </is>
+      </c>
+      <c r="J327" t="inlineStr">
+        <is>
+          <t>생활용품/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>327</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>집에서 간편하게 충전하는 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://naver.me/xslfAFd2</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251124_168/1763968762791QsHSS_PNG/12674323526927895_1553026111.png</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>간편 충전 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>칫솔 속 세균 걱정되시나요? 집에서 쉽고 빠르게 충전해 청결을 지키세요.</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>집에서 간편 충전 칫솔살균기 추천, 청결 관리 필수템</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>간편한 충전 방식으로 집에서 손쉽게 칫솔을 살균하여 청결한 구강 관리를 돕는 칫솔살균기 추천 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>칫솔살균기,충전식칫솔살균기,구강관리,집에서사용,세균제거,칫솔살균,간편충전</t>
+        </is>
+      </c>
+      <c r="J328" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>328</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>칫솔을 청결하게 지켜주는 휴대용 휴대 아이템</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://naver.me/G02cCRTA</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251001_256/1759283258438mUSsP_JPEG/13728717274370336_533321072.jpg</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>휴대용 칫솔 살균기</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>외출 시 칫솔 청결 걱정 끝! 간편하게 휴대하며 깨끗함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>칫솔 청결 휴대용 케이스 추천 - 깔끔하게 관리하세요</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>외출 시 칫솔을 위생적으로 보관할 수 있는 휴대용 아이템으로 간편하게 청결을 유지합니다.</t>
+        </is>
+      </c>
+      <c r="I329" t="inlineStr">
+        <is>
+          <t>칫솔케이스,휴대용칫솔통,칫솔보관,위생칫솔,여행용칫솔케이스</t>
+        </is>
+      </c>
+      <c r="J329" t="inlineStr">
+        <is>
+          <t>위생용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>329</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편한 휴대폰소독기 사용법</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://naver.me/G5Pm1WTz</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220425_89/1650894035469sCgsR_JPEG/52029931188685548_1626230221.jpg</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>간편 휴대폰 소독기</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 스마트폰 청결이 걱정되시나요? 언제 어디서나 깨끗하게 소독하세요.</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>출퇴근길 휴대폰소독기 사용법 추천 - 간편한 스마트폰 소독</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 간편하게 휴대폰을 깨끗하게 소독하는 방법을 소개합니다. 스마트폰 청결에 신경 쓰는 분들에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I330" t="inlineStr">
+        <is>
+          <t>휴대폰소독기,스마트폰소독,휴대폰청결,출퇴근소독,사용법,간편소독,휴대용소독기</t>
+        </is>
+      </c>
+      <c r="J330" t="inlineStr">
+        <is>
+          <t>생활용품/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>330</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>에스테틱 업소 필수품, 자외선 수건 살균기의 휴대성</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://naver.me/xLseZCQt</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231124_238/1700832322886WMpbq_JPEG/28135006761875050_665139029.jpg</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>휴대용 자외선 수건 살균기</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>깨끗한 위생을 위한 필수 아이템, 언제 어디서나 간편하게 수건을 살균하세요.</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>에스테틱 업소 필수 자외선 수건 살균기 휴대용 추천</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>에스테틱 업소에서 위생을 지키는 자외선 수건 살균기입니다. 휴대가 간편해 언제 어디서나 깨끗한 수건을 유지할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I331" t="inlineStr">
+        <is>
+          <t>에스테틱,자외선살균기,수건살균기,휴대용살균기,위생관리,업소필수</t>
+        </is>
+      </c>
+      <c r="J331" t="inlineStr">
+        <is>
+          <t>에스테틱/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>331</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>운동 후 신발을 빠르게 건조하고 살균하는 편리한 신발 스타일러</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://naver.me/5AgC8JPb</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240830_94/1724945476887cYp8o_JPEG/50145569590671388_1220978015.jpg</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>운동화 빠른 건조와 살균</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 신발 걱정 없이 빠르게 건조하고 살균해 청결하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>운동 후 신발 스타일러로 빠른 건조와 살균 추천</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 신발을 빠르게 건조하고 살균하여 청결하게 관리할 수 있는 신발 스타일러입니다. 편리한 사용으로 쾌적한 신발 환경 유지에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>운동화 건조기,신발 살균기,신발 스타일러,운동 후 신발 관리,빠른 신발 건조,살균 신발 건조기</t>
+        </is>
+      </c>
+      <c r="J332" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>332</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>운동 후 휴대용 구강세정기로 깔끔한 마무리하기</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://naver.me/GZ6rqzm1</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_248/1761276428010sqEV8_JPEG/33810872320662127_1106136919.jpg</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>운동 후 휴대용 구강세정기</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>운동 후 입안 청결이 걱정되시나요? 휴대용 구강세정기로 깔끔하게 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>운동 후 휴대용 구강세정기로 입안 깔끔하게 마무리 추천</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>운동 후 휴대하기 편한 구강세정기로 입안을 청결하게 관리하세요. 간편한 사용법으로 언제 어디서나 활용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I333" t="inlineStr">
+        <is>
+          <t>휴대용 구강세정기, 운동 후 구강관리, 입안 청결, 휴대 간편 구강세정기, 구강 위생, 운동용 구강세정기</t>
+        </is>
+      </c>
+      <c r="J333" t="inlineStr">
+        <is>
+          <t>헬스/구강관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>333</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>운동 후 빠르게 건조하고 살균하는 스타일에어의 장점</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://naver.me/G9pTEC19</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251218_233/1766044751615AHVdP_JPEG/43457833704754297_696634848.jpg</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>운동복 빠른건조 살균</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 옷 냄새와 세균 고민 없이 스타일에어로 쾌적하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>스타일에어 운동복 빠른 건조와 살균 추천</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 옷의 냄새와 세균을 효과적으로 제거하는 스타일에어로 쾌적하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>스타일에어,운동복 건조,살균,냄새제거,운동 후 관리</t>
+        </is>
+      </c>
+      <c r="J334" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>334</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>운동 후에도 안심! 휴대용 UV 자외선 살균기로 위생 챙기기</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlb7QzPo</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200516_65/1589610452982hBQiX_JPEG/26971995611326808_911477727.jpg</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>휴대용 UV 자외선 살균기</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>운동 후 불안한 위생 걱정, 간편한 휴대용 UV 살균기로 깨끗하게 케어하세요.</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>운동 후 위생 관리 추천 휴대용 UV 자외선 살균기 구매</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>운동 후 손쉽게 사용하는 휴대용 UV 자외선 살균기로 위생 걱정 없이 깨끗하게 관리하세요. 간편하고 안전한 위생 케어 도구입니다.</t>
+        </is>
+      </c>
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>휴대용 자외선 살균기,UV 살균기,운동 위생,휴대용 살균기,손살균,위생관리</t>
+        </is>
+      </c>
+      <c r="J335" t="inlineStr">
+        <is>
+          <t>위생/헬스</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>335</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>UV-C 기술로 운동 후 칫솔을 깨끗하게 관리하는 방법</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://naver.me/ID3QYJXb</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250814_280/1755158725997kyPj9_JPEG/3796318116698175_201338981.jpg</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 UV-C 살균</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>운동 후 세균 걱정 없이 칫솔을 안전하게 관리하세요. UV-C 기술로 깨끗함을 유지해 드립니다.</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>UV-C 기술 활용한 운동 후 칫솔 안전 관리법 추천</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔을 UV-C 기술로 깨끗하고 위생적으로 관리해 세균 걱정 없이 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>UV-C 칫솔살균, 운동 후 칫솔관리, 칫솔 세균제거, 위생 칫솔, 건강 관리</t>
+        </is>
+      </c>
+      <c r="J336" t="inlineStr">
+        <is>
+          <t>건강관리/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>336</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>화장실 공간 절약에 좋은 벽걸이형 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://naver.me/FdonjNIM</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241014_229/1728916636265MFCln_JPEG/__uv_uv___resize.jpg</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>벽걸이 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>좁은 화장실 공간도 깔끔하게! 벽걸이형 칫솔살균기로 깨끗한 위생을 지켜보세요.</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>벽걸이형 칫솔살균기 추천 화장실 공간 절약용 위생기기</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>좁은 화장실 공간에 최적화된 벽걸이형 칫솔살균기로 깔끔하고 위생적인 관리가 가능합니다. 공간 절약과 청결을 동시에 만족시켜줍니다.</t>
+        </is>
+      </c>
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>벽걸이형 칫솔살균기,칫솔 살균,화장실 공간 절약,위생기기,칫솔관리,청결용품</t>
+        </is>
+      </c>
+      <c r="J337" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>337</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>출퇴근 전 간편하게 챙기는 욕실 칫솔살균기 팁</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://naver.me/FwjWV1XZ</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241011_234/1728653926036qdMD2_JPEG/WDM_W8B7630_resize.jpg</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>간편 욕실 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>출퇴근 전 칫솔 위생 걱정 끝! 간편하게 살균해 건강한 미소를 지켜보세요.</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>출퇴근 필수 욕실 칫솔살균기 추천, 간편 위생 관리</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>출퇴근 전 간편하게 칫솔을 살균해 위생 걱정 없이 건강한 미소를 유지하세요. 소형으로 욕실 어디에나 설치 가능해 실용적입니다.</t>
+        </is>
+      </c>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>칫솔살균기,욕실용품,칫솔위생,출퇴근필수,간편살균,건강미소,소형살균기</t>
+        </is>
+      </c>
+      <c r="J338" t="inlineStr">
+        <is>
+          <t>욕실/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>338</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>운동 후 전동 칫솔 살균기로 위생적인 관리법</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://naver.me/xXwZfdm3</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241011_279/1728658256741VjRId_JPEG/WDM_W99DBE3_resize.jpg</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 살균</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔에 남은 세균 걱정 없이 위생적으로 관리하세요. 깔끔한 구강 건강을 위해 꼭 필요한 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>운동 후 전동 칫솔 살균기 추천, 위생적 구강 관리법</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 세균 걱정 없이 간편하게 살균하여 위생적인 구강 관리를 도와주는 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>전동칫솔, 칫솔살균기, 구강관리, 위생제품, 운동후관리</t>
+        </is>
+      </c>
+      <c r="J339" t="inlineStr">
+        <is>
+          <t>건강/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>339</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 간편하게 휴대 가능한 프롬비 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ZSbGwp2</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251201_51/1764578577506CqQS9_PNG/111543845316792026_1951245759.png</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>간편 휴대 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 깨끗한 칫솔 관리가 고민이라면, 휴대가 쉬운 프롬비 칫솔살균기로 위생 걱정을 덜어보세요.</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>프롬비 칫솔살균기 휴대용 추천 출퇴근 위생관리</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>출퇴근 시 간편한 휴대와 깨끗한 칫솔 살균으로 위생 걱정을 덜어줍니다. 휴대용 칫솔살균기로 청결관리가 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>프롬비, 칫솔살균기, 휴대용, 출퇴근, 위생관리, 칫솔청결, 휴대간편, 살균기추천</t>
+        </is>
+      </c>
+      <c r="J340" t="inlineStr">
+        <is>
+          <t>생활용품/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>340</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>집에서 간편하게 충전하는 칫솔살균기 추천</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://naver.me/xslfAFd2</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251124_168/1763968762791QsHSS_PNG/12674323526927895_1553026111.png</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>간편 충전 칫솔살균기</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>칫솔 위생 걱정 끝! 집에서 간편하게 충전하며 깨끗하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>집에서 간편하게 충전하는 칫솔살균기 추천, 위생 관리 필수템</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>칫솔 위생 걱정을 덜어주는 칫솔살균기로 간편 충전과 깨끗한 관리가 가능합니다. 가족 모두 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>칫솔살균기,칫솔위생,충전식살균기,위생관리,가정용살균기,칫솔관리</t>
+        </is>
+      </c>
+      <c r="J341" t="inlineStr">
+        <is>
+          <t>위생/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>341</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>운동 후에도 신경 쓰이는 칫솔을 깨끗하게 하는 휴대용 살균기</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://naver.me/FHVd82GL</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231220_97/1703039542245hIDz7_JPEG/104175440939395322_1940114033.jpg</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 살균기</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>운동 후에도 칫솔 위생이 걱정된다면, 휴대용 살균기로 깨끗하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>운동 후 칫솔 위생 관리 휴대용 살균기 추천</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>운동 후에도 칫솔을 깨끗하게 유지하는 휴대용 살균기로 언제 어디서나 위생 관리를 간편하게 하세요.</t>
+        </is>
+      </c>
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>휴대용 살균기,칫솔 살균기,운동 후 칫솔 관리,칫솔 위생,휴대용 위생기</t>
+        </is>
+      </c>
+      <c r="J342" t="inlineStr">
+        <is>
+          <t>위생/헬스</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>342</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 간편하게 사용할 수 있는 저온 가열식 가습기</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://naver.me/xumtTVW6</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251212_253/1765533253007x9CRl_JPEG/41151299491326722_1218782561.jpg</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>저온 가열식 간편 가습기</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 간편하게 촉촉함을 유지하세요. 저온 가열식으로 안전한 가습을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>출퇴근 길 저온 가열식 가습기 추천</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 간편하게 사용할 수 있는 저온 가열식 가습기로 안전하고 쾌적한 실내 환경을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>가습기,저온가열식,출퇴근,간편사용,안전가습,실내습도조절</t>
+        </is>
+      </c>
+      <c r="J343" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>343</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>출퇴근길 골프 연습에 적합한 볼빅 플라이온 4구 세트</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQik9G3g</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251202_108/176464942858726UYR_JPEG/18754969627384816_727862273.jpg</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>출퇴근용 골프 연습볼 4구</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>출퇴근길 짧은 시간에도 골프 연습을 완벽하게! 볼빅 플라이온 4구 세트로 실력 향상을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>출퇴근길 골프 연습 추천 볼빅 플라이온 4구 세트 할인 구매</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>볼빅 플라이온 4구 세트로 출퇴근 시간 짧은 골프 연습에도 실력 향상에 도움을 줍니다. 휴대가 간편한 골프 연습용 볼입니다.</t>
+        </is>
+      </c>
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>볼빅, 플라이온, 골프 연습, 출퇴근 연습, 골프볼 세트, 골프 용품, 실력 향상</t>
+        </is>
+      </c>
+      <c r="J344" t="inlineStr">
+        <is>
+          <t>골프/스포츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>344</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>간편하게 설치하는 난방텐트, 집에서 편안한 휴대용 공간</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://naver.me/5u9fZjpb</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250925_238/1758798052124RC17z_JPEG/10370016234276854_1777386343.jpg</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>간편 설치 난방 텐트</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>추운 날씨, 집 안에서도 따뜻하고 편안한 공간을 원하시나요? 간편한 설치로 온기 가득한 휴대용 난방 텐트입니다.</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>간편 설치 휴대용 난방텐트 추천, 집에서 따뜻한 공간 만들기</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>간편하게 설치 가능한 휴대용 난방텐트로 집안에서도 따뜻하고 아늑한 공간을 제공합니다. 추운 날씨에 실내 난방 보조용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>난방텐트,휴대용난방텐트,실내텐트,난방보조,온열텐트,따뜻한실내,간편설치,홈캠핑</t>
+        </is>
+      </c>
+      <c r="J345" t="inlineStr">
+        <is>
+          <t>난방/홈캠핑</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>345</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>수면 시간을 더 포근하게 만드는 난방 텐트의 매력</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://naver.me/GagBxt3p</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251031_219/1761890680656TqoSn_PNG/17099738451677415_195885521.png</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>포근한 수면 난방 텐트</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>추운 밤에도 따뜻하게 감싸주는 난방 텐트로 편안한 숙면을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>난방 텐트 추천 수면 시간을 더 포근하게 만드는 제품</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>추운 밤에도 따뜻하게 감싸주는 난방 텐트로 편안한 숙면을 도와줍니다. 겨울철 집안 어디서나 사용 가능해 실용적입니다.</t>
+        </is>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>난방텐트,수면텐트,난방용품,겨울용품,숙면도우미,포근한잠,텐트난방</t>
+        </is>
+      </c>
+      <c r="J346" t="inlineStr">
+        <is>
+          <t>가전/침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>346</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>겨울철 실내 난방텐트 착용감과 보온성 비교해봤어요</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://naver.me/5r3biKkO</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251105_46/1762338327981HG3g1_JPEG/874295975826462_969390051.jpg</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>겨울철 보온 난방텐트</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>추운 겨울, 실내에서도 따뜻하게 머무르고 싶다면 보온성 뛰어난 난방텐트를 선택하세요.</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>겨울철 실내 난방텐트 보온성 비교 추천</t>
+        </is>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>추운 겨울 실내에서 따뜻하게 머물 수 있는 보온성 좋은 난방텐트를 비교해 소개합니다. 착용감과 효율성을 고려한 선택 가이드입니다.</t>
+        </is>
+      </c>
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>난방텐트,실내난방,보온텐트,겨울템트,난방용품,겨울보온</t>
+        </is>
+      </c>
+      <c r="J347" t="inlineStr">
+        <is>
+          <t>난방/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>347</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식 시간, 방한텐트에서 느끼는 따뜻함</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://naver.me/FDGOUdrI</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20180928_95/snsnumber1_15381245135395cV4F_JPEG/61430814158992040_577471647.jpg</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>따뜻한 방한텐트 휴식</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>출퇴근 후 차가운 바깥 걱정 없이, 방한텐트에서 편안한 온기를 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식, 방한텐트로 따뜻함 추천</t>
+        </is>
+      </c>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>출퇴근 후 찬 바람 걱정 없이 방한텐트에서 편안하고 따뜻한 휴식을 제공합니다. 겨울철 실내외 온기 유지에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>출퇴근, 방한텐트, 따뜻한휴식, 온기, 겨울용텐트, 실내텐트, 휴식공간</t>
+        </is>
+      </c>
+      <c r="J348" t="inlineStr">
+        <is>
+          <t>생활용품/텐트</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>348</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>실내 보온에 탁월한 원터치 난방텐트, 출퇴근 후 휴식에 딱</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://naver.me/5sGYlA1e</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251110_241/1762753149055232Ch_PNG/17441192030941110_367153971.png</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>원터치 난방텐트</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>추운 실내에 따뜻함을 더하는 난방텐트로 퇴근 후 휴식을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>원터치 난방텐트 실내 보온 추천, 출퇴근 후 휴식에 딱</t>
+        </is>
+      </c>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>실내 추위 걱정 없이 편안한 휴식을 돕는 원터치 난방텐트로 퇴근 후 따뜻하게 쉴 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>난방텐트,원터치텐트,실내보온,휴식템트,겨울텐트,난방용품,온열텐트</t>
+        </is>
+      </c>
+      <c r="J349" t="inlineStr">
+        <is>
+          <t>생활가전/난방용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>349</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식 공간으로 활용하는 스위트 플레이텐트</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://naver.me/xcATmMvJ</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250331_186/1743390479339KVavf_JPEG/31283975422409586_871236657.jpg</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>편안한 휴식 공간 텐트</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸과 마음을 위한 아늑한 휴식 공간, 집에서도 간편하게 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>스위트 플레이텐트 출퇴근 후 휴식 추천 아늑한 홈 공간</t>
+        </is>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸과 마음을 위한 아늑한 휴식 공간, 집에서 간편하게 휴식을 즐길 수 있는 플레이텐트입니다.</t>
+        </is>
+      </c>
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>스위트 플레이텐트, 휴식 공간, 출퇴근 휴식, 홈 플레이텐트, 아늑한 텐트, 간편 설치, 집안 휴식</t>
+        </is>
+      </c>
+      <c r="J350" t="inlineStr">
+        <is>
+          <t>생활용품/휴식</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>350</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>더블 사이즈 방한용 텐트로 편안한 휴식 공간 만들기</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://naver.me/GNREztT7</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241022_52/1729595873009hAGKM_JPEG/main_image_resize.jpg</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>더블 사이즈 방한 텐트</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>춥고 바람 부는 날에도 따뜻하게 쉴 수 있는 넉넉한 방한 텐트로 편안한 휴식 공간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>더블 사이즈 방한용 텐트 추천 - 따뜻한 휴식 공간 만들기</t>
+        </is>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>넉넉한 크기의 더블 사이즈 방한 텐트로 추위와 바람을 막아 따뜻하고 편안한 휴식 공간을 제공합니다. 가족 캠핑이나 야외 활동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>더블 사이즈 텐트, 방한 텐트, 겨울 캠핑, 방풍 텐트, 휴식 공간, 야외 텐트, 가족 캠핑</t>
+        </is>
+      </c>
+      <c r="J351" t="inlineStr">
+        <is>
+          <t>캠핑/방한</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>351</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>슈퍼싱글 사이즈로 집 안 어디서든 편리한 보온 텐트</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://naver.me/xv6VXmnP</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231108_72/1699416855049K0mw3_JPEG/13356121891583604_190548832.jpg</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>슈퍼싱글 보온 텐트</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>집 안 어디서나 따뜻하게, 슈퍼싱글 보온 텐트로 쾌적한 공간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>슈퍼싱글 보온 텐트 집안 어디서든 따뜻하게 추천</t>
+        </is>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>슈퍼싱글 사이즈 보온 텐트로 집안 어디서든 쾌적하고 따뜻한 공간을 만들 수 있습니다. 간편 설치로 실내 생활을 더 편리하게 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>보온텐트,슈퍼싱글텐트,실내용텐트,집안텐트,따뜻한텐트,보온용텐트,실내보온,편리한텐트</t>
+        </is>
+      </c>
+      <c r="J352" t="inlineStr">
+        <is>
+          <t>가정용품/보온</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>352</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식 시간에 좋은 방풍 난방 텐트</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://naver.me/FwjgudQB</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231108_183/1699417102467l83YH_JPEG/19770830424171726_80191518.jpg</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>따뜻한 방풍 난방 텐트</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>출퇴근 후 추위를 막아주는 방풍 텐트로 포근한 휴식을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식용 방풍 난방 텐트 추천</t>
+        </is>
+      </c>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>출퇴근 후 추운 날씨에도 포근한 휴식을 도와주는 방풍 난방 텐트입니다. 간편 설치로 실내외 모두 사용 가능해 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>방풍텐트,난방텐트,휴식템트,출퇴근용품,겨울용품,방한텐트</t>
+        </is>
+      </c>
+      <c r="J353" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-22 05:13)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J353"/>
+  <dimension ref="A1:J406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18085,6 +18085,2656 @@
         </is>
       </c>
     </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>353</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>8중 필터가 적용된 닥터제로 샤워기헤드 사용 후기</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://naver.me/FswMoetJ</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250826_226/1756193150503T6cDW_JPEG/45009920297856469_919990096.jpg</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>8중 필터 샤워기</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>깨끗한 물로 피부 고민까지 해결해보세요. 8중 필터로 안심하고 사용하는 샤워기입니다.</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>8중 필터 닥터제로 샤워기헤드 사용 후기 추천</t>
+        </is>
+      </c>
+      <c r="H354" t="inlineStr">
+        <is>
+          <t>8중 필터로 깨끗한 물을 제공해 피부 고민을 완화하고 안심하고 사용할 수 있는 닥터제로 샤워기헤드입니다.</t>
+        </is>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>샤워기,샤워기헤드,필터샤워기,닥터제로,피부관리,깨끗한물,샤워기추천</t>
+        </is>
+      </c>
+      <c r="J354" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>354</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>샤워기헤드 교체로 녹물 걱정 없이 출퇴근 준비</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1m6uLGw</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250717_277/1752715115631iwrkb_PNG/86847917111930370_1598608558.png</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>녹물 걱정 없는 샤워기헤드</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>출퇴근 전 깨끗한 샤워를 원한다면 녹물 없는 샤워기헤드로 건강한 습관을 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>녹물 없는 샤워기헤드 교체로 건강한 출퇴근 준비 추천</t>
+        </is>
+      </c>
+      <c r="H355" t="inlineStr">
+        <is>
+          <t>녹물 걱정 없이 깨끗한 물로 샤워할 수 있는 샤워기헤드로 매일 건강한 습관을 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>샤워기헤드,녹물제거,깨끗한물,건강샤워,교체용샤워기</t>
+        </is>
+      </c>
+      <c r="J355" t="inlineStr">
+        <is>
+          <t>욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>355</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>출퇴근 전 상쾌한 기분, 4단 필터 샤워기의 힘</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://naver.me/xpBFjyXW</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250612_167/1749705923470qXM5l_JPEG/25324025951444757_1181802633.jpg</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>상쾌한 4단 필터 샤워기</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>출퇴근길 피로를 씻어내는 4단 필터 샤워기로 깨끗하고 상쾌한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>출퇴근 전 상쾌한 기분을 위한 4단 필터 샤워기 추천</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>4단 필터가 불순물을 걸러내어 깨끗한 물로 출퇴근 전 피로를 씻어내고 상쾌한 하루를 시작할 수 있는 샤워기입니다.</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>4단 필터 샤워기, 상쾌한 샤워, 깨끗한 물, 피로 해소, 출퇴근 샤워기</t>
+        </is>
+      </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>생활/위생</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>356</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>출퇴근 후 운동 후 깨끗한 물로 리프레시하는 샤워기 추천</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gf0Fr4Kc</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230726_149/1690336329830yu827_JPEG/744018671355859_1762111595.jpg</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>깨끗한 물 샤워기</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>출퇴근과 운동 후, 불순물 없는 깨끗한 물로 상쾌하게 리프레시하세요.</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>출퇴근 운동 후 깨끗한 물 샤워기 추천으로 상쾌한 리프레시</t>
+        </is>
+      </c>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>출퇴근과 운동 후에 불순물 없는 깨끗한 물로 피부를 상쾌하게 관리할 수 있는 샤워기입니다. 건강한 라이프스타일에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>샤워기,깨끗한물,운동후샤워,출퇴근리프레시,피부관리,정수샤워기,건강생활</t>
+        </is>
+      </c>
+      <c r="J357" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>357</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로 풀기 좋은 수압상승 샤워기 선택법</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://naver.me/5owf0LmH</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231103_65/1698972127761BVT9F_JPEG/23233352176719783_655586231.jpg</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>피로회복 수압상승 샤워기</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 피로, 강력한 수압으로 말끔하게 풀어보세요. 상쾌한 하루의 시작과 마무리를 돕습니다.</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>출퇴근 피로 해소 수압상승 샤워기 추천</t>
+        </is>
+      </c>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>강력한 수압으로 출퇴근 후 쌓인 피로를 풀어주는 샤워기 추천, 상쾌한 하루 시작과 마무리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>수압상승 샤워기, 피로 해소, 출퇴근 샤워, 강력 수압, 샤워기 추천, 피로 풀기, 샤워 용품</t>
+        </is>
+      </c>
+      <c r="J358" t="inlineStr">
+        <is>
+          <t>생활용품/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>358</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>집에서도 스파 같은 고압 샤워를 즐기는 방법</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://naver.me/FhfFuBXj</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230103_183/1672730919641OgKqh_JPEG/73866815368639841_1187014424.jpg</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>집에서도 즐기는 고압 샤워</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>집에서도 스파처럼 시원한 고압 샤워로 피로를 풀고 상쾌함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>고압 샤워기 추천 집에서도 스파 같은 시원한 샤워 즐기기</t>
+        </is>
+      </c>
+      <c r="H359" t="inlineStr">
+        <is>
+          <t>집에서도 스파처럼 시원한 고압 샤워기로 피로를 효과적으로 풀고 상쾌한 기분을 느껴보세요. 간편하게 설치 가능한 샤워기입니다.</t>
+        </is>
+      </c>
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>고압 샤워기,스파 샤워,집에서 고압 샤워,시원한 샤워,피로 해소,상쾌함,욕실용품</t>
+        </is>
+      </c>
+      <c r="J359" t="inlineStr">
+        <is>
+          <t>욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>359</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>욕실 분위기를 바꾸는 수압 좋은 샤워기 헤드</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://naver.me/59UglCDR</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210806_135/1628208397436DWBf2_JPEG/29344240152840990_58729648.jpg</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>강력 수압 샤워기 헤드</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>약한 수압에 답답했던 당신, 강력한 수압으로 상쾌한 샤워 시간을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>수압 좋은 샤워기 헤드 추천, 욕실 분위기 혁신</t>
+        </is>
+      </c>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>약한 수압 문제를 해결해주는 강력한 샤워기 헤드로 쾌적한 샤워 환경을 제공합니다. 욕실 분위기를 새롭게 바꾸고 싶은 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>샤워기,수압 좋은 샤워기,욕실용품,샤워기헤드,수압강화,욕실 분위기,샤워기 교체,수압 문제 해결</t>
+        </is>
+      </c>
+      <c r="J360" t="inlineStr">
+        <is>
+          <t>욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>360</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>AI 기술이 적용된 세비앙 샤워기로 집에서 편안함을</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://naver.me/5DDdZmMQ</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210203_55/1612314355377q2xwd_JPEG/13450189143019508_956228451.jpg</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>AI 자동 온도 조절 샤워기</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻한 샤워를 원하는 당신을 위해, AI가 온도를 자동 조절해 쾌적한 목욕 시간을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>AI 기술 적용 세비앙 샤워기 추천, 자동 온도 조절로 편안함</t>
+        </is>
+      </c>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>AI 온도 자동 조절 기능으로 추운 날씨에도 쾌적한 샤워를 제공하는 세비앙 샤워기입니다. 집에서 편안한 목욕 시간을 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>세비앙 샤워기, AI 샤워기, 자동 온도 조절, 따뜻한 샤워, 쾌적한 목욕, 집에서 샤워</t>
+        </is>
+      </c>
+      <c r="J361" t="inlineStr">
+        <is>
+          <t>욕실,생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>361</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>출퇴근 후 도레이 샤워기로 모발과 피부를 건강하게 케어</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://naver.me/xCtbjYV8</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230106_59/1672973070178a2jPT_JPEG/74108968879451275_2117507430.jpg</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>모발과 피부 건강 샤워기</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로한 모발과 피부를 부드럽게 케어해주는 샤워기로 상쾌함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>출퇴근 후 도레이 샤워기 추천, 건강한 모발과 피부 케어</t>
+        </is>
+      </c>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로한 모발과 피부를 부드럽게 관리해주는 도레이 샤워기로 상쾌함과 촉촉함을 동시에 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>도레이샤워기,모발케어,피부케어,출퇴근샤워기,샤워기추천,건강한피부,상쾌한샤워</t>
+        </is>
+      </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>생활/욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>362</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>스마트 기능이 돋보이는 세비앙 샤워기로 쾌적한 샤워 타임</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://naver.me/GcKxAq8N</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20190711_242/cebien_1562833635633kTfL4_JPEG/193470205221114_1786022386.jpg</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>스마트 샤워기 쾌적한 세정</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>물 절약은 물론 청결까지 챙기는 스마트 샤워기로 상쾌한 샤워 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>스마트 세비앙 샤워기 추천 물 절약과 청결 관리</t>
+        </is>
+      </c>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>스마트 기능이 적용된 세비앙 샤워기로 물 절약뿐만 아니라 청결한 샤워 환경을 제공합니다. 쾌적하고 상쾌한 샤워 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>스마트샤워기,세비앙,물절약,청결관리,샤워기추천,욕실용품</t>
+        </is>
+      </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>욕실/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>363</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>집에서도 쉽게 누리는 두피 마사지와 절수 효과</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://naver.me/5R4lA5DL</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240503_48/1714715392972UYWKU_PNG/115851281641758368_1027845630.png</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>편안한 두피 마사지</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>일상 속 두피 고민, 집에서 간편하게 관리해보세요. 절수 효과로 환경까지 생각한 스마트 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>두피 마사지기 절수 효과로 집에서 간편 관리 추천</t>
+        </is>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>집에서 쉽게 두피 마사지를 경험하며 절수 효과로 환경까지 고려한 스마트한 두피 관리기입니다.</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>두피 마사지, 절수, 두피 관리, 집에서 마사지, 환경 친화, 스마트 두피기기</t>
+        </is>
+      </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>건강/뷰티</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>364</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로를 씻어내는 소프롱 샤워기 헤드</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://naver.me/xQitJg07</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200724_144/15955753094714wBSK_JPEG/32936852094189456_1709929947.jpg</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>피로 해소 샤워기 헤드</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>하루 종일 쌓인 피로, 상쾌한 물줄기로 말끔히 씻어내세요.</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>소프롱 샤워기 헤드 추천 출퇴근 후 피로 해소용</t>
+        </is>
+      </c>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>소프롱 샤워기 헤드로 상쾌한 물줄기를 경험하며 출퇴근 후 쌓인 피로를 효과적으로 씻어내 보세요.</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>소프롱,샤워기,샤워기헤드,피로해소,출퇴근,상쾌한샤워</t>
+        </is>
+      </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>365</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>출퇴근 후 상쾌함을 주는 수압상승 샤워기 사용기</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://naver.me/x0XeOHgx</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250427_184/1745764104795F2mJv_JPEG/273804197159851_1358893843.jpg</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>수압상승 상쾌 샤워기</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로한 당신, 강력한 수압으로 상쾌함을 느껴보세요. 매일의 샤워가 힐링 타임으로 변합니다.</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>수압상승 샤워기 추천 출퇴근 후 상쾌한 힐링 샤워 용품</t>
+        </is>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>강력한 수압으로 출퇴근 후 피로를 해소하는 샤워기입니다. 매일 상쾌한 힐링 타임을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>수압상승 샤워기, 상쾌한 샤워, 피로해소, 출퇴근, 힐링 샤워, 욕실용품, 샤워기 추천</t>
+        </is>
+      </c>
+      <c r="J366" t="inlineStr">
+        <is>
+          <t>욕실/샤워기</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>366</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>출퇴근 후 녹물제거 샤워기로 피부를 부드럽게 케어</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://naver.me/GsowBmGl</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230224_272/1677215500538vSp0T_JPEG/4518184365595438_1825950055.jpg</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>녹물제거 샤워기로 피부케어</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>출퇴근 후 녹물 걱정 없이 부드러운 피부를 케어해보세요. 깨끗한 물로 건강한 샤워 시간을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>출퇴근 후 녹물제거 샤워기 추천, 피부 부드럽게 케어</t>
+        </is>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>녹물 걱정 없이 깨끗한 물로 피부를 부드럽게 케어하는 샤워기로 건강한 샤워 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>녹물제거 샤워기, 피부케어, 깨끗한샤워, 출퇴근필수, 건강샤워기</t>
+        </is>
+      </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>367</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>출퇴근 후 스트레스 완화에 좋은 클라리스트 미스트샤워기</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://naver.me/FivePtcY</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250210_198/1739174932010dwbkc_JPEG/73307720154051791_1353795410.jpg</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>스트레스 완화 미스트샤워기</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 스트레스를 부드러운 미스트로 풀어보세요. 상쾌한 샤워로 하루를 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>클라리스트 미스트샤워기 출퇴근 스트레스 완화 추천</t>
+        </is>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 스트레스를 부드러운 미스트로 완화하는 클라리스트 미스트샤워기입니다. 상쾌한 샤워로 하루를 편안하게 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>미스트샤워기,스트레스완화,출퇴근피로,샤워기추천,상쾌한샤워</t>
+        </is>
+      </c>
+      <c r="J368" t="inlineStr">
+        <is>
+          <t>건강,생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>368</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>리필필터 교체로 샤워기 성능 오래 유지하는 법</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://naver.me/FpPkw3E8</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250211_178/1739239723772gAg7p_JPEG/491033913287228_1413590909.jpg</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>샤워기 필터 교체법</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>깨끗한 물로 상쾌한 샤워, 필터 교체로 청결함과 성능을 오래 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>리필필터 교체로 샤워기 성능 오래 유지하는 법 추천</t>
+        </is>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>깨끗한 물로 상쾌한 샤워를 즐기고, 필터 교체로 샤워기 성능과 청결함을 오래 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>리필필터, 샤워기필터, 필터교체, 샤워청결, 물필터, 샤워기성능, 수질관리</t>
+        </is>
+      </c>
+      <c r="J369" t="inlineStr">
+        <is>
+          <t>생활용품/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>369</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>출퇴근 후 상쾌함을 더해주는 프리미엄 미스트샤워기 사용기</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://naver.me/59UglCTa</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250211_27/1739239698049fNli5_JPEG/54255512934056154_2067882630.jpg</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>상쾌함 선사 미스트샤워기</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸과 마음을 편안하게 감싸주는 미스트샤워기로 상쾌한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>프리미엄 미스트샤워기 추천 출퇴근 후 상쾌함 더하기</t>
+        </is>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸과 마음을 편안하게 감싸주는 프리미엄 미스트샤워기로 상쾌한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>미스트샤워기,프리미엄샤워기,상쾌함,출퇴근피로해소,편안한샤워,바디케어</t>
+        </is>
+      </c>
+      <c r="J370" t="inlineStr">
+        <is>
+          <t>건강,생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>370</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>출퇴근 전 샤워 시간을 단축하는 고압 샤워기 활용법</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://naver.me/FGE63kIp</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250614_75/17498760629664f4fD_JPEG/84008896093604606_2114264486.jpg</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>고압 샤워기로 빠른 세정</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>출퇴근 시간 부족에 지친 당신을 위한 고압 샤워기로 빠르고 시원한 세정 효과를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>고압 샤워기 추천 출퇴근 시간 단축 효과</t>
+        </is>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>출퇴근 시간 부족으로 바쁜 직장인에게 적합한 고압 샤워기로 빠르고 효율적인 세정 효과를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>고압 샤워기,샤워 시간 단축,출퇴근 샤워,빠른 세정,직장인 샤워,샤워기 추천</t>
+        </is>
+      </c>
+      <c r="J371" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>371</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>6개 필터 구성으로 오랫동안 쾌적한 샤워 경험</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://naver.me/GPln23iN</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220121_298/1642752765856cqQfN_JPEG/43888661579244996_1099116077.jpg</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>6중 필터 쾌적샤워</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>오래 써도 변하지 않는 6중 필터로 깨끗하고 상쾌한 샤워를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>오래가는 6중 필터 샤워기 추천 - 쾌적한 샤워 경험</t>
+        </is>
+      </c>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>6개 필터 구성으로 깨끗하고 상쾌한 샤워를 오랫동안 즐길 수 있는 제품으로 가족 모두에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>샤워기, 6중 필터, 깨끗한 샤워, 쾌적한 샤워, 샤워기 추천, 필터샤워기, 욕실용품</t>
+        </is>
+      </c>
+      <c r="J372" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>372</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 샤워도 데일리 필터 샤워기로 신선하게</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://naver.me/x5m72BEo</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250721_93/1753072340287iPdqP_PNG/87205119429611061_2057728688.png</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>데일리 필터 샤워기</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 샤워도 깨끗하고 상쾌하게, 피부 고민 없이 신선함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 샤워에도 좋은 데일리 필터 샤워기 추천</t>
+        </is>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>출퇴근 전 빠른 샤워에도 깨끗하고 상쾌한 사용감을 제공하는 필터 샤워기입니다. 피부 자극 걱정 없이 신선함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>필터 샤워기,데일리 샤워기,출퇴근 샤워,피부 보호,신선한 샤워</t>
+        </is>
+      </c>
+      <c r="J373" t="inlineStr">
+        <is>
+          <t>생활용품/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>373</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>샤워기필터가 포함된 제품으로 깨끗한 물로 건강한 출퇴근 준비</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://naver.me/5AgCu4BZ</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250620_273/1750403065360YOW8n_JPEG/84535943891484202_697412586.jpg</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>깨끗한 물 샤워기필터</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>피부와 모발 고민 끝! 샤워기 필터로 건강한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>샤워기필터 포함 제품으로 깨끗한 물 건강한 출퇴근 추천</t>
+        </is>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>샤워기 필터로 피부와 모발 건강을 지키며 깨끗한 물로 상쾌한 하루를 시작할 수 있는 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>샤워기필터,깨끗한물,피부관리,모발건강,출퇴근준비,건강샤워기</t>
+        </is>
+      </c>
+      <c r="J374" t="inlineStr">
+        <is>
+          <t>생활/욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>374</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로 풀기 좋은 수압강한 샤워기 헤드</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://naver.me/FivePt8B</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20201208_296/1607428351356aNGE4_JPEG/8564246896146635_2063322137.jpg</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>수압강한 피로 해소 샤워기</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 피로를 수압 세기로 시원하게 풀어보세요. 매일 상쾌함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로 풀기 좋은 수압강한 샤워기 헤드 추천</t>
+        </is>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>수압이 강한 샤워기 헤드로 출퇴근 후 쌓인 피로를 시원하게 해소하세요. 매일 상쾌한 샤워 경험을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>샤워기, 수압강한 샤워기, 피로해소, 출퇴근 필수품, 홈케어, 욕실용품</t>
+        </is>
+      </c>
+      <c r="J375" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>375</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로를 씻어내는 수압 상승 샤워기 사용 경험</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://naver.me/IxKe06ja</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251203_237/1764742133713owlRT_JPEG/50817559537326970_2080526736.jpg</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>강력 수압 피로 해소 샤워기</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>출퇴근 후 쌓인 피로를 시원한 수압으로 씻어내세요. 매일 상쾌한 시작과 마무리를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>수압 상승 샤워기 추천 출퇴근 후 피로 해소에 탁월</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>강력한 수압으로 출퇴근 후 몸에 쌓인 피로를 효과적으로 씻어내는 샤워기로 상쾌한 하루를 시작하고 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>샤워기,수압샤워기,피로해소,출퇴근,목욕용품,욕실용품,상쾌한샤워</t>
+        </is>
+      </c>
+      <c r="J376" t="inlineStr">
+        <is>
+          <t>생활용품/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>376</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>집에서 간편히 석회수를 제거하는 샤워필터 알아보기</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://naver.me/GuDxCK2I</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250409_87/17441663752859OE5i_PNG/7154606408128641_767976720.png</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>간편 석회수 제거 샤워필터</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>석회수로 인한 피부 건조와 머리카락 손상, 집에서 쉽게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>간편한 석회수 제거 샤워필터 추천 - 집에서 쉽게 설치</t>
+        </is>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>석회수로 인한 피부 건조와 머리카락 손상을 집에서 간편히 해결할 수 있는 샤워필터입니다. 건강한 피부와 모발 관리를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>석회수제거,샤워필터,피부보호,머리카락손상방지,홈케어,간편설치,물정수</t>
+        </is>
+      </c>
+      <c r="J377" t="inlineStr">
+        <is>
+          <t>생활용품/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>377</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>국내생산 홈앤미 샤워기로 출퇴근 후 피로 풀기</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://naver.me/FswMoeVl</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251121_216/1763683265685YVITs_JPEG/92198622725448597_1117810433.jpg</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>피로 회복 샤워기</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>하루의 피로를 시원하게 씻어내고 싶은 당신을 위한 국내 생산 샤워기입니다.</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>국내생산 홈앤미 샤워기 피로해소 추천</t>
+        </is>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>출퇴근 후 하루 피로를 시원하게 씻어내는 국내 생산 홈앤미 샤워기입니다. 집에서 편안한 샤워 시간을 경험해 보세요.</t>
+        </is>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>국내생산,홈앤미,샤워기,피로해소,출퇴근,목욕용품,욕실용품,건강생활,편안한샤워</t>
+        </is>
+      </c>
+      <c r="J378" t="inlineStr">
+        <is>
+          <t>욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>378</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>출퇴근 후 상쾌함을 더하는 아쿠아듀오 샤워기필터</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://naver.me/x9zEVOlE</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241212_139/1733987102434iHXcA_JPEG/68120048561229868_329020713.jpg</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>상쾌한 출퇴근 샤워필터</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피곤한 피부와 머리를 깨끗하게, 아쿠아듀오 샤워필터로 상쾌함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>아쿠아듀오 샤워기필터 추천 출퇴근 후 상쾌함 유지</t>
+        </is>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>피곤한 피부와 머리를 깨끗하게 관리하는 아쿠아듀오 샤워기필터로 매일 출퇴근 후 상쾌함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>샤워기필터,아쿠아듀오,피부관리,머리관리,출퇴근,상쾌함,청결,수질정화</t>
+        </is>
+      </c>
+      <c r="J379" t="inlineStr">
+        <is>
+          <t>생활,욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>379</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>온오프 기능으로 간편한 두피 마사지와 청결 유지</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gpl8r35O</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250401_168/1743488728009hMRI2_PNG/24096811571058699_2126470277.png</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>간편 두피 마사지 케어</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>바쁜 일상 속 두피 청결과 마사지 고민을 한 번에 해결해보세요, 편리한 온오프 기능으로 쉽게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>간편 온오프 두피 마사지기 추천으로 청결 관리</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>편리한 온오프 기능으로 바쁜 일상에도 쉽게 두피 마사지와 청결을 관리할 수 있는 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>두피마사지,두피청결,온오프기능,간편사용,헤어케어,마사지기,청결유지</t>
+        </is>
+      </c>
+      <c r="J380" t="inlineStr">
+        <is>
+          <t>뷰티/헤어케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>380</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>가정용 필터샤워기와 2M 호스로 넉넉한 휴대성까지</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ZSb1CQJ</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250725_297/1753455591445x4tJi_PNG/87588356572425325_405207826.png</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>깨끗한 물 필터샤워기</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>수도물 속 불순물을 걸러 깨끗한 샤워를 원한다면 필터샤워기로 건강한 목욕을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>가정용 필터샤워기 2M 호스 포함 깨끗한 샤워 추천</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>수도물 속 불순물을 걸러 건강한 목욕이 가능한 가정용 필터샤워기와 2M 호스로 휴대성과 사용 편리성을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>필터샤워기,가정용샤워기,정수샤워기,샤워기호스,건강목욕,깨끗한수도물</t>
+        </is>
+      </c>
+      <c r="J381" t="inlineStr">
+        <is>
+          <t>욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>381</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>환경과 건강을 생각하는 사람들을 위한 ACF 필터 리필 세트</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://naver.me/5owf0Lgk</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250721_215/1753072364695u4a83_PNG/40270971565994998_1288476524.png</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>깨끗한 공기 필터 리필</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>공기 오염 걱정 없이 건강한 숨결을 지키세요. 환경까지 생각한 필터 리필 세트입니다.</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>ACF 필터 리필 세트 건강과 환경을 위한 추천</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>환경과 건강을 동시에 고려한 ACF 필터 리필 세트로 깨끗한 공기를 유지하세요. 가족 모두 안심하고 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>ACF필터,리필세트,공기정화,환경친화,건강케어,실내공기,알러지예방</t>
+        </is>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>환경,건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>382</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>출퇴근 후 닥터피엘 아토샤워헤드로 개운한 샤워 경험</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://naver.me/F5aNsmiV</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251201_24/1764570249917kuyuJ_PNG/98703190062911922_874182136.png</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>개운한 아토샤워헤드</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로와 피부 고민을 한 번에 해결해보세요. 청결하고 상쾌한 샤워로 하루를 리셋하세요.</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>닥터피엘 아토샤워헤드 출퇴근 후 개운한 샤워 추천</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로와 피부 고민을 해결해주는 닥터피엘 아토샤워헤드로 청결하고 상쾌한 샤워를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>닥터피엘, 아토샤워헤드, 샤워기, 피부케어, 출퇴근피로, 청결샤워, 상쾌한샤워</t>
+        </is>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>생활/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>383</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>물때 걱정 없는 PVC 호스와 함께한 출퇴근 샤워 시간</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://naver.me/xI1CFibo</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250120_233/1737361834591QAokM_JPEG/5701833608693595_1162823873.jpg</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>물때 걱정 없는 PVC 호스</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>물때로 불편했던 샤워 시간을 쾌적하게! 깨끗한 PVC 호스로 매일 상쾌한 출퇴근 샤워를 즐기세요.</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>물때 걱정 없는 PVC 호스 출퇴근 샤워 추천</t>
+        </is>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>물때 걱정 없이 깨끗한 PVC 호스로 쾌적한 출퇴근 샤워 시간을 즐기세요. 위생적인 샤워 환경을 찾는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>PVC호스,물때걱정없음,샤워용품,출퇴근샤워,위생샤워,쾌적샤워,욕실용품</t>
+        </is>
+      </c>
+      <c r="J384" t="inlineStr">
+        <is>
+          <t>욕실/샤워</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>384</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>출퇴근 전 간편하게 염소 필터로 수돗물 관리하기</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://naver.me/IM4XZqFg</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231010_261/16969210731712ASVt_JPEG/42352283965250216_1096032435.jpg</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>염소 필터 수돗물 관리</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>출퇴근 후에도 안심할 수 있는 깨끗한 물, 염소 제거로 건강한 수돗물을 간편하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>출퇴근 전 간편 염소 필터 추천, 건강한 수돗물 관리</t>
+        </is>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>출퇴근 전후 간편하게 염소를 제거해 깨끗하고 건강한 수돗물을 제공합니다. 누구나 쉽게 사용할 수 있어 안심하고 물을 마실 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>염소 필터, 수돗물 관리, 깨끗한 물, 건강한 물, 간편 필터, 염소 제거, 출퇴근, 물 정수</t>
+        </is>
+      </c>
+      <c r="J385" t="inlineStr">
+        <is>
+          <t>주방/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>385</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>알루미늄 샤워기헤드와 긴 호스로 편리한 욕실 환경 만들기</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://naver.me/GvfsWS3M</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241114_154/1731567006294v2E88_JPEG/3460175300067150_2130451052.jpg</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>편리한 알루미늄 샤워기</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>긴 호스로 자유로운 샤워, 매일 편안한 욕실 시간을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>알루미늄 샤워기헤드 긴 호스 욕실환경 개선 추천</t>
+        </is>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>알루미늄 재질 샤워기헤드와 긴 호스로 편리하고 자유로운 샤워 사용감을 제공합니다. 편안한 욕실 환경을 원하시는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>알루미늄 샤워기헤드, 긴 호스 샤워기, 욕실용품, 편리한 샤워, 욕실 환경개선</t>
+        </is>
+      </c>
+      <c r="J386" t="inlineStr">
+        <is>
+          <t>욕실/샤워기</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>386</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>출퇴근 후 상쾌함을 더하는 필터 샤워기헤드 선택법</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://naver.me/xYvxNdJd</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251219_237/1766119911328MSTp1_JPEG/41737957803595154_1271039617.jpg</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>상쾌함 더하는 샤워기헤드</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로한 몸을 상쾌하게 해주는 필터 샤워기헤드로 매일 상쾌한 샤워 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>상쾌함을 더하는 필터 샤워기헤드 추천과 선택법</t>
+        </is>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로 회복에 도움되는 필터 샤워기헤드로 매일 상쾌한 샤워를 즐겨보세요. 건강한 피부와 깨끗한 물 사용에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>필터 샤워기헤드,샤워기 추천,피로 회복 샤워기,청결 샤워기,상쾌한 샤워</t>
+        </is>
+      </c>
+      <c r="J387" t="inlineStr">
+        <is>
+          <t>생활/욕실용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>387</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>밀크씨슬 함유한 건강 보조제로 하루를 시작해보세요</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://naver.me/xF2K47Ej</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250815_233/17552488561978w0Jj_JPEG/36664050173282778_2053253080.jpg</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>밀크씨슬 간 건강 보조제</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>피로하고 지친 간을 위한 밀크씨슬, 건강한 하루를 다시 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>밀크씨슬 건강 보조제 추천, 피로 회복에 좋은 간 건강 제품</t>
+        </is>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>피로하고 지친 간을 위한 밀크씨슬 함유 건강 보조제입니다. 간 건강 유지와 활력 증진에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>밀크씨슬,건강보조제,간건강,피로회복,비타민,영양제</t>
+        </is>
+      </c>
+      <c r="J388" t="inlineStr">
+        <is>
+          <t>건강보조제/간건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>388</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>휴대가 편한 슬림카페 다이어트커피, 언제 어디서나 간편하게</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://naver.me/5QiwsQPG</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250815_64/1755249215362UVglo_JPEG/6282904486238430_451963844.jpg</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>간편 슬림 다이어트커피</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>언제 어디서나 간편하게 즐기며 건강한 다이어트를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>휴대가 편한 슬림카페 다이어트커피 추천, 간편한 다이어트 음료</t>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>언제 어디서나 간편하게 즐기는 슬림카페 다이어트커피로 건강한 다이어트를 지원합니다. 휴대가 편리해 외출 시에도 부담 없이 섭취 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>다이어트커피,슬림카페,휴대용커피,건강음료,다이어트음료,간편커피</t>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t>건강/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>389</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>운동 전후로 체지방감소 효과를 기대하는 다이어트보조제 활용법</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://naver.me/FtG2oL71</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220610_276/16548327660848MQoH_JPEG/55968661084178299_999993883.jpg</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>운동 효과 극대화 체지방감소</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>운동 전후 식단만으로 부족한 지방 연소, 체지방 감소를 도와 건강한 다이어트를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>체지방감소 다이어트보조제 활용법 운동 전후 추천</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>운동 전후 체지방 감소를 돕는 다이어트보조제로 효과적인 지방 연소와 건강한 다이어트를 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>체지방감소,다이어트보조제,지방연소,운동보조제,건강다이어트</t>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>다이어트/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>390</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>운동 효과를 높이는 체지방 분해 보조제 사용 후기</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://naver.me/xafpT7xn</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250723_172/1753247488467Cepmd_JPEG/26193299570339009_1025687634.jpg</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>체지방 분해 보조제</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>운동해도 체지방이 잘 빠지지 않아 고민인 분들에게 체지방 분해를 도와주는 효과적인 보조제입니다.</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>운동 효과를 높이는 체지방 분해 보조제 추천</t>
+        </is>
+      </c>
+      <c r="H391" t="inlineStr">
+        <is>
+          <t>체지방 분해를 촉진해 운동 효과를 높이고 싶은 분들에게 적합한 체지방 분해 보조제입니다. 꾸준한 운동과 함께 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>체지방 분해, 운동 보조제, 체중 감량, 다이어트 보조제, 건강 보조 식품</t>
+        </is>
+      </c>
+      <c r="J391" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>391</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>하루 한포로 관리하는 예비 신부를 위한 가르시니아 커피</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://naver.me/xquwb70l</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241222_63/1734850272025BEMze_JPEG/4063858900926849_580976780.jpg</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>예비 신부를 위한 가르시니아 커피</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>하루 한포로 간편하게 관리하며 자신감 넘치는 예비 신부 준비를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>가르시니아 커피 하루 한포로 예비 신부 관리 추천</t>
+        </is>
+      </c>
+      <c r="H392" t="inlineStr">
+        <is>
+          <t>예비 신부를 위한 간편한 하루 한포 가르시니아 커피로 자신감 있는 준비를 도와드립니다. 건강한 다이어트 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>가르시니아커피,예비신부,다이어트커피,간편관리,다이어트보조제</t>
+        </is>
+      </c>
+      <c r="J392" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>392</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>다이어트 중 휴대하기 좋은 가르시니아 제품 후기</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://naver.me/FGE63kKd</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240718_124/1721260015203XIp1A_JPEG/3954300607385183_1159429439.jpg</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>다이어트 가르시니아 휴대용</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>다이어트 중 간편하게 챙기는 가르시니아로 체중 관리 고민을 덜어보세요.</t>
+        </is>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>다이어트 휴대용 가르시니아 추천 후기 및 구매 가이드</t>
+        </is>
+      </c>
+      <c r="H393" t="inlineStr">
+        <is>
+          <t>간편하게 휴대하며 다이어트 중 체중 관리를 돕는 가르시니아 제품입니다. 체중 감량을 원하는 분께 적합한 건강 보조식품입니다.</t>
+        </is>
+      </c>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>가르시니아,다이어트보조제,체중관리,건강보조식품,휴대용다이어트,체중감량,다이어트후기</t>
+        </is>
+      </c>
+      <c r="J393" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>393</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>운동할 때 체지방 감소를 지원하는 그린몬스터 가르시니아</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://naver.me/xfYQbji6</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250508_150/1746690660709i4QOS_JPEG/80823428837522799_1004659686.jpg</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>운동 체지방 감소 지원</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>운동해도 체지방이 잘 빠지지 않아 고민인 분들께, 체지방 감소를 효과적으로 돕는 가르시니아입니다.</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>운동 체지방 감소 그린몬스터 가르시니아 추천</t>
+        </is>
+      </c>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>운동 후에도 체지방 감소에 어려움을 겪는 분들을 위한 가르시니아로, 효과적인 체지방 관리에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>체지방감소,가르시니아,운동보조제,체지방관리,다이어트보조</t>
+        </is>
+      </c>
+      <c r="J394" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>394</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>운동할 때 도움되는 슬림밸런스와 비오틴의 역할</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://naver.me/FMTz9PQ3</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241112_141/1731373447425WejIG_JPEG/65506317571828100_1490088266.jpg</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>운동 효과 돕는 슬림밸런스</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>운동 후 지친 몸에 슬림밸런스와 비오틴으로 활력을 더하세요. 건강한 탄력 유지에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>운동 도움 슬림밸런스와 비오틴 추천 활력 유지</t>
+        </is>
+      </c>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t>운동 후 지친 몸에 슬림밸런스와 비오틴으로 활력을 더하고 건강한 탄력 유지에 도움을 줍니다. 꾸준한 운동 후 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>슬림밸런스,비오틴,운동보조,활력제,탄력유지,건강보조제</t>
+        </is>
+      </c>
+      <c r="J395" t="inlineStr">
+        <is>
+          <t>건강보조제</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>395</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>꾸준한 체지방 감소에 도움 주는 가르시니아의 효과적 사용법</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEird9wg</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250508_7/1746690677337ctoNC_JPEG/27322000147683797_1554222345.jpg</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>체지방 감소 도움</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>꾸준한 체지방 감소에 어려움을 느끼는 분들을 위해 가르시니아가 효과적으로 작용합니다. 건강한 다이어트를 시작해보세요.</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>가르시니아 체지방 감소 효과적 사용법 추천</t>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>꾸준한 체지방 감소에 도움을 주는 가르시니아의 효과적인 사용법과 건강한 다이어트 방법을 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>가르시니아, 체지방 감소, 다이어트, 건강보조제, 식이조절, 체중관리</t>
+        </is>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>396</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 간편하게 챙기는 다이어트 보조제</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://naver.me/FUQSi8Kv</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241112_86/1731373595252Ujg4l_JPEG/11439350025450052_1192888972.jpg</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>간편 다이어트 보조제</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>출퇴근 길 바쁜 일상 속에도 건강한 다이어트를 도와줍니다. 간편하게 챙겨 효과를 경험해 보세요.</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>출퇴근 길 간편 다이어트 보조제 추천</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 시간에도 쉽게 챙기는 다이어트 보조제로 건강한 체중 관리를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>다이어트,보조제,출퇴근,건강관리,간편섭취,체중감량,운동보조</t>
+        </is>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>397</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>다이어트 중간 통화 시간에 간편히 챙기는 슬림핑크</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://naver.me/x8DSkyIv</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250815_90/1755248747248THQBw_JPEG/68628729097927935_1932579.jpg</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>간편 다이어트 보조제</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>바쁜 일상 속 간편하게 챙기는 다이어트 보조제로 건강한 체중 관리 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>슬림핑크 다이어트 보조제 건강한 체중 관리 추천</t>
+        </is>
+      </c>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>바쁜 일상 중간 통화 시간에 간편하게 섭취하는 다이어트 보조제로 건강한 체중 관리에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>슬림핑크,다이어트보조제,체중관리,건강,간편복용</t>
+        </is>
+      </c>
+      <c r="J398" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>398</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>탄수화물컷 효과로 운동 전 후 부담 줄여보세요</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://naver.me/G6QGRcqN</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230314_268/1678780098932kh77f_JPEG/79915941617181148_1527616821.jpg</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>탄수화물 부담 줄이는 컷팅</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>운동 전후 탄수화물 걱정 없이 가볍게! 부담을 줄여 슬림한 몸매를 꿈꾸는 당신을 응원합니다.</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>탄수화물컷 보조제 운동 전후 부담 감소 추천</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>운동 전후 탄수화물 걱정 없이 가볍게 섭취해 부담을 줄이고 슬림한 몸매 유지에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>탄수화물컷, 운동보조제, 다이어트, 탄수화물관리, 슬림몸매, 운동전후, 체중조절</t>
+        </is>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>건강보조제</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>399</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>착용감 걱정 없이 꾸준히 챙기는 고함량 가르시니아</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://naver.me/5W9XUW1t</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250317_77/1742188685439VMX4B_JPEG/76321586457350692_1791619449.jpg</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>부담 없는 고함량 가르시니아</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>착용감 걱정 없이 매일 간편하게 챙기며 건강 관리하세요. 꾸준한 섭취로 더욱 효과적인 케어를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>고함량 가르시니아 건강관리 추천 상품</t>
+        </is>
+      </c>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t>편안한 착용감으로 매일 간편하게 섭취 가능하며 꾸준한 복용으로 건강 관리를 돕는 가르시니아입니다.</t>
+        </is>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>가르시니아,건강관리,고함량,꾸준한섭취,편안한착용감,건강보조제</t>
+        </is>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>건강/영양제</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>400</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>운동 전 가르시니아 섭취로 다이어트 효과 높이기</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://naver.me/GOhp63XJ</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241022_104/1729582808633U9F2k_JPEG/77171285978295048_857167025.jpg</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>운동 전 다이어트 보조제</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>운동 효과를 높이고 싶은 당신을 위해, 가르시니아로 건강한 체중 관리를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>운동 전 가르시니아 섭취로 다이어트 효과 높이기 추천</t>
+        </is>
+      </c>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>운동 효과를 극대화하고 건강한 체중 관리를 원하는 분께 가르시니아 섭취를 추천합니다. 자연 성분으로 체지방 감소에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>가르시니아,다이어트,운동보조제,체중관리,건강보조식품</t>
+        </is>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>건강,다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>401</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>가르시니아로 운동 후에도 효과적인 체지방 관리법</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://naver.me/x4GplNys</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241022_22/17295827884996SXKg_JPEG/10067930901400049_1026045168.jpg</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>운동 후 체지방 관리</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>운동 후에도 체지방 걱정 없이 건강하게 관리하세요. 효과적인 지방 분해로 만족스러운 몸매를 완성해드립니다.</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>가르시니아로 운동 후 체지방 관리법 추천</t>
+        </is>
+      </c>
+      <c r="H402" t="inlineStr">
+        <is>
+          <t>운동 후에도 체지방 걱정 없이 건강한 체지방 관리를 원한다면 가르시니아를 활용한 효과적인 지방 분해법을 소개합니다.</t>
+        </is>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>가르시니아,체지방관리,운동후관리,지방분해,건강관리,다이어트보조제</t>
+        </is>
+      </c>
+      <c r="J402" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>402</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>통화 중에도 간편하게 마시는 가르시니아 다이어트 음료</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://naver.me/546eKHRt</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250920_38/1758374223600Biw1Q_PNG/8465170568445646_296496640.png</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>간편 다이어트 음료</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>바쁜 통화 시간에도 간편하게 마셔 다이어트 걱정을 덜어보세요.</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>가르시니아 다이어트 음료 통화 중 간편 섭취 추천</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>통화 중에도 간편하게 마실 수 있는 가르시니아 다이어트 음료로 바쁜 일상 속 다이어트 부담을 줄여보세요.</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>가르시니아,다이어트음료,간편섭취,체중관리,건강음료,휴대용음료</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>다이어트/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>403</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>운동 효과를 높여주는 다이어트보조제 가르시니아 활용법</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1m6uLjA</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250317_128/1742188551570y2GJD_JPEG/76321415686012759_1509359898.jpg</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>운동과 함께하는 다이어트보조제</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>운동 효과를 극대화하고 싶나요? 가르시니아가 체지방 감소를 도와 당신의 다이어트를 응원합니다.</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>운동 효과 높이는 다이어트보조제 가르시니아 추천</t>
+        </is>
+      </c>
+      <c r="H404" t="inlineStr">
+        <is>
+          <t>가르시니아는 체지방 감소에 도움을 주어 운동 효과를 극대화하는 다이어트보조제로, 건강한 다이어트를 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>가르시니아,다이어트보조제,운동효과증대,체지방감소,건강다이어트</t>
+        </is>
+      </c>
+      <c r="J404" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>404</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>운동 전후로 섭취하는 감비책 다이어트보조제의 효과</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://naver.me/GCgCJQ0H</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240205_178/1707114861077Pc5ao_JPEG/108250759763292670_859977881.jpg</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>운동 전후 다이어트보조제</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>운동 전후 체지방 관리를 쉽고 효과적으로 도와줘, 다이어트 고민을 해결해 드립니다.</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>감비책 다이어트보조제 운동 전후 섭취 추천</t>
+        </is>
+      </c>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>운동 전후로 간편하게 섭취해 체지방 관리에 도움을 주는 감비책 다이어트보조제입니다. 다이어트 고민을 효과적으로 해결할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>감비책,다이어트보조제,체지방관리,운동전,운동후,다이어트,체중감량,건강관리</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>405</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>가르시니아 다이어트보조제로 꾸준한 체중 관리하기</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://naver.me/GziIdZa4</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250317_77/1742188501200GKzkX_JPEG/51663629212623390_464609201.jpg</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>꾸준한 체중 관리</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>다이어트가 어렵게만 느껴지나요? 가르시니아로 체중 관리를 쉽고 꾸준하게 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>가르시니아 다이어트보조제 추천 꾸준한 체중 관리</t>
+        </is>
+      </c>
+      <c r="H406" t="inlineStr">
+        <is>
+          <t>가르시니아 다이어트보조제로 체중 관리를 쉽고 꾸준하게 도와드리며 건강한 다이어트를 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>가르시니아,다이어트,체중관리,다이어트보조제,건강관리,체중감량,식욕억제,다이어트영양제</t>
+        </is>
+      </c>
+      <c r="J406" t="inlineStr">
+        <is>
+          <t>건강/다이어트</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-22 18:47)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J406"/>
+  <dimension ref="A1:J444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20735,6 +20735,1906 @@
         </is>
       </c>
     </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>406</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>해외여행 필수품, RFID차단 기능의 여권 케이스 사용 후기</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://naver.me/59Ug0Ox3</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250904_23/1756954382230QN0yH_JPEG/91087168592205771_1685880555.jpg</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>안심 여권 RFID 케이스</t>
+        </is>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>해외여행 중 개인정보 도난 걱정 없이 안전하게 여권을 보호하세요.</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>해외여행 필수 RFID차단 여권 케이스 추천 및 사용 후기</t>
+        </is>
+      </c>
+      <c r="H407" t="inlineStr">
+        <is>
+          <t>여행 중 개인정보 보호에 탁월한 RFID차단 기능의 여권 케이스로 안전하게 여권을 보관하세요.</t>
+        </is>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>해외여행,여권케이스,RFID차단,개인정보보호,여행필수품,안전여행</t>
+        </is>
+      </c>
+      <c r="J407" t="inlineStr">
+        <is>
+          <t>여행용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>407</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 좋은 RFID 차단 가죽 파우치</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://naver.me/FjCtYDQu</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230802_199/1690983816506T5Eko_JPEG/1845157370384854_1862008070.jpg</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>RFID 차단 가죽 파우치</t>
+        </is>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>출퇴근길 소중한 카드 정보 보호, 세련된 가죽 파우치로 안심하세요.</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>RFID 차단 가죽 파우치 출퇴근길 카드 보호 추천</t>
+        </is>
+      </c>
+      <c r="H408" t="inlineStr">
+        <is>
+          <t>출퇴근길 카드 정보를 안전하게 지키는 세련된 RFID 차단 가죽 파우치로 소중한 개인정보를 보호하세요.</t>
+        </is>
+      </c>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>RFID 차단, 가죽 파우치, 카드 보호, 출퇴근 필수품, 개인정보 보안</t>
+        </is>
+      </c>
+      <c r="J408" t="inlineStr">
+        <is>
+          <t>소품/보안</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>408</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>출퇴근할 때도 부담 없는 가죽 여권 지갑 커버 추천</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://naver.me/GnR95snI</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240801_207/1722498060508ORyaW_JPEG/3160855241573347_2083437562.jpg</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>가죽 여권 지갑 커버</t>
+        </is>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>출퇴근할 때도 가볍고 실용적인 가죽 여권 지갑으로 소지품 관리를 간편하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>출퇴근용 가죽 여권 지갑 커버 추천 실용적 휴대용</t>
+        </is>
+      </c>
+      <c r="H409" t="inlineStr">
+        <is>
+          <t>가볍고 실용적인 가죽 여권 지갑으로 출퇴근 시 소지품을 간편하게 관리할 수 있어 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>가죽 여권 지갑,출퇴근 지갑,실용적인 여권 커버,휴대용 지갑,여권 케이스</t>
+        </is>
+      </c>
+      <c r="J409" t="inlineStr">
+        <is>
+          <t>여권지갑/출퇴근</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>409</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편리한 접이식 여행용 가방 활용법</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://naver.me/FFaEWl5y</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220820_45/1660986000125xzhoR_JPEG/62121842838106457_194365616.jpg</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>접이식 여행용 가방</t>
+        </is>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>출퇴근길과 여행에 모두 편리한 접이식 가방으로 무거움 걱정 없이 간편하게 휴대하세요.</t>
+        </is>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>출퇴근길 편리한 접이식 여행용 가방 추천</t>
+        </is>
+      </c>
+      <c r="H410" t="inlineStr">
+        <is>
+          <t>가볍고 접이식 디자인으로 출퇴근과 여행 시 휴대가 간편한 다용도 가방입니다.</t>
+        </is>
+      </c>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>접이식가방,여행용가방,출퇴근가방,휴대용가방,경량가방,멀티가방</t>
+        </is>
+      </c>
+      <c r="J410" t="inlineStr">
+        <is>
+          <t>가방/여행</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>410</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 손쉬운 휴대가 가능한 명품 여권 지갑</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://naver.me/xJGkJMys</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241122_172/1732271212399ABuuF_PNG/4871076481185730_1640305877.png</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>컴팩트 명품 여권 지갑</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 부담 없는 휴대성으로 안전하게 여권과 소지품을 보관하세요.</t>
+        </is>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>출퇴근용 명품 여권 지갑 추천, 휴대성 좋은 가죽 지갑</t>
+        </is>
+      </c>
+      <c r="H411" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 손쉽게 휴대 가능한 명품 여권 지갑으로 안전하게 여권과 소지품을 보관하세요. 실용적인 디자인과 뛰어난 내구성이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>명품 여권 지갑, 출퇴근 지갑, 휴대용 여권 케이스, 안전한 지갑, 가죽 여권 지갑</t>
+        </is>
+      </c>
+      <c r="J411" t="inlineStr">
+        <is>
+          <t>여권/지갑</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>411</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간단 청소에 딱 좋은 밀대 걸레 활용법</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://naver.me/xI1CNFmh</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240214_289/1707876130968rQldr_JPEG/109011958790044915_1745793694.jpg</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>간편 출퇴근 밀대 청소</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후 간단한 청소가 어려우셨나요? 밀대 걸레로 빠르고 깨끗하게 청소하세요.</t>
+        </is>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간단 청소에 좋은 밀대 걸레 활용법 추천</t>
+        </is>
+      </c>
+      <c r="H412" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후에도 간편하게 사용할 수 있는 밀대 걸레로 빠르고 깨끗한 청소를 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>밀대걸레,간단청소,출퇴근청소,빠른청소,청소도구</t>
+        </is>
+      </c>
+      <c r="J412" t="inlineStr">
+        <is>
+          <t>생활용품/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>412</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>출장과 출퇴근 시에도 편리한 여행 지갑 활용법</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://naver.me/xVGjkdht</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_6/1765263856579S7PWG_JPEG/99396719681309744_1144324174.jpg</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>여행과 출퇴근 지갑</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>출장과 일상 속 간편한 휴대, 다양한 카드와 현금 수납으로 걱정 없이 편리함을 누리세요.</t>
+        </is>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>출장과 출퇴근에 편리한 여행 지갑 추천 및 활용법</t>
+        </is>
+      </c>
+      <c r="H413" t="inlineStr">
+        <is>
+          <t>출장과 일상 출퇴근 시 간편하게 휴대할 수 있는 여행 지갑으로 다양한 카드와 현금을 쉽게 수납해 편리함을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>여행지갑,출장용지갑,출퇴근지갑,카드수납,현금수납,간편휴대,여행필수품,편리한지갑</t>
+        </is>
+      </c>
+      <c r="J413" t="inlineStr">
+        <is>
+          <t>여행/가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>413</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>등원길에 딱 좋은 나이키 키즈 가방 선택 팁</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://naver.me/GkUqt4B3</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250115_277/1736922002970voHNz_JPEG/71054854119951384_1144685863.jpg</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>아이 등원 가방 추천</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>아이의 등원길 고민 끝! 가벼우면서도 실용적인 가방으로 편안한 등원길을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>나이키 키즈 가방 추천, 등원길에 딱 맞는 가방 선택법</t>
+        </is>
+      </c>
+      <c r="H414" t="inlineStr">
+        <is>
+          <t>가볍고 실용적인 나이키 키즈 가방으로 아이의 등원길 고민을 해결하세요. 편안한 착용감과 넉넉한 수납공간이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>나이키 키즈 가방,어린이가방,등원길 가방,어린이 백팩,가볍고 실용적인 가방</t>
+        </is>
+      </c>
+      <c r="J414" t="inlineStr">
+        <is>
+          <t>키즈/가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>414</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>가벼운 키즈 백팩으로 출퇴근길 학원 갈 때도 편안해요</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://naver.me/FqZysG4C</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220803_199/1659494773685AdjxN_JPEG/60630619362228643_1273724754.jpg</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>가벼운 키즈 백팩</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>출퇴근길과 학원 이동 시 무거움 없이 편안한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>가벼운 키즈 백팩 추천 출퇴근길과 학원용 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H415" t="inlineStr">
+        <is>
+          <t>가벼운 키즈 백팩은 출퇴근길과 학원 갈 때 무게 부담 없이 편안함을 선사합니다. 아이들의 이동이 더욱 쾌적해집니다.</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>키즈백팩,가벼운백팩,어린이백팩,학원가방,출퇴근백팩,아동가방,편안한백팩</t>
+        </is>
+      </c>
+      <c r="J415" t="inlineStr">
+        <is>
+          <t>키즈/가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>415</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>실속형 물걸레밀대와 함께하는 집안 청소 루틴</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gf0FgrW3</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231220_159/1703057638266jeTC5_JPEG/104193421940228109_1869244370.jpg</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>효율적인 물걸레 청소</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>번거로운 집안 청소를 간편하게! 실속형 물걸레밀대로 깨끗하고 쾌적한 공간을 만드세요.</t>
+        </is>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>실속형 물걸레밀대 추천, 집안 청소 간편 해결</t>
+        </is>
+      </c>
+      <c r="H416" t="inlineStr">
+        <is>
+          <t>실속형 물걸레밀대로 집안 청소를 간편하고 깨끗하게 완성하세요. 쾌적한 공간 유지에 적합한 실용 도구입니다.</t>
+        </is>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>물걸레밀대, 집안 청소, 실속형, 청소용품, 간편 청소, 쾌적 공간, 바닥 청소</t>
+        </is>
+      </c>
+      <c r="J416" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>416</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>출퇴근 전 빠른 청소에 좋은 원터치 밀대 사용기</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://naver.me/x6xmvJaC</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250721_287/1753072598377B2VVK_PNG/87205446711432891_2131706487.png</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>원터치 밀대 청소기</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 길 손쉽게 청소하고 싶은 당신을 위한 빠른 원터치 밀대입니다.</t>
+        </is>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>출퇴근 빠른 청소 원터치 밀대 추천 - 손쉬운 사용법</t>
+        </is>
+      </c>
+      <c r="H417" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길 간편하게 청소할 수 있는 원터치 밀대로 빠르고 효율적인 청소를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>출퇴근 청소, 원터치 밀대, 빠른 청소, 간편 청소, 가정용 밀대</t>
+        </is>
+      </c>
+      <c r="J417" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>417</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>출퇴근 후 빠른 청소에 적합한 스프레이 밀대 추천</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://naver.me/xAAMsfyl</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200825_4/1598328027712Fdn1g_PNG/35691416230201822_1643894096.png</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>빠른 출퇴근 청소용 스프레이밀대</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>출퇴근 후 바쁜 시간에도 간편하게 청소하세요. 스프레이 밀대로 빠르고 깨끗한 집안 관리가 가능합니다.</t>
+        </is>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>출퇴근 후 빠른 청소에 좋은 스프레이 밀대 추천</t>
+        </is>
+      </c>
+      <c r="H418" t="inlineStr">
+        <is>
+          <t>출퇴근 후 바쁜 시간에도 간편하게 사용하는 스프레이 밀대로 빠르고 깨끗한 청소를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>스프레이 밀대,빠른 청소,출퇴근 청소,간편 청소,홈케어</t>
+        </is>
+      </c>
+      <c r="J418" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>418</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>멀티 파우치로 휴대품을 체계적으로 분류하는 팁</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://naver.me/IFG5Aox8</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250131_235/17382989169177lC3b_JPEG/669384049305367_35158766.jpg</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>체계적 휴대품 분류 파우치</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>휴대품이 뒤섞여 고민이라면 멀티 파우치로 깔끔하게 정리해보세요. 간편한 수납으로 언제나 편리합니다.</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>멀티 파우치 휴대품 정리 추천, 간편한 수납 팁</t>
+        </is>
+      </c>
+      <c r="H419" t="inlineStr">
+        <is>
+          <t>깔끔한 휴대품 정리를 돕는 멀티 파우치로 언제나 편리하게 수납하세요. 소지품 관리에 적합한 실용적인 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>멀티파우치,휴대품정리,수납팁,간편수납,여행파우치,소지품정리,파우치추천</t>
+        </is>
+      </c>
+      <c r="J419" t="inlineStr">
+        <is>
+          <t>생활용품/수납</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>419</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>출퇴근 가방 안 깔끔하게, 방수 여행용 세면도구 파우치 추천</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://naver.me/FdonYlao</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250718_39/1752811971665CV5KJ_JPEG/86944772965982402_698004058.jpg</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>방수 여행용 세면 파우치</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>출퇴근과 여행 시 세면도구 정리 고민 끝! 방수 기능으로 깔끔하게 보관하세요.</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>출퇴근 가방 방수 세면도구 파우치 추천, 깔끔한 정리 솔루션</t>
+        </is>
+      </c>
+      <c r="H420" t="inlineStr">
+        <is>
+          <t>출퇴근과 여행 시 세면도구를 방수 파우치로 깔끔하게 보관할 수 있는 실용적인 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>방수 파우치, 세면도구 파우치, 출퇴근 가방, 여행용 파우치, 깔끔한 수납</t>
+        </is>
+      </c>
+      <c r="J420" t="inlineStr">
+        <is>
+          <t>여행용품/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>420</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>차량용 세차 밀대 하나로 손쉬운 휴대와 사용 경험</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://naver.me/xKtxHyUj</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251205_75/17649214726671ULQN_PNG/99654131612718635_488594249.png</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>간편 차량용 세차 밀대</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>차 세척이 번거로우셨나요? 이 밀대 하나로 손쉽게 깨끗한 차량 관리하세요.</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>차량용 세차 밀대 추천 손쉬운 휴대와 간편 세척</t>
+        </is>
+      </c>
+      <c r="H421" t="inlineStr">
+        <is>
+          <t>차량용 세차 밀대로 쉽고 빠르게 차량을 깨끗이 관리하세요. 휴대가 간편해 언제 어디서나 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>차량용 세차 밀대,자동차 세척,휴대용 세차 도구,간편 세척,차량 관리</t>
+        </is>
+      </c>
+      <c r="J421" t="inlineStr">
+        <is>
+          <t>자동차/세차용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>421</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>막대걸레와 극세사 리필 세트로 출퇴근 전 빠른 청소 팁</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://naver.me/F9hSJ3Yw</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251218_37/1766023562255g0W0g_JPEG/100156412356330737_2034941853.jpg</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>빠른 청소 막대걸레 세트</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 시간도 깨끗하게! 막대걸레와 극세사 리필로 번거로움 없이 청소하세요.</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>막대걸레와 극세사 리필 세트 추천 출퇴근 전 빠른 청소</t>
+        </is>
+      </c>
+      <c r="H422" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 시간에도 효과적인 청소가 가능한 막대걸레와 극세사 리필 세트로 번거로움 없이 간편하게 청소하세요.</t>
+        </is>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>막대걸레,극세사리필,빠른청소,출퇴근청소,간편청소,청소세트</t>
+        </is>
+      </c>
+      <c r="J422" t="inlineStr">
+        <is>
+          <t>생활용품/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>422</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>운동 후 깔끔한 관리, 건습분리 세면파우치 활용법</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://naver.me/5owfBDex</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240705_296/1720107389567deFKo_JPEG/45296663414843189_892214716.jpg</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>운동 후 깔끔한 세면파우치</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 용품과 마른 용품을 깔끔하게 분리해 관리할 수 있어 편리합니다.</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>운동 후 건습분리 세면파우치 추천, 깔끔한 관리법</t>
+        </is>
+      </c>
+      <c r="H423" t="inlineStr">
+        <is>
+          <t>운동 후 젖은 용품과 마른 용품을 분리해 편리하게 관리할 수 있는 건습분리 세면파우치입니다.</t>
+        </is>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>건습분리, 세면파우치, 운동용품관리, 깔끔한파우치, 분리수납</t>
+        </is>
+      </c>
+      <c r="J423" t="inlineStr">
+        <is>
+          <t>운동/용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>423</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>운동복부터 일상 소지품까지 정리하기 좋은 여행 파우치</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://naver.me/FE3Tjmq5</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250407_17/1744024057957dGtE2_JPEG/78156999071930984_482468358.jpg</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>다용도 여행 소품 파우치</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>여행 중 흩어지는 소지품, 깔끔하게 정리하고 싶다면 이 파우치로 손쉽게 정리하세요.</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>여행 파우치 추천 운동복부터 일상 소지품 정리용</t>
+        </is>
+      </c>
+      <c r="H424" t="inlineStr">
+        <is>
+          <t>여행 중 흩어지는 소지품을 깔끔하게 정리해주는 파우치로 편리하게 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>여행파우치,소지품정리,운동복파우치,여행용파우치,휴대용파우치</t>
+        </is>
+      </c>
+      <c r="J424" t="inlineStr">
+        <is>
+          <t>여행용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>424</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 부담 없는 초등학생 사첼형 책가방 추천</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://naver.me/5eZxH6rz</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250813_145/1755071641136X8uof_JPEG/6p24P_102078_1.jpg</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>초등 사첼형 책가방</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>출퇴근길 포근한 착용감으로 아이 부담 줄이고, 실용적 수납으로 편리함까지 챙겨주세요.</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>출퇴근길 부담 없는 초등학생 사첼형 책가방 추천</t>
+        </is>
+      </c>
+      <c r="H425" t="inlineStr">
+        <is>
+          <t>포근한 착용감과 실용적인 수납 공간으로 초등학생 아이가 편안하게 사용할 수 있는 사첼형 책가방입니다. 출퇴근길에도 부담 없이 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>초등학생책가방,사첼형가방,책가방추천,어린이가방,실용적인가방,부담없는가방,출퇴근길가방</t>
+        </is>
+      </c>
+      <c r="J425" t="inlineStr">
+        <is>
+          <t>가방/학생용</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>425</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>넉넉한 수납 공간의 대형 캐리어로 해외여행 준비 끝</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://naver.me/FRu9shSs</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241018_39/1729207590502mBoB6_JPEG/63340440633299439_967847229.jpg</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>넉넉한 대형 캐리어</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>많은 짐도 걱정 없는 넉넉한 수납 공간으로 해외여행 준비를 간편하게 해보세요.</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>넉넉한 수납 대형 캐리어 추천 해외여행 준비 완벽</t>
+        </is>
+      </c>
+      <c r="H426" t="inlineStr">
+        <is>
+          <t>넉넉한 수납 공간을 갖춘 대형 캐리어로 많은 짐도 간편하게 정리하세요. 해외여행 준비에 적합한 캐리어입니다.</t>
+        </is>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>대형캐리어,수납공간,해외여행,여행가방,여행캐리어,넉넉한수납</t>
+        </is>
+      </c>
+      <c r="J426" t="inlineStr">
+        <is>
+          <t>여행가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>426</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>간편한 회전과 조절로 운동 후 집 청소가 한결 수월해졌어요</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://naver.me/GWiv3WC6</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230321_65/1679365545298PqX8U_JPEG/80501433998402638_463328027.jpg</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>회전 조절로 간편 청소</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>운동 후에도 손쉽게 회전 조절로 쌓인 먼지를 깨끗하게 청소하세요. 집안일이 한결 편해집니다.</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>운동 후 청소용 회전 조절 청소기 추천</t>
+        </is>
+      </c>
+      <c r="H427" t="inlineStr">
+        <is>
+          <t>운동 후에도 간편한 회전과 조절 기능으로 집안 먼지를 효과적으로 청소할 수 있어 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>청소기,회전 청소기,집 청소,운동 후 청소,간편 조절,먼지 제거,가정용 청소기</t>
+        </is>
+      </c>
+      <c r="J427" t="inlineStr">
+        <is>
+          <t>가전/청소기</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>427</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>가벼운 벨크로 막대걸레 휴대하며 빠른 청소법</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://naver.me/FJIVqOhc</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250403_142/1743662866997Vg65z_JPEG/14189721834390307_70317861.jpg</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>가벼운 휴대용 막대걸레</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>빠르고 간편한 청소로 시간 절약! 어디서나 손쉽게 깨끗함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>가벼운 벨크로 막대걸레 추천 빠른 휴대용 청소법</t>
+        </is>
+      </c>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>가벼운 벨크로 막대걸레로 간편하고 빠른 청소가 가능합니다. 휴대가 용이해 어디서든 깨끗하게 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>가벼운 막대걸레, 벨크로 청소기, 휴대용 청소용품, 빠른 청소, 간편 청소법</t>
+        </is>
+      </c>
+      <c r="J428" t="inlineStr">
+        <is>
+          <t>생활용품/청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>428</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>가벼운 밀대걸레로 출퇴근 후 간편한 청소</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fr0yPijU</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250502_46/1746175728362FNKbL_JPEG/26807051164498691_1079860948.jpg</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>가벼운 밀대걸레로 간편청소</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에도 부담 없는 가벼운 밀대걸레로 빠르고 깨끗한 청소를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>가벼운 밀대걸레 추천 출퇴근 후 간편 청소용</t>
+        </is>
+      </c>
+      <c r="H429" t="inlineStr">
+        <is>
+          <t>가벼운 밀대걸레로 출퇴근 후 부담 없이 빠르고 깨끗한 청소를 할 수 있어 실용적입니다.</t>
+        </is>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>가벼운 밀대걸레,간편 청소,출퇴근 청소,청소 도구,빠른 청소</t>
+        </is>
+      </c>
+      <c r="J429" t="inlineStr">
+        <is>
+          <t>생활/청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>429</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>휴대가 편리한 나일론 소재 폴더블 토트백 추천</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://naver.me/FE3TjmXd</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250106_188/17361558669602uE4k_JPEG/70288745103982351_1670159072.jpg</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>경량 접이식 나일론 토트백</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>가볍고 접을 수 있어 휴대가 간편한 토트백으로 언제 어디서나 스타일을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>휴대가 편리한 나일론 폴더블 토트백 추천 및 할인</t>
+        </is>
+      </c>
+      <c r="H430" t="inlineStr">
+        <is>
+          <t>가볍고 접을 수 있어 휴대가 간편한 나일론 토트백으로 언제 어디서나 스타일리시하게 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>나일론토트백,폴더블토트백,휴대용가방,가벼운가방,접이식가방,여행가방,데일리백</t>
+        </is>
+      </c>
+      <c r="J430" t="inlineStr">
+        <is>
+          <t>패션/가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>430</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>초등학생 맞춤 아디다스 키즈 백팩, 출퇴근길 가방으로도 좋아요</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://naver.me/GWiv3fps</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250731_93/17539246656856KWEC_PNG/63239350878220_1549208197.png</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>초등학생 맞춤 키즈 백팩</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>아이의 학교 생활과 출퇴근길을 편안하게! 튼튼하고 실용적인 백팩으로 고민 끝.</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>초등학생 맞춤 아디다스 키즈 백팩 추천, 실용적인 등하교 가방</t>
+        </is>
+      </c>
+      <c r="H431" t="inlineStr">
+        <is>
+          <t>튼튼하고 편안한 아디다스 키즈 백팩으로 초등학생 아이의 학교 생활과 출퇴근길을 지원합니다. 실용적인 디자인으로 활용도 높아요.</t>
+        </is>
+      </c>
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>아디다스, 키즈 백팩, 초등학생 가방, 등하교 가방, 실용적인 백팩, 튼튼한 가방, 출퇴근 백팩</t>
+        </is>
+      </c>
+      <c r="J431" t="inlineStr">
+        <is>
+          <t>학교용품/가방</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>431</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>운동 후 반자동 대걸레로 깔끔한 바닥 유지법</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://naver.me/G02cnp3i</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230603_272/1685770693154ykSxb_JPEG/22613145968898573_920123709.jpg</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>운동 후 대걸레 청소법</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>운동 후 땀과 먼지 걱정 마세요. 반자동 대걸레로 간편하게 바닥을 깨끗하게 유지해드립니다.</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>운동 후 반자동 대걸레 추천, 간편한 바닥 청소법</t>
+        </is>
+      </c>
+      <c r="H432" t="inlineStr">
+        <is>
+          <t>운동 후 땀과 먼지 걱정을 덜어주는 반자동 대걸레로 쉽고 빠르게 바닥을 청결하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>운동 후 청소,반자동 대걸레,바닥 청소,간편 청소,땀 먼지 제거,홈 클리닝</t>
+        </is>
+      </c>
+      <c r="J432" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>432</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>찌든때도 걱정 없는 물걸레패드로 깨끗한 집 만들기</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://naver.me/xafprTiA</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250730_126/17538416002610qrbE_JPEG/26441464334625869_981279472.jpg</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>찌든때 제거 물걸레패드</t>
+        </is>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>잘 지워지지 않는 찌든때, 걱정 마세요. 깨끗한 집을 위한 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>찌든때 제거 물걸레패드 추천으로 깨끗한 집 만들기</t>
+        </is>
+      </c>
+      <c r="H433" t="inlineStr">
+        <is>
+          <t>찌든때도 쉽게 제거 가능한 물걸레패드로 집안을 깨끗하게 관리하세요. 청소가 어려운 구석까지 말끔히 청소하는 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>물걸레패드, 찌든때 제거, 청소용품, 집 청소, 깨끗한 집, 바닥 청소, 생활용품</t>
+        </is>
+      </c>
+      <c r="J433" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>433</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>가족 모두를 위한 RFID 차단 여권케이스의 휴대 편리성</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://naver.me/F3YJCAyU</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251027_179/1761549165767QPCGp_PNG/3801594892088752_1879957588.png</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>안전한 RFID 차단 여권지갑</t>
+        </is>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>여행 중 RFID 도난 걱정 없이 가족 모두의 소중한 개인정보를 안전하게 지키세요.</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>가족용 RFID 차단 여권케이스 휴대 편리성 추천</t>
+        </is>
+      </c>
+      <c r="H434" t="inlineStr">
+        <is>
+          <t>여행 시 RFID 스캔 방지로 가족 모두 개인정보를 안전하게 보호하는 여권케이스입니다. 휴대가 간편해 편리합니다.</t>
+        </is>
+      </c>
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>RFID차단,여권케이스,여행용품,가족안전,개인정보보호,휴대용케이스,여행필수품</t>
+        </is>
+      </c>
+      <c r="J434" t="inlineStr">
+        <is>
+          <t>여행/보안</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>434</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>해킹방지 커버로 휴대폰과 함께 안전하게 휴대하는 방법</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://naver.me/xydF4bqS</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230919_215/1695084268146CSpH1_JPEG/765052289834778_292264096.jpg</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>휴대폰 해킹방지 커버</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>개인 정보 유출 걱정 없이 안전하게 휴대폰을 보호하세요. 해킹 방지 커버로 안심하고 외출할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>해킹방지 커버로 휴대폰 안전하게 보호하는 방법 추천</t>
+        </is>
+      </c>
+      <c r="H435" t="inlineStr">
+        <is>
+          <t>개인 정보 유출 걱정 없이 휴대폰을 안전하게 보호할 수 있는 해킹방지 커버로 안심 외출하세요.</t>
+        </is>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>해킹방지,휴대폰보호,개인정보보호,안전커버,모바일보안,스마트폰커버</t>
+        </is>
+      </c>
+      <c r="J435" t="inlineStr">
+        <is>
+          <t>보안/모바일</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>435</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 안전하게 들고 다니는 RFID 차단 가죽 지갑</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://naver.me/GziIFlTL</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241203_105/1733198207024Qqquc_JPEG/13397820911573677_1668845250.jpg</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>RFID 차단 가죽 지갑</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>출퇴근 길 소중한 개인정보를 안전하게 보호하세요. 스타일과 보안을 한 번에 갖춘 지갑입니다.</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>RFID 차단 가죽 지갑 추천 안전한 출퇴근용 지갑</t>
+        </is>
+      </c>
+      <c r="H436" t="inlineStr">
+        <is>
+          <t>출퇴근길 개인정보 보호에 최적화된 RFID 차단 기능과 세련된 가죽 디자인으로 안전하고 편리한 지갑입니다.</t>
+        </is>
+      </c>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>RFID 차단,가죽 지갑,출퇴근 지갑,개인정보 보호,안전 지갑,남성 지갑,여성 지갑</t>
+        </is>
+      </c>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>패션/지갑</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>436</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 편리한 RFID차단 기능의 여권지갑</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://naver.me/52c18F6g</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230809_221/1691551489558LEbgb_JPEG/2412830421553901_996217029.jpg</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>RFID 차단 여권지갑</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>여권과 카드 정보를 안전하게 지키며 출퇴근길도 안심하세요. 편리한 수납으로 여행과 일상 모두 완벽합니다.</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>RFID차단 기능 여권지갑 추천 출퇴근 시 안전한 카드 보관</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>여권과 카드 정보를 안전하게 보호하는 RFID차단 여권지갑으로 출퇴근과 여행 시 편리하고 안심할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>RFID차단,여권지갑,안전한 카드보관,출퇴근,여행용 지갑</t>
+        </is>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>여행/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>437</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>휴대하기 좋은 가죽 소재의 RFID차단 여권케이스 추천</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ixbWs3J</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250429_184/1745853521115kQpMr_JPEG/79986298663323096_239939128.jpg</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>가죽 RFID 여권케이스</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>여권 분실 걱정 없이 스마트하게 여행하세요. 슬림한 가죽 케이스로 안전과 스타일을 동시에!}</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>휴대하기 좋은 가죽 RFID차단 여권케이스 추천</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>슬림한 가죽 소재로 제작된 RFID차단 여권케이스로, 분실 걱정 없이 안전하고 스타일리시한 여행을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>여권케이스,RIFD차단,가죽케이스,여행용지갑,슬림케이스,여권보호,안전여행</t>
+        </is>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>여행용품/가죽</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>438</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 청소포 세트 활용하기</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://naver.me/FtGrO2MF</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251218_58/17660227519178ndML_JPEG/35138634030849847_707710269.jpg</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>간편 출퇴근 청소포</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후에도 간편하게 청소를 끝내세요. 청소 고민을 덜어주는 실속 세트입니다.</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편 청소포 세트 추천으로 빠른 청소 해결</t>
+        </is>
+      </c>
+      <c r="H439" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근 후에 간편하게 사용할 수 있는 청소포 세트로 쉽고 빠른 청소를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>청소포,간편청소,출퇴근후청소,청소세트,실속청소포</t>
+        </is>
+      </c>
+      <c r="J439" t="inlineStr">
+        <is>
+          <t>생활/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>439</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>운동 후 집에서 밀대로 바닥 습기 싹 제거</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://naver.me/GwSOYfvw</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230116_183/16738754068617BMsn_JPEG/75011249469875568_754103415.jpg</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>운동 후 습기 제거 밀대</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>운동 후 땀으로 눅눅해진 바닥, 빠르게 습기를 제거해 쾌적한 집안을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>운동 후 바닥 습기 제거용 밀대 추천, 쾌적한 집안 유지</t>
+        </is>
+      </c>
+      <c r="H440" t="inlineStr">
+        <is>
+          <t>운동 후 눅눅해진 바닥의 습기를 빠르게 제거해 쾌적한 실내 환경을 만들어 줍니다. 집에서 간편하게 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>운동 후 바닥 습기, 바닥 밀대, 습기 제거, 집안 청소, 빠른 건조</t>
+        </is>
+      </c>
+      <c r="J440" t="inlineStr">
+        <is>
+          <t>생활용품/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>440</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>출퇴근 전 빠른 청소에 좋은 밀대 청소기 추천</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://naver.me/FCrjFZ24</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20190527_129/kencoceo@gmail.com_1558938959760dABm5_JPEG/41657818608533250_657950075.jpg</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>빠른 출퇴근 밀대 청소기</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 시간에 간편하게 청소하고 싶은 분들에게 딱 맞는 밀대 청소기입니다. 바쁜 일상 속 청결을 쉽게 지켜보세요.</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>출퇴근 전 빠른 청소용 밀대 청소기 추천</t>
+        </is>
+      </c>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>출퇴근 전 짧은 시간에 간편한 청소가 가능한 밀대 청소기로 바쁜 일상 속에서도 깔끔함을 유지할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>밀대청소기,빠른청소,간편청소,출퇴근청소,실내청소,바쁜일상,청소기추천</t>
+        </is>
+      </c>
+      <c r="J441" t="inlineStr">
+        <is>
+          <t>가전,청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>441</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>가벼운 물걸레밀대 휴대하며 운동 후 바닥 닦기</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://naver.me/xumxSF5E</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251219_218/1766124592723XSy8h_JPEG/100257516635638541_626982472.jpg</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>가벼운 휴대용 물걸레밀대</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>운동 후 바닥 청소가 번거로우셨나요? 가볍고 편리한 물걸레밀대로 깔끔한 청소를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>가벼운 물걸레밀대 추천 운동 후 바닥 청소용</t>
+        </is>
+      </c>
+      <c r="H442" t="inlineStr">
+        <is>
+          <t>운동 후 바닥 청소를 간편하게 도와주는 가벼운 물걸레밀대입니다. 휴대가 편리해 언제 어디서든 깔끔하게 청소할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>물걸레밀대,가벼운밀대,운동후청소,휴대용청소도구,바닥청소</t>
+        </is>
+      </c>
+      <c r="J442" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>442</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>집안 청소가 쉬워지는 원터치 밀대 사용 후기</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://naver.me/FaOghe71</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241117_133/1731773267496Dw0Vv_JPEG/13273621339997313_1344770132.jpg</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>간편 원터치 밀대 청소</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>청소가 번거로웠다면 원터치 밀대로 간편하게 해결하세요. 손쉽게 집안 구석구석 깨끗해집니다.</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>원터치 밀대 청소 도구 추천으로 집안 청소 간편 해결</t>
+        </is>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>원터치 밀대로 손쉽게 집안 곳곳을 청소하세요. 간편한 사용법으로 청소 시간이 단축되고 깨끗하게 관리할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>원터치 밀대,청소 도구,간편 청소,집안 청소,밀대 추천,바닥청소,청소 용품</t>
+        </is>
+      </c>
+      <c r="J443" t="inlineStr">
+        <is>
+          <t>청소용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>443</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>업소용 대형 밀대, 강당 청소도 문제없어요</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://naver.me/GxLYSriL</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250319_112/1742363410837PJ0Dy_JPEG/36906156031243463_1098766749.jpg</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>업소용 대형 밀대</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>넓은 강당 청소도 쉽고 빠르게! 힘들이지 않고 깔끔한 바닥을 완성해 드립니다.</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>업소용 대형 밀대 추천, 강당 청소도 문제없이 빠르게</t>
+        </is>
+      </c>
+      <c r="H444" t="inlineStr">
+        <is>
+          <t>넓은 강당 및 대형 공간 청소에 적합한 업소용 대형 밀대입니다. 힘들이지 않고 깔끔한 바닥을 완성해 줍니다.</t>
+        </is>
+      </c>
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>업소용 밀대, 대형 밀대, 강당 청소, 청소용품, 바닥 청소, 대형 청소도구</t>
+        </is>
+      </c>
+      <c r="J444" t="inlineStr">
+        <is>
+          <t>청소/업소용</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-26 10:49)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J444"/>
+  <dimension ref="A1:J512"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22635,6 +22635,3406 @@
         </is>
       </c>
     </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>444</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>웅진 하늘보리 무라벨로 산뜻하게 마시는 보리차 경험</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://naver.me/xwwqaJRC</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240624_100/1719192332127bN5jb_PNG/67989840948385601_1345515016.png</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>산뜻한 무라벨 보리차</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>답답한 갈증을 시원하게 해소하는 산뜻한 무라벨 보리차로 깔끔한 맛을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>웅진 하늘보리 무라벨 보리차 깔끔한 갈증 해소 추천</t>
+        </is>
+      </c>
+      <c r="H445" t="inlineStr">
+        <is>
+          <t>산뜻하고 깔끔한 맛의 무라벨 보리차로 답답한 갈증을 시원하게 해소해주는 웅진 하늘보리를 만나보세요.</t>
+        </is>
+      </c>
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>웅진 하늘보리, 무라벨 보리차, 갈증 해소, 깔끔한 맛, 건강 음료</t>
+        </is>
+      </c>
+      <c r="J445" t="inlineStr">
+        <is>
+          <t>음료/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>445</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>침향명가 쌍화차로 하루를 건강하게 시작해요</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://naver.me/F2nuqP9O</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241007_240/1728281631148B5gsM_JPEG/16763555077355548_1436053499.jpg</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>하루 건강 쌍화차</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>피로하고 기운 없을 때 쌍화차 한잔으로 활력을 되찾아보세요.</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>침향명가 쌍화차 건강 시작 추천</t>
+        </is>
+      </c>
+      <c r="H446" t="inlineStr">
+        <is>
+          <t>피로 회복과 활력 충전에 좋은 침향명가 쌍화차로 하루를 상쾌하게 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>침향명가, 쌍화차, 건강차, 피로회복, 활력충전, 전통차</t>
+        </is>
+      </c>
+      <c r="J446" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>446</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>귤피차로 상쾌한 하루 시작하는 법</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://naver.me/xWznb5fA</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241129_14/1732872042459krwnk_JPEG/67004827598424723_1781685910.jpg</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>상쾌한 귤피차로 활력충전</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>귤피의 자연스러운 상큼함으로 지친 하루에 활력을 더하세요. 상쾌한 시작을 원한다면 이 차가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>귤피차 상쾌한 하루 시작 추천 자연 상큼함</t>
+        </is>
+      </c>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>귤피차로 지친 하루에 자연스러운 상큼함과 활력을 더하세요. 상쾌한 아침 시작에 좋은 건강 차입니다.</t>
+        </is>
+      </c>
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>귤피차,상쾌한차,건강차,자연상큼,활력증진,아침차,귤차</t>
+        </is>
+      </c>
+      <c r="J447" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>447</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>포근한 양털 극세사 이불로 따뜻한 겨울밤 보내기</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://naver.me/5TQAUVJC</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251017_104/1760674427180Oz96h_JPEG/14849679981967227_1667841524.JPG</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>포근한 양털 극세사 이불</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>차가운 겨울밤, 포근한 양털 극세사 이불로 따뜻함을 느껴보세요. 당신의 숙면을 책임집니다.</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>포근한 양털 극세사 이불로 따뜻한 겨울밤 추천</t>
+        </is>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>포근한 양털 극세사 이불로 차가운 겨울밤에도 따뜻하게 숙면할 수 있습니다. 부드러운 촉감과 우수한 보온성이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>양털이불,극세사이불,겨울이불,포근한이불,따뜻한이불,숙면이불,보온이불</t>
+        </is>
+      </c>
+      <c r="J448" t="inlineStr">
+        <is>
+          <t>침구/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>448</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>임산부도 안심하고 마시는 국산 생강차 추천</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://naver.me/5sGTh61B</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241129_102/1732876046130dEvq1_JPEG/42948874896799527_1178596958.jpg</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>임산부 안심 생강차</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>임신 중에도 걱정 없이 즐길 수 있는 순수 국산 생강차로 따뜻한 건강을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>임산부도 안심 국산 생강차 추천, 건강한 따뜻함</t>
+        </is>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>임신 중에도 안전하게 마실 수 있는 순수 국산 생강차로 건강과 따뜻함을 동시에 챙길 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>임산부생강차,국산생강차,임신중음료,건강음료,따뜻한차</t>
+        </is>
+      </c>
+      <c r="J449" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>449</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>출근길에 정읍 쌍화차 진액으로 활기 충전하기</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ZSx8tyd</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251128_18/1764291642295bn9Kf_JPEG/98424500938760244_1270736987.jpg</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>활기 충전 쌍화차 진액</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>출근길 피로와 스트레스를 달래고, 하루 종일 활기찬 에너지를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>출근길 활기 충전 쌍화차 진액 추천</t>
+        </is>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>출근길 피로와 스트레스를 완화하고 하루 종일 활기와 에너지를 선사하는 쌍화차 진액입니다.</t>
+        </is>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>출근길,쌍화차,쌍화차 진액,피로 해소,스트레스 완화,에너지 보충,건강음료</t>
+        </is>
+      </c>
+      <c r="J450" t="inlineStr">
+        <is>
+          <t>건강음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>450</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>출퇴근길 활력 챙기는 정읍 쌍화차 진액 이야기</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://naver.me/5dA46bIW</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251128_250/1764291799435gAELQ_JPEG/98424713661323385_733027965.jpg</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>출퇴근 활력 쌍화차</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>지친 출퇴근길, 쌍화차 진액으로 활력을 채워보세요. 편리한 휴대로 언제든 힘 나는 하루를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>출퇴근길 활력 챙기는 정읍 쌍화차 진액 추천</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>지친 출퇴근길에 간편하게 즐기는 정읍 쌍화차 진액으로 활력을 더하세요. 휴대가 편리해 언제든지 힘나는 하루를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>쌍화차,정읍쌍화차,출퇴근활력,건강음료,진액,휴대용차,피로회복,한방음료</t>
+        </is>
+      </c>
+      <c r="J451" t="inlineStr">
+        <is>
+          <t>건강/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>451</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>극세사이불로 포근한 겨울밤 보내기</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://naver.me/FkL0QQcl</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251107_157/1762482160525J9DVA_JPEG/39461885613659734_966175733.jpg</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>극세사 포근 이불</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>찬바람 걱정 없이 포근한 겨울밤, 극세사 이불로 따뜻함을 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>극세사이불 따뜻함 가득 겨울철 추천 이불 구매</t>
+        </is>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>찬바람 걱정 없이 포근한 극세사 이불로 겨울밤 따뜻하게 보내세요.</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>극세사이불,겨울이불,포근한이불,따뜻한침구,겨울침구</t>
+        </is>
+      </c>
+      <c r="J452" t="inlineStr">
+        <is>
+          <t>침구</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>452</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 따뜻한 설약산 쌍화차 한 잔</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://naver.me/xLsADb0P</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240109_95/1704781943676OA5WV_JPEG/32084627490806281_654386819.jpg</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>출퇴근 따뜻한 쌍화차</t>
+        </is>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길, 몸과 마음을 따뜻하게 채워주는 설약산 쌍화차로 하루를 활기차게 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>출퇴근 길 따뜻한 설약산 쌍화차 추천</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길 몸과 마음을 따뜻하게 해주는 설약산 쌍화차로 활기찬 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>설약산,쌍화차,출퇴근,따뜻한음료,건강차,활력,한방차</t>
+        </is>
+      </c>
+      <c r="J453" t="inlineStr">
+        <is>
+          <t>건강차/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>453</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>겨울철 우주전열 동파방지기 착용 후기</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://naver.me/FwjiHsmv</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241217_31/1734418054618E5ad1_JPEG/13813849723769849_1415684602.jpg</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>겨울철 동파 방지기</t>
+        </is>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>추운 겨울, 동파 걱정 없이 따뜻함을 유지하세요. 안전하고 효과적인 전열기로 걱정을 덜어드립니다.</t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t>겨울철 우주전열 동파방지기 추천 - 안전한 겨울 난방 솔루션</t>
+        </is>
+      </c>
+      <c r="H454" t="inlineStr">
+        <is>
+          <t>겨울철 동파 걱정 없이 안전하게 사용할 수 있는 우주전열 동파방지기로 집안을 따뜻하게 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>동파방지기,우주전열,겨울난방,동파예방,전열기,안전난방,겨울용품</t>
+        </is>
+      </c>
+      <c r="J454" t="inlineStr">
+        <is>
+          <t>난방/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>454</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>쌍화차 진액으로 하루 시작하는 건강 루틴</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://naver.me/FGExgtIj</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241007_173/1728281159866Xnb8F_JPEG/13466125642859210_2088804952.jpg</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>하루 활력 쌍화차 진액</t>
+        </is>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>바쁜 아침, 지친 몸에 쌍화차 진액 한 잔으로 건강한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>쌍화차 진액 건강 루틴 추천, 바쁜 아침 활력 충전</t>
+        </is>
+      </c>
+      <c r="H455" t="inlineStr">
+        <is>
+          <t>쌍화차 진액으로 아침 건강 관리에 도움을 주며, 바쁜 일상 속 지친 몸에 활력을 더합니다.</t>
+        </is>
+      </c>
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>쌍화차, 건강 루틴, 진액, 아침 음료, 활력 충전, 피로 회복, 전통차</t>
+        </is>
+      </c>
+      <c r="J455" t="inlineStr">
+        <is>
+          <t>건강/차</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>455</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>아침 출근길, 생강청 한잔으로 건강 챙기기</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://naver.me/xwwqaJzE</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240906_37/1725596048530vIgYT_JPEG/15949466535486035_538780801.jpg</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>생강청으로 활기충전</t>
+        </is>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>출근길 피로와 감기 걱정을 생강청 한 잔으로 날려보세요. 자연의 따뜻한 건강 비결을 담았습니다.</t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>아침 출근길 생강청으로 건강 챙기기 추천</t>
+        </is>
+      </c>
+      <c r="H456" t="inlineStr">
+        <is>
+          <t>출근길 피로와 감기 예방에 좋은 자연생강청, 간편하게 마시며 건강을 지키세요.</t>
+        </is>
+      </c>
+      <c r="I456" t="inlineStr">
+        <is>
+          <t>생강청,출근길,건강챙기기,피로회복,감기예방,자연성분,음료</t>
+        </is>
+      </c>
+      <c r="J456" t="inlineStr">
+        <is>
+          <t>건강/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>456</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>국내산 생강차로 건강한 하루 시작하기</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://naver.me/GDL29Ymy</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250919_297/17582471036928WGbO_JPEG/8338050696555187_1334539117.jpg</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>국내산 생강 건강차</t>
+        </is>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>몸도 마음도 편안해지는 국내산 생강차로 건강한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>국내산 생강차로 건강한 하루 시작하기 추천</t>
+        </is>
+      </c>
+      <c r="H457" t="inlineStr">
+        <is>
+          <t>국내산 생강차로 몸과 마음을 편안하게 해주는 건강 음료를 만나보세요. 일상에 상쾌함과 활력을 더합니다.</t>
+        </is>
+      </c>
+      <c r="I457" t="inlineStr">
+        <is>
+          <t>국내산 생강차,생강차,건강음료,편안한차,면역강화,자연재료</t>
+        </is>
+      </c>
+      <c r="J457" t="inlineStr">
+        <is>
+          <t>건강식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>457</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>도라지 생강차로 목 건강 챙기기 좋은 선택</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://naver.me/5FES5a69</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250724_141/1753331244269c2b5l_JPEG/50359580391045185_594662318.jpg</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>목 건강 도라지 생강차</t>
+        </is>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>목이 자주 아플 때, 도라지 생강차로 부드럽게 케어하세요. 자연의 힘으로 건강을 지켜드립니다.</t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>도라지 생강차 추천 목 건강 챙기기 좋은 선택</t>
+        </is>
+      </c>
+      <c r="H458" t="inlineStr">
+        <is>
+          <t>목이 자주 아플 때 도라지 생강차로 부드럽게 케어하세요. 자연 성분으로 건강한 목을 지켜드립니다.</t>
+        </is>
+      </c>
+      <c r="I458" t="inlineStr">
+        <is>
+          <t>도라지 생강차,목 건강,자연차,목 케어,건강차</t>
+        </is>
+      </c>
+      <c r="J458" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>458</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>국내산 배도라지차로 건강한 하루를 시작해요</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://naver.me/FzsZGFWH</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240213_139/1707791072039OGO7a_JPEG/35093755923080030_755062530.jpg</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>국내산 배도라지차 건강차</t>
+        </is>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t>목 건강과 면역 걱정될 때, 부드럽고 상쾌한 배도라지차로 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>국내산 배도라지차 건강차 추천 - 목 건강과 면역 강화에</t>
+        </is>
+      </c>
+      <c r="H459" t="inlineStr">
+        <is>
+          <t>국내산 배도라지차로 목 건강을 지키고 면역력을 높여주는 부드럽고 상쾌한 건강차입니다. 하루 시작에 좋은 음료로 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I459" t="inlineStr">
+        <is>
+          <t>배도라지차,국내산차,목건강차,면역강화차,건강음료</t>
+        </is>
+      </c>
+      <c r="J459" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>459</v>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>배도라지차 티백으로 하루를 건강하게 시작해요</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://naver.me/FeNRGM1i</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221111_69/1668165718905VWApD_JPEG/69301552727708719_730058829.jpg</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>배도라지차로 건강한 시작</t>
+        </is>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t>피로하고 목이 답답할 때 배도라지차 한 잔으로 상쾌함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>배도라지차 티백 추천 건강한 하루 시작</t>
+        </is>
+      </c>
+      <c r="H460" t="inlineStr">
+        <is>
+          <t>피로와 목 답답함에 좋은 배도라지차 티백으로 상쾌한 하루를 시작하세요. 간편한 티백으로 언제든 즐길 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I460" t="inlineStr">
+        <is>
+          <t>배도라지차, 티백, 건강차, 목 건강, 피로 해소, 상쾌함, 허브차, 음료</t>
+        </is>
+      </c>
+      <c r="J460" t="inlineStr">
+        <is>
+          <t>건강/차</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>460</v>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>감기 걸렸을 때 집에서 생강청 한 잔의 힘</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://naver.me/GkU3uadw</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240617_290/1718619725343rk6fw_JPEG/55498208266751246_588896069.jpg</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>따뜻한 감기 완화 생강청</t>
+        </is>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t>감기로 힘든 날, 집에서 간편하게 생강청 한 잔으로 몸을 따뜻하게 해보세요. 빠른 건강 회복에 도움을 드립니다.</t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>감기 생강청 한 잔으로 집에서 건강 회복 추천</t>
+        </is>
+      </c>
+      <c r="H461" t="inlineStr">
+        <is>
+          <t>감기로 힘든 날 간편하게 집에서 마시는 생강청으로 몸을 따뜻하게 하고 빠른 건강 회복에 도움을 드립니다.</t>
+        </is>
+      </c>
+      <c r="I461" t="inlineStr">
+        <is>
+          <t>감기,생강청,건강회복,따뜻한음료,집에서간편</t>
+        </is>
+      </c>
+      <c r="J461" t="inlineStr">
+        <is>
+          <t>건강/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>461</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>고농축 생강청으로 몸을 따뜻하게 감싸보세요</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://naver.me/FhfL3P5y</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231012_287/16970765397909TPvt_JPEG/27877140722994300_2094553161.jpg</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>고농축 생강청 온열 효과</t>
+        </is>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>차가운 몸을 따뜻하게 감싸주는 고농축 생강청으로 건강과 활력을 되찾으세요.</t>
+        </is>
+      </c>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t>고농축 생강청 건강 활력 추천</t>
+        </is>
+      </c>
+      <c r="H462" t="inlineStr">
+        <is>
+          <t>고농축 생강청으로 차가운 몸을 따뜻하게 감싸고 건강과 활력을 높여보세요. 간편한 섭취로 일상에 활력을 더합니다.</t>
+        </is>
+      </c>
+      <c r="I462" t="inlineStr">
+        <is>
+          <t>고농축 생강청,생강청 건강,몸 따뜻하게,활력보충,건강 음료</t>
+        </is>
+      </c>
+      <c r="J462" t="inlineStr">
+        <is>
+          <t>건강식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>462</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>목감기에 좋은 따뜻한 계피 생강차 한잔</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gso2qkrW</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250821_159/1755768464047YXGgm_JPEG/40953429839266928_423378625.jpg</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>따뜻한 계피 생강차</t>
+        </is>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>목감기로 힘든 당신에게, 따뜻한 계피 생강차가 편안한 휴식을 선물합니다.</t>
+        </is>
+      </c>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t>목감기 완화에 좋은 계피 생강차 추천</t>
+        </is>
+      </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>목감기로 불편한 목을 따뜻한 계피 생강차가 부드럽게 감싸줍니다. 휴식과 건강을 동시에 챙기세요.</t>
+        </is>
+      </c>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>목감기,계피생강차,따뜻한차,숙면,건강차,목휴식,면역력</t>
+        </is>
+      </c>
+      <c r="J463" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>463</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>제주 청귤청으로 상큼한 에이드 한잔 즐기기</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://naver.me/5OtyxOqf</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230722_234/1690031021858hEBOm_JPEG/40277439368070612_1906966841.jpg</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>상큼 제주 청귤 에이드</t>
+        </is>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>달콤 쌉싸름한 제주 청귤청으로 집에서도 상큼한 에이드 맛을 간편하게 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>제주 청귤청으로 상큼한 에이드 만들기 추천</t>
+        </is>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>달콤 쌉싸름한 제주 청귤청으로 집에서도 간편하게 상큼한 에이드를 즐겨보세요. 건강한 홈카페 음료로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I464" t="inlineStr">
+        <is>
+          <t>제주청귤청,에이드만들기,상큼한음료,홈카페,과일청,제주과일</t>
+        </is>
+      </c>
+      <c r="J464" t="inlineStr">
+        <is>
+          <t>음료/과일청</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>464</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>전통 쌍화차로 건강한 하루 시작해요</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://naver.me/5SSQcqk4</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241204_26/1733298708741Mnskk_JPEG/5452845837548796_1181273498.jpg</t>
+        </is>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>전통 쌍화차로 건강 챙기기</t>
+        </is>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>피로와 스트레스에 지친 당신, 전통 쌍화차로 활기찬 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>전통 쌍화차로 건강한 하루 시작 추천</t>
+        </is>
+      </c>
+      <c r="H465" t="inlineStr">
+        <is>
+          <t>피로와 스트레스 완화를 돕는 전통 쌍화차로 활기찬 하루를 시작해보세요. 건강 관리에 좋은 전통 음료입니다.</t>
+        </is>
+      </c>
+      <c r="I465" t="inlineStr">
+        <is>
+          <t>전통 쌍화차, 피로회복, 스트레스 완화, 건강 음료, 한방차</t>
+        </is>
+      </c>
+      <c r="J465" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>465</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>센서형 열선으로 겨울철 배관 동파 걱정 끝</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://naver.me/x6xylquK</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251224_73/1766549541980YnthQ_JPEG/14525534996386451_1284115973.jpg</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>센서 열선 배관 보호</t>
+        </is>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>겨울철 배관 동파 걱정 없이 안전하게 지키세요. 센서형 열선으로 스마트한 난방 솔루션을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>센서형 열선으로 겨울철 배관 동파 걱정 없이 안전하게 추천</t>
+        </is>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>센서형 열선을 사용해 겨울철 배관 동파를 예방하세요. 스마트 난방 솔루션으로 안전하고 효율적인 난방 관리에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>센서형 열선, 배관 동파 예방, 겨울철 난방, 스마트 난방, 배관 보온</t>
+        </is>
+      </c>
+      <c r="J466" t="inlineStr">
+        <is>
+          <t>난방/배관</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>466</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>모과청과 레몬 생강 수제청으로 건강한 하루 시작해요</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://naver.me/F2nuqPJ6</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230715_7/1689398730892rTnsy_JPEG/4915219190794987_2067540992.jpg</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>상큼한 모과 레몬 생강청</t>
+        </is>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t>몸을 따뜻하게 하고 면역력을 챙기는 자연수제청으로 건강한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G467" t="inlineStr">
+        <is>
+          <t>모과청과 레몬 생강 수제청으로 건강한 하루 시작 추천</t>
+        </is>
+      </c>
+      <c r="H467" t="inlineStr">
+        <is>
+          <t>모과청, 레몬, 생강의 자연 원료로 만든 수제청은 면역력 강화와 체온 유지에 도움을 줍니다. 건강한 습관을 시작하기 좋은 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I467" t="inlineStr">
+        <is>
+          <t>모과청, 레몬, 생강, 수제청, 면역력, 건강음료, 자연수제, 건강관리</t>
+        </is>
+      </c>
+      <c r="J467" t="inlineStr">
+        <is>
+          <t>건강/음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>467</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>임산부도 안심하고 마실 수 있는 그린 루이보스티 추천</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://naver.me/GcKrI1ex</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250114_163/1736835160470W2rn0_JPEG/381095285362304_518993906.jpg</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>임산부용 그린 루이보스티</t>
+        </is>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>임산부도 안심하고 즐길 수 있는 건강한 루이보스티로 하루를 편안하게 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G468" t="inlineStr">
+        <is>
+          <t>임산부도 안심 그린 루이보스티 추천 건강차 구매</t>
+        </is>
+      </c>
+      <c r="H468" t="inlineStr">
+        <is>
+          <t>임산부도 안심하고 마실 수 있는 건강한 그린 루이보스티로 하루를 편안하게 시작하세요. 카페인 걱정 없이 즐기기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I468" t="inlineStr">
+        <is>
+          <t>그린 루이보스티,임산부차,카페인 없음,건강차,허브차,임산부 추천</t>
+        </is>
+      </c>
+      <c r="J468" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>468</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>따뜻함을 더하는 극세사 겨울 이불 사용기</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://naver.me/GxLTvvuo</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221014_194/1665727893330doCx6_JPEG/66863789054466131_982598869.JPG</t>
+        </is>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>포근한 극세사 겨울 이불</t>
+        </is>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>찬바람에도 끄떡없는 극세사 이불로 따뜻함 가득, 편안한 잠자리를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t>극세사 겨울 이불 추천 따뜻함 가득한 포근한 겨울이불</t>
+        </is>
+      </c>
+      <c r="H469" t="inlineStr">
+        <is>
+          <t>찬바람에도 따뜻함을 유지하는 극세사 겨울 이불로 편안한 잠자리를 선사합니다. 부드러운 촉감과 보온성이 뛰어난 겨울용 이불입니다.</t>
+        </is>
+      </c>
+      <c r="I469" t="inlineStr">
+        <is>
+          <t>극세사이불,겨울이불,따뜻한이불,겨울침구,포근한이불,보온이불,침실용이불</t>
+        </is>
+      </c>
+      <c r="J469" t="inlineStr">
+        <is>
+          <t>침구류/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>469</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>한파에도 포근한 극세사 겨울 이불 추천</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://naver.me/GWiqjjPj</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20201115_33/1605367296878qBuQR_JPEG/6503080585163488_1950567508.JPG</t>
+        </is>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>한파 대비 극세사 겨울이불</t>
+        </is>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t>찬바람 걱정 없이 포근함을 선사하는 극세사 이불로 따뜻한 겨울 준비하세요.</t>
+        </is>
+      </c>
+      <c r="G470" t="inlineStr">
+        <is>
+          <t>한파에도 포근한 극세사 겨울 이불 추천으로 따뜻함 유지</t>
+        </is>
+      </c>
+      <c r="H470" t="inlineStr">
+        <is>
+          <t>찬바람 걱정 없이 부드럽고 따뜻한 극세사 이불로 겨울철 포근함을 선사합니다. 실용적이고 가볍게 사용 가능한 겨울 이불을 찾는 분께 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>극세사 이불,겨울 이불,포근한 이불,따뜻한 이불,한파 대비 이불,부드러운 겨울 이불</t>
+        </is>
+      </c>
+      <c r="J470" t="inlineStr">
+        <is>
+          <t>침구/계절용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>470</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>임산부도 안전하게 즐기는 그린 루이보스티 허브차</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://naver.me/xktnfElC</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240805_187/1722841769925n47Yn_JPEG/69215348983757424_1718355489.JPG</t>
+        </is>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>임산부용 안전 허브티</t>
+        </is>
+      </c>
+      <c r="F471" t="inlineStr">
+        <is>
+          <t>임산부도 안심하고 마실 수 있는 무카페인 그린 루이보스티로 건강한 하루를 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G471" t="inlineStr">
+        <is>
+          <t>임산부도 안전한 그린 루이보스티 허브차 추천</t>
+        </is>
+      </c>
+      <c r="H471" t="inlineStr">
+        <is>
+          <t>무카페인 그린 루이보스티 허브차로 임산부도 안심하고 마실 수 있으며, 건강한 일상을 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I471" t="inlineStr">
+        <is>
+          <t>그린루이보스티,임산부차,무카페인허브차,건강차,허브티</t>
+        </is>
+      </c>
+      <c r="J471" t="inlineStr">
+        <is>
+          <t>건강/차</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>471</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>하루 한 잔, 유기농 도라지차로 건강 챙기기</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://naver.me/GwSMkuZa</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240225_234/1708837911683eQEJS_JPEG/36140595492190541_810407892.jpg</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>유기농 도라지차 건강차</t>
+        </is>
+      </c>
+      <c r="F472" t="inlineStr">
+        <is>
+          <t>힘든 하루, 도라지차 한 잔으로 활력을 충전하세요. 자연의 건강함을 담아 몸과 마음을 케어합니다.</t>
+        </is>
+      </c>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t>하루 한 잔 유기농 도라지차 건강 관리 추천</t>
+        </is>
+      </c>
+      <c r="H472" t="inlineStr">
+        <is>
+          <t>유기농 도라지차로 피로 회복과 면역력 증진에 도움을 주며 일상 속 건강을 지켜줍니다.</t>
+        </is>
+      </c>
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>유기농 도라지차, 건강차, 피로회복, 면역력증진, 자연건강, 도라지 음료</t>
+        </is>
+      </c>
+      <c r="J472" t="inlineStr">
+        <is>
+          <t>건강음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>472</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>출근길에 간편하게 즐기는 배도라지차 한잔</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://naver.me/xquarVCT</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250217_231/17397740180499FAqa_JPEG/10282055199597087_1003253005.jpg</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>출근길 간편 배도라지차</t>
+        </is>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t>바쁜 아침, 간편하게 마시는 배도라지차로 활기찬 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr">
+        <is>
+          <t>출근길 간편 배도라지차 추천으로 활기찬 하루 시작</t>
+        </is>
+      </c>
+      <c r="H473" t="inlineStr">
+        <is>
+          <t>바쁜 아침에 간편하게 즐길 수 있는 배도라지차로 건강한 하루를 시작하세요. 피로 회복과 면역력 증진에 도움됩니다.</t>
+        </is>
+      </c>
+      <c r="I473" t="inlineStr">
+        <is>
+          <t>배도라지차,간편음료,아침음료,건강차,피로회복,면역력증진,출근길음료</t>
+        </is>
+      </c>
+      <c r="J473" t="inlineStr">
+        <is>
+          <t>음료/건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>473</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>오미자차로 건강한 하루 시작하기</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://naver.me/FxCtifno</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250217_30/17397799946681S5Ug_JPEG/32015003248316212_2072686942.jpg</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>상쾌한 오미자 건강차</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>피로하고 지친 일상에 상큼한 오미자차 한 잔으로 활력을 찾아보세요.</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t>오미자차 건강한 하루 시작하기 추천</t>
+        </is>
+      </c>
+      <c r="H474" t="inlineStr">
+        <is>
+          <t>상큼한 오미자차 한 잔으로 피로한 일상에 활력을 더하세요. 건강 관리에 적합한 음료입니다.</t>
+        </is>
+      </c>
+      <c r="I474" t="inlineStr">
+        <is>
+          <t>오미자차, 건강음료, 피로회복, 자연차, 상큼한차</t>
+        </is>
+      </c>
+      <c r="J474" t="inlineStr">
+        <is>
+          <t>건강음료</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>474</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>국산 대추차 티백으로 건강한 하루 시작하기</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://naver.me/GreaIrQg</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251120_163/1763614589216TdcMR_JPEG/61092723772271708_1366188997.jpg</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>건강 대추차 티백</t>
+        </is>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t>바쁜 일상 속 힘들 때, 국산 대추차로 몸과 마음에 건강을 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t>국산 대추차 티백 건강한 하루 시작 추천</t>
+        </is>
+      </c>
+      <c r="H475" t="inlineStr">
+        <is>
+          <t>국산 대추차 티백으로 바쁜 일상 속 건강을 챙기고 마음의 여유를 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="I475" t="inlineStr">
+        <is>
+          <t>국산대추차,대추차티백,건강차,한방차,힐링음료</t>
+        </is>
+      </c>
+      <c r="J475" t="inlineStr">
+        <is>
+          <t>건강차</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>475</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>닥터포포 올인원 바디워시로 상쾌한 아침을 시작해보세요</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Qi7RUVD</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230508_253/1683523227768QfbrO_JPEG/12241788568690015_1711174330.jpg</t>
+        </is>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>상쾌한 올인원 바디워시</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>피부 고민 없이 깔끔하게, 하루를 상쾌하게 시작하고 싶다면 이 올인원 바디워시가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>닥터포포 올인원 바디워시 추천, 상쾌한 아침 시작</t>
+        </is>
+      </c>
+      <c r="H476" t="inlineStr">
+        <is>
+          <t>피부 고민 없이 깔끔하게 사용 가능한 닥터포포 올인원 바디워시로 하루를 산뜻하게 시작하세요. 민감한 피부에도 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I476" t="inlineStr">
+        <is>
+          <t>닥터포포, 올인원 바디워시, 바디클렌저, 상쾌한 바디워시, 피부관리, 데일리 바디워시</t>
+        </is>
+      </c>
+      <c r="J476" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>476</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>수영 후 피부를 지켜주는 염소제거 바디워시 사용기</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://naver.me/F3YX0Cyq</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250214_185/1739521794697AD6Mk_PNG/13957607813165967_1722259381.png</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>수영 후 염소케어 바디워시</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>수영 후 피부 자극 걱정 끝, 염소 잔여물 없이 부드럽게 케어해 줍니다.</t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t>수영 후 피부 지킴이 염소제거 바디워시 추천</t>
+        </is>
+      </c>
+      <c r="H477" t="inlineStr">
+        <is>
+          <t>수영 후 남은 염소 잔여물을 부드럽게 제거해 피부 자극을 줄여줍니다. 민감한 피부도 안심하고 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I477" t="inlineStr">
+        <is>
+          <t>염소제거,바디워시,수영후케어,피부진정,민감피부,클렌징,보습</t>
+        </is>
+      </c>
+      <c r="J477" t="inlineStr">
+        <is>
+          <t>뷰티/스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>477</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>그루밍랩 올인원 바디 샴푸로 깔끔한 샤워 루틴 만들기</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://naver.me/G6Qth1Jr</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250627_153/1750988501096zwlon_PNG/5561560220604580_612289974.png</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>올인원 바디 샴푸</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>피부 고민 없이 간편한 샤워를 원한다면, 하나로 끝나는 올인원 바디 샴푸를 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t>그루밍랩 올인원 바디 샴푸로 간편한 샤워 추천</t>
+        </is>
+      </c>
+      <c r="H478" t="inlineStr">
+        <is>
+          <t>그루밍랩 올인원 바디 샴푸로 피부 고민 없이 깔끔한 샤워 루틴을 완성하세요. 간편하게 하나로 청결과 보습을 동시에 관리할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I478" t="inlineStr">
+        <is>
+          <t>그루밍랩,올인원 바디 샴푸,바디클렌저,샤워용품,피부보습,간편샤워,남성바디샴푸,피부관리</t>
+        </is>
+      </c>
+      <c r="J478" t="inlineStr">
+        <is>
+          <t>바디케어/샤워용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>478</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>수분 가득 속광토너로 촉촉한 피부 완성하기</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://naver.me/GbAFfPTh</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250715_57/1752539081224v2Ja4_JPEG/28941523354805732_1202933094.jpg</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>수분 충전 촉촉 속광토너</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>건조한 피부에 꼭 맞는 수분 가득 속광토너로 촉촉하고 빛나는 피부를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t>수분 가득 속광토너로 촉촉한 피부 완성하기 추천</t>
+        </is>
+      </c>
+      <c r="H479" t="inlineStr">
+        <is>
+          <t>건조한 피부에 적합한 수분 가득 속광토너로 촉촉하고 빛나는 피부를 가꾸세요. 매일 사용하기 좋은 수분 토너입니다.</t>
+        </is>
+      </c>
+      <c r="I479" t="inlineStr">
+        <is>
+          <t>속광토너,수분토너,촉촉한피부,건조피부케어,피부보습</t>
+        </is>
+      </c>
+      <c r="J479" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>479</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>엘지생활건강 수퍼테크로 깨끗한 세탁 경험하기</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://naver.me/517NOHhK</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241210_259/1733811626632dDVch_PNG/16718292218145902_1296557479.png</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>강력 세탁력 세제</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>때를 확실히 지우고 깨끗한 세탁을 원한다면, 수퍼테크가 답입니다.</t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t>엘지생활건강 수퍼테크 세탁세제 추천 깨끗한 세탁 경험</t>
+        </is>
+      </c>
+      <c r="H480" t="inlineStr">
+        <is>
+          <t>때를 확실히 제거하고 깨끗한 세탁을 원하는 분들에게 적합한 엘지생활건강 수퍼테크 세탁세제입니다. 강력한 세탁력으로 신선한 세탁 경험을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I480" t="inlineStr">
+        <is>
+          <t>엘지생활건강,수퍼테크,세탁세제,깨끗한세탁,때제거,세탁추천,세탁용품</t>
+        </is>
+      </c>
+      <c r="J480" t="inlineStr">
+        <is>
+          <t>생활용품/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>480</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>피부 깊숙이 수분을 채우는 속광토너 사용법</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://naver.me/5ow5VHFf</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250718_139/1752798739095lUmHl_JPEG/19726570586421607_1865008403.jpg</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>속광 수분 토너</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>건조하고 칙칙한 피부에 즉각적인 수분과 촉촉한 광채를 선사해 보세요.</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>속광토너 피부 깊숙이 수분 충전하는 사용법 추천</t>
+        </is>
+      </c>
+      <c r="H481" t="inlineStr">
+        <is>
+          <t>속광토너로 건조한 피부에 즉각적인 수분과 촉촉한 광채를 채워 환하고 건강한 피부를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I481" t="inlineStr">
+        <is>
+          <t>속광토너,수분토너,피부수분,촉촉한피부,광채토너,건조피부,토너사용법</t>
+        </is>
+      </c>
+      <c r="J481" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>481</v>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>세라마이드 토너로 촉촉한 피부 관리하기</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlbDqx3O</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221114_154/1668394834421hxBBf_JPEG/69530730148830853_141829253.jpg</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>세라마이드 촉촉 토너</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>건조하고 거칠어진 피부에 깊은 수분감을 채워 부드럽고 건강한 피부로 가꿔보세요.</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>세라마이드 토너로 촉촉한 피부 관리 추천</t>
+        </is>
+      </c>
+      <c r="H482" t="inlineStr">
+        <is>
+          <t>건조하고 거친 피부에 깊은 수분감을 채워 부드럽고 건강한 피부로 가꿔줍니다. 매일 사용하는 피부 관리 토너로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I482" t="inlineStr">
+        <is>
+          <t>세라마이드,토너,촉촉한피부,수분보습,피부관리,건강한피부</t>
+        </is>
+      </c>
+      <c r="J482" t="inlineStr">
+        <is>
+          <t>스킨케어/토너</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>482</v>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>기념일에 딱 맞는 핸드 앤 바디 워시 선물 추천</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://naver.me/F4LMqVUO</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231108_258/1699417182746hJzXx_JPEG/13270048637862448_1045257954.jpg</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>기념일용 핸드바디 워시</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>특별한 날, 부드럽고 촉촉한 핸드 앤 바디 워시로 소중한 분께 감사의 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>기념일 선물 추천 핸드 앤 바디 워시 구매 가이드</t>
+        </is>
+      </c>
+      <c r="H483" t="inlineStr">
+        <is>
+          <t>부드럽고 촉촉한 핸드 앤 바디 워시로 특별한 기념일에 소중한 분께 감사의 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="I483" t="inlineStr">
+        <is>
+          <t>기념일선물,핸드앤바디워시,선물추천,보습케어,촉촉한바디워시</t>
+        </is>
+      </c>
+      <c r="J483" t="inlineStr">
+        <is>
+          <t>기념일/뷰티</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>483</v>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>비건 바디워시로 민감한 피부도 촉촉하게 케어해요</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://naver.me/xBMJQmfh</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251222_116/1766365451465tWcnu_JPEG/76488732339196560_1297190941.jpg</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>민감 피부 촉촉 바디워시</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없이 부드럽게 케어해주는 비건 바디워시로 촉촉함을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t>비건 바디워시 추천 민감 피부 촉촉한 바디케어</t>
+        </is>
+      </c>
+      <c r="H484" t="inlineStr">
+        <is>
+          <t>민감한 피부도 부드럽게 관리할 수 있는 비건 바디워시로 촉촉한 피부를 유지하세요. 안심하고 사용할 수 있는 순한 성분이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I484" t="inlineStr">
+        <is>
+          <t>비건 바디워시, 민감 피부, 촉촉한 바디케어, 순한 바디워시, 피부 보습</t>
+        </is>
+      </c>
+      <c r="J484" t="inlineStr">
+        <is>
+          <t>뷰티/바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>484</v>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>꾸준한 수분 공급으로 촉촉한 피부 만드는 그린푸드 토너</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://naver.me/xhlC2qkZ</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230912_101/1694507881817YL0l8_JPEG/8396739625932187_434637330.jpg</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>촉촉 수분 그린푸드 토너</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>건조한 피부에 지속적인 수분을 채워주어 하루 종일 촉촉함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>그린푸드 토너 추천 꾸준한 수분 공급 촉촉한 피부 완성</t>
+        </is>
+      </c>
+      <c r="H485" t="inlineStr">
+        <is>
+          <t>건조한 피부에 지속적으로 수분을 공급해 하루 종일 촉촉함을 유지하는 그린푸드 토너입니다. 민감한 피부에도 안심하고 사용 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I485" t="inlineStr">
+        <is>
+          <t>그린푸드,토너,수분공급,촉촉한피부,건성피부,스킨케어,보습,피부진정,민감성피부</t>
+        </is>
+      </c>
+      <c r="J485" t="inlineStr">
+        <is>
+          <t>스킨케어/보습</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>485</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>엘지생활건강 테크 파워 액체세제로 깨끗한 세탁을 경험해보세요</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Bwj9bLf</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230205_31/1675608239516AEfan_PNG/2910923353599488_1608149617.png</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>강력 세탁 파워 액체세제</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>땀과 찌든 때도 깨끗하게, 상쾌한 세탁을 원한다면 이 제품이 딱이에요.</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>엘지생활건강 테크 파워 액체세제 추천 깨끗한 세탁</t>
+        </is>
+      </c>
+      <c r="H486" t="inlineStr">
+        <is>
+          <t>땀과 찌든 때까지 말끔히 세탁해주는 액체세제로, 상쾌한 세탁 후기를 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I486" t="inlineStr">
+        <is>
+          <t>엘지생활건강, 테크파워, 액체세제, 깨끗한세탁, 찌든때제거, 상쾌한세탁, 세탁세제</t>
+        </is>
+      </c>
+      <c r="J486" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>486</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 딥클린으로 깨끗한 세탁 경험하기</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://naver.me/FjCnsYFw</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230425_292/1682384845934vQcyi_JPEG/35156816916761457_2042029041.jpg</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>딥클린 세탁 세제</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>옷의 묵은 때와 얼룩 걱정 끝! 헨켈 퍼실 딥클린으로 깨끗한 세탁을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 딥클린 세탁세제 추천 깨끗한 세탁 경험</t>
+        </is>
+      </c>
+      <c r="H487" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 딥클린으로 묵은 때와 얼룩까지 깨끗하게 세탁하세요. 뛰어난 세정력으로 옷감 손상 걱정 없이 안심 세탁이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="I487" t="inlineStr">
+        <is>
+          <t>헨켈,퍼실,딥클린,세탁세제,깨끗한세탁,얼룩제거,묵은때,세탁추천</t>
+        </is>
+      </c>
+      <c r="J487" t="inlineStr">
+        <is>
+          <t>생활/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>487</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>산양유 성분으로 피부에 자극 없이 촉촉하게</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbJl3Rm</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250901_26/175668442092049y5k_JPEG/74000491859115632_35322206.jpg</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>산양유 촉촉 보습 케어</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>민감한 피부도 산양유로 자극 없이 촉촉하게 케어하세요. 하루종일 촉촉함을 유지해드립니다.</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>산양유 성분 촉촉한 피부 케어 추천</t>
+        </is>
+      </c>
+      <c r="H488" t="inlineStr">
+        <is>
+          <t>민감한 피부도 부담 없이 사용할 수 있는 산양유 성분으로 촉촉한 피부 케어를 도와줍니다. 하루 종일 촉촉함 유지에 효과적입니다.</t>
+        </is>
+      </c>
+      <c r="I488" t="inlineStr">
+        <is>
+          <t>산양유,촉촉한피부,민감피부,피부케어,보습크림,자극없음,스킨케어</t>
+        </is>
+      </c>
+      <c r="J488" t="inlineStr">
+        <is>
+          <t>피부케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>488</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>히알루론산으로 촉촉한 피부 완성한 스킨토너 이야기</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://naver.me/5tftVyZJ</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230407_4/1680860479959sdO53_JPEG/8paW9_100068_1.jpg</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>촉촉한 히알루론산 토너</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>건조한 피부에 깊은 수분을 채워 하루 종일 촉촉함을 유지해 줍니다.</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>히알루론산 스킨토너 추천, 촉촉한 피부 완성</t>
+        </is>
+      </c>
+      <c r="H489" t="inlineStr">
+        <is>
+          <t>히알루론산 함유로 깊은 수분을 공급하여 건조한 피부를 하루 종일 촉촉하게 유지해 줍니다. 모든 피부 타입에 적합한 스킨토너입니다.</t>
+        </is>
+      </c>
+      <c r="I489" t="inlineStr">
+        <is>
+          <t>히알루론산,스킨토너,촉촉한피부,수분공급,건성피부,피부보습,기초화장품</t>
+        </is>
+      </c>
+      <c r="J489" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>489</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>부케가르니 모이스처 바디워시로 촉촉한 피부 느껴보세요</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Qi7RUCe</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241106_235/1730883555904onTxV_JPEG/10965527644390372_979791515.jpg</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>촉촉한 모이스처 바디워시</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>건조한 피부에 부드럽게 스며들어 하루 종일 촉촉함을 유지해줍니다.</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>부케가르니 모이스처 바디워시 촉촉한 피부 추천</t>
+        </is>
+      </c>
+      <c r="H490" t="inlineStr">
+        <is>
+          <t>부케가르니 모이스처 바디워시는 건조한 피부에 부드럽게 흡수되어 하루 종일 촉촉함을 유지해줍니다.</t>
+        </is>
+      </c>
+      <c r="I490" t="inlineStr">
+        <is>
+          <t>부케가르니,모이스처,바디워시,촉촉한피부,보습,스킨케어,건조피부</t>
+        </is>
+      </c>
+      <c r="J490" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>490</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>부드러운 약산성 포뮬러로 매일 상쾌한 샤워 타임</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://naver.me/xktn4CJ0</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_260/1729729268682uHFws_JPEG/63862172811086960_674702177.jpg</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>부드러운 약산성 샤워젤</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없이, 부드러운 약산성 포뮬러로 매일 상쾌한 샤워를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>부드러운 약산성 포뮬러 샤워젤 추천 - 매일 상쾌한 피부 관리</t>
+        </is>
+      </c>
+      <c r="H491" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 부드러운 약산성 포뮬러로 매일 상쾌한 샤워 시간을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I491" t="inlineStr">
+        <is>
+          <t>약산성, 샤워젤, 민감피부, 부드러운, 상쾌한, 피부관리, 매일사용, 보습</t>
+        </is>
+      </c>
+      <c r="J491" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>491</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>출퇴근 후 상쾌함을 지켜주는 부케가르니 바디워시</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://naver.me/FNIXYLpS</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250114_27/17368354267242gQMW_JPEG/19126041632763729_1035396254.jpg</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>상쾌함 유지 바디워시</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>출퇴근 후에도 상쾌함이 오래가길 원하나요? 부케가르니 바디워시가 산뜻한 하루를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>부케가르니 바디워시 추천 출퇴근 후 상쾌함 유지</t>
+        </is>
+      </c>
+      <c r="H492" t="inlineStr">
+        <is>
+          <t>부케가르니 바디워시는 출퇴근 후에도 산뜻하고 깨끗한 피부를 유지해주는 바디워시입니다. 하루 종일 상쾌함을 원하는 분께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I492" t="inlineStr">
+        <is>
+          <t>부케가르니,바디워시,상쾌함,출퇴근,피부관리,산뜻함,하루상쾌</t>
+        </is>
+      </c>
+      <c r="J492" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>492</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>운동 후 땀 냄새 잡는 올인원 바디워시 사용기</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://naver.me/5mh0TyHh</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250317_194/1742201637569NzcxT_JPEG/3471211378440063_1517548718.jpg</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>운동 후 땀 냄새 제거 바디워시</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>땀 냄새 때문에 불편하셨나요? 이 올인원 바디워시로 상쾌하게 클리어하세요.</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>운동 후 땀 냄새 잡는 올인원 바디워시 추천</t>
+        </is>
+      </c>
+      <c r="H493" t="inlineStr">
+        <is>
+          <t>운동 후 불쾌한 땀 냄새를 효과적으로 제거하는 올인원 바디워시로 상쾌함을 유지하세요. 피부 자극 없이 깔끔한 클렌징에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I493" t="inlineStr">
+        <is>
+          <t>운동 후 바디워시, 땀 냄새 제거, 올인원 바디워시, 상쾌한 샤워, 피부 자극 적음</t>
+        </is>
+      </c>
+      <c r="J493" t="inlineStr">
+        <is>
+          <t>바디케어/샤워용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>493</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>라벤더머스크향 바디워시로 촉촉한 샤워시간을</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://naver.me/GiaBgk89</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250630_35/1751255449162r5CgQ_JPEG/8738468954039493_778787331.jpg</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>촉촉한 라벤더 바디워시</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>건조한 피부에 진정과 보습을 선사하는 라벤더머스크향 바디워시로 부드러운 샤워 시간을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t>라벤더머스크향 바디워시 촉촉한 피부 보습 추천</t>
+        </is>
+      </c>
+      <c r="H494" t="inlineStr">
+        <is>
+          <t>건조한 피부에 진정과 보습을 제공하는 라벤더머스크향 바디워시로 부드럽고 산뜻한 샤워 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I494" t="inlineStr">
+        <is>
+          <t>라벤더머스크,바디워시,보습,진정,촉촉한샤워,건성피부,피부진정,향기로운바디워시</t>
+        </is>
+      </c>
+      <c r="J494" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>494</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>아기 옷에도 안심하고 쓰는 중성세제 이야기</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://naver.me/F16xzvix</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250527_116/17483233509763DnSG_JPEG/82456172308998266_590843927.jpg</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>아기 옷 안심 중성세제</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>민감한 아기 피부에도 안전한 중성세제로 부드럽고 깨끗하게 세탁하세요.</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>아기 옷 중성세제 추천 안전하게 세탁하기</t>
+        </is>
+      </c>
+      <c r="H495" t="inlineStr">
+        <is>
+          <t>민감한 아기 피부도 걱정 없는 중성세제로 부드럽고 깨끗한 세탁을 경험하세요. 아기 옷 전용 세제로 안전 케어를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>중성세제,아기옷세탁,민감피부,안전세제,부드러운세탁</t>
+        </is>
+      </c>
+      <c r="J495" t="inlineStr">
+        <is>
+          <t>아기용품/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>495</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>민감한 피부를 위한 아크네 티트리 바디 워시 사용후기</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://naver.me/xWznOaqs</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230302_115/1677735880274Kim8h_JPEG/78871715102894722_370226551.jpg</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>민감 피부 진정 바디워시</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>예민한 피부, 자극 없이 깨끗하게 관리하고 싶다면 아크네 티트리 바디워시가 답입니다.</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>민감한 피부 아크네 티트리 바디 워시 추천 사용후기</t>
+        </is>
+      </c>
+      <c r="H496" t="inlineStr">
+        <is>
+          <t>예민한 피부도 자극 없이 깨끗하게 관리 가능한 아크네 티트리 바디 워시로 피부 트러블 완화에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>아크네 바디워시, 티트리, 민감한 피부, 트러블케어, 저자극, 바디 클렌저, 피부 진정</t>
+        </is>
+      </c>
+      <c r="J496" t="inlineStr">
+        <is>
+          <t>바디케어/민감성</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>496</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>등드름 고민 완화에 도움되는 고보습 바디워시 사용기</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://naver.me/x6xyjv9O</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241211_20/1733895952435KHTL5_JPEG/68028718856390770_2031058973.jpg</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>등드름 완화 고보습 바디워시</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>등드름으로 고민하는 피부를 부드럽고 촉촉하게 케어해주는 고보습 바디워시입니다.</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>등드름 고민 완화 고보습 바디워시 추천 및 구매 가이드</t>
+        </is>
+      </c>
+      <c r="H497" t="inlineStr">
+        <is>
+          <t>등드름 피부를 부드럽고 촉촉하게 케어하는 고보습 바디워시로 민감한 피부에도 사용하기 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>등드름,바디워시,고보습,피부케어,촉촉한,민감피부,여드름완화</t>
+        </is>
+      </c>
+      <c r="J497" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n">
+        <v>497</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>헨켈 9중효소 세탁세제로 깨끗한 빨래 완성해요</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgBmS9rj</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230413_244/1681362590082qOrPp_JPEG/8665273956031618_490760756.jpg</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>9중효소 세탁세제</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>겹겹이 쌓인 얼룩도 깨끗하게, 헨켈 9중효소 세탁세제로 완벽한 빨래를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>헨켈 9중효소 세탁세제 깨끗한 빨래 추천</t>
+        </is>
+      </c>
+      <c r="H498" t="inlineStr">
+        <is>
+          <t>헨켈 9중효소 세탁세제로 겹겹이 쌓인 얼룩도 완벽하게 제거해 주는 깨끗한 세탁을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>헨켈,세탁세제,9중효소,얼룩제거,빨래,깨끗한세탁,효소세제</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr">
+        <is>
+          <t>생활/세제</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n">
+        <v>498</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 엑스퍼트로 깔끔한 세탁 경험</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fwji0hEe</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250414_253/1744591215038Y2zaq_JPEG/9315771180712750_1495509724.jpg</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>강력 얼룩 제거 세제</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>지긋지긋한 얼룩과 냄새 걱정 없이 깨끗한 세탁을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 엑스퍼트 세탁세제 추천 - 얼룩·냄새 제거 탁월</t>
+        </is>
+      </c>
+      <c r="H499" t="inlineStr">
+        <is>
+          <t>헨켈 퍼실 엑스퍼트로 지긋지긋한 얼룩과 냄새 없이 깨끗한 세탁을 간편하게 경험하세요. 강력한 세정력으로 세탁 효율을 높입니다.</t>
+        </is>
+      </c>
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>헨켈,퍼실,세탁세제,얼룩제거,냄새제거,깨끗한세탁,세탁용품</t>
+        </is>
+      </c>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>세탁/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n">
+        <v>499</v>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>로즈워터 미스트로 하루 종일 촉촉한 피부 유지하기</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://naver.me/FxCtVNVe</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251129_172/17643502715496D3qK_PNG/98483211679437613_33548241.png</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>하루종일 촉촉한 로즈미스트</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>건조한 피부에 즉각 수분을 채워 하루 종일 촉촉함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>로즈워터 미스트로 하루 종일 촉촉한 피부 유지 추천</t>
+        </is>
+      </c>
+      <c r="H500" t="inlineStr">
+        <is>
+          <t>건조한 피부에 즉각 수분을 공급하여 하루 종일 촉촉함을 유지하는 로즈워터 미스트입니다. 민감한 피부에도 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I500" t="inlineStr">
+        <is>
+          <t>로즈워터,미스트,수분미스트,촉촉한피부,수분공급,피부보습,건조피부,스킨케어</t>
+        </is>
+      </c>
+      <c r="J500" t="inlineStr">
+        <is>
+          <t>스킨케어/피부관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n">
+        <v>500</v>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>에필로우 어성초 토너로 저자극 수분 케어하기</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Kq3r0eR</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251020_207/1760941088808tX2O6_JPEG/15904103087635725_398640114.jpg</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>저자극 수분 토너</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심, 에필로우 어성초 토너로 촉촉한 수분 케어를 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>에필로우 어성초 토너 저자극 수분 케어 추천</t>
+        </is>
+      </c>
+      <c r="H501" t="inlineStr">
+        <is>
+          <t>민감한 피부에도 안심할 수 있는 에필로우 어성초 토너로 촉촉한 수분 케어를 경험해보세요. 부드러운 저자극 포뮬러로 매일 사용 가능.</t>
+        </is>
+      </c>
+      <c r="I501" t="inlineStr">
+        <is>
+          <t>에필로우,어성초 토너,저자극 토너,수분 케어,민감 피부,스킨케어,수분 토너,피부 진정</t>
+        </is>
+      </c>
+      <c r="J501" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n">
+        <v>501</v>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>건성피부에 깊은 보습을 선사하는 히알루론산 세럼</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEihR3R7</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250904_79/1756996294415tjAs1_PNG/91129231525037280_76164624.png</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>깊은 보습 히알루론산 세럼</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>건조한 피부에 촉촉함을 더해주는 히알루론산 세럼으로 한층 부드럽고 건강한 피부를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>건성피부용 히알루론산 세럼 깊은 보습 추천</t>
+        </is>
+      </c>
+      <c r="H502" t="inlineStr">
+        <is>
+          <t>건조한 피부에 풍부한 촉촉함을 선사하는 히알루론산 세럼으로 부드럽고 건강한 피부 관리를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>히알루론산,건성피부,보습세럼,피부보습,촉촉한피부,스킨케어,피부영양</t>
+        </is>
+      </c>
+      <c r="J502" t="inlineStr">
+        <is>
+          <t>뷰티/스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n">
+        <v>502</v>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>산양유 함유 밀크토너로 촉촉한 피부 유지하기</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://naver.me/FDGCZOBE</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250521_59/1747810921573guQwH_JPEG/81943840727095270_476550322.jpg</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>산양유 촉촉 밀크토너</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>건조한 피부 고민을 산양유 밀크토너로 촉촉하게 케어해보세요. 부드러운 보습으로 하루 종일 건강한 피부를 유지할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>산양유 함유 밀크토너로 촉촉한 피부 유지 추천</t>
+        </is>
+      </c>
+      <c r="H503" t="inlineStr">
+        <is>
+          <t>산양유 밀크토너로 건조한 피부를 부드럽게 보습해 하루 종일 건강하고 촉촉한 피부를 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>산양유,밀크토너,촉촉한피부,보습,건성피부,스킨케어,피부케어,수분공급</t>
+        </is>
+      </c>
+      <c r="J503" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="n">
+        <v>503</v>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>속건조 걱정 없이 촉촉한 히알루론산 세럼 사용법</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://naver.me/52c5OubX</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250905_275/1757054601879j2PnF_PNG/91187435326822884_77300759.png</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>속건조 완화 히알루론산 세럼</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>속부터 촉촉한 보습을 원한다면 이 세럼으로 건조함 걱정을 씻어내세요.</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>촉촉한 히알루론산 세럼 사용법 추천, 속건조 걱정 없이</t>
+        </is>
+      </c>
+      <c r="H504" t="inlineStr">
+        <is>
+          <t>속부터 깊은 보습을 원하는 분께 적합한 히알루론산 세럼입니다. 건조함 없이 촉촉한 피부 관리에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I504" t="inlineStr">
+        <is>
+          <t>히알루론산,보습세럼,속건조,수분공급,피부관리,촉촉한피부,세럼사용법</t>
+        </is>
+      </c>
+      <c r="J504" t="inlineStr">
+        <is>
+          <t>스킨케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="n">
+        <v>504</v>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>유세린 더머토클린 토너로 피부 진정 효과 경험하기</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://naver.me/xpBA0eq6</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241011_151/17286041304319l9aV_JPEG/62736987548599813_1511811946.jpg</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>피부 진정 토너</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>민감한 피부도 편안하게, 유세린 더머토클린 토너로 피부 진정을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>유세린 더머토클린 토너 피부 진정 추천</t>
+        </is>
+      </c>
+      <c r="H505" t="inlineStr">
+        <is>
+          <t>민감한 피부도 편안하게 진정시키는 유세린 더머토클린 토너로 건강한 피부 관리에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>유세린,더머토클린,토너,피부진정,민감피부,스킨케어,저자극,피부관리</t>
+        </is>
+      </c>
+      <c r="J505" t="inlineStr">
+        <is>
+          <t>스킨케어/토너</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="n">
+        <v>505</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>실내건조 세탁에 적합한 살림백서 세제 후기</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://naver.me/xafRhr08</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220619_254/1655647765684HEnFk_JPEG/56783593278113932_371089839.jpg</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>실내건조용 세탁세제</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>실내에서 빨래가 잘 마르지 않아 고민이시죠? 이 세제 하나면 깔끔하고 상쾌한 세탁을 경험할 수 있어요.</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>실내건조 세탁에 좋은 살림백서 세제 추천</t>
+        </is>
+      </c>
+      <c r="H506" t="inlineStr">
+        <is>
+          <t>실내건조 세탁에 적합한 살림백서 세제로 깔끔하고 상쾌한 세탁을 경험하세요. 빠른 건조와 우수한 세척력을 자랑합니다.</t>
+        </is>
+      </c>
+      <c r="I506" t="inlineStr">
+        <is>
+          <t>실내건조, 살림백서, 세탁세제, 상쾌한세탁, 세척력, 빨래건조, 생활용품</t>
+        </is>
+      </c>
+      <c r="J506" t="inlineStr">
+        <is>
+          <t>생활/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="n">
+        <v>506</v>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>천연 유래 성분으로 안심하고 쓰는 액체 세탁세제</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://naver.me/xktn4CDP</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231122_156/1700650320386Nx6lN_JPEG/12332399589473356_226591414.jpg</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>자연성분 안심 세탁세제</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>민감한 피부도 걱정 없이 사용 가능한 천연 유래 성분 세탁세제로 깨끗한 세탁을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>천연 유래 성분 액체 세탁세제 추천 - 민감 피부 안심 세탁</t>
+        </is>
+      </c>
+      <c r="H507" t="inlineStr">
+        <is>
+          <t>민감한 피부도 안심하고 사용할 수 있는 천연 유래 성분의 액체 세탁세제로 깨끗한 세탁 효과를 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="I507" t="inlineStr">
+        <is>
+          <t>천연세탁세제, 액체세탁세제, 민감피부, 친환경세제, 무향세제, 피부안심, 세탁용품</t>
+        </is>
+      </c>
+      <c r="J507" t="inlineStr">
+        <is>
+          <t>생활/세제</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="n">
+        <v>507</v>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>딥클린파워 액체 세제로 깨끗한 세탁 경험하기</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://naver.me/5DDtO9wF</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240903_105/172534822884243pjc_JPEG/39665500662925325_314883325.jpg</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>강력 액체 세탁 세제</t>
+        </is>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>옷감 속 깊이 침투해 얼룩과 냄새를 말끔히 제거해 드려요. 깨끗한 세탁으로 하루를 상쾌하게 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>딥클린파워 액체 세제 추천 깨끗한 세탁 솔루션</t>
+        </is>
+      </c>
+      <c r="H508" t="inlineStr">
+        <is>
+          <t>옷감 깊은 곳까지 침투하는 딥클린파워 액체 세제로 얼룩과 냄새를 효과적으로 제거해 상쾌한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I508" t="inlineStr">
+        <is>
+          <t>딥클린파워, 액체세제, 세탁세제, 얼룩제거, 냄새제거, 깨끗한세탁, 세탁용품</t>
+        </is>
+      </c>
+      <c r="J508" t="inlineStr">
+        <is>
+          <t>생활/세탁</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="n">
+        <v>508</v>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>나드 바디워시로 집에서도 향기로운 힐링 타임</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://naver.me/G8h90VxT</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250314_82/1741923264981ME9Nn_JPEG/21596665333435375_258880686.jpg</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>집에서 즐기는 향기 바디워시</t>
+        </is>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>피로한 일상 속에서도 향기로운 힐링을 경험하세요. 촉촉하고 부드러운 피부 케어를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>나드 바디워시 추천 힐링과 촉촉한 피부 케어</t>
+        </is>
+      </c>
+      <c r="H509" t="inlineStr">
+        <is>
+          <t>나드 바디워시로 집에서도 편안한 힐링 타임을 즐기고 촉촉한 피부를 관리하세요. 피로 회복에 도움을 주는 부드러운 세정제입니다.</t>
+        </is>
+      </c>
+      <c r="I509" t="inlineStr">
+        <is>
+          <t>나드,바디워시,향기로운,피부케어,촉촉한,힐링,피로회복,부드러운세정제</t>
+        </is>
+      </c>
+      <c r="J509" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="n">
+        <v>509</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>등드름 완화를 위한 약산성 바디워시 선택기</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://naver.me/xdjFobhq</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240715_282/1721007653634nQInG_JPEG/68596105981665843_835104506.jpg</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>약산성 바디워시로 등드름 케어</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>등드름 고민, 자극 없는 약산성 바디워시로 깨끗하게 관리하세요. 민감한 피부에도 안심입니다.</t>
+        </is>
+      </c>
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>등드름 완화 약산성 바디워시 추천, 민감피부 관리용</t>
+        </is>
+      </c>
+      <c r="H510" t="inlineStr">
+        <is>
+          <t>등드름 고민에 자극 없는 약산성 바디워시로 깨끗하고 건강한 피부 관리가 가능합니다. 민감한 피부도 안심하고 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>등드름, 약산성 바디워시, 민감피부, 피부관리, 여드름완화, 바디클렌저, 피부진정</t>
+        </is>
+      </c>
+      <c r="J510" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="n">
+        <v>510</v>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>나드 퍼퓸드 바디워시로 상쾌한 출퇴근 시작하기</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://naver.me/F6nTACux</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250410_297/1744257526598i4JXJ_JPEG/90283369299203542_1802911345.jpg</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>상쾌한 아침 바디워시</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>출퇴근길 상쾌함으로 하루를 시작하세요. 피로를 씻어내고 기분 좋은 향기로 활력을 불어넣습니다.</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>나드 퍼퓸드 바디워시 추천으로 상쾌한 출퇴근 시작하기</t>
+        </is>
+      </c>
+      <c r="H511" t="inlineStr">
+        <is>
+          <t>나드 퍼퓸드 바디워시로 출퇴근길 상쾌함을 경험하세요. 피로 회복과 기분 좋은 향기로 활력을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>나드,퍼퓸드 바디워시,바디워시,상쾌한 바디워시,출퇴근 바디워시,활력,피로 회복</t>
+        </is>
+      </c>
+      <c r="J511" t="inlineStr">
+        <is>
+          <t>바디케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="n">
+        <v>511</v>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>피부 진정에 좋은 티트리 바디워시 경험기</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://naver.me/xPUmxGzR</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250206_105/1738818262683pPBuv_JPEG/19343053506527629_1733378206.jpg</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>피부 진정 티트리 바디워시</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>피부가 자주 가렵고 예민하다면 티트리 바디워시로 편안한 진정을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>피부 진정용 티트리 바디워시 추천, 민감 피부에 효과적</t>
+        </is>
+      </c>
+      <c r="H512" t="inlineStr">
+        <is>
+          <t>예민하고 가려운 피부를 위한 티트리 바디워시로 부드럽고 편안한 진정을 경험하세요. 피부 보호에 적합한 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I512" t="inlineStr">
+        <is>
+          <t>티트리 바디워시,피부 진정,민감 피부,가려움 완화,천연 성분,스킨케어,바디클렌저</t>
+        </is>
+      </c>
+      <c r="J512" t="inlineStr">
+        <is>
+          <t>스킨케어/바디워시</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2025-12-29 02:50)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J512"/>
+  <dimension ref="A1:J582"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26035,6 +26035,3506 @@
         </is>
       </c>
     </row>
+    <row r="513">
+      <c r="A513" t="n">
+        <v>512</v>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>출퇴근길 필수, 플레이보이 쿨 드로우즈 세트 리뷰</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://naver.me/GFC1r8CJ</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230726_57/1690338469301WyByC_JPEG/2859286086072784_1831005046.jpg</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>쿨링 드로즈 세트</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>출퇴근길 땀 고민 끝! 시원하고 쾌적한 플레이보이 드로즈로 하루 종일 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>출퇴근길 필수 플레이보이 쿨 드로우즈 세트 추천</t>
+        </is>
+      </c>
+      <c r="H513" t="inlineStr">
+        <is>
+          <t>출퇴근길 땀 걱정 없이 시원하고 쾌적한 플레이보이 쿨 드로우즈 세트로 하루 종일 편안함을 경험해 보세요.</t>
+        </is>
+      </c>
+      <c r="I513" t="inlineStr">
+        <is>
+          <t>플레이보이,쿨드로우즈,출퇴근필수,남성속옷,시원한속옷</t>
+        </is>
+      </c>
+      <c r="J513" t="inlineStr">
+        <is>
+          <t>속옷/남성</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="n">
+        <v>513</v>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 부담 없는 심리스 디자인 팬티 추천</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://naver.me/5FESv4hY</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250425_238/1745571641311llU44_JPEG/79704418833426552_888476132.jpg</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>심리스 부담 없는 팬티</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>출퇴근 시에도 편안함을 선사하는 심리스 팬티로 하루 종일 깔끔한 착용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>출퇴근 길 편안한 심리스 디자인 팬티 추천</t>
+        </is>
+      </c>
+      <c r="H514" t="inlineStr">
+        <is>
+          <t>하루 종일 깔끔하고 편안한 착용감을 제공하는 심리스 팬티로 출퇴근 시 부담 없이 착용하세요.</t>
+        </is>
+      </c>
+      <c r="I514" t="inlineStr">
+        <is>
+          <t>심리스 팬티, 출퇴근 팬티, 편안한 팬티, 일상 팬티, 깔끔한 팬티</t>
+        </is>
+      </c>
+      <c r="J514" t="inlineStr">
+        <is>
+          <t>패션,속옷</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="n">
+        <v>514</v>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>베이직하우스 2팩 긴팔 티셔츠, 휴대와 관리가 편리해요</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://naver.me/G8h9HL7K</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241014_26/1728877112411pwhGV_JPEG/63009917524409383_1712541107.jpg</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>편안한 2팩 긴팔 티셔츠</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>간편한 휴대와 손쉬운 관리로 언제 어디서나 편안하게 입을 수 있어요.</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>베이직하우스 2팩 긴팔 티셔츠 편리한 휴대와 관리 추천</t>
+        </is>
+      </c>
+      <c r="H515" t="inlineStr">
+        <is>
+          <t>간편한 휴대와 손쉬운 관리가 가능한 베이직하우스 2팩 긴팔 티셔츠로 편안한 착용감을 경험해 보세요.</t>
+        </is>
+      </c>
+      <c r="I515" t="inlineStr">
+        <is>
+          <t>베이직하우스,긴팔티셔츠,2팩티셔츠,간편휴대,손쉬운관리,편안한착용,기본티셔츠</t>
+        </is>
+      </c>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>패션/상의</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="n">
+        <v>515</v>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 좋은 기모 처리된 빅사이즈 츄리닝</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://naver.me/FRuNAgud</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241027_230/1729961748126fNYMy_JPEG/64094684730065177_1101283505.jpg</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>따뜻한 빅사이즈 츄리닝</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길에도 따뜻함을 유지하는 기모 처리 빅사이즈 츄리닝으로 편안함을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>기모 빅사이즈 츄리닝 추천 출퇴근길 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H516" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길에도 따뜻하게 입을 수 있는 기모 처리된 빅사이즈 츄리닝으로 편안함과 보온성을 동시에 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I516" t="inlineStr">
+        <is>
+          <t>빅사이즈 츄리닝,기모 츄리닝,출퇴근 옷,편안한 츄리닝,겨울 츄리닝,남녀공용 츄리닝</t>
+        </is>
+      </c>
+      <c r="J516" t="inlineStr">
+        <is>
+          <t>패션/상의</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="n">
+        <v>516</v>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>아노락과 조거팬츠 세트로 가볍게 운동할 때 입기 좋아요</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://naver.me/GMPg2smz</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251122_176/1763762411613SnlfW_JPEG/18443146539256066_1910660863.jpeg</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>가벼운 운동 아노락 세트</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>편안한 착용감으로 가벼운 운동에 딱! 스타일과 활동성을 동시에 챙겨보세요.</t>
+        </is>
+      </c>
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>아노락 조거팬츠 세트 운동복 추천 가벼운 착용감</t>
+        </is>
+      </c>
+      <c r="H517" t="inlineStr">
+        <is>
+          <t>편안한 착용감과 활동성을 겸비한 아노락과 조거팬츠 세트로 가벼운 운동에 최적화된 스타일을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I517" t="inlineStr">
+        <is>
+          <t>아노락,조거팬츠,운동복,세트상품,가벼운운동,편안한착용감,활동성</t>
+        </is>
+      </c>
+      <c r="J517" t="inlineStr">
+        <is>
+          <t>운동복,세트</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="n">
+        <v>517</v>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>운동할 때도 편안한 덤블 플리스 아노락 착용 후기</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://naver.me/5M5z2yVS</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251122_190/1763762279904OclxE_JPEG/110806343592085327_2112386859.jpeg</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>운동용 편안한 덤블 플리스</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>운동 중에도 따뜻하고 부드러운 착용감으로 편안함을 선사합니다. 활동성을 높여주는 아노락 스타일을 만나보세요.</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>운동할 때 편안한 덤블 플리스 아노락 추천</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>운동 시에도 따뜻하고 부드러운 덤블 플리스 아노락으로 편안함과 활동성을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="I518" t="inlineStr">
+        <is>
+          <t>덤블 플리스,아노락,운동복,편안한 착용감,활동성,따뜻한 옷,스포츠웨어</t>
+        </is>
+      </c>
+      <c r="J518" t="inlineStr">
+        <is>
+          <t>스포츠웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="n">
+        <v>518</v>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>출퇴근 길에도 편리한 세미 와이드 조거 팬츠 스타일</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://naver.me/GUmSN6tS</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250928_167/1759037232435yTigk_PNG/79662161464881750_1872096006.png</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>편안한 세미 와이드 조거 팬츠</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>출퇴근길 활동량 많은 당신에게 딱 맞는 편안함과 스타일을 동시에! 하루 종일 쾌적하게 입어요.</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>출퇴근 세미 와이드 조거 팬츠 편안한 착용 추천</t>
+        </is>
+      </c>
+      <c r="H519" t="inlineStr">
+        <is>
+          <t>출퇴근길 활동적인 분들을 위한 세미 와이드 조거 팬츠로 편안함과 세련된 스타일을 동시에 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>조거팬츠,세미와이드,출퇴근팬츠,편안한바지,활동적인옷</t>
+        </is>
+      </c>
+      <c r="J519" t="inlineStr">
+        <is>
+          <t>패션/팬츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="n">
+        <v>519</v>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>커플 선물로 좋은 랄프로렌 울 머플러 추천</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://naver.me/xcAawYgw</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251031_10/1761899861060WsY5Q_JPEG/80203167987569373_1354871713.jpg</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>포근한 울 머플러</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>추운 겨울, 사랑하는 사람과 따뜻함을 나누고 싶다면 부드러운 울 머플러로 특별한 커플 선물을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>커플 선물 추천 랄프로렌 울 머플러로 따뜻한 겨울 준비</t>
+        </is>
+      </c>
+      <c r="H520" t="inlineStr">
+        <is>
+          <t>부드러운 울 소재로 제작된 랄프로렌 머플러로 겨울철 사랑하는 이와 따뜻함을 나누세요. 커플 선물로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>랄프로렌, 울 머플러, 커플 선물, 겨울 머플러, 따뜻한 선물, 남녀 공용, 겨울 액세서리</t>
+        </is>
+      </c>
+      <c r="J520" t="inlineStr">
+        <is>
+          <t>패션/커플선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="n">
+        <v>520</v>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 없는 겨울목도리 선택 팁</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://naver.me/FoIN76XV</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240903_274/1725354712769VsalW_JPEG/53560851585874223_809957736.jpg</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>출퇴근 추위 방한 목도리</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>출퇴근길 차가운 바람으로부터 목을 보호하세요. 따뜻하고 편안한 겨울 목도리로 추위를 걱정 없이 보내세요.</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>출퇴근길 겨울목도리 선택 팁 추천, 추위 걱정 없는 보온 아이템</t>
+        </is>
+      </c>
+      <c r="H521" t="inlineStr">
+        <is>
+          <t>출퇴근길 차가운 바람으로부터 목을 보호하는 따뜻하고 편안한 겨울 목도리 선택법을 알려드립니다.</t>
+        </is>
+      </c>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>겨울목도리,출퇴근목도리,보온목도리,따뜻한목도리,목보호,추위예방,겨울패션</t>
+        </is>
+      </c>
+      <c r="J521" t="inlineStr">
+        <is>
+          <t>패션/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="n">
+        <v>521</v>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>운동할 때도 좋은 베이직 트레이닝 팬츠 착용 후기</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://naver.me/GNRklwvc</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251127_86/1764225548444DCC4O_JPEG/2341315771862281_585412848.jpg</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>편안한 베이직 트레이닝 팬츠</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>운동할 때 불편함 없이 편안함을 느껴보세요. 일상과 운동 모두에 딱 맞는 팬츠입니다.</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>운동할 때 편안한 베이직 트레이닝 팬츠 추천</t>
+        </is>
+      </c>
+      <c r="H522" t="inlineStr">
+        <is>
+          <t>운동과 일상 모두에 적합한 베이직 트레이닝 팬츠로 편안한 착용감을 경험하세요. 활동적인 라이프스타일에 알맞은 팬츠입니다.</t>
+        </is>
+      </c>
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>트레이닝팬츠,운동복,편안한팬츠,베이직팬츠,일상복,운동용팬츠,편안한착용감</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr">
+        <is>
+          <t>운동복/팬츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="n">
+        <v>522</v>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>휴대가 간편한 1+1 남자 반목티로 스타일 완성하기</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://naver.me/GdlmrHyV</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241231_258/1735592390321ByHmv_JPEG/10076057340085717_653951886.jpg</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>남자 반목티 1+1 세트</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>간편하게 스타일을 완성하는 반목티, 두 개 세트로 더욱 경제적입니다. 깔끔한 디자인으로 매일 입기 좋아요.</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>휴대가 간편한 1+1 남자 반목티 세트 추천</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>간편하게 스타일을 완성할 수 있는 남자 반목티 1+1 세트로 깔끔하고 편안한 데일리룩을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I523" t="inlineStr">
+        <is>
+          <t>남자반목티, 1+1세트, 남성패션, 데일리룩, 간편스타일, 반목티, 깔끔한 디자인, 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>남성패션/상의</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="n">
+        <v>523</v>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>커플 아이템으로 좋은 겨울 기모 머플러 활용법</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://naver.me/GJ5ih8Zf</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221107_160/16677895563483xbFK_PNG/28750475259358926_2027323707.jpg</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 기모 머플러</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>찬 바람에 얼어붙은 목을 부드럽게 감싸주는 기모 머플러로 겨울 데이트를 더 특별하게 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>커플 아이템 겨울 기모 머플러 추천, 따뜻한 데이트 필수품</t>
+        </is>
+      </c>
+      <c r="H524" t="inlineStr">
+        <is>
+          <t>겨울 찬바람을 부드럽게 감싸주는 기모 머플러로 커플 데이트에 따뜻함과 스타일을 더해보세요.</t>
+        </is>
+      </c>
+      <c r="I524" t="inlineStr">
+        <is>
+          <t>커플 아이템,겨울 머플러,기모 머플러,따뜻한 데이트,겨울 액세서리,목 보호</t>
+        </is>
+      </c>
+      <c r="J524" t="inlineStr">
+        <is>
+          <t>패션/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="n">
+        <v>524</v>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>출퇴근길 필수 아이템, 커플 수술 머플러 활용법</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEih9NdS</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241121_4/1732179443539ggb16_GIF/53855139713302472_531518611.gif</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>따뜻한 커플 수술 머플러</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>출퇴근길 찬 바람에 고민이라면, 포근한 커플 수술 머플러로 따뜻함을 더하세요.</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>출퇴근 필수 커플 수술 머플러 추천 - 따뜻한 겨울 외출</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>찬 바람 걱정 없이 출퇴근길에 따뜻함을 선사하는 커플 수술 머플러, 포근한 착용감과 스타일을 동시에 잡았습니다.</t>
+        </is>
+      </c>
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>커플 머플러, 출퇴근용 머플러, 겨울 머플러, 수술 머플러, 따뜻한 머플러</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr">
+        <is>
+          <t>패션/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="n">
+        <v>525</v>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>포근한 기모 소재 조거팬츠로 일상 휴대와 활동성 높이기</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://naver.me/5XpIfzpl</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230601_222/16856140799842e7MD_JPEG/5133300660789642_368376206.jpg</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>포근한 기모 조거팬츠</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>차가운 날씨에 따뜻함과 편안함을 동시에! 일상 활동에 딱 맞는 기모 조거팬츠로 스타일과 실용성을 모두 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>포근한 기모 조거팬츠 추천, 따뜻하고 편안한 일상복</t>
+        </is>
+      </c>
+      <c r="H526" t="inlineStr">
+        <is>
+          <t>차가운 날씨에도 따뜻하고 활동성이 좋은 기모 조거팬츠로 일상에서 편안한 착용감을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>기모조거팬츠,기모팬츠,조거팬츠,따뜻한바지,편안한팬츠,겨울바지,활동복,일상복</t>
+        </is>
+      </c>
+      <c r="J526" t="inlineStr">
+        <is>
+          <t>패션/팬츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="n">
+        <v>526</v>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>출퇴근길 스타일 완성하는 남자폴라티 활용 팁</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://naver.me/x1mvL1mP</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251028_27/1761647649589pMfQV_PNG/4859078514905144_1707670059.png</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>출퇴근 남자폴라티 코디법</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>출퇴근룩 고민 끝! 편안하면서도 세련된 남자폴라티 스타일링 팁으로 매일 신경 쓰지 않아도 멋진 하루를 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>출퇴근길 스타일 완성 남자폴라티 추천 및 활용 팁</t>
+        </is>
+      </c>
+      <c r="H527" t="inlineStr">
+        <is>
+          <t>편안하고 세련된 남자폴라티로 출퇴근룩을 완성하는 스타일링 팁을 소개합니다. 매일 간편하게 멋진 하루를 준비하세요.</t>
+        </is>
+      </c>
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>남자폴라티,출퇴근룩,남자패션,폴라티코디,스타일팁,편안한의류,데일리룩</t>
+        </is>
+      </c>
+      <c r="J527" t="inlineStr">
+        <is>
+          <t>패션/남성</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="n">
+        <v>527</v>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>실크핏 잠옷 입고 집에서 느끼는 최상의 휴식 시간</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://naver.me/G3P63iXh</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251127_113/1764226625365ekuoz_JPEG/68625903213883871_893332471.jpg</t>
+        </is>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>실크 부드러운 잠옷</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>하루의 피로를 감싸주는 부드러운 실크 잠옷으로 집에서 최고의 휴식을 누려보세요.</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>실크핏 잠옷 추천, 부드러운 휴식용 실크 잠옷 구매</t>
+        </is>
+      </c>
+      <c r="H528" t="inlineStr">
+        <is>
+          <t>부드러운 실크 소재로 제작된 실크핏 잠옷으로 집에서 편안하고 고급스러운 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I528" t="inlineStr">
+        <is>
+          <t>실크잠옷,부드러운잠옷,휴식잠옷,실크핏,편안한잠옷,홈웨어,실크잠옷추천</t>
+        </is>
+      </c>
+      <c r="J528" t="inlineStr">
+        <is>
+          <t>잠옷/홈웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="n">
+        <v>528</v>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>출퇴근길에 세련됨을 더하는 맞춤 자동차키링 경험</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://naver.me/5EnZyeRo</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210625_47/1624607124940WdWY1_JPEG/25743020368553851_1773214130.jpg</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>맞춤 자동차키링 세련된 디자인</t>
+        </is>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>출퇴근길 지루한 순간, 세련된 맞춤 키링으로 특별함을 더하세요. 당신의 개성을 완성합니다.</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>맞춤 자동차키링 추천 출퇴근길 세련된 키링 구매</t>
+        </is>
+      </c>
+      <c r="H529" t="inlineStr">
+        <is>
+          <t>출퇴근길에 개성 있는 맞춤 자동차키링으로 세련된 스타일을 완성하세요. 일상의 소소한 특별함을 더해줍니다.</t>
+        </is>
+      </c>
+      <c r="I529" t="inlineStr">
+        <is>
+          <t>맞춤 키링,자동차 키링,출퇴근길 액세서리,세련된 키링,개성 키링</t>
+        </is>
+      </c>
+      <c r="J529" t="inlineStr">
+        <is>
+          <t>액세서리/자동차</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="n">
+        <v>529</v>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>튼튼한 장우산과 나무손잡이로 운동 후에도 편안한 휴대감</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fr0pOsZz</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230526_99/168503295296750ihO_PNG/9699761746796461_1506484008.png</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>튼튼한 장우산 편안한 휴대</t>
+        </is>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>운동 후에도 가볍고 편안하게 쓸 수 있는 튼튼한 장우산, 나무손잡이로 품격까지 챙겼어요.</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>튼튼한 장우산 나무손잡이 운동 후 휴대 편리 추천</t>
+        </is>
+      </c>
+      <c r="H530" t="inlineStr">
+        <is>
+          <t>운동 후에도 편안하게 사용할 수 있는 튼튼한 장우산입니다. 나무손잡이로 고급스러운 품격을 더해 휴대하기 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I530" t="inlineStr">
+        <is>
+          <t>장우산,튼튼한우산,나무손잡이,운동후우산,휴대용우산,고급우산,편안한우산</t>
+        </is>
+      </c>
+      <c r="J530" t="inlineStr">
+        <is>
+          <t>우산/생활</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="n">
+        <v>530</v>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편한 와이드핏 조거팬츠 추천해요</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://naver.me/ximuhKwv</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251114_147/1763105086495CvSLI_JPEG/17282849959703274_532436093.jpg</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>편안한 와이드 조거팬츠</t>
+        </is>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 편안함을 놓치지 마세요. 와이드핏으로 자유로운 움직임을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>편안한 와이드핏 조거팬츠 추천, 출퇴근 길에도 자유로운 착용감</t>
+        </is>
+      </c>
+      <c r="H531" t="inlineStr">
+        <is>
+          <t>와이드핏 조거팬츠로 출퇴근길에도 편안한 움직임을 경험하세요. 넉넉한 핏이 자유로운 활동성을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I531" t="inlineStr">
+        <is>
+          <t>조거팬츠,와이드핏,출퇴근용팬츠,편한바지,일상복,활동적인바지,직장인스타일</t>
+        </is>
+      </c>
+      <c r="J531" t="inlineStr">
+        <is>
+          <t>패션/팬츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="n">
+        <v>531</v>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>운동할 때도 편한 오버핏 무지맨투맨의 매력</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fbqnwbzj</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251203_61/1764740025325p5N9q_JPEG/17452908482558476_1869996506.jpg</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>운동용 오버핏 맨투맨</t>
+        </is>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>편안한 착용감으로 운동 중에도 자유롭게 움직여 보세요. 스타일과 실용성을 동시에 챙긴 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>운동용 오버핏 무지맨투맨 추천, 편안한 착용감과 스타일</t>
+        </is>
+      </c>
+      <c r="H532" t="inlineStr">
+        <is>
+          <t>편안한 착용감과 함께 운동 시 자유로운 움직임이 가능한 오버핏 무지맨투맨으로 스타일과 실용성을 겸비했습니다.</t>
+        </is>
+      </c>
+      <c r="I532" t="inlineStr">
+        <is>
+          <t>오버핏,무지맨투맨,운동복,편안한착용감,스포츠웨어,캐주얼</t>
+        </is>
+      </c>
+      <c r="J532" t="inlineStr">
+        <is>
+          <t>패션/운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="n">
+        <v>532</v>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>휴대성 좋은 남자골덴바지로 외출 준비 끝</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://naver.me/xlbDrGC7</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251203_50/1764739944327B4rJm_JPEG/2864454151287579_1313301688.jpg</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>편안한 남성 골덴 팬츠</t>
+        </is>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>휴대성 좋고 부드러운 골덴바지로 어디서나 편안한 착용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>휴대성 좋은 남자골덴바지 추천, 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H533" t="inlineStr">
+        <is>
+          <t>부드럽고 휴대성 좋은 남자 골덴바지로 외출 시 편안함을 더해주는 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I533" t="inlineStr">
+        <is>
+          <t>남자 골덴바지, 휴대성 바지, 편안한 바지, 외출용 바지, 부드러운 골덴바지</t>
+        </is>
+      </c>
+      <c r="J533" t="inlineStr">
+        <is>
+          <t>패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="n">
+        <v>533</v>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>비스트모드 기모 후드로 따뜻하게 휴대하며 통화하기</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gq94QP8q</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251031_235/1761879469000VRdHL_JPEG/96012357698609829_849709413.jpg</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>기모 후드로 따뜻한 통화</t>
+        </is>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻하게 입고 휴대폰 통화까지 편안하게 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>비스트모드 기모 후드 추천 따뜻한 착용과 휴대폰 통화용</t>
+        </is>
+      </c>
+      <c r="H534" t="inlineStr">
+        <is>
+          <t>비스트모드 기모 후드는 추운 날씨에도 따뜻한 착용감과 휴대폰 통화 편리함을 제공합니다. 일상 외출용으로 적합한 후드입니다.</t>
+        </is>
+      </c>
+      <c r="I534" t="inlineStr">
+        <is>
+          <t>비스트모드,기모후드,따뜻한후드,휴대폰통화,겨울옷,편안한후드</t>
+        </is>
+      </c>
+      <c r="J534" t="inlineStr">
+        <is>
+          <t>패션/겨울의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="n">
+        <v>534</v>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>출퇴근길 쁘띠 아이보리 목도리가 전하는 포근한 온기</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://naver.me/5cqusf8d</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251217_124/1765930556983BQmh8_JPEG/100063441039363008_1224587440.jpg</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>포근한 아이보리 목도리</t>
+        </is>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길, 따뜻한 목도리로 포근함을 챙기세요. 가벼운 착용감으로 하루 종일 편안합니다.</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>출퇴근길 쁘띠 아이보리 목도리 추천, 따뜻한 포근함 제공</t>
+        </is>
+      </c>
+      <c r="H535" t="inlineStr">
+        <is>
+          <t>가벼운 착용감으로 하루 종일 편안한 출퇴근길 쁘띠 아이보리 목도리로 따뜻함을 챙기세요.</t>
+        </is>
+      </c>
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>목도리,출퇴근,겨울목도리,아이보리목도리,따뜻한목도리,겨울패션,패션소품</t>
+        </is>
+      </c>
+      <c r="J535" t="inlineStr">
+        <is>
+          <t>패션/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="n">
+        <v>535</v>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>운동 중 체온 유지에 좋은 푸마 웜셀 상하의 세트 추천</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://naver.me/FNIX1A7K</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251218_126/17660318493351DjP4_JPEG/20129939367818004_1630708739.jpg</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr">
+        <is>
+          <t>운동 중 체온 유지 세트</t>
+        </is>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>운동할 때 체온 걱정되시죠? 푸마 웜셀 상하의로 따뜻하고 편안한 운동을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G536" t="inlineStr">
+        <is>
+          <t>푸마 웜셀 상하의 세트 운동 체온 유지 추천</t>
+        </is>
+      </c>
+      <c r="H536" t="inlineStr">
+        <is>
+          <t>운동 중 체온을 효과적으로 유지해주는 푸마 웜셀 상하의 세트로 따뜻하고 편안한 활동을 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I536" t="inlineStr">
+        <is>
+          <t>푸마, 웜셀, 운동복, 체온유지, 상하의세트, 스포츠웨어, 따뜻한운동복</t>
+        </is>
+      </c>
+      <c r="J536" t="inlineStr">
+        <is>
+          <t>운동복/스포츠웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="n">
+        <v>536</v>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>부드러운 감촉의 골덴바지로 편안한 휴대성 경험</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://naver.me/xDCuSpJr</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251102_165/17620701100322GVyU_PNG/96203073159518038_453992078.png</t>
+        </is>
+      </c>
+      <c r="E537" t="inlineStr">
+        <is>
+          <t>편안한 골덴 바지</t>
+        </is>
+      </c>
+      <c r="F537" t="inlineStr">
+        <is>
+          <t>부드러운 감촉의 골덴 원단으로 하루 종일 편안함을 느껴보세요. 휴대하기도 간편해 언제 어디서나 착용 가능해요.</t>
+        </is>
+      </c>
+      <c r="G537" t="inlineStr">
+        <is>
+          <t>부드러운 감촉 골덴바지 편안함과 휴대성 추천</t>
+        </is>
+      </c>
+      <c r="H537" t="inlineStr">
+        <is>
+          <t>부드러운 골덴 원단으로 하루 종일 편안한 착용감을 제공하며, 휴대가 간편해 언제 어디서나 편리하게 입을 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I537" t="inlineStr">
+        <is>
+          <t>골덴바지,부드러운원단,편안한바지,휴대용바지,데일리팬츠</t>
+        </is>
+      </c>
+      <c r="J537" t="inlineStr">
+        <is>
+          <t>패션/바지</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="n">
+        <v>537</v>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>활동성 좋은 와이드 데님, 운동할 때도 부담 없어요</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://naver.me/GFC1r8BN</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251017_269/1760688756081vT2i8_JPEG/33508810207914007_485001687.jpg</t>
+        </is>
+      </c>
+      <c r="E538" t="inlineStr">
+        <is>
+          <t>편안한 활동 와이드 데님</t>
+        </is>
+      </c>
+      <c r="F538" t="inlineStr">
+        <is>
+          <t>운동할 때도 편안하게 움직이고 싶은 당신을 위한 와이드 데님, 부담 없이 스타일 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G538" t="inlineStr">
+        <is>
+          <t>활동성 좋은 와이드 데님 추천, 운동 시 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H538" t="inlineStr">
+        <is>
+          <t>운동할 때도 편안한 와이드 데님으로 자유로운 활동성과 스타일을 동시에 챙기세요. 부담 없이 일상 및 운동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I538" t="inlineStr">
+        <is>
+          <t>와이드 데님,운동용 청바지,활동성 좋은 바지,편안한 데님,캐주얼 팬츠</t>
+        </is>
+      </c>
+      <c r="J538" t="inlineStr">
+        <is>
+          <t>패션/데님</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="n">
+        <v>538</v>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 딱 맞는 오버핏 빅사이즈 후드집업 추천</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://naver.me/5DDtmRjJ</t>
+        </is>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240827_63/1724746061413GFIoF_JPEG/11511803900983745_203240835.jpg</t>
+        </is>
+      </c>
+      <c r="E539" t="inlineStr">
+        <is>
+          <t>오버핏 빅사이즈 후드집업</t>
+        </is>
+      </c>
+      <c r="F539" t="inlineStr">
+        <is>
+          <t>출퇴근 길 불편한 옷차림 고민 끝! 편안하고 스타일리시한 오버핏 후드집업으로 하루를 산뜻하게 시작하세요.</t>
+        </is>
+      </c>
+      <c r="G539" t="inlineStr">
+        <is>
+          <t>오버핏 빅사이즈 후드집업 추천 출퇴근 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H539" t="inlineStr">
+        <is>
+          <t>출퇴근 길에 편안함과 스타일을 동시에! 빅사이즈 오버핏 후드집업으로 쾌적한 하루를 시작하세요.</t>
+        </is>
+      </c>
+      <c r="I539" t="inlineStr">
+        <is>
+          <t>오버핏,빅사이즈,후드집업,출퇴근,편안한,스타일리시,남녀공용,캐주얼</t>
+        </is>
+      </c>
+      <c r="J539" t="inlineStr">
+        <is>
+          <t>패션/아우터</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="n">
+        <v>539</v>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>통화할 때도 편안한 나이키 긴 바지의 매력</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://naver.me/I5yadX5Z</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250801_25/1754028149208AFzPL_JPEG/8488088024906455_1006621690.jpg</t>
+        </is>
+      </c>
+      <c r="E540" t="inlineStr">
+        <is>
+          <t>통화 중 편안한 긴 바지</t>
+        </is>
+      </c>
+      <c r="F540" t="inlineStr">
+        <is>
+          <t>장시간 착용해도 불편함 없는 부드러운 소재로, 통화 중에도 쾌적한 착용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G540" t="inlineStr">
+        <is>
+          <t>통화할 때도 편안한 나이키 긴 바지 추천</t>
+        </is>
+      </c>
+      <c r="H540" t="inlineStr">
+        <is>
+          <t>부드러운 소재로 장시간 착용해도 쾌적하며, 통화 중에도 편안한 나이키 긴 바지입니다.</t>
+        </is>
+      </c>
+      <c r="I540" t="inlineStr">
+        <is>
+          <t>나이키 긴 바지,편안한 바지,운동복,부드러운 소재,장시간 착용,통화용 바지</t>
+        </is>
+      </c>
+      <c r="J540" t="inlineStr">
+        <is>
+          <t>패션/스포츠웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="n">
+        <v>540</v>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻하게, 나이키 경량 패딩 조끼 착용 후기</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://naver.me/5BwjCdcu</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251223_264/176647312256610PfV_JPEG/42241424665063474_1760797052.jpg</t>
+        </is>
+      </c>
+      <c r="E541" t="inlineStr">
+        <is>
+          <t>경량 패딩 조끼로 따뜻함 유지</t>
+        </is>
+      </c>
+      <c r="F541" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 가볍고 따뜻하게 입고 싶다면 이 경량 패딩 조끼가 딱입니다. 편안한 착용감으로 일상 추위를 막아줍니다.</t>
+        </is>
+      </c>
+      <c r="G541" t="inlineStr">
+        <is>
+          <t>나이키 경량 패딩 조끼 추천, 추운 겨울 따뜻하게 착용하기</t>
+        </is>
+      </c>
+      <c r="H541" t="inlineStr">
+        <is>
+          <t>가볍고 따뜻한 나이키 경량 패딩 조끼는 추운 날씨에도 편안한 착용감을 제공하며 일상 추위를 효과적으로 막아줍니다.</t>
+        </is>
+      </c>
+      <c r="I541" t="inlineStr">
+        <is>
+          <t>나이키,경량패딩,패딩조끼,겨울패션,따뜻한옷,겨울외투,남녀공용,방한용품</t>
+        </is>
+      </c>
+      <c r="J541" t="inlineStr">
+        <is>
+          <t>패션/아우터</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="n">
+        <v>541</v>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>겨울 커플 아이템으로 자연스러운 스타일 완성</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://naver.me/GJ5ih8OE</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241127_264/1732668592518joqRp_PNG/78005473255052832_99514055.png</t>
+        </is>
+      </c>
+      <c r="E542" t="inlineStr">
+        <is>
+          <t>겨울 커플 스타일</t>
+        </is>
+      </c>
+      <c r="F542" t="inlineStr">
+        <is>
+          <t>추운 겨울, 자연스러운 커플 스타일로 따뜻함과 세련됨을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G542" t="inlineStr">
+        <is>
+          <t>겨울 커플 아이템으로 자연스러운 스타일 완성 추천</t>
+        </is>
+      </c>
+      <c r="H542" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 자연스러운 커플 스타일을 완성해주는 아이템으로 따뜻함과 세련됨을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="I542" t="inlineStr">
+        <is>
+          <t>겨울커플,커플아이템,겨울패션,자연스러운스타일,따뜻한커플룩,세련된겨울코디</t>
+        </is>
+      </c>
+      <c r="J542" t="inlineStr">
+        <is>
+          <t>패션/커플</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="n">
+        <v>542</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>운동 후에도 편안한 나이키 면 티셔츠 추천</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://naver.me/Goi7Pk2b</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251223_60/1766474057487Owegz_JPEG/76597338348471018_1602677092.jpg</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>운동 후 편안한 면 티셔츠</t>
+        </is>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>운동 후에도 피부에 부드럽고 편안한 면 티셔츠로 쾌적함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G543" t="inlineStr">
+        <is>
+          <t>운동 후에도 편안한 나이키 면 티셔츠 추천</t>
+        </is>
+      </c>
+      <c r="H543" t="inlineStr">
+        <is>
+          <t>운동 후에도 부드럽고 쾌적한 착용감을 제공하는 나이키 면 티셔츠로 편안함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I543" t="inlineStr">
+        <is>
+          <t>나이키,면티셔츠,운동복,편안한티셔츠,운동후티셔츠,스포츠웨어</t>
+        </is>
+      </c>
+      <c r="J543" t="inlineStr">
+        <is>
+          <t>운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="n">
+        <v>543</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>가볍고 따뜻한 남자 코듀로이 팬츠 휴대성 체크</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://naver.me/5yWnAHB7</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250207_249/1738918462131i6IrF_JPEG/21278455127709725_728531916.jpg</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>가볍고 따뜻한 남성 코듀로이 팬츠</t>
+        </is>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>춥고 무거운 겨울 팬츠가 불편하셨나요? 가볍고 따뜻한 코듀로이 팬츠로 편안함을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G544" t="inlineStr">
+        <is>
+          <t>가볍고 따뜻한 남자 코듀로이 팬츠 추천</t>
+        </is>
+      </c>
+      <c r="H544" t="inlineStr">
+        <is>
+          <t>겨울철 무거운 팬츠 대신 가볍고 따뜻한 코듀로이 팬츠로 편안함과 휴대성을 동시에 누려보세요.</t>
+        </is>
+      </c>
+      <c r="I544" t="inlineStr">
+        <is>
+          <t>남자코듀로이팬츠,겨울팬츠,가벼운팬츠,따뜻한팬츠,휴대성바지,편안한바지,남성팬츠</t>
+        </is>
+      </c>
+      <c r="J544" t="inlineStr">
+        <is>
+          <t>패션/남성의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="n">
+        <v>544</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>운동할 때 가볍고 쾌적한 초경량 쇼츠 추천해요</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://naver.me/5Qi7QhuX</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250722_180/17531535729608N8xE_JPEG/39970542798889521_1328972599.jpg</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>가벼운 초경량 운동 쇼츠</t>
+        </is>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>운동 중 무거움과 답답함 걱정 끝! 가벼워 자유로운 움직임을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G545" t="inlineStr">
+        <is>
+          <t>초경량 운동 쇼츠 가볍고 쾌적해 추천해요</t>
+        </is>
+      </c>
+      <c r="H545" t="inlineStr">
+        <is>
+          <t>운동 시 무거움 없이 자유로운 움직임을 지원하는 초경량 쇼츠로 쾌적한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I545" t="inlineStr">
+        <is>
+          <t>초경량 쇼츠,운동 쇼츠,가벼운 반바지,운동복,쿨링 쇼츠,남성 운동복,여성 운동복</t>
+        </is>
+      </c>
+      <c r="J545" t="inlineStr">
+        <is>
+          <t>운동복/쇼츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="n">
+        <v>545</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>빅사이즈 겨울바지로 출퇴근길도 쾌적하게</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://naver.me/xBMJI5w5</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251001_212/1759315844191pcXdI_JPEG/13868123728124705_1870989508.jpg</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>빅사이즈 겨울 출근 바지</t>
+        </is>
+      </c>
+      <c r="F546" t="inlineStr">
+        <is>
+          <t>추운 겨울 출퇴근길에도 따뜻하고 편안한 빅사이즈 바지로 쾌적함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G546" t="inlineStr">
+        <is>
+          <t>빅사이즈 겨울바지 추천 출퇴근길 따뜻하고 편안하게</t>
+        </is>
+      </c>
+      <c r="H546" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 쾌적하고 따뜻하게 입는 빅사이즈 겨울바지로 출퇴근길 편안함을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I546" t="inlineStr">
+        <is>
+          <t>빅사이즈,겨울바지,출퇴근바지,따뜻한바지,편안한바지,겨울패션,남성빅사이즈,여성빅사이즈</t>
+        </is>
+      </c>
+      <c r="J546" t="inlineStr">
+        <is>
+          <t>의류/겨울패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="n">
+        <v>546</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>모크넥 반목폴라로 편안한 휴대성과 스타일 완성</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://naver.me/xI1XiQel</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221028_132/1666948160481NMJvv_JPEG/68083988293599129_1256860273.jpg</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>편안한 모크넥 반목폴라</t>
+        </is>
+      </c>
+      <c r="F547" t="inlineStr">
+        <is>
+          <t>목을 부드럽게 감싸주는 모크넥으로 따뜻함과 스타일을 동시에 챙겨보세요.</t>
+        </is>
+      </c>
+      <c r="G547" t="inlineStr">
+        <is>
+          <t>모크넥 반목폴라 추천, 편안한 착용감과 따뜻함</t>
+        </is>
+      </c>
+      <c r="H547" t="inlineStr">
+        <is>
+          <t>목을 부드럽게 감싸주는 모크넥 반목폴라로 따뜻함과 스타일을 모두 갖춘 실용적인 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I547" t="inlineStr">
+        <is>
+          <t>모크넥,반목폴라,따뜻한폴라,편안한착용,가을패션,남녀공용,스타일폴라</t>
+        </is>
+      </c>
+      <c r="J547" t="inlineStr">
+        <is>
+          <t>패션/상의</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="n">
+        <v>547</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>트레이닝 팬츠로 통화 중에도 활동하기 좋아요</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://naver.me/I5yadXy6</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240509_22/1715249392000twvof_JPEG/42552075863124979_1286528457.jpg</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>활동 편안 트레이닝 팬츠</t>
+        </is>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>통화 중에도 자유로운 움직임을 원한다면, 편안한 착용감의 트레이닝 팬츠가 정답입니다.</t>
+        </is>
+      </c>
+      <c r="G548" t="inlineStr">
+        <is>
+          <t>트레이닝 팬츠 추천 통화 중 활동 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H548" t="inlineStr">
+        <is>
+          <t>통화 중에도 자유로운 움직임을 돕는 편안한 트레이닝 팬츠입니다. 활동성이 뛰어나 일상생활에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I548" t="inlineStr">
+        <is>
+          <t>트레이닝팬츠,편안한팬츠,활동적인바지,운동복,일상팬츠</t>
+        </is>
+      </c>
+      <c r="J548" t="inlineStr">
+        <is>
+          <t>패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="n">
+        <v>548</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>출퇴근길에 딱 좋은 나이키 후드티 스타일링</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://naver.me/xhlCa4lk</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250320_93/1742459981875N8KTX_JPEG/50837273687194780_58258140.jpg</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>편안한 출퇴근 후드티</t>
+        </is>
+      </c>
+      <c r="F549" t="inlineStr">
+        <is>
+          <t>출퇴근길 찬바람에도 따뜻하고 편안한 착용감을 원한다면, 이 후드티가 딱입니다.</t>
+        </is>
+      </c>
+      <c r="G549" t="inlineStr">
+        <is>
+          <t>출퇴근길 딱 좋은 나이키 후드티 추천 및 스타일링 팁</t>
+        </is>
+      </c>
+      <c r="H549" t="inlineStr">
+        <is>
+          <t>찬바람 부는 출퇴근길에도 편안하고 따뜻한 착용감을 제공하는 나이키 후드티입니다. 실용적이고 스타일리시한 데일리룩에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I549" t="inlineStr">
+        <is>
+          <t>나이키 후드티, 출퇴근 패션, 따뜻한 후드티, 편안한 옷차림, 데일리룩, 가을 후드티, 스타일링 팁</t>
+        </is>
+      </c>
+      <c r="J549" t="inlineStr">
+        <is>
+          <t>패션/아우터</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="n">
+        <v>549</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>출퇴근길 겨울 방한 패딩머플러로 포근함 유지하기</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://naver.me/GScAJh9y</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241222_41/1734843468910xAexC_JPEG/2928497033566451_860674312.jpg</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>겨울 방한 패딩머플러</t>
+        </is>
+      </c>
+      <c r="F550" t="inlineStr">
+        <is>
+          <t>출퇴근 시 차가운 바람을 막아주는 포근한 패딩머플러로 따뜻함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="G550" t="inlineStr">
+        <is>
+          <t>출퇴근용 겨울 방한 패딩머플러 추천, 따뜻함 유지</t>
+        </is>
+      </c>
+      <c r="H550" t="inlineStr">
+        <is>
+          <t>출퇴근길 차가운 바람을 효과적으로 막아주는 겨울용 패딩머플러로 따뜻하고 포근하게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I550" t="inlineStr">
+        <is>
+          <t>패딩머플러,겨울방한,출퇴근용,따뜻한머플러,겨울패션</t>
+        </is>
+      </c>
+      <c r="J550" t="inlineStr">
+        <is>
+          <t>패션/방한</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="n">
+        <v>550</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>세미와이드 핏이라 활동성 좋은 운동용 데님</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://naver.me/xAACEqV8</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251017_58/1760690406823K2t0q_JPEG/2503800583515077_1483002917.jpg</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>활동성 좋은 세미와이드 운동용 데님</t>
+        </is>
+      </c>
+      <c r="F551" t="inlineStr">
+        <is>
+          <t>운동할 때도 편안함이 필요하죠? 세미와이드 핏으로 움직임을 자유롭게 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G551" t="inlineStr">
+        <is>
+          <t>세미와이드 핏 운동용 데님 편안한 활동성 추천</t>
+        </is>
+      </c>
+      <c r="H551" t="inlineStr">
+        <is>
+          <t>운동 시 편안한 착용감을 제공하는 세미와이드 핏 데님으로 자유로운 움직임이 가능합니다. 활동적인 분들께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I551" t="inlineStr">
+        <is>
+          <t>세미와이드 핏,운동용 데님,활동성 좋은 바지,편안한 데님,캐주얼 바지</t>
+        </is>
+      </c>
+      <c r="J551" t="inlineStr">
+        <is>
+          <t>패션,운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="n">
+        <v>551</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>운동할 때 추천하는 헬스용 기모조거팬츠 후기</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://naver.me/FvQgbUEf</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240509_55/17152481239167IB2q_JPEG/116384012603204987_1078256589.jpg</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>운동용 기모 조거팬츠</t>
+        </is>
+      </c>
+      <c r="F552" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻하게 운동하고 싶으신가요? 이 기모 조거팬츠로 편안함과 보온을 동시에 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G552" t="inlineStr">
+        <is>
+          <t>운동용 기모조거팬츠 추천, 따뜻하고 편안한 겨울 운동복</t>
+        </is>
+      </c>
+      <c r="H552" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 따뜻하게 보온하며 편안한 착용감을 제공하는 기모 조거팬츠로 겨울 운동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I552" t="inlineStr">
+        <is>
+          <t>기모조거팬츠,운동복,겨울운동,헬스팬츠,보온조거팬츠,편안한운동복</t>
+        </is>
+      </c>
+      <c r="J552" t="inlineStr">
+        <is>
+          <t>운동복/팬츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="n">
+        <v>552</v>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>휴대하기 좋은 푸마 러너핏 드로즈, 어디서든 활용 가능</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://naver.me/FfBOQuef</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251218_281/17660318493866mDJM_JPEG/96371595371130549_1502229446.jpg</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>편안한 휴대용 러너핏 드로즈</t>
+        </is>
+      </c>
+      <c r="F553" t="inlineStr">
+        <is>
+          <t>언제 어디서나 편안함이 필요한 당신을 위한 가벼운 러너핏 드로즈로 일상 속 자신감을 채우세요.</t>
+        </is>
+      </c>
+      <c r="G553" t="inlineStr">
+        <is>
+          <t>휴대용 푸마 러너핏 드로즈 추천, 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H553" t="inlineStr">
+        <is>
+          <t>가볍고 편안한 푸마 러너핏 드로즈로 언제 어디서나 자신감을 높이세요. 활동적인 일상에 적합한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I553" t="inlineStr">
+        <is>
+          <t>푸마,러너핏,드로즈,편안한속옷,휴대용속옷,일상속옷,남성속옷</t>
+        </is>
+      </c>
+      <c r="J553" t="inlineStr">
+        <is>
+          <t>패션/언더웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="n">
+        <v>553</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>운동 후 휴식 시간에 딱 좋은 편한 기모 슬랙스</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://naver.me/GCgqQnvi</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231113_164/1699867060820oAMbQ_JPEG/12416727591751234_2094529882.jpg</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>편안한 기모 슬랙스</t>
+        </is>
+      </c>
+      <c r="F554" t="inlineStr">
+        <is>
+          <t>운동 후에도 편안함을 놓치고 싶지 않은 당신을 위한 따뜻한 기모 슬랙스입니다.</t>
+        </is>
+      </c>
+      <c r="G554" t="inlineStr">
+        <is>
+          <t>운동 후 휴식용 따뜻한 기모 슬랙스 추천</t>
+        </is>
+      </c>
+      <c r="H554" t="inlineStr">
+        <is>
+          <t>운동 후 편안한 휴식을 위해 제작된 따뜻한 기모 슬랙스입니다. 부드러운 소재로 포근한 착용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I554" t="inlineStr">
+        <is>
+          <t>기모슬랙스,운동후슬랙스,편안한바지,따뜻한바지,휴식용바지</t>
+        </is>
+      </c>
+      <c r="J554" t="inlineStr">
+        <is>
+          <t>패션/운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="n">
+        <v>554</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 스타일 살리는 나이키 패딩 파카</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://naver.me/FXkG92k9</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251217_94/1765935006051pV1sV_JPEG/43348088135133595_1609088381.jpg</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 패딩 파카</t>
+        </is>
+      </c>
+      <c r="F555" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 스타일과 보온성 모두 챙기고 싶은 당신을 위한 완벽한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G555" t="inlineStr">
+        <is>
+          <t>나이키 패딩 파카 겨울 스타일 추천 - 따뜻한 보온성</t>
+        </is>
+      </c>
+      <c r="H555" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 스타일과 보온성을 모두 갖춘 나이키 패딩 파카로 편안하고 세련된 겨울 패션을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I555" t="inlineStr">
+        <is>
+          <t>나이키,패딩,파카,겨울패션,보온성,스타일,겨울외투,남성패딩,여성패딩</t>
+        </is>
+      </c>
+      <c r="J555" t="inlineStr">
+        <is>
+          <t>패션/겨울</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="n">
+        <v>555</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>워싱 디테일로 멋스럽게 입는 데님팬츠 이야기</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://naver.me/5lfkEixf</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251108_178/1762597629860Qavkh_JPEG/9231431080407949_763830790.jpg</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>멋스러운 워싱 데님팬츠</t>
+        </is>
+      </c>
+      <c r="F556" t="inlineStr">
+        <is>
+          <t>평범한 데님은 싫다면, 워싱 디테일로 스타일을 살려보세요. 감각적인 핏으로 자신감이 올라갑니다.</t>
+        </is>
+      </c>
+      <c r="G556" t="inlineStr">
+        <is>
+          <t>워싱 디테일 데님팬츠 추천, 스타일과 핏 모두 만족</t>
+        </is>
+      </c>
+      <c r="H556" t="inlineStr">
+        <is>
+          <t>워싱 디테일로 멋스럽고 감각적인 데님팬츠입니다. 자신감 있는 스타일링을 원하는 분들께 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I556" t="inlineStr">
+        <is>
+          <t>데님팬츠,워싱데님,멋스러운팬츠,감각적인핏,남성데님,여성데님,캐주얼룩</t>
+        </is>
+      </c>
+      <c r="J556" t="inlineStr">
+        <is>
+          <t>패션/의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="n">
+        <v>556</v>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>남녀공용 면티로 편하게 운동할 때 입기 좋아요</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://naver.me/xydGL6lH</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20191216_122/1576500581260NByNW_JPEG/13862914818054153_367223989.jpg</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>편안한 남녀공용 면티</t>
+        </is>
+      </c>
+      <c r="F557" t="inlineStr">
+        <is>
+          <t>운동할 때 불편함 없는 부드러운 면 소재로 하루종일 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G557" t="inlineStr">
+        <is>
+          <t>남녀공용 면티 편안한 운동복 추천</t>
+        </is>
+      </c>
+      <c r="H557" t="inlineStr">
+        <is>
+          <t>부드러운 면 소재로 제작되어 운동 시 편안함을 제공하는 남녀공용 면티입니다. 활동적인 하루에도 부담 없이 착용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I557" t="inlineStr">
+        <is>
+          <t>남녀공용,면티,운동복,편안한티셔츠,부드러운소재,캐주얼웨어,데일리웨어</t>
+        </is>
+      </c>
+      <c r="J557" t="inlineStr">
+        <is>
+          <t>운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="n">
+        <v>557</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 부담 없는 운동복, 블랙몬스터핏 추천</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://naver.me/FkL3XG7T</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250206_75/1738818981800eEohA_JPEG/71259936055384_46327553.jpg</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>출퇴근 운동복 추천</t>
+        </is>
+      </c>
+      <c r="F558" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편안한 운동복으로 하루 종일 쾌적함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G558" t="inlineStr">
+        <is>
+          <t>출퇴근길 부담 없는 운동복 블랙몬스터핏 추천</t>
+        </is>
+      </c>
+      <c r="H558" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 편안한 블랙몬스터핏 운동복으로 하루 종일 쾌적하게 활동하세요. 실용적인 디자인과 편안한 착용감이 돋보입니다.</t>
+        </is>
+      </c>
+      <c r="I558" t="inlineStr">
+        <is>
+          <t>운동복,출퇴근운동복,블랙몬스터핏,편안한운동복,일상복,운동웨어</t>
+        </is>
+      </c>
+      <c r="J558" t="inlineStr">
+        <is>
+          <t>운동복/일상복</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="n">
+        <v>558</v>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>빅사이즈 남성용 와이드 슬랙스로 운동할 때도 편해요</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://naver.me/5h1aYsu4</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251028_294/1761644940173IIIT1_JPEG/2487418835474141_241270634.jpg</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>빅사이즈 남성 와이드 슬랙스</t>
+        </is>
+      </c>
+      <c r="F559" t="inlineStr">
+        <is>
+          <t>넉넉한 사이즈와 와이드 핏으로 편안함을 느껴보세요. 운동할 때도 자유롭게 움직일 수 있어 만족스러워요.</t>
+        </is>
+      </c>
+      <c r="G559" t="inlineStr">
+        <is>
+          <t>빅사이즈 남성용 와이드 슬랙스 추천 편안한 운동복</t>
+        </is>
+      </c>
+      <c r="H559" t="inlineStr">
+        <is>
+          <t>넉넉한 빅사이즈와 와이드 핏으로 남성에게 편안함을 제공하며 운동 시에도 자유로운 움직임을 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I559" t="inlineStr">
+        <is>
+          <t>빅사이즈,남성슬랙스,와이드핏,운동복,편안한바지,빅사이즈남성,슬랙스추천</t>
+        </is>
+      </c>
+      <c r="J559" t="inlineStr">
+        <is>
+          <t>패션/남성의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="n">
+        <v>559</v>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>러닝과 헬스 모두 소화하는 다용도 운동복 이야기</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://naver.me/FFaMdzah</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_25/17297326606349nx4g_JPEG/63865591731134712_1455770870.jpg</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>러닝&amp;헬스 다용도 운동복</t>
+        </is>
+      </c>
+      <c r="F560" t="inlineStr">
+        <is>
+          <t>운동할 때마다 불편했나요? 러닝과 헬스에 모두 편안한 다용도 운동복으로 최적의 움직임을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G560" t="inlineStr">
+        <is>
+          <t>러닝과 헬스 모두 소화하는 다용도 운동복 추천</t>
+        </is>
+      </c>
+      <c r="H560" t="inlineStr">
+        <is>
+          <t>러닝과 헬스에 모두 적합한 다용도 운동복으로 편안한 착용감과 자유로운 움직임을 제공합니다. 다양한 운동에 최적화된 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I560" t="inlineStr">
+        <is>
+          <t>운동복,다용도운동복,러닝복,헬스복,편안한운동복,운동웨어,스포츠웨어</t>
+        </is>
+      </c>
+      <c r="J560" t="inlineStr">
+        <is>
+          <t>운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="n">
+        <v>560</v>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>짧은목도리 형태의 남자 캐시미어 머플러 휴대와 보관법</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://naver.me/GJ5ih8Z4</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231220_290/1703062137707Wf8CI_JPEG/104198033430835259_1308403619.jpg</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>포근한 남성 캐시미어 머플러</t>
+        </is>
+      </c>
+      <c r="F561" t="inlineStr">
+        <is>
+          <t>차가운 날씨에도 목을 따뜻하게 감싸주어 겨울 외출이 즐거워집니다. 가볍고 휴대가 편해 어디서나 간편히 보관하세요.</t>
+        </is>
+      </c>
+      <c r="G561" t="inlineStr">
+        <is>
+          <t>남자 캐시미어 짧은목도리 머플러 추천, 따뜻한 겨울 필수품</t>
+        </is>
+      </c>
+      <c r="H561" t="inlineStr">
+        <is>
+          <t>가볍고 부드러운 캐시미어 소재로 겨울철 목을 따뜻하게 감싸주며, 휴대와 보관이 간편한 남성용 짧은목도리 머플러입니다.</t>
+        </is>
+      </c>
+      <c r="I561" t="inlineStr">
+        <is>
+          <t>남자 목도리, 캐시미어 머플러, 짧은목도리, 겨울 머플러, 휴대용 목도리, 따뜻한 머플러</t>
+        </is>
+      </c>
+      <c r="J561" t="inlineStr">
+        <is>
+          <t>패션/겨울용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="n">
+        <v>561</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>연말 크리스마스에 어울리는 고급스러운 숄 목도리 추천</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://naver.me/5dA49UhI</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250531_244/1748637321220Ca4m4_JPEG/82770162365708984_1054816897.jpeg</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>고급스러운 숄 목도리</t>
+        </is>
+      </c>
+      <c r="F562" t="inlineStr">
+        <is>
+          <t>연말과 크리스마스에 어울리는 따뜻한 숄 목도리로 스타일과 보온을 동시에 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G562" t="inlineStr">
+        <is>
+          <t>연말 크리스마스 고급 숄 목도리 추천으로 따뜻함과 스타일 완성</t>
+        </is>
+      </c>
+      <c r="H562" t="inlineStr">
+        <is>
+          <t>연말과 크리스마스 시즌에 어울리는 고급스러운 숄 목도리로 따뜻함과 멋진 스타일을 동시에 챙기세요.</t>
+        </is>
+      </c>
+      <c r="I562" t="inlineStr">
+        <is>
+          <t>연말 목도리,크리스마스 숄,고급 목도리,따뜻한 스카프,겨울 액세서리,여성 목도리,남성 숄</t>
+        </is>
+      </c>
+      <c r="J562" t="inlineStr">
+        <is>
+          <t>겨울패션/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="n">
+        <v>562</v>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>부드러운 감촉의 울머플러로 겨울 운동 후 휴대용으로 좋아요</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://naver.me/GYG90gMo</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_228/1765269910613I9Nib_JPEG/4116169668984464_1800646980.JPG</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>부드러운 울머플러</t>
+        </is>
+      </c>
+      <c r="F563" t="inlineStr">
+        <is>
+          <t>운동 후 쌀쌀한 겨울, 부드러운 울머플러로 따뜻함을 유지하세요. 가볍고 휴대하기 좋아요.</t>
+        </is>
+      </c>
+      <c r="G563" t="inlineStr">
+        <is>
+          <t>부드러운 울머플러 겨울 운동용 추천 따뜻한 휴대용</t>
+        </is>
+      </c>
+      <c r="H563" t="inlineStr">
+        <is>
+          <t>운동 후 쌀쌀한 겨울에도 부드러운 울머플러로 따뜻함을 유지할 수 있어요. 가볍고 휴대하기 좋아 활용도가 높습니다.</t>
+        </is>
+      </c>
+      <c r="I563" t="inlineStr">
+        <is>
+          <t>울머플러,겨울머플러,운동용머플러,부드러운머플러,휴대용머플러,따뜻한머플러,겨울패션,겨울소품</t>
+        </is>
+      </c>
+      <c r="J563" t="inlineStr">
+        <is>
+          <t>겨울/패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="n">
+        <v>563</v>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>커플 선물로 좋은 겨울용 예쁜 미니목도리</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://naver.me/xdjFPX8p</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251016_161/1760623976991YGGTt_JPEG/67216740334686619_1221438390.JPG</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 미니목도리</t>
+        </is>
+      </c>
+      <c r="F564" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 부담 없이 포근한 커플 미니목도리로 특별한 선물을 준비해보세요.</t>
+        </is>
+      </c>
+      <c r="G564" t="inlineStr">
+        <is>
+          <t>커플 선물 겨울용 미니목도리 추천, 포근한 데일리 아이템</t>
+        </is>
+      </c>
+      <c r="H564" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 부담 없이 착용 가능한 커플용 미니목도리로 따뜻함과 스타일을 동시에 챙겨보세요.</t>
+        </is>
+      </c>
+      <c r="I564" t="inlineStr">
+        <is>
+          <t>커플목도리,미니목도리,겨울목도리,커플선물,포근한목도리,겨울패션,목도리추천</t>
+        </is>
+      </c>
+      <c r="J564" t="inlineStr">
+        <is>
+          <t>패션/목도리</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="n">
+        <v>564</v>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>소중한 강아지와 고양이 얼굴 키링으로 마음을 전해요</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://naver.me/xXw56ltu</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250212_298/1739319922382rplWR_JPEG/73452722526998419_2061161191.jpg</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>강아지 고양이 얼굴 키링</t>
+        </is>
+      </c>
+      <c r="F565" t="inlineStr">
+        <is>
+          <t>반려동물의 사랑스러운 얼굴을 담아 소중한 마음을 전하세요. 특별한 선물로 딱 좋아요.</t>
+        </is>
+      </c>
+      <c r="G565" t="inlineStr">
+        <is>
+          <t>소중한 강아지와 고양이 얼굴 키링 추천 특별 선물</t>
+        </is>
+      </c>
+      <c r="H565" t="inlineStr">
+        <is>
+          <t>반려동물의 귀여운 얼굴을 담아 마음을 전하는 키링으로 특별한 선물이 가능합니다. 강아지와 고양이 애호가에게 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I565" t="inlineStr">
+        <is>
+          <t>강아지 키링,고양이 키링,반려동물 선물,애완동물 액세서리,특별한 선물</t>
+        </is>
+      </c>
+      <c r="J565" t="inlineStr">
+        <is>
+          <t>애완용품/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="n">
+        <v>565</v>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>운동 후에도 부담 없는 와이드 밴딩 팬츠 활용법</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://naver.me/F3YXHxOO</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251001_288/17593200467620Kb50_PNG/24914495885957850_712121420.png</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>편안한 와이드 밴딩팬츠</t>
+        </is>
+      </c>
+      <c r="F566" t="inlineStr">
+        <is>
+          <t>운동 후에도 불편함 없이 편안한 와이드 밴딩팬츠로 활동성을 높이세요.</t>
+        </is>
+      </c>
+      <c r="G566" t="inlineStr">
+        <is>
+          <t>편안한 와이드 밴딩 팬츠 활용법 추천</t>
+        </is>
+      </c>
+      <c r="H566" t="inlineStr">
+        <is>
+          <t>운동 후에도 부담 없이 착용 가능한 편안한 와이드 밴딩 팬츠로 활동성을 높이고 일상에서도 활용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I566" t="inlineStr">
+        <is>
+          <t>와이드 밴딩 팬츠,운동복,편안한 팬츠,활동성 좋은 팬츠,운동 후 팬츠</t>
+        </is>
+      </c>
+      <c r="J566" t="inlineStr">
+        <is>
+          <t>패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="n">
+        <v>566</v>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>출퇴근용 겨울 와이드 밴딩 청바지 추천</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://naver.me/II4c8s4w</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251105_115/1762330603925WpHdU_JPEG/96463492666087289_573857834.jpg</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>겨울용 와이드 밴딩 청바지</t>
+        </is>
+      </c>
+      <c r="F567" t="inlineStr">
+        <is>
+          <t>출퇴근 길도 따뜻하고 편안하게, 겨울철 필수 와이드 밴딩 청바지로 스타일을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G567" t="inlineStr">
+        <is>
+          <t>출퇴근용 겨울 와이드 밴딩 청바지 추천, 따뜻하고 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H567" t="inlineStr">
+        <is>
+          <t>겨울철 출퇴근용 와이드 밴딩 청바지로 따뜻하고 편안한 착용감을 경험하세요. 스타일과 실용성을 동시에 갖춘 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I567" t="inlineStr">
+        <is>
+          <t>겨울 청바지, 와이드 밴딩 청바지, 출퇴근 패션, 따뜻한 청바지, 편안한 바지</t>
+        </is>
+      </c>
+      <c r="J567" t="inlineStr">
+        <is>
+          <t>패션/청바지</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="n">
+        <v>567</v>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>집 근처 공원에서 가볍게 운동할 때 좋은 러닝 쇼츠</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://naver.me/xJGBgVGj</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250527_153/1748328090720Fup9D_JPEG/76917717801745974_1608780613.jpg</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>가볍고 편안한 러닝 쇼츠</t>
+        </is>
+      </c>
+      <c r="F568" t="inlineStr">
+        <is>
+          <t>운동할 때 답답한 옷차림이 고민이라면, 통기성 좋은 러닝 쇼츠로 쾌적함을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G568" t="inlineStr">
+        <is>
+          <t>통기성 좋은 러닝 쇼츠 추천, 집 근처 공원 운동에 적합</t>
+        </is>
+      </c>
+      <c r="H568" t="inlineStr">
+        <is>
+          <t>가벼운 운동에 적합한 통기성 좋은 러닝 쇼츠로 쾌적한 착용감을 경험해 보세요. 집 근처 공원 산책이나 달리기에 최적입니다.</t>
+        </is>
+      </c>
+      <c r="I568" t="inlineStr">
+        <is>
+          <t>러닝쇼츠,운동복,통기성,가벼운운동,운동용반바지,공원운동,러닝웨어</t>
+        </is>
+      </c>
+      <c r="J568" t="inlineStr">
+        <is>
+          <t>운동복/러닝</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="n">
+        <v>568</v>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>운동할 때 제격인 조거 팬츠 추천드려요</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://naver.me/5SSQJ7S0</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_274/1729733411570eRwoO_JPEG/4295345704461212_58253742.jpg</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>편안한 운동 조거 팬츠</t>
+        </is>
+      </c>
+      <c r="F569" t="inlineStr">
+        <is>
+          <t>운동할 때 편안함과 스타일 모두 놓치기 싫다면 꼭 필요한 조거 팬츠입니다.</t>
+        </is>
+      </c>
+      <c r="G569" t="inlineStr">
+        <is>
+          <t>운동할 때 제격인 조거 팬츠 추천 - 편안한 스타일</t>
+        </is>
+      </c>
+      <c r="H569" t="inlineStr">
+        <is>
+          <t>운동 시 편안함과 스타일을 동시에 갖춘 조거 팬츠로 활동성을 높이고 일상복으로도 활용하기 좋은 제품입니다.</t>
+        </is>
+      </c>
+      <c r="I569" t="inlineStr">
+        <is>
+          <t>조거팬츠,운동복,편안한바지,스포츠웨어,캐주얼팬츠</t>
+        </is>
+      </c>
+      <c r="J569" t="inlineStr">
+        <is>
+          <t>운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="n">
+        <v>569</v>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>운동할 때 최적화된 트리코트 조거 팬츠 추천</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://naver.me/FVSYoTSr</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20210928_82/16328095487713Poow_JPEG/33945394489861761_996892351.jpg</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>운동 최적화 트리코트 조거팬츠</t>
+        </is>
+      </c>
+      <c r="F570" t="inlineStr">
+        <is>
+          <t>땀과 움직임에 완벽하게 맞춰진 조거 팬츠로, 편안함과 스타일을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G570" t="inlineStr">
+        <is>
+          <t>운동할 때 최적화된 트리코트 조거 팬츠 추천</t>
+        </is>
+      </c>
+      <c r="H570" t="inlineStr">
+        <is>
+          <t>땀과 움직임에 완벽하게 맞춰진 트리코트 조거 팬츠로 편안함과 스타일을 동시에 누릴 수 있습니다. 일상 운동과 야외 활동에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I570" t="inlineStr">
+        <is>
+          <t>트리코트,조거팬츠,운동복,편안한 팬츠,스타일 팬츠,트레이닝,활동복,스포츠웨어</t>
+        </is>
+      </c>
+      <c r="J570" t="inlineStr">
+        <is>
+          <t>운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="n">
+        <v>570</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>출퇴근길을 따뜻하게 만드는 미니 쁘띠 목도리</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://naver.me/x6xyk8ee</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241127_187/1732672695942U2beW_PNG/66805502052796842_1865423638.png</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>포근한 미니 목도리</t>
+        </is>
+      </c>
+      <c r="F571" t="inlineStr">
+        <is>
+          <t>출퇴근길 찬바람에 시린 목, 작고 가벼운 미니 목도리로 따뜻함을 더하세요.</t>
+        </is>
+      </c>
+      <c r="G571" t="inlineStr">
+        <is>
+          <t>출퇴근길 미니 쁘띠 목도리 추천 따뜻한 목 보호</t>
+        </is>
+      </c>
+      <c r="H571" t="inlineStr">
+        <is>
+          <t>가벼운 미니 쁘띠 목도리로 출퇴근길 찬바람을 막아주어 목을 따뜻하게 보호합니다. 작고 컴팩트한 디자인이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I571" t="inlineStr">
+        <is>
+          <t>목도리,미니목도리,쁘띠목도리,출퇴근용,따뜻한목도리,경량목도리,목보호</t>
+        </is>
+      </c>
+      <c r="J571" t="inlineStr">
+        <is>
+          <t>패션/액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="n">
+        <v>571</v>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>제임스딘 드로즈, 운동할 때도 땀 흡수 잘 되는 속옷</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://naver.me/GbAF7BDm</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250612_102/1749717293220qb0EA_JPEG/4173911010195187_481928943.jpg</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>땀 흡수 운동용 드로즈</t>
+        </is>
+      </c>
+      <c r="F572" t="inlineStr">
+        <is>
+          <t>운동 중 땀 걱정 없이 쾌적함을 유지하세요. 편안한 착용감으로 활동성을 높여줍니다.</t>
+        </is>
+      </c>
+      <c r="G572" t="inlineStr">
+        <is>
+          <t>제임스딘 드로즈 운동용 쾌적 속옷 추천</t>
+        </is>
+      </c>
+      <c r="H572" t="inlineStr">
+        <is>
+          <t>운동 중 땀 흡수가 뛰어나 쾌적함을 유지하고 편안한 착용감으로 활동성을 높여줍니다.</t>
+        </is>
+      </c>
+      <c r="I572" t="inlineStr">
+        <is>
+          <t>제임스딘, 드로즈, 운동속옷, 땀흡수, 쾌적속옷, 편안한속옷, 남성속옷</t>
+        </is>
+      </c>
+      <c r="J572" t="inlineStr">
+        <is>
+          <t>속옷/운동</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="n">
+        <v>572</v>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>운동할 때 최적화된 쿨링 기능성 무지 티셔츠 추천</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://naver.me/GreahXmL</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241024_179/1729732283604IzBcR_JPEG/63865214709757452_2120109612.jpg</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>운동 쾌적 쿨링 티셔츠</t>
+        </is>
+      </c>
+      <c r="F573" t="inlineStr">
+        <is>
+          <t>운동 중 땀 때문에 불편할 때, 시원한 쿨링 기능이 쾌적함을 유지해 줍니다.</t>
+        </is>
+      </c>
+      <c r="G573" t="inlineStr">
+        <is>
+          <t>운동용 쿨링 기능성 무지 티셔츠 추천 - 시원한 착용감</t>
+        </is>
+      </c>
+      <c r="H573" t="inlineStr">
+        <is>
+          <t>운동 중 땀으로 인한 불편함을 줄여주는 쿨링 기능성 무지 티셔츠로 쾌적한 착용감을 제공합니다. 활동적인 라이프스타일에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I573" t="inlineStr">
+        <is>
+          <t>운동티셔츠,쿨링티셔츠,기능성티셔츠,무지티셔츠,스포츠웨어,여름운동복</t>
+        </is>
+      </c>
+      <c r="J573" t="inlineStr">
+        <is>
+          <t>운동복/티셔츠</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="n">
+        <v>573</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 작지만 특별한 키링으로 기분 전환</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://naver.me/Gq94QP5m</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251222_246/1766362556130Bs9aN_JPEG/46496787899978546_914785932.jpg</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>작고 특별한 기분 전환 키링</t>
+        </is>
+      </c>
+      <c r="F574" t="inlineStr">
+        <is>
+          <t>출퇴근길 지루함을 달래줄 작고 특별한 키링으로 기분까지 산뜻하게 바꿔보세요.</t>
+        </is>
+      </c>
+      <c r="G574" t="inlineStr">
+        <is>
+          <t>작지만 특별한 키링 추천, 출퇴근길 기분 전환 아이템</t>
+        </is>
+      </c>
+      <c r="H574" t="inlineStr">
+        <is>
+          <t>출퇴근길 지루함을 달래줄 작고 특별한 키링으로 일상에 산뜻함을 더하세요. 작은 변화로 기분 전환을 원하시는 분들께 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I574" t="inlineStr">
+        <is>
+          <t>키링,출퇴근길 키링,기분 전환 아이템,작은 키링,일상용 키링</t>
+        </is>
+      </c>
+      <c r="J574" t="inlineStr">
+        <is>
+          <t>액세서리</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="n">
+        <v>574</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>겨울철 따뜻하게 입기 좋은 밴딩기모바지 소개</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://naver.me/5h1aYsu9</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251016_110/1760548491967iJVAm_PNG/43455157513832045_894974845.png</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>따뜻한 밴딩 기모바지</t>
+        </is>
+      </c>
+      <c r="F575" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻하고 편안한 밴딩 기모바지로 하루 종일 쾌적한 착용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G575" t="inlineStr">
+        <is>
+          <t>겨울철 따뜻하게 입기 좋은 밴딩기모바지 추천</t>
+        </is>
+      </c>
+      <c r="H575" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 편안하고 따뜻한 착용감을 제공하는 밴딩 기모바지로 하루 종일 쾌적함을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I575" t="inlineStr">
+        <is>
+          <t>밴딩기모바지,겨울바지,기모바지,따뜻한바지,편안한바지,겨울옷,겨울패션,겨울코디</t>
+        </is>
+      </c>
+      <c r="J575" t="inlineStr">
+        <is>
+          <t>겨울의류</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="n">
+        <v>575</v>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>편안한 착용감과 보온성을 겸비한 남자 기모 골덴바지</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://naver.me/50JM9bJq</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251027_206/1761572019579iqoaW_JPEG/8333562561349489_66055258.jpg</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>남성 기모 골덴바지</t>
+        </is>
+      </c>
+      <c r="F576" t="inlineStr">
+        <is>
+          <t>추운 날씨에도 편안하게 입을 수 있는 따뜻한 기모 골덴바지로 겨울 나기 걱정을 덜어보세요.</t>
+        </is>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>남자 기모 골덴바지 추천 겨울철 편안한 보온 바지</t>
+        </is>
+      </c>
+      <c r="H576" t="inlineStr">
+        <is>
+          <t>기모 골덴바지로 보온성과 편안한 착용감을 모두 갖춘 겨울용 남성 바지입니다. 추운 날씨에 적합한 따뜻한 소재를 사용했습니다.</t>
+        </is>
+      </c>
+      <c r="I576" t="inlineStr">
+        <is>
+          <t>기모골덴바지,남자골덴바지,겨울바지,보온바지,편안한바지,기모바지</t>
+        </is>
+      </c>
+      <c r="J576" t="inlineStr">
+        <is>
+          <t>겨울패션/남성</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="n">
+        <v>576</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>부드러운 머플러와 함께하는 겨울 운동 시간</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://naver.me/5xapXzgH</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241015_217/1728959353033qQrbN_JPEG/5446661160273028_854136038.jpg</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>포근한 겨울 운동 머플러</t>
+        </is>
+      </c>
+      <c r="F577" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 따뜻함을 유지하며 운동할 수 있는 부드러운 머플러로 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>추운 겨울 운동용 부드러운 머플러 추천</t>
+        </is>
+      </c>
+      <c r="H577" t="inlineStr">
+        <is>
+          <t>겨울 운동 시 따뜻함과 편안함을 제공하는 부드러운 머플러로 추위 걱정 없이 활동하세요.</t>
+        </is>
+      </c>
+      <c r="I577" t="inlineStr">
+        <is>
+          <t>겨울 머플러,운동 머플러,따뜻한 머플러,부드러운 머플러,겨울 운동용품</t>
+        </is>
+      </c>
+      <c r="J577" t="inlineStr">
+        <is>
+          <t>패션/운동용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="n">
+        <v>577</v>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>겨울작업에도 적합한 퀄팅패딩 잠바의 활동성</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fm36hi27</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241213_20/1734083035014IylQB_JPEG/49098699603587041_308975377.jpg</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr">
+        <is>
+          <t>겨울철 활동성 퀄팅패딩</t>
+        </is>
+      </c>
+      <c r="F578" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 편안한 움직임을 돕는 퀄팅패딩으로 작업 중에도 따뜻함과 활동성을 모두 챙기세요.</t>
+        </is>
+      </c>
+      <c r="G578" t="inlineStr">
+        <is>
+          <t>겨울작업용 퀄팅패딩 잠바 추천, 따뜻한 활동성 확보</t>
+        </is>
+      </c>
+      <c r="H578" t="inlineStr">
+        <is>
+          <t>추운 겨울 작업에도 적합한 퀄팅패딩 잠바로 편안한 움직임과 뛰어난 보온성을 제공합니다. 작업복으로도 손색없는 활동성을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I578" t="inlineStr">
+        <is>
+          <t>퀄팅패딩, 겨울작업, 작업복, 보온잠바, 활동성, 따뜻한잠바</t>
+        </is>
+      </c>
+      <c r="J578" t="inlineStr">
+        <is>
+          <t>겨울의류/작업복</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="n">
+        <v>578</v>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>활동성 좋은 밴딩청바지로 운동할 때도 부담 없이</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://naver.me/xZjbd6Vm</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251219_48/1766141114484Gu4x4_PNG/100274077565253058_1662471698.png</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr">
+        <is>
+          <t>운동도 편안한 밴딩청바지</t>
+        </is>
+      </c>
+      <c r="F579" t="inlineStr">
+        <is>
+          <t>활동량 많은 날에도 불편함 없이 쫀득한 착용감을 제공합니다. 부담 없이 운동과 일상을 모두 즐기세요.</t>
+        </is>
+      </c>
+      <c r="G579" t="inlineStr">
+        <is>
+          <t>활동성 좋은 밴딩청바지 추천 - 편안한 운동과 일상용</t>
+        </is>
+      </c>
+      <c r="H579" t="inlineStr">
+        <is>
+          <t>쫀득한 착용감으로 활동량 많은 날에도 편안하게 입을 수 있는 밴딩청바지입니다. 운동과 일상 모두 부담 없이 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I579" t="inlineStr">
+        <is>
+          <t>밴딩청바지,운동복,편안한청바지,활동성,일상복,남녀공용,신축성,캐주얼</t>
+        </is>
+      </c>
+      <c r="J579" t="inlineStr">
+        <is>
+          <t>패션/청바지</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="n">
+        <v>579</v>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>운동복으로 출퇴근길도 편안하게 보내는 방법</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://naver.me/GnRyOlRo</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250626_243/17509149576606pm2s_PNG/26085240458988858_1429110069.png</t>
+        </is>
+      </c>
+      <c r="E580" t="inlineStr">
+        <is>
+          <t>출퇴근용 편안한 운동복</t>
+        </is>
+      </c>
+      <c r="F580" t="inlineStr">
+        <is>
+          <t>출퇴근길 불편함은 이제 그만, 편안함과 활동성을 동시에 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G580" t="inlineStr">
+        <is>
+          <t>운동복 출퇴근길 추천, 편안함과 활동성 모두 갖춘 스타일</t>
+        </is>
+      </c>
+      <c r="H580" t="inlineStr">
+        <is>
+          <t>출퇴근길의 불편함을 해결해주는 운동복으로 편안하고 활동적인 하루를 시작하세요. 누구나 부담 없이 입기 좋은 디자인입니다.</t>
+        </is>
+      </c>
+      <c r="I580" t="inlineStr">
+        <is>
+          <t>운동복, 출퇴근복, 편안한 옷, 활동적인 복장, 데일리웨어</t>
+        </is>
+      </c>
+      <c r="J580" t="inlineStr">
+        <is>
+          <t>패션/운동복</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="n">
+        <v>580</v>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>겨울 외출 필수품, 패딩목도리의 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://naver.me/FHVg1Co1</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251030_299/17618070412693IBeH_JPEG/9783034272407597_123816286.jpg</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr">
+        <is>
+          <t>따뜻한 겨울 패딩목도리</t>
+        </is>
+      </c>
+      <c r="F581" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 포근한 착용감으로 외출 걱정 끝, 따뜻함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G581" t="inlineStr">
+        <is>
+          <t>겨울 외출 필수 패딩목도리 추천, 편안한 착용감과 따뜻함</t>
+        </is>
+      </c>
+      <c r="H581" t="inlineStr">
+        <is>
+          <t>추운 겨울에도 포근한 착용감을 제공하는 패딩목도리로 따뜻하게 외출하세요. 실용적이고 부드러운 겨울 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I581" t="inlineStr">
+        <is>
+          <t>패딩목도리,겨울목도리,보온목도리,패딩,겨울외출,따뜻한목도리,편안한착용감</t>
+        </is>
+      </c>
+      <c r="J581" t="inlineStr">
+        <is>
+          <t>겨울/패션</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="n">
+        <v>581</v>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>운동 중에도 태그미 커플키링으로 스마트 연결</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://naver.me/FGExkQwD</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251201_169/17645832181733EuuU_PNG/98716158249500001_2104017671.png</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr">
+        <is>
+          <t>스마트 커플키링 운동중 연결</t>
+        </is>
+      </c>
+      <c r="F582" t="inlineStr">
+        <is>
+          <t>운동 중에도 사랑을 연결하는 스마트 커플키링으로 소중한 사람과 항상 함께하세요.</t>
+        </is>
+      </c>
+      <c r="G582" t="inlineStr">
+        <is>
+          <t>운동 중에도 태그미 커플키링 스마트 연결 추천</t>
+        </is>
+      </c>
+      <c r="H582" t="inlineStr">
+        <is>
+          <t>운동 중에도 소중한 사람과 항상 연결되는 스마트 커플키링으로 편리한 소통과 사랑을 지속하세요.</t>
+        </is>
+      </c>
+      <c r="I582" t="inlineStr">
+        <is>
+          <t>커플키링,스마트키링,운동용 키링,태그미,커플선물,사랑연결,스마트악세사리</t>
+        </is>
+      </c>
+      <c r="J582" t="inlineStr">
+        <is>
+          <t>커플액세서리</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All-in-one: update products & pages (2026-01-19 12:25)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -2,31 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="13140" yWindow="5970" windowWidth="23820" windowHeight="14715" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
       <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +56,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +81,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,13 +444,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J682"/>
+  <dimension ref="A1:J753"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A683" sqref="A683"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <cols>
+    <col width="45.25" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -34535,7 +34558,3558 @@
         </is>
       </c>
     </row>
+    <row r="683">
+      <c r="A683" t="n">
+        <v>682</v>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>호텔 수건 같은 부드러운 타월로 통화 후 손닦기 좋은 선택</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://naver.me/F3Y8bDH7</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230628_78/1687924669614HSJ8W_JPEG/1089944589840563_1767513167.jpg</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr">
+        <is>
+          <t>호텔 부드러운 손타월</t>
+        </is>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>통화 후 손을 닦기 딱 좋은 부드러운 호텔 수건 느낌, 피부 자극 없이 편안함을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>호텔 수건 같은 부드러운 타월 추천 - 통화 후 손닦기용</t>
+        </is>
+      </c>
+      <c r="H683" t="inlineStr">
+        <is>
+          <t>호텔 수건처럼 부드러운 타월로 통화 후 손을 편안하게 닦아주는 제품입니다. 피부 자극 없이 누구나 사용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I683" t="inlineStr">
+        <is>
+          <t>부드러운 타월,호텔 수건,손 닦기,피부 자극 없는 타월,통화 후 타월</t>
+        </is>
+      </c>
+      <c r="J683" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="n">
+        <v>683</v>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>3개월분 비타민B12와 아연, 꾸준한 영양 보충법</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://naver.me/5JG9AHyx</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230816_293/1692150480888krngp_JPEG/6826070257218395_1868163127.jpg</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>비타민B12와 아연 3개월분</t>
+        </is>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>에너지와 면역력 고민에 딱 맞는 비타민B12와 아연으로 건강을 꾸준히 지키세요.</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>3개월분 비타민B12와 아연 영양제 추천, 건강 유지 간편 구매</t>
+        </is>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>에너지 증진과 면역력 강화를 위한 비타민B12와 아연 3개월분으로 꾸준한 건강 관리를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I684" t="inlineStr">
+        <is>
+          <t>비타민B12,아연,영양제,면역력,에너지보충,건강관리,3개월분</t>
+        </is>
+      </c>
+      <c r="J684" t="inlineStr">
+        <is>
+          <t>건강/영양제</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="n">
+        <v>684</v>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>캠핑 때 즐기기 좋은 신선한 우대갈비 찜 이야기</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://naver.me/x7jJ3cWq</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221116_74/1668557377543UurAY_JPEG/69693212359783973_733947479.jpg</t>
+        </is>
+      </c>
+      <c r="E685" t="inlineStr">
+        <is>
+          <t>신선한 우대갈비 찜</t>
+        </is>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>캠핑 음식 고민 끝! 부드럽고 신선한 우대갈비 찜으로 특별한 맛을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
+        <is>
+          <t>캠핑 추천 신선한 우대갈비 찜 할인 구매</t>
+        </is>
+      </c>
+      <c r="H685" t="inlineStr">
+        <is>
+          <t>캠핑에 딱 맞는 부드럽고 신선한 우대갈비 찜으로 간편하게 맛있는 식사를 즐기세요. 캠핑 음식 고민을 해결해드립니다.</t>
+        </is>
+      </c>
+      <c r="I685" t="inlineStr">
+        <is>
+          <t>캠핑음식,우대갈비찜,신선한갈비,부드러운갈비,캠핑요리,특별한맛</t>
+        </is>
+      </c>
+      <c r="J685" t="inlineStr">
+        <is>
+          <t>캠핑/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="n">
+        <v>685</v>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>출퇴근 전 켜두기 좋은 벽걸이형 컨벡션히터 추천</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://naver.me/GWiYV5GV</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_87/1761279481661Qx5Me_JPEG/20721100855900162_2100783670.jpg</t>
+        </is>
+      </c>
+      <c r="E686" t="inlineStr">
+        <is>
+          <t>벽걸이형 컨벡션히터</t>
+        </is>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>추운 출퇴근길에도 따뜻함을 미리 준비하세요. 공간 절약형 벽걸이 히터로 쾌적한 온기를 즐기세요.</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>출퇴근 전 켜두기 좋은 벽걸이형 컨벡션히터 추천</t>
+        </is>
+      </c>
+      <c r="H686" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 미리 따뜻함을 준비할 수 있는 공간 절약형 벽걸이 컨벡션히터로 쾌적한 온기를 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I686" t="inlineStr">
+        <is>
+          <t>컨벡션히터,벽걸이히터,출퇴근용히터,작은공간히터,난방기구,공간절약히터</t>
+        </is>
+      </c>
+      <c r="J686" t="inlineStr">
+        <is>
+          <t>난방기구/벽걸이히터</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="n">
+        <v>686</v>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>정성 가득한 한우 찜갈비, 설날 선물로 추천해요</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://naver.me/FQyvsitb</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240115_236/1705298091421odgzP_PNG/106433871088985342_1953932693.png</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr">
+        <is>
+          <t>부드러운 한우 찜갈비</t>
+        </is>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>가족과 함께 맛있는 설날을! 정성 가득한 한우 찜갈비로 특별한 순간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>정성 가득한 한우 찜갈비 설날 선물 추천</t>
+        </is>
+      </c>
+      <c r="H687" t="inlineStr">
+        <is>
+          <t>가족과 함께하는 설날, 정성 가득한 한우 찜갈비로 특별한 맛과 행복을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="I687" t="inlineStr">
+        <is>
+          <t>한우찜갈비, 설날선물, 명절음식, 가족식사, 특별한선물</t>
+        </is>
+      </c>
+      <c r="J687" t="inlineStr">
+        <is>
+          <t>설날/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="n">
+        <v>687</v>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 준비하는 한우 구이 요리</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://naver.me/GBvr9y8T</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240816_53/1723814121665ghsnG_PNG/70773646461639925_1239251959.png</t>
+        </is>
+      </c>
+      <c r="E688" t="inlineStr">
+        <is>
+          <t>간편 한우 구이 맛있게</t>
+        </is>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>출퇴근 후 빠르게 준비해 고소한 한우 구이로 지친 하루를 맛있게 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>한우 구이 간편 조리법 추천 - 출퇴근 후 빠른 한우 요리</t>
+        </is>
+      </c>
+      <c r="H688" t="inlineStr">
+        <is>
+          <t>출퇴근 후 간편하게 준비할 수 있는 고소한 한우 구이로 하루를 맛있게 마무리하세요. 빠른 조리와 풍부한 맛이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I688" t="inlineStr">
+        <is>
+          <t>한우 구이,간편 요리,출퇴근 요리,한우 맛집,빠른 한우,홈쿡,저녁 식사,고기 요리</t>
+        </is>
+      </c>
+      <c r="J688" t="inlineStr">
+        <is>
+          <t>한우/요리</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="n">
+        <v>688</v>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>6M 연장 호스로 어려운 배관도 깨끗하게 세척</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://naver.me/xNnfUNAe</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220916_167/1663277817256BgxfB_JPEG/64413596959806116_1234983577.jpg</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>6M 연장 배관 세척 호스</t>
+        </is>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>배관 청소가 어려워 고민이라면 6M 연장 호스로 깔끔하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>6M 연장 호스로 배관 청소 쉽고 깨끗하게 추천</t>
+        </is>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>6M 연장 호스로 배관 청소가 어려운 부분도 손쉽게 깔끔하게 세척할 수 있어 집안 관리에 효과적입니다.</t>
+        </is>
+      </c>
+      <c r="I689" t="inlineStr">
+        <is>
+          <t>배관 청소, 6M 연장 호스, 배관 세척, 집안 관리, 청소 도구</t>
+        </is>
+      </c>
+      <c r="J689" t="inlineStr">
+        <is>
+          <t>생활/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="n">
+        <v>689</v>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>고압세척기로 집안 배관 청소가 한결 쉬워졌어요</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://naver.me/GnRfAU59</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220915_44/1663195281597l6Bxr_JPEG/64331116413114522_1570410935.jpg</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr">
+        <is>
+          <t>집안 배관 깨끗이 청소</t>
+        </is>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>배관 막힘, 냄새 고민 끝! 고압세척기로 쉽고 빠르게 집안 청결을 지키세요.</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>고압세척기 배관 청소 추천 - 집안 배관 막힘 해결</t>
+        </is>
+      </c>
+      <c r="H690" t="inlineStr">
+        <is>
+          <t>고압세척기로 배관 막힘과 냄새 문제를 간편하게 해결해 보세요. 집안 배관 청소를 쉽고 빠르게 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I690" t="inlineStr">
+        <is>
+          <t>고압세척기, 배관청소, 집안청소, 배관막힘, 냄새제거, 청소기기, 주방청소</t>
+        </is>
+      </c>
+      <c r="J690" t="inlineStr">
+        <is>
+          <t>생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="n">
+        <v>690</v>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>명절 선물로 제격인 7.5kg 나주배 세트 소개</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fr0658Uh</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250907_55/1757254047088KGtmi_JPEG/10848959219834333_1151914422.jpg</t>
+        </is>
+      </c>
+      <c r="E691" t="inlineStr">
+        <is>
+          <t>신선한 7.5kg 나주배 세트</t>
+        </is>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>명절 선물 고민 끝! 달콤하고 신선한 나주배로 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>명절 선물 추천 7.5kg 나주배 세트 신선하고 달콤한 구매</t>
+        </is>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>신선하고 달콤한 나주배 7.5kg 세트로 명절 선물 고민을 해결하세요. 건강한 과일로 온 가족이 함께 즐기기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I691" t="inlineStr">
+        <is>
+          <t>명절선물,나주배,과일선물,신선한배,달콤한과일,과일세트,가족선물</t>
+        </is>
+      </c>
+      <c r="J691" t="inlineStr">
+        <is>
+          <t>명절/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="n">
+        <v>691</v>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>정성 가득한 한우 등심으로 특별한 명절 상차림 완성</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://naver.me/GNR028cD</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221118_146/1668748995088DI8je_JPEG/69884778792702594_1294477324.jpg</t>
+        </is>
+      </c>
+      <c r="E692" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 등심</t>
+        </is>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>정성 가득한 한우 등심으로 명절 상차림을 특별하게 완성하세요. 가족의 행복한 순간을 함께하세요.</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>한우 등심 명절 상차림 추천 - 정성 가득한 특별한 식사</t>
+        </is>
+      </c>
+      <c r="H692" t="inlineStr">
+        <is>
+          <t>한우 등심으로 명절 상차림을 더욱 특별하게 완성하세요. 가족과 함께하는 행복한 순간에 안성맞춤입니다.</t>
+        </is>
+      </c>
+      <c r="I692" t="inlineStr">
+        <is>
+          <t>한우 등심, 명절 상차림, 특별한 식사, 가족 모임, 고급 한우</t>
+        </is>
+      </c>
+      <c r="J692" t="inlineStr">
+        <is>
+          <t>명절/한우</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="n">
+        <v>692</v>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>노즐과 호스를 연결해 배관 청소를 손쉽게 끝내는 방법</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fm3zXUk5</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221229_260/1672300873205Aq3Rw_JPEG/73436708021923847_1060564037.jpg</t>
+        </is>
+      </c>
+      <c r="E693" t="inlineStr">
+        <is>
+          <t>배관 청소 간편 노즐</t>
+        </is>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>더러운 배관 청소가 걱정되시나요? 노즐과 호스로 쉽고 깔끔하게 해결하세요.</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
+        <is>
+          <t>노즐과 호스로 쉽고 깔끔한 배관 청소 추천</t>
+        </is>
+      </c>
+      <c r="H693" t="inlineStr">
+        <is>
+          <t>노즐과 호스를 연결해 더러운 배관 청소를 간편하고 효율적으로 해결하세요. 가정용 배관 청소에 적합한 도구입니다.</t>
+        </is>
+      </c>
+      <c r="I693" t="inlineStr">
+        <is>
+          <t>배관청소, 노즐, 호스, 배관관리, 청소도구, 가정용, 간편청소, 위생관리</t>
+        </is>
+      </c>
+      <c r="J693" t="inlineStr">
+        <is>
+          <t>생활/청소</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="n">
+        <v>693</v>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>고당도 한라봉으로 건강한 통화 시간을 즐기세요</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://naver.me/FtGi6wpW</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251211_72/17654463844670SDju_JPEG/18372445982762337_1641180196.jpg</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>달콤한 고당도 한라봉</t>
+        </is>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>상큼한 한라봉으로 지친 일상에 활력을! 건강한 달콤함을 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>고당도 한라봉 건강한 통화 시간 추천</t>
+        </is>
+      </c>
+      <c r="H694" t="inlineStr">
+        <is>
+          <t>상큼하고 달콤한 고당도 한라봉으로 지친 일상에 활력을 더하세요. 건강한 간식으로 인기입니다.</t>
+        </is>
+      </c>
+      <c r="I694" t="inlineStr">
+        <is>
+          <t>한라봉,고당도과일,건강간식,달콤한과일,면역력증진,비타민C</t>
+        </is>
+      </c>
+      <c r="J694" t="inlineStr">
+        <is>
+          <t>과일/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="n">
+        <v>694</v>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>출퇴근길에도 좋은 휴고스 벽걸이 난로 사용기</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://naver.me/G5PYHZWZ</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_190/1761279824595F2bUi_JPEG/26873173707539593_1421592921.jpg</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>효율적인 벽걸이 난로</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>출퇴근길 추위 걱정 없이 따뜻하게! 공간 절약형 난로로 쾌적한 겨울을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>휴고스 벽걸이 난로 추천 출퇴근길 따뜻한 공간 절약형 난로</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>출퇴근길 쾌적한 난방을 위한 휴고스 벽걸이 난로는 공간 절약형 디자인과 효율적인 온열 기능이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I695" t="inlineStr">
+        <is>
+          <t>휴고스 난로,벽걸이 난로,출퇴근 난방,공간 절약 난로,겨울 난로</t>
+        </is>
+      </c>
+      <c r="J695" t="inlineStr">
+        <is>
+          <t>가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="n">
+        <v>695</v>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>투뿔한우 설로인, 구이용으로 가족과 맛있는 시간</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://naver.me/5wNGUhqt</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250826_196/1756172286966NqL4q_JPEG/2313950102036927_1345584054.jpg</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 설로인 구이</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>가족과 함께하는 특별한 식사, 부드럽고 풍부한 맛의 한우 설로인이 고민 없이 즐거운 먹거리를 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>투뿔한우 설로인 구이 추천, 가족과 맛있는 시간</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>부드럽고 풍부한 맛의 투뿔한우 설로인으로 가족과 특별한 식사를 즐기세요. 구이용으로 최적화된 프리미엄 한우입니다.</t>
+        </is>
+      </c>
+      <c r="I696" t="inlineStr">
+        <is>
+          <t>투뿔한우, 설로인, 구이용한우, 가족식사, 한우추천, 프리미엄한우</t>
+        </is>
+      </c>
+      <c r="J696" t="inlineStr">
+        <is>
+          <t>한우/고기</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="n">
+        <v>696</v>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>출퇴근 길 간편하게 에너지바로 힘 충전하기</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://naver.me/ximTrXom</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260113_76/1768283373246Um9QI_JPEG/5541569061100749_2047489314.jpg</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>출퇴근 에너지바 충전</t>
+        </is>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길 간편한 에너지바로 지친 몸에 활력을 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>출퇴근 에너지바 추천으로 간편하게 힘 충전하세요</t>
+        </is>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에 간편하게 먹을 수 있는 에너지바로 지친 몸에 활력을 채워주는 건강 간식입니다.</t>
+        </is>
+      </c>
+      <c r="I697" t="inlineStr">
+        <is>
+          <t>에너지바,출퇴근간식,간편식,건강간식,활력충전</t>
+        </is>
+      </c>
+      <c r="J697" t="inlineStr">
+        <is>
+          <t>간편식</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="n">
+        <v>697</v>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>프리미엄 감귤로 건강한 출퇴근 간식을 준비해요</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://naver.me/GuD15osJ</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251022_77/17610961738270yeF1_JPEG/2203337644051844_1752172532.jpg</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>상큼한 건강 감귤 간식</t>
+        </is>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>피곤한 출퇴근길, 상큼한 감귤로 활력을 채워보세요. 간편하게 건강을 지킬 수 있어요.</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>프리미엄 감귤로 건강한 출퇴근 간식 추천</t>
+        </is>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>상큼한 프리미엄 감귤로 피곤한 출퇴근길에 활력을 더하세요. 간편하게 건강 간식을 즐길 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I698" t="inlineStr">
+        <is>
+          <t>프리미엄 감귤, 출퇴근 간식, 건강 간식, 상큼한 과일, 간편 간식</t>
+        </is>
+      </c>
+      <c r="J698" t="inlineStr">
+        <is>
+          <t>간식/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="n">
+        <v>698</v>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>명절 선물로 추천하는 달콤한 시나노골드 사과 세트</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fbq1P955</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260101_82/1767267448808x2DaU_PNG/11766445743486775_1333664845.png</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>달콤한 시나노골드 사과세트</t>
+        </is>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>설날맞이 선물로 좋은 달콤하고 신선한 시나노골드 사과 세트로 사랑을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>명절 선물 추천 시나노골드 사과 세트 할인 구매</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>설날 맞이 달콤하고 신선한 시나노골드 사과 세트로 특별한 명절 선물을 준비하세요. 가족과 지인에게 건강한 마음을 전하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I699" t="inlineStr">
+        <is>
+          <t>시나노골드,사과세트,명절선물,설날선물,과일선물,신선한사과,달콤한사과</t>
+        </is>
+      </c>
+      <c r="J699" t="inlineStr">
+        <is>
+          <t>명절/과일선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="n">
+        <v>699</v>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>산지직송 딸기로 기분 좋은 출퇴근 간식</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fdof2JI0</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251209_266/1765245382490zWxUQ_JPEG/14836934153257533_237965246.jpg</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>상큼한 산지직송 딸기</t>
+        </is>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 신선한 딸기로 기분 전환하세요. 달콤함이 에너지를 채워줍니다.</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>산지직송 딸기 출퇴근 간식 추천, 신선한 달콤함 가득</t>
+        </is>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>신선한 산지직송 딸기로 출퇴근길 기분 전환하세요. 간편한 간식으로 에너지를 채워줍니다.</t>
+        </is>
+      </c>
+      <c r="I700" t="inlineStr">
+        <is>
+          <t>산지직송,딸기,출퇴근간식,신선한과일,간편간식,달콤한간식,에너지충전</t>
+        </is>
+      </c>
+      <c r="J700" t="inlineStr">
+        <is>
+          <t>간식/과일</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="n">
+        <v>700</v>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>투뿔 소고기로 특별한 어버이날 선물 준비하기</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://naver.me/xzlJCFRs</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250106_117/1736152797355nDvwq_JPEG/70285738497904845_1046362743.jpg</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>프리미엄 투뿔 소고기</t>
+        </is>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>어버이날, 건강과 맛을 선물하세요. 정성 가득한 투뿔 소고기로 특별한 순간을 완성합니다.</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>투뿔 소고기 어버이날 선물 추천, 건강과 맛 모두 만족</t>
+        </is>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>투뿔 소고기로 어버이날 건강과 맛을 동시에 챙길 수 있는 특별한 선물입니다. 정성 가득한 품질로 특별한 순간을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I701" t="inlineStr">
+        <is>
+          <t>투뿔 소고기, 어버이날 선물, 건강 선물, 고급 소고기, 특별한 선물</t>
+        </is>
+      </c>
+      <c r="J701" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="n">
+        <v>701</v>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>명절 선물로 좋은 한라명작 1.2kg 한우세트</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://naver.me/xydMkJoh</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250106_166/1736150691494QbEPy_JPEG/70283539285086981_951853215.jpg</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 세트</t>
+        </is>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>명절 선물 고민 끝! 신선하고 풍부한 맛의 한우로 특별한 감사의 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>명절 선물 추천 한라명작 1.2kg 한우세트 할인 구매</t>
+        </is>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>신선한 1.2kg 한우세트로 명절 선물 고민 없이 감사의 마음을 전하세요. 풍부한 맛과 고품질 한우로 특별한 선물이 됩니다.</t>
+        </is>
+      </c>
+      <c r="I702" t="inlineStr">
+        <is>
+          <t>한우세트,명절선물,한라명작,고급한우,선물세트,1.2kg한우,감사선물,프리미엄한우</t>
+        </is>
+      </c>
+      <c r="J702" t="inlineStr">
+        <is>
+          <t>명절/선물세트</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="n">
+        <v>702</v>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>공간을 효율적으로 쓰는 벽걸이 히터 설치 후기</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://naver.me/5M5OfwTs</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251024_185/1761279317936TW155_JPEG/819334742292654_806162743.jpg</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>공간 절약 벽걸이 히터</t>
+        </is>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>좁은 공간에서도 따뜻함을 포기하지 마세요. 벽걸이 히터로 효율적인 난방을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>벽걸이 히터 추천 공간 효율적 난방 설치 후기</t>
+        </is>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>좁은 공간에 적합한 벽걸이 히터로 효율적인 난방이 가능합니다. 간편한 설치와 공간 절약에 적합해 따뜻한 환경을 유지하세요.</t>
+        </is>
+      </c>
+      <c r="I703" t="inlineStr">
+        <is>
+          <t>벽걸이 히터, 난방효율, 공간절약, 설치후기, 따뜻한 집, 효율난방, 벽걸이온풍기</t>
+        </is>
+      </c>
+      <c r="J703" t="inlineStr">
+        <is>
+          <t>가전/난방</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="n">
+        <v>703</v>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>출퇴근 준비 시간을 줄여주는 보만 스팀다리미 사용법</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://naver.me/GoihlO10</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20200416_17/1587024838465i3AAj_JPEG/24385577098078436_2090441662.jpg</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>빠른 출근용 스팀다리미</t>
+        </is>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>출퇴근 준비 시간을 줄이고 깔끔한 옷차림을 완성하세요. 쉽고 빠른 사용으로 매일 아침이 편안해집니다.</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>보만 스팀다리미 사용법으로 출퇴근 준비 시간 단축 추천</t>
+        </is>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>보만 스팀다리미는 쉽고 빠르게 옷차림을 정리해 매일 아침 출퇴근 준비 시간을 줄여줍니다. 간편한 사용법으로 편안한 일상을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="I704" t="inlineStr">
+        <is>
+          <t>보만,스팀다리미,출퇴근준비,다리미사용법,빠른다림질,옷관리,간편가전</t>
+        </is>
+      </c>
+      <c r="J704" t="inlineStr">
+        <is>
+          <t>생활가전</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="n">
+        <v>704</v>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 한우 설로인 구이로 활력 충전하기</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://naver.me/5IivMgGH</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_42/1736592727976wb9iD_JPEG/20754741779743894_1724877240.jpg</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>활력 충전 한우 설로인 구이</t>
+        </is>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 든든한 한우 설로인 구이로 에너지 가득 활력을 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>한우 설로인 구이로 활력 충전 추천</t>
+        </is>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 든든한 한우 설로인 구이로 에너지 충전과 활력 회복에 도움을 줍니다.</t>
+        </is>
+      </c>
+      <c r="I705" t="inlineStr">
+        <is>
+          <t>한우,설로인,한우구이,활력충전,에너지보충,출퇴근간식,건강식</t>
+        </is>
+      </c>
+      <c r="J705" t="inlineStr">
+        <is>
+          <t>식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="n">
+        <v>705</v>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>밍크융털 수면잠옷으로 통화할 때도 따뜻하게</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://naver.me/5mh5J3Qo</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260109_142/1767949226925H6fwM_JPEG/78097676726548975_768366443.jpg</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>포근한 밍크융털 잠옷</t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>추운 밤에도 끄덕없는 따뜻함, 수면 잠옷으로 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>밍크융털 수면잠옷 따뜻함 추천</t>
+        </is>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>밍크융털 소재로 한겨울에도 따뜻하게 입을 수 있는 수면잠옷으로 편안한 휴식을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I706" t="inlineStr">
+        <is>
+          <t>밍크융털,수면잠옷,겨울잠옷,보온잠옷,따뜻한잠옷</t>
+        </is>
+      </c>
+      <c r="J706" t="inlineStr">
+        <is>
+          <t>잠옷/홈웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>706</v>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>출퇴근 후 이너리즘 밍크 수면바지로 휴식 시간 즐기기</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://naver.me/5KqGjd4m</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20231206_118/1701841544494QUHgO_JPEG/102977387194511590_93984543.jpg</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>포근한 밍크 수면바지</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식을 원하신다면 부드러운 밍크 수면바지로 하루의 피로를 날려보세요.</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식 이너리즘 밍크 수면바지 추천</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>부드러운 이너리즘 밍크 수면바지로 출퇴근 후 편안한 휴식을 즐기세요. 하루 피로를 효과적으로 풀어주는 실내복입니다.</t>
+        </is>
+      </c>
+      <c r="I707" t="inlineStr">
+        <is>
+          <t>이너리즘,밍크 수면바지,편안한 휴식,출퇴근,실내복,수면바지</t>
+        </is>
+      </c>
+      <c r="J707" t="inlineStr">
+        <is>
+          <t>수면복</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>707</v>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>통화 중에도 선물 고민 없이 선택한 설날 한우 세트</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://naver.me/xxFbzfHy</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251230_205/1767072008008JwQ0p_PNG/117769532996332599_757614155.png</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>설날 선물 한우 세트</t>
+        </is>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>소중한 분께 특별한 설날 선물, 한우 세트로 고민 없이 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>설날 한우 세트 추천 통화 중에도 선물 고민 해결</t>
+        </is>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>설날 선물 고민 없이 특별한 한우 세트로 소중한 분께 마음을 전하세요. 고품질 한우로 가족에게 특별한 명절을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I708" t="inlineStr">
+        <is>
+          <t>설날 선물,한우 세트,명절 선물,프리미엄 한우,가족 선물,한우 구매,설날 추천,명절 한우</t>
+        </is>
+      </c>
+      <c r="J708" t="inlineStr">
+        <is>
+          <t>설날/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="n">
+        <v>708</v>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>통화 중에도 선물 고민 없이 선택한 설날 한우 세트</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://naver.me/xxFbzfHy</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251230_205/1767072008008JwQ0p_PNG/117769532996332599_757614155.png</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>설날 선물 한우 세트</t>
+        </is>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>설 선물 고민 끝! 신선한 한우 세트로 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>설날 한우 세트 추천, 통화 중에도 선물 고민 없이 선택하세요</t>
+        </is>
+      </c>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>신선한 한우 세트로 설날 선물 고민을 간편하게 해결하세요. 가족과 지인에게 마음을 전하기 좋은 명절 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I709" t="inlineStr">
+        <is>
+          <t>설날선물,한우세트,명절선물,신선한한우,한우선물,설날한우,한우구매</t>
+        </is>
+      </c>
+      <c r="J709" t="inlineStr">
+        <is>
+          <t>설날/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="n">
+        <v>709</v>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>비 오는 날에도 선명한 시야를 위한 자동차 유리 관리법</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://naver.me/xWzql1Gp</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20241018_18/1729235881321h0liH_JPEG/63368816461429016_70990470.jpg</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>비오는 날 선명한 유리 관리</t>
+        </is>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>비 오는 날 시야가 흐려 고민이라면, 자동차 유리 관리법으로 안전한 드라이빙을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>비 오는 날 자동차 유리 관리법 추천 안전한 시야 확보</t>
+        </is>
+      </c>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>비 오는 날에도 선명한 시야를 위한 자동차 유리 관리법으로 안전 운전을 도와드립니다. 간편한 관리법으로 쾌적한 드라이빙 환경을 만들어 보세요.</t>
+        </is>
+      </c>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>자동차 유리, 유리 관리법, 비 오는 날 시야, 안전 운전, 자동차 관리</t>
+        </is>
+      </c>
+      <c r="J710" t="inlineStr">
+        <is>
+          <t>자동차관리</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="n">
+        <v>710</v>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 딱 맞는 수면잠옷 추천</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://naver.me/xrC52tZO</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260112_225/1768218693846i3Nih_JPEG/81707952172063538_694076858.jpg</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>편안한 휴식 수면잠옷</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>하루의 피로를 부드럽게 감싸주는 수면잠옷으로 편안한 휴식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>출퇴근 후 휴식에 딱 맞는 수면잠옷 추천 - 편안한 수면</t>
+        </is>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>부드러운 소재로 하루 피로를 풀어주는 수면잠옷으로 편안한 휴식을 돕습니다. 출퇴근 후 휴식 시간에 적합한 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>수면잠옷,출퇴근,휴식,편안한잠옷,수면의류,집에서입는옷,피로회복</t>
+        </is>
+      </c>
+      <c r="J711" t="inlineStr">
+        <is>
+          <t>잠옷/편안함</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="n">
+        <v>711</v>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>설날 선물로 좋은 마장동 한우 선물 세트, 맛과 품질의 비결</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbgn70K</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260103_220/1767397746877Yd4oU_PNG/21846957667466438_127974687.png</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>최상급 마장동 한우 세트</t>
+        </is>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>설날 특별한 선물로 품질 좋은 마장동 한우로 가족의 입맛을 사로잡아보세요.</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>설날 선물 추천 마장동 한우 선물 세트 맛과 품질</t>
+        </is>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>설날 가족 선물로 좋은 마장동 한우 선물 세트로 신선하고 풍부한 맛을 즐기세요. 품질 좋은 한우로 특별한 명절을 완성합니다.</t>
+        </is>
+      </c>
+      <c r="I712" t="inlineStr">
+        <is>
+          <t>설날선물,마장동한우,한우선물세트,명절선물,가족선물,한우맛집</t>
+        </is>
+      </c>
+      <c r="J712" t="inlineStr">
+        <is>
+          <t>설날/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="n">
+        <v>712</v>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 좋은 구이용 한우 선물세트 활용법</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://naver.me/5CFNfvGM</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251105_169/1762302985687lcE7L_JPEG/80606292631494242_399949605.jpg</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>지친 몸 힐링 한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로에 지친 당신을 위한 건강한 한우로 활력을 충전해보세요.</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>출퇴근 피로 회복에 좋은 구이용 한우 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 영양가 높은 구이용 한우 선물세트로 건강과 활력을 채워보세요. 간편하게 즐길 수 있어 일상 식사로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I713" t="inlineStr">
+        <is>
+          <t>한우,구이용한우,한우선물세트,피로회복,건강식,출퇴근,활력</t>
+        </is>
+      </c>
+      <c r="J713" t="inlineStr">
+        <is>
+          <t>식품/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="n">
+        <v>713</v>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>설날 선물로 좋은 마장동 한우 선물 세트, 맛과 품질의 비결</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbgn70K</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260103_220/1767397746877Yd4oU_PNG/21846957667466438_127974687.png</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>프리미엄 마장동 한우 세트</t>
+        </is>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>설날 특별한 선물, 신선하고 부드러운 마장동 한우로 가족의 행복을 채워보세요.</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>설날 선물 추천 마장동 한우 선물 세트 맛과 품질</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>신선하고 부드러운 마장동 한우 선물 세트로 설날 가족의 행복을 가득 채우세요. 고급 선물용으로 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I714" t="inlineStr">
+        <is>
+          <t>설날선물,한우선물세트,마장동한우,고급선물,명절선물,소고기,신선식품</t>
+        </is>
+      </c>
+      <c r="J714" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="n">
+        <v>714</v>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>직장인 출퇴근 후에 즐기는 투뿔 숙성한우 스테이크</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://naver.me/G1mhj8N3</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_211/1720395611635zPhvg_JPEG/31289291941500558_1720856556.jpg</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>투뿔 숙성한우 스테이크</t>
+        </is>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸에 풍부한 육즙과 부드러운 식감으로 특별한 힐링을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>투뿔 숙성한우 스테이크 직장인 힐링 추천</t>
+        </is>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 직장인을 위한 풍부한 육즙과 부드러운 식감의 투뿔 숙성한우 스테이크로 특별한 힐링을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>숙성한우,투뿔한우,스테이크,직장인추천,출퇴근후간식,육즙가득,부드러운식감</t>
+        </is>
+      </c>
+      <c r="J715" t="inlineStr">
+        <is>
+          <t>음식/간식</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="n">
+        <v>715</v>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>체크 패턴이 돋보이는 이너리즘 수면바지 추천</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://naver.me/5En1EkDl</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221205_239/1670227759613vC9kV_JPEG/71363602302792285_1662957356.jpg</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>포근한 체크 수면바지</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>차가운 밤, 따뜻한 체크 수면바지로 편안한 잠자리를 만들어보세요. 이너리즘의 부드러운 감촉이 하루의 피로를 녹여드립니다.</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>체크 패턴 이너리즘 수면바지 추천, 편안한 숙면을 위한 선택</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>이너리즘 체크 수면바지는 부드러운 감촉과 따뜻한 보온성으로 포근한 잠자리를 선사합니다. 차가운 밤에도 편안하게 착용하기 좋습니다.</t>
+        </is>
+      </c>
+      <c r="I716" t="inlineStr">
+        <is>
+          <t>이너리즘,수면바지,체크패턴,편안한수면,따뜻한바지,숙면용바지,부드러운수면복</t>
+        </is>
+      </c>
+      <c r="J716" t="inlineStr">
+        <is>
+          <t>수면웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="n">
+        <v>716</v>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>2kg 대용량 LA갈비로 설날 명절 준비 완벽하게 마무리하기</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://naver.me/5asWE81f</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_59/1720403498896AbObJ_PNG/945707466979107_665950170.png</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>2kg 대용량 LA갈비</t>
+        </is>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>넉넉한 양으로 가족 모임 걱정 끝! 설날 명절 준비를 완벽하게 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>2kg 대용량 LA갈비 설날 명절 준비 추천</t>
+        </is>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>2kg 대용량 LA갈비로 가족 모임 걱정 없이 넉넉한 양을 준비하세요. 설날 명절 준비를 완벽하게 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="I717" t="inlineStr">
+        <is>
+          <t>LA갈비,대용량갈비,설날명절,가족모임,명절준비,2kg갈비</t>
+        </is>
+      </c>
+      <c r="J717" t="inlineStr">
+        <is>
+          <t>명절/한우</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="n">
+        <v>717</v>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>가족과 함께 맛보는 LA갈비의 특별한 맛</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://naver.me/5r3Rid1h</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240202_283/1706867245040UizPK_JPEG/108003028724874416_1035578210.jpg</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>가족과 즐기는 LA갈비</t>
+        </is>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>가족 모임에 안성맞춤인 LA갈비로 특별한 맛의 행복을 나누세요.</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>가족과 함께하는 LA갈비 추천, 특별한 맛 할인 구매</t>
+        </is>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>가족 모임에 최적화된 LA갈비로 특별한 맛과 행복을 나누세요. 신선한 재료로 풍미 가득한 가족 식사에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I718" t="inlineStr">
+        <is>
+          <t>LA갈비,가족모임,특별한맛,한식,바베큐,신선한고기,맛있는고기,가족식사</t>
+        </is>
+      </c>
+      <c r="J718" t="inlineStr">
+        <is>
+          <t>음식/고기</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="n">
+        <v>718</v>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>마장동 숙성로스로 완성하는 특별한 저녁 식사</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://naver.me/x2cvneZX</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250228_208/1740694115536Xhl34_JPEG/47249825932196547_1421438944.jpg</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>숙성로스 고기 한 상</t>
+        </is>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>특별한 저녁, 신선한 숙성로스로 풍성한 식탁 완성해보세요.</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>마장동 숙성로스 추천, 특별한 저녁 식사 완성</t>
+        </is>
+      </c>
+      <c r="H719" t="inlineStr">
+        <is>
+          <t>마장동에서 신선하게 숙성한 로스로 풍성하고 특별한 저녁 식사를 즐겨보세요. 고소하고 부드러운 맛이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>마장동,숙성로스,저녁식사,특별한식사,신선한고기,풍성한식탁</t>
+        </is>
+      </c>
+      <c r="J719" t="inlineStr">
+        <is>
+          <t>식품/고기</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>719</v>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물세트로 특별한 출퇴근 도시락 준비하기</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://naver.me/FfBHNiXl</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240112_240/17050411800423xifl_PNG/106177022673966491_1564965846.png</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>소중한 사람과 함께하는 특별한 식사, 신선한 투뿔 한우로 건강하고 맛있는 도시락을 완성하세요.</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물세트 추천, 특별한 출퇴근 도시락 완성하기</t>
+        </is>
+      </c>
+      <c r="H720" t="inlineStr">
+        <is>
+          <t>신선한 투뿔 한우로 건강하고 맛있는 출퇴근 도시락을 준비하세요. 소중한 사람과 함께 특별한 식사를 즐기기에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I720" t="inlineStr">
+        <is>
+          <t>투뿔한우,한우선물세트,도시락재료,건강식,출퇴근도시락,특별한선물</t>
+        </is>
+      </c>
+      <c r="J720" t="inlineStr">
+        <is>
+          <t>선물세트/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>720</v>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물세트로 특별한 출퇴근 도시락 준비하기</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://naver.me/FfBHNiXl</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240112_240/17050411800423xifl_PNG/106177022673966491_1564965846.png</t>
+        </is>
+      </c>
+      <c r="E721" t="inlineStr">
+        <is>
+          <t>프리미엄 투뿔 한우 세트</t>
+        </is>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>출퇴근 도시락에 든든한 한 끼, 투뿔 한우로 특별한 맛과 건강을 선물하세요.</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물세트로 출퇴근 도시락 추천</t>
+        </is>
+      </c>
+      <c r="H721" t="inlineStr">
+        <is>
+          <t>투뿔 한우 선물세트로 출퇴근 도시락을 더욱 특별하게 준비하세요. 신선한 한우로 든든한 한 끼를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I721" t="inlineStr">
+        <is>
+          <t>투뿔한우,선물세트,출퇴근도시락,한우도시락,건강식,한우추천</t>
+        </is>
+      </c>
+      <c r="J721" t="inlineStr">
+        <is>
+          <t>식품/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="n">
+        <v>721</v>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>풋파일로 집에서도 간편한 뒤꿈치 굳은살 케어</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://naver.me/FW0SBrvQ</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250430_271/17459995425983QQQX_JPEG/89971664727595_583972751.jpg</t>
+        </is>
+      </c>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>뒤꿈치 굳은살 간편케어</t>
+        </is>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>거칠고 딱딱한 뒤꿈치 고민, 집에서 쉽고 빠르게 매끄럽게 케어하세요.</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>풋파일 추천 집에서 간편한 뒤꿈치 굳은살 케어</t>
+        </is>
+      </c>
+      <c r="H722" t="inlineStr">
+        <is>
+          <t>거칠고 딱딱한 뒤꿈치 굳은살을 집에서도 쉽고 빠르게 매끄럽게 관리하는 풋파일입니다. 간편한 사용으로 꾸준한 케어에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I722" t="inlineStr">
+        <is>
+          <t>풋파일,뒤꿈치케어,굳은살제거,발관리,홈케어,발각질제거,풋케어,발건강</t>
+        </is>
+      </c>
+      <c r="J722" t="inlineStr">
+        <is>
+          <t>뷰티/케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="n">
+        <v>722</v>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>마장동에서 온 신선한 투뿔한우, 집에서 특별한 식사 경험</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://naver.me/x5m5HcXf</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_175/1736597878436V7jNs_JPEG/8565368481611108_1280498002.jpg</t>
+        </is>
+      </c>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>신선한 투뿔한우 스테이크</t>
+        </is>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>집에서도 즐기는 마장동 직송 투뿔한우로 특별한 식사 시간을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>마장동 투뿔한우 추천, 집에서 신선한 한우 맛보기</t>
+        </is>
+      </c>
+      <c r="H723" t="inlineStr">
+        <is>
+          <t>마장동에서 직송한 신선한 투뿔한우로 집에서 특별한 식사를 즐겨보세요. 고품질 한우를 간편하게 만나볼 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I723" t="inlineStr">
+        <is>
+          <t>마장동, 투뿔한우, 신선한 한우, 집에서 한우, 특별한 식사, 한우 추천</t>
+        </is>
+      </c>
+      <c r="J723" t="inlineStr">
+        <is>
+          <t>한우/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="n">
+        <v>723</v>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>운동 후 뷰티끄랩 투웨이 발각질제거기로 발 관리하기</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://naver.me/xdjhyiiC</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221221_168/16716003391477ukwz_JPEG/72736227859010256_1495902461.jpg</t>
+        </is>
+      </c>
+      <c r="E724" t="inlineStr">
+        <is>
+          <t>운동 후 발 각질 제거</t>
+        </is>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>운동 후 거칠어진 발을 부드럽게 관리해 보세요. 깔끔한 발 피부로 자신감을 되찾아 드립니다.</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>운동 후 뷰티끄랩 투웨이 발각질제거기 추천</t>
+        </is>
+      </c>
+      <c r="H724" t="inlineStr">
+        <is>
+          <t>운동으로 거칠어진 발 피부를 부드럽게 관리해주는 뷰티끄랩 투웨이 발각질제거기입니다. 깔끔한 발 피부로 자신감을 되찾으세요.</t>
+        </is>
+      </c>
+      <c r="I724" t="inlineStr">
+        <is>
+          <t>발각질제거기,운동후피부관리,뷰티끄랩,발관리,투웨이발각질제거기</t>
+        </is>
+      </c>
+      <c r="J724" t="inlineStr">
+        <is>
+          <t>뷰티/퍼스널케어</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="n">
+        <v>724</v>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>맞춤 주문 호텔수건으로 출퇴근 준비를 완성하다</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://naver.me/GHYFnszi</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_184/1736587711088NW09B_JPEG/87791555057789157_1147789636.jpg</t>
+        </is>
+      </c>
+      <c r="E725" t="inlineStr">
+        <is>
+          <t>포근한 맞춤 호텔수건</t>
+        </is>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>매일 아침, 부드러운 호텔수건으로 상쾌한 출근 준비를 완성해 보세요.</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>맞춤 주문 호텔수건으로 부드러운 출근 준비 추천</t>
+        </is>
+      </c>
+      <c r="H725" t="inlineStr">
+        <is>
+          <t>매일 아침 부드럽고 흡수력 좋은 맞춤 주문 호텔수건으로 상쾌한 출근 준비를 도와드립니다. 실용적이고 고급스러운 터치감이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I725" t="inlineStr">
+        <is>
+          <t>호텔수건,맞춤수건,출근준비,부드러운수건,흡수력좋은수건</t>
+        </is>
+      </c>
+      <c r="J725" t="inlineStr">
+        <is>
+          <t>홈리빙/욕실</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="n">
+        <v>725</v>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>긴팔 수면 잠옷으로 출퇴근 후 휴식 시간을 더욱 아늑하게</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://naver.me/xR2OFeiU</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251001_250/17592947364724CLgH_JPEG/3538710971471043_1595756783.jpg</t>
+        </is>
+      </c>
+      <c r="E726" t="inlineStr">
+        <is>
+          <t>포근한 긴팔 수면 잠옷</t>
+        </is>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식을 원한다면 부드러운 긴팔 잠옷으로 하루를 따뜻하게 마무리하세요.</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>긴팔 수면 잠옷 추천, 출퇴근 후 편안한 휴식에 적합</t>
+        </is>
+      </c>
+      <c r="H726" t="inlineStr">
+        <is>
+          <t>부드러운 긴팔 잠옷으로 출퇴근 후 휴식을 따뜻하고 편안하게 만들어 줍니다. 아늑한 착용감이 특징입니다.</t>
+        </is>
+      </c>
+      <c r="I726" t="inlineStr">
+        <is>
+          <t>긴팔 잠옷,수면 잠옷,편안한 잠옷,출퇴근 잠옷,아늑한 잠옷</t>
+        </is>
+      </c>
+      <c r="J726" t="inlineStr">
+        <is>
+          <t>잠옷/홈웨어</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="n">
+        <v>726</v>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>커플 수면 잠옷으로 함께하는 달콤한 홈웨어 데이트</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://naver.me/GcKsUBaT</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251001_26/1759296431456fAeFY_JPEG/9661792553309763_1234632757.jpg</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr">
+        <is>
+          <t>편안한 커플 수면 잠옷</t>
+        </is>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>함께 입는 편안한 잠옷으로 포근한 밤과 달콤한 홈 데이트를 즐겨보세요.</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>커플 수면 잠옷 추천, 달콤한 홈웨어 데이트</t>
+        </is>
+      </c>
+      <c r="H727" t="inlineStr">
+        <is>
+          <t>함께 입는 커플 수면 잠옷으로 편안하고 포근한 밤을 보내고 달콤한 홈 데이트를 즐기세요.</t>
+        </is>
+      </c>
+      <c r="I727" t="inlineStr">
+        <is>
+          <t>커플잠옷,수면잠옷,홈웨어,커플홈웨어,잠옷세트,포근한잠옷,편안한잠옷,홈데이트</t>
+        </is>
+      </c>
+      <c r="J727" t="inlineStr">
+        <is>
+          <t>홈웨어/잠옷</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="n">
+        <v>727</v>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>설 명절 소중한 사람과 나누는 투뿔 한우의 맛</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://naver.me/xAAc5G0y</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250106_226/1736150569911uNt3o_JPEG/51159063933769078_295223677.jpg</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr">
+        <is>
+          <t>명절 소중한 투뿔 한우</t>
+        </is>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>설 명절, 가족과 함께하는 최고의 한우 맛으로 특별한 순간을 더욱 풍성하게 만드세요.</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>설 명절 추천 투뿔 한우, 풍성한 가족 식사</t>
+        </is>
+      </c>
+      <c r="H728" t="inlineStr">
+        <is>
+          <t>설 명절 소중한 사람과 함께 즐기는 투뿔 한우로 특별한 순간을 더욱 풍성하게 만드세요. 가족 모임에 가장 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I728" t="inlineStr">
+        <is>
+          <t>설 명절,투뿔 한우,한우 맛,가족 식사,명절 선물</t>
+        </is>
+      </c>
+      <c r="J728" t="inlineStr">
+        <is>
+          <t>명절/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="n">
+        <v>728</v>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>출퇴근 전 빠른 커피 한잔, 위즈웰 자동 핸드 드립 세트 추천</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://naver.me/G28spFMK</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230324_238/1679615995648hHgpg_JPEG/qm6Ec_102817_1.jpg</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr">
+        <is>
+          <t>빠른 출근 커피 드립 세트</t>
+        </is>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>바쁜 아침에도 빠르고 간편하게 신선한 커피를 즐기세요. 출퇴근길 커피 고민 끝!</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>위즈웰 자동 핸드 드립 세트 빠른 커피 추천</t>
+        </is>
+      </c>
+      <c r="H729" t="inlineStr">
+        <is>
+          <t>출퇴근길 바쁜 아침에도 신선하고 간편하게 즐기는 자동 핸드 드립 커피 세트로 커피 고민을 해결하세요.</t>
+        </is>
+      </c>
+      <c r="I729" t="inlineStr">
+        <is>
+          <t>자동핸드드립,커피세트,출퇴근커피,간편커피,신선커피,빠른커피</t>
+        </is>
+      </c>
+      <c r="J729" t="inlineStr">
+        <is>
+          <t>커피/주방</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="n">
+        <v>729</v>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>가족과 함께 즐기는 명절 꽃갈비 선물 이야기</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://naver.me/xOdWBPDl</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230907_80/1694062474349Gs1Hh_JPEG/1107766880238636_1531823951.jpg</t>
+        </is>
+      </c>
+      <c r="E730" t="inlineStr">
+        <is>
+          <t>명절 가족 꽃갈비 선물</t>
+        </is>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>소중한 가족과 함께하는 명절, 맛있는 꽃갈비로 특별한 시간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
+        <is>
+          <t>가족과 함께 즐기는 명절 꽃갈비 선물 추천</t>
+        </is>
+      </c>
+      <c r="H730" t="inlineStr">
+        <is>
+          <t>소중한 가족과 함께하는 명절에 맛있는 꽃갈비로 특별한 시간을 선사하세요. 고품질 갈비로 가족 식사에 적합한 선물입니다.</t>
+        </is>
+      </c>
+      <c r="I730" t="inlineStr">
+        <is>
+          <t>명절선물,꽃갈비,가족식사,명절음식,갈비선물</t>
+        </is>
+      </c>
+      <c r="J730" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="n">
+        <v>730</v>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>감사박스에 담긴 마음, 명절 선물로 딱 좋아요</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://naver.me/5jBoPC8F</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260112_197/1768213792922TxC8s_JPEG/22894527870296529_444502902.jpg</t>
+        </is>
+      </c>
+      <c r="E731" t="inlineStr">
+        <is>
+          <t>감사 마음 선물 세트</t>
+        </is>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>소중한 분들께 감사의 마음을 전하세요. 명절에 딱 맞는 특별한 선물입니다.</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>감사박스 명절 선물로 추천하는 특별한 마음 전하기</t>
+        </is>
+      </c>
+      <c r="H731" t="inlineStr">
+        <is>
+          <t>소중한 분들께 감사의 마음을 전하는 명절 선물용 박스입니다. 특별한 마음을 담아 선물하기에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I731" t="inlineStr">
+        <is>
+          <t>감사박스,명절선물,감사의마음,특별한선물,선물추천,명절선물세트</t>
+        </is>
+      </c>
+      <c r="J731" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="n">
+        <v>731</v>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>선물세트로 따뜻한 마음을 전하는 구정 맞이 선택</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://naver.me/G7CAdxjN</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260113_223/1768268190266LBwuS_JPEG/4751635388318500_697929344.jpg</t>
+        </is>
+      </c>
+      <c r="E732" t="inlineStr">
+        <is>
+          <t>구정 맞이 따뜻한 선물세트</t>
+        </is>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>소중한 이에게 마음을 전할 완벽한 선물세트로 따뜻한 설날 분위기를 선사하세요.</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>구정 맞이 따뜻한 마음 전하는 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H732" t="inlineStr">
+        <is>
+          <t>설날 분위기를 더욱 따뜻하게 만드는 완벽한 선물세트로 소중한 이에게 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="I732" t="inlineStr">
+        <is>
+          <t>구정선물세트,설날선물,따뜻한선물,선물추천,명절선물</t>
+        </is>
+      </c>
+      <c r="J732" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="n">
+        <v>732</v>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>투뿔 한우 한정세트로 가족과 즐기는 건강한 외식</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://naver.me/Fm3zXU7f</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20251111_89/1762827002459qKPlh_JPEG/2496457400875908_1605784555.jpg</t>
+        </is>
+      </c>
+      <c r="E733" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 세트</t>
+        </is>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>가족과 함께하는 특별한 외식, 신선하고 건강한 한우로 행복한 시간을 만드세요.</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>투뿔 한우 한정세트 가족외식 추천 건강한 미식</t>
+        </is>
+      </c>
+      <c r="H733" t="inlineStr">
+        <is>
+          <t>가족과 함께 즐기는 신선한 투뿔 한우 한정세트로 건강하고 특별한 외식을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I733" t="inlineStr">
+        <is>
+          <t>투뿔한우,한정세트,가족외식,건강한한우,신선한고기,특별한외식,미식세트</t>
+        </is>
+      </c>
+      <c r="J733" t="inlineStr">
+        <is>
+          <t>외식/고기</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="n">
+        <v>733</v>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>출퇴근 후 피로한 발 뒤꿈치, 굳은살 제거로 상쾌하게</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://naver.me/xhlGYWWM</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240528_124/1716880006689a20Pc_JPEG/118015895400020214_724515494.jpg</t>
+        </is>
+      </c>
+      <c r="E734" t="inlineStr">
+        <is>
+          <t>피로한 발 뒤꿈치 굳은살 제거</t>
+        </is>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 발을 상쾌하게 케어해주는 굳은살 제거 솔루션으로 편안함을 느껴보세요.</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>출퇴근 후 발 뒤꿈치 굳은살 제거 추천, 상쾌한 발 케어</t>
+        </is>
+      </c>
+      <c r="H734" t="inlineStr">
+        <is>
+          <t>출퇴근으로 지친 발 뒤꿈치의 굳은살을 효과적으로 제거하여 편안함을 선사하는 솔루션입니다. 상쾌한 하루를 위한 필수 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="I734" t="inlineStr">
+        <is>
+          <t>발뒤꿈치,굳은살제거,발케어,피로해소,출퇴근,편안함,상쾌함</t>
+        </is>
+      </c>
+      <c r="J734" t="inlineStr">
+        <is>
+          <t>건강/뷰티</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="n">
+        <v>734</v>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>파이프크리닝호스로 집안 하수구 깔끔하게 관리하기</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://naver.me/5FEdc3NX</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20221229_117/1672297043758sSKrx_JPEG/73432823482644631_616679119.jpg</t>
+        </is>
+      </c>
+      <c r="E735" t="inlineStr">
+        <is>
+          <t>집안 하수구 청소 호스</t>
+        </is>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>막힌 하수구 고민, 파이프크리닝호스로 간편히 해결하세요. 깔끔한 관리를 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>하수구 막힘 해결 파이프크리닝호스 추천 및 구매</t>
+        </is>
+      </c>
+      <c r="H735" t="inlineStr">
+        <is>
+          <t>간편하게 하수구 막힘을 해결하는 파이프크리닝호스로 집안 배수관을 청결하게 관리하세요.</t>
+        </is>
+      </c>
+      <c r="I735" t="inlineStr">
+        <is>
+          <t>파이프크리닝호스,하수구청소,막힌하수구해결,집안배수관관리,하수구관리</t>
+        </is>
+      </c>
+      <c r="J735" t="inlineStr">
+        <is>
+          <t>청소/생활용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="n">
+        <v>735</v>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>부채살의 부드러운 맛을 집에서 즐기는 방법</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://naver.me/F9ha1ECZ</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220812_57/1660267565596YR2l3_JPEG/61403411288097468_1297543586.jpg</t>
+        </is>
+      </c>
+      <c r="E736" t="inlineStr">
+        <is>
+          <t>집에서 즐기는 부채살</t>
+        </is>
+      </c>
+      <c r="F736" t="inlineStr">
+        <is>
+          <t>부드러운 부채살의 풍미를 집에서 간편하게 즐기고 싶은 당신을 위한 완벽한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G736" t="inlineStr">
+        <is>
+          <t>부채살 부드러운 맛 집에서 즐기기 추천 방법</t>
+        </is>
+      </c>
+      <c r="H736" t="inlineStr">
+        <is>
+          <t>부드러운 부채살의 진한 풍미를 집에서 간편하게 즐기기 좋은 방법입니다. 가족과 함께하는 특별한 식사에 적합합니다.</t>
+        </is>
+      </c>
+      <c r="I736" t="inlineStr">
+        <is>
+          <t>부채살, 부드러운 고기, 집에서 요리, 간편 조리, 풍미 가득, 가족 식사, 고기 요리</t>
+        </is>
+      </c>
+      <c r="J736" t="inlineStr">
+        <is>
+          <t>고기/요리</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="n">
+        <v>736</v>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>긴팔 키즈 수면 잠옷, 아이 통화 중에도 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://naver.me/565MPriY</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250915_63/1757925624009AhsQT_JPEG/92058572165383142_377319152.jpg</t>
+        </is>
+      </c>
+      <c r="E737" t="inlineStr">
+        <is>
+          <t>아이용 편안한 긴팔 잠옷</t>
+        </is>
+      </c>
+      <c r="F737" t="inlineStr">
+        <is>
+          <t>아이 통화 중에도 편안한 착용감의 긴팔 수면 잠옷으로 편안한 잠자리를 선사해요.</t>
+        </is>
+      </c>
+      <c r="G737" t="inlineStr">
+        <is>
+          <t>긴팔 키즈 수면 잠옷 추천 편안한 착용감</t>
+        </is>
+      </c>
+      <c r="H737" t="inlineStr">
+        <is>
+          <t>아이 통화 중에도 편안한 착용감을 제공하는 긴팔 키즈 수면 잠옷으로 쾌적한 잠자리를 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I737" t="inlineStr">
+        <is>
+          <t>키즈 수면 잠옷,긴팔 잠옷,아이 잠옷,편안한 잠옷,아동 수면복</t>
+        </is>
+      </c>
+      <c r="J737" t="inlineStr">
+        <is>
+          <t>키즈웨어/잠옷</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="n">
+        <v>737</v>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>명절 선물세트, 전통장식과 함께 전하는 마음</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://naver.me/5wNGUhzX</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260113_186/1768300012124UaQgP_JPEG/48457631110096998_730051055.jpg</t>
+        </is>
+      </c>
+      <c r="E738" t="inlineStr">
+        <is>
+          <t>전통장식 명절 선물세트</t>
+        </is>
+      </c>
+      <c r="F738" t="inlineStr">
+        <is>
+          <t>특별한 명절, 소중한 마음을 전하는 전통장식과 선물세트로 사랑을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G738" t="inlineStr">
+        <is>
+          <t>명절 선물세트 전통장식과 함께 마음 전하기 추천</t>
+        </is>
+      </c>
+      <c r="H738" t="inlineStr">
+        <is>
+          <t>전통장식과 함께하는 명절 선물세트로 소중한 마음을 전하세요. 가족과 지인들에게 의미 있는 선물이 됩니다.</t>
+        </is>
+      </c>
+      <c r="I738" t="inlineStr">
+        <is>
+          <t>명절 선물세트,전통장식,명절 선물,가족 선물,명절 추천,전통 선물,특별한 선물</t>
+        </is>
+      </c>
+      <c r="J738" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="n">
+        <v>738</v>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>투뿔한우 선물세트로 감사의 마음을 전하세요</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://naver.me/xGFhsK7b</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250111_57/1736598055212aFRE2_JPEG/70730970335598878_142773343.jpg</t>
+        </is>
+      </c>
+      <c r="E739" t="inlineStr">
+        <is>
+          <t>프리미엄 투뿔한우 선물세트</t>
+        </is>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
+          <t>소중한 분께 최고의 맛과 품질을 선물하세요. 특별한 감사의 마음을 담아드립니다.</t>
+        </is>
+      </c>
+      <c r="G739" t="inlineStr">
+        <is>
+          <t>투뿔한우 선물세트 추천 최고의 맛과 품질 선물</t>
+        </is>
+      </c>
+      <c r="H739" t="inlineStr">
+        <is>
+          <t>투뿔한우 선물세트로 소중한 분께 감사의 마음을 전하세요. 품질 좋은 한우로 특별한 선물을 완성합니다.</t>
+        </is>
+      </c>
+      <c r="I739" t="inlineStr">
+        <is>
+          <t>투뿔한우,선물세트,한우선물,감사선물,명절선물,프리미엄한우</t>
+        </is>
+      </c>
+      <c r="J739" t="inlineStr">
+        <is>
+          <t>선물/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="n">
+        <v>739</v>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>브루클린 스타일 명품 호텔 수건, 출퇴근 후 피로를 부드럽게 달래줘요</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://naver.me/G5PYHZDx</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250715_5/1752566911923wSfup_JPEG/36377843888357111_1143029479.jpg</t>
+        </is>
+      </c>
+      <c r="E740" t="inlineStr">
+        <is>
+          <t>명품 호텔 수건</t>
+        </is>
+      </c>
+      <c r="F740" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 프리미엄 수건으로 피로를 날려보세요.</t>
+        </is>
+      </c>
+      <c r="G740" t="inlineStr">
+        <is>
+          <t>브루클린 스타일 명품 호텔 수건 추천, 부드러운 피로 회복</t>
+        </is>
+      </c>
+      <c r="H740" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 감싸주는 브루클린 스타일 명품 호텔 수건으로 부드럽고 쾌적한 휴식을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="I740" t="inlineStr">
+        <is>
+          <t>브루클린 스타일, 명품 호텔 수건, 프리미엄 수건, 피로회복, 출퇴근, 부드러운 수건, 고급 수건</t>
+        </is>
+      </c>
+      <c r="J740" t="inlineStr">
+        <is>
+          <t>생활/수건</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="n">
+        <v>740</v>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>간편한 휴대용 에너지바, 운동할 때 딱 좋아요</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://naver.me/GagH7D4a</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260113_233/1768275534281wpa5o_JPEG/78423984006384043_1186804354.jpg</t>
+        </is>
+      </c>
+      <c r="E741" t="inlineStr">
+        <is>
+          <t>운동용 휴대 에너지바</t>
+        </is>
+      </c>
+      <c r="F741" t="inlineStr">
+        <is>
+          <t>운동 중 간편하게 에너지를 보충하고 싶다면 딱 맞는 간편 휴대용 에너지바입니다.</t>
+        </is>
+      </c>
+      <c r="G741" t="inlineStr">
+        <is>
+          <t>간편한 휴대용 에너지바 운동 중 에너지 보충 추천</t>
+        </is>
+      </c>
+      <c r="H741" t="inlineStr">
+        <is>
+          <t>운동할 때 간편하게 섭취 가능한 휴대용 에너지바로 빠른 에너지 보충에 적합합니다. 활동적인 라이프스타일에 최적화된 간식입니다.</t>
+        </is>
+      </c>
+      <c r="I741" t="inlineStr">
+        <is>
+          <t>휴대용 에너지바,운동 간식,에너지 보충,간편 에너지바,스포츠 간식</t>
+        </is>
+      </c>
+      <c r="J741" t="inlineStr">
+        <is>
+          <t>운동/에너지</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="n">
+        <v>741</v>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>고급선물포장된 기삼전복, 소중한 분께 전하는 마음</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://naver.me/GMP8beUB</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240730_69/17223028898088OCMX_JPEG/16690646809654166_465245087.jpg</t>
+        </is>
+      </c>
+      <c r="E742" t="inlineStr">
+        <is>
+          <t>신선한 고급 기삼전복</t>
+        </is>
+      </c>
+      <c r="F742" t="inlineStr">
+        <is>
+          <t>소중한 분께 신선한 기삼전복으로 특별한 감동을 전하세요. 고급 포장으로 마음까지 담았습니다.</t>
+        </is>
+      </c>
+      <c r="G742" t="inlineStr">
+        <is>
+          <t>고급선물포장 기삼전복 추천, 소중한 분을 위한 특별한 선물</t>
+        </is>
+      </c>
+      <c r="H742" t="inlineStr">
+        <is>
+          <t>신선한 기삼전복을 고급 포장하여 소중한 분께 특별한 감동을 전하는 선물용 전복입니다.</t>
+        </is>
+      </c>
+      <c r="I742" t="inlineStr">
+        <is>
+          <t>기삼전복,선물전복,고급포장,신선전복,특별한선물,감동선물</t>
+        </is>
+      </c>
+      <c r="J742" t="inlineStr">
+        <is>
+          <t>선물/식품</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="n">
+        <v>742</v>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>명절에 사랑받는 소고기 육회, 가족과 함께하는 시간</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://naver.me/GKbgn7ql</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250326_201/1742949569579qinqD_JPEG/5926313666178271_1656623347.jpg</t>
+        </is>
+      </c>
+      <c r="E743" t="inlineStr">
+        <is>
+          <t>신선한 소고기 육회</t>
+        </is>
+      </c>
+      <c r="F743" t="inlineStr">
+        <is>
+          <t>명절에 가족과 함께 즐기는 신선한 소고기 육회로 특별한 시간을 만들어보세요.</t>
+        </is>
+      </c>
+      <c r="G743" t="inlineStr">
+        <is>
+          <t>명절 소고기 육회 추천, 가족과 함께하는 신선한 맛</t>
+        </is>
+      </c>
+      <c r="H743" t="inlineStr">
+        <is>
+          <t>명절에 가족과 함께 신선한 소고기 육회를 즐기며 특별한 시간을 보내세요. 건강하고 고급진 맛으로 추천합니다.</t>
+        </is>
+      </c>
+      <c r="I743" t="inlineStr">
+        <is>
+          <t>소고기육회,명절음식,가족식사,신선한육회,한우육회</t>
+        </is>
+      </c>
+      <c r="J743" t="inlineStr">
+        <is>
+          <t>명절/음식</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>743</v>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>각질 고민 끝, 편리한 발꿈치 각질 제거기 사용법</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://naver.me/GT6JwWWb</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20220110_76/1641780388882cpX12_JPEG/42916172588825224_442210156.jpg</t>
+        </is>
+      </c>
+      <c r="E744" t="inlineStr">
+        <is>
+          <t>효과 빠른 발꿈치 각질 제거</t>
+        </is>
+      </c>
+      <c r="F744" t="inlineStr">
+        <is>
+          <t>발꿈치 각질 때문에 고민이라면, 간편하게 사용하는 각질 제거기로 매끈한 발을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>각질 고민 끝 발꿈치 각질 제거기 추천 사용법 안내</t>
+        </is>
+      </c>
+      <c r="H744" t="inlineStr">
+        <is>
+          <t>발꿈치 각질 제거기로 간편하게 각질을 관리하고 매끄러운 발 피부를 유지하세요. 사용법도 쉬워 누구나 손쉽게 사용할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="I744" t="inlineStr">
+        <is>
+          <t>발꿈치,각질제거기,각질관리,발관리,각질제거,피부관리,발꿈치각질</t>
+        </is>
+      </c>
+      <c r="J744" t="inlineStr">
+        <is>
+          <t>뷰티/건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>744</v>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>호텔수건처럼 부드러운 메리츠 수건 추천</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://naver.me/GEiljs7d</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250129_144/17381230023337npgE_JPEG/49761904351032185_92738464.jpg</t>
+        </is>
+      </c>
+      <c r="E745" t="inlineStr">
+        <is>
+          <t>호텔식 부드러운 수건</t>
+        </is>
+      </c>
+      <c r="F745" t="inlineStr">
+        <is>
+          <t>매일 피부에 닿는 수건, 부드러움이 달라야 편안함이 있습니다. 메리츠 수건으로 집에서도 호텔 느낌을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>호텔수건처럼 부드러운 메리츠 수건 추천, 집에서도 호텔감성</t>
+        </is>
+      </c>
+      <c r="H745" t="inlineStr">
+        <is>
+          <t>부드러운 메리츠 수건으로 피부에 편안함을 선사하며, 집에서도 호텔 같은 고급스러운 사용감을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I745" t="inlineStr">
+        <is>
+          <t>메리츠 수건,부드러운 수건,호텔 수건,피부 친화적,고급 수건,호텔 감성,수건 추천</t>
+        </is>
+      </c>
+      <c r="J745" t="inlineStr">
+        <is>
+          <t>생활용품/수건</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="n">
+        <v>745</v>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>통기성이 뛰어난 호텔수건, 대나무섬유의 매력</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://naver.me/GBvr9yZ4</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240708_144/1720401268374ixyeY_JPEG/19110258398959642_1120965771.jpg</t>
+        </is>
+      </c>
+      <c r="E746" t="inlineStr">
+        <is>
+          <t>쾌적한 통기 대나무 수건</t>
+        </is>
+      </c>
+      <c r="F746" t="inlineStr">
+        <is>
+          <t>땀과 습기로 답답한 수건 고민 끝! 대나무섬유로 산뜻한 사용감을 경험해보세요.</t>
+        </is>
+      </c>
+      <c r="G746" t="inlineStr">
+        <is>
+          <t>통기성 좋은 대나무섬유 호텔수건 추천</t>
+        </is>
+      </c>
+      <c r="H746" t="inlineStr">
+        <is>
+          <t>대나무섬유로 제작된 호텔수건으로 땀과 습기를 효과적으로 흡수해 산뜻한 사용감을 제공합니다.</t>
+        </is>
+      </c>
+      <c r="I746" t="inlineStr">
+        <is>
+          <t>호텔수건,대나무섬유,통기성수건,흡습수건,산뜻한수건</t>
+        </is>
+      </c>
+      <c r="J746" t="inlineStr">
+        <is>
+          <t>생활용품/수건</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="n">
+        <v>746</v>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>밤새 포근하게, 키즈 수면 잠옷의 중요성</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://naver.me/FNIprQar</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250915_67/1757925625886FVWr8_JPEG/92058574072473218_222578381.jpg</t>
+        </is>
+      </c>
+      <c r="E747" t="inlineStr">
+        <is>
+          <t>아이 편안한 수면 잠옷</t>
+        </is>
+      </c>
+      <c r="F747" t="inlineStr">
+        <is>
+          <t>밤새 뒤척이는 아이를 위한 포근한 잠옷, 편안한 수면을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>키즈 수면 잠옷 추천, 밤새 포근한 아이 잠자리</t>
+        </is>
+      </c>
+      <c r="H747" t="inlineStr">
+        <is>
+          <t>아이의 편안한 수면을 돕는 포근한 키즈 수면 잠옷으로 밤새 뒤척임 없이 숙면을 지원합니다.</t>
+        </is>
+      </c>
+      <c r="I747" t="inlineStr">
+        <is>
+          <t>키즈수면잠옷,아동파자마,편안한잠옷,포근한수면,어린이잠옷,수면도움옷</t>
+        </is>
+      </c>
+      <c r="J747" t="inlineStr">
+        <is>
+          <t>키즈/잠옷</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="n">
+        <v>747</v>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>호두정과가 더해진 특별한 한결맛담 명절 선물세트</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://naver.me/xv6lXjoB</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20260112_178/1768205544586J59t6_JPEG/50635835252722267_1896513983.jpg</t>
+        </is>
+      </c>
+      <c r="E748" t="inlineStr">
+        <is>
+          <t>고소한 호두 정과 선물세트</t>
+        </is>
+      </c>
+      <c r="F748" t="inlineStr">
+        <is>
+          <t>명절 고민, 고소한 호두 정과로 풀어보세요. 건강한 맛으로 특별한 선물이 됩니다.</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>호두정과가 더해진 한결맛담 명절 선물세트 추천</t>
+        </is>
+      </c>
+      <c r="H748" t="inlineStr">
+        <is>
+          <t>고소한 호두 정과가 포함된 한결맛담 명절 선물세트로 건강한 맛과 특별한 마음을 전하세요.</t>
+        </is>
+      </c>
+      <c r="I748" t="inlineStr">
+        <is>
+          <t>호두정과,명절선물세트,한결맛담,건강선물,고소한간식</t>
+        </is>
+      </c>
+      <c r="J748" t="inlineStr">
+        <is>
+          <t>명절/선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="n">
+        <v>748</v>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식, 수면 잠옷바지 추천</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://naver.me/5BwXf6Ir</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250313_72/1741833107914HRtux_JPEG/17019559995477385_1823353566.jpg</t>
+        </is>
+      </c>
+      <c r="E749" t="inlineStr">
+        <is>
+          <t>편안한 수면 잠옷바지</t>
+        </is>
+      </c>
+      <c r="F749" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 편안한 잠옷바지로 숙면을 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="G749" t="inlineStr">
+        <is>
+          <t>출퇴근 후 편안한 휴식, 수면 잠옷바지 추천</t>
+        </is>
+      </c>
+      <c r="H749" t="inlineStr">
+        <is>
+          <t>출퇴근 후 지친 몸을 부드럽게 감싸주는 편안한 수면 잠옷바지로 편안한 휴식과 숙면을 도와드립니다.</t>
+        </is>
+      </c>
+      <c r="I749" t="inlineStr">
+        <is>
+          <t>수면바지,잠옷바지,편안한잠옷,숙면,출퇴근휴식,부드러운잠옷,홈웨어</t>
+        </is>
+      </c>
+      <c r="J749" t="inlineStr">
+        <is>
+          <t>잠옷/수면</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="n">
+        <v>749</v>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>설명절 선물용으로 손색없는 투뿔 한우 소고기 케이크</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://naver.me/G1mhj8qs</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20250401_121/1743444033935ksete_PNG/5333854596653683_517695447.png</t>
+        </is>
+      </c>
+      <c r="E750" t="inlineStr">
+        <is>
+          <t>프리미엄 한우 소고기 케이크</t>
+        </is>
+      </c>
+      <c r="F750" t="inlineStr">
+        <is>
+          <t>설명절 고민 끝! 특별한 투뿔 한우로 가족과 친구에게 품격 있는 선물을 전하세요.</t>
+        </is>
+      </c>
+      <c r="G750" t="inlineStr">
+        <is>
+          <t>설명절 선물용 투뿔 한우 소고기 케이크 추천</t>
+        </is>
+      </c>
+      <c r="H750" t="inlineStr">
+        <is>
+          <t>품격 있는 투뿔 한우 소고기 케이크로 설명절 가족과 친구 선물 고민 끝! 특별한 맛과 고급스러움을 선사합니다.</t>
+        </is>
+      </c>
+      <c r="I750" t="inlineStr">
+        <is>
+          <t>투뿔한우,설명절선물,한우케이크,소고기선물,가족선물,친구선물</t>
+        </is>
+      </c>
+      <c r="J750" t="inlineStr">
+        <is>
+          <t>설명절,선물</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="n">
+        <v>750</v>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>손에 들고 다니기 좋은 다용도 지압기로 휴대성까지 챙겼어요</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://naver.me/xPUXjBtm</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20240820_276/1724142405090gnBBU_PNG/57615273843911422_605455763.png</t>
+        </is>
+      </c>
+      <c r="E751" t="inlineStr">
+        <is>
+          <t>휴대용 다용도 지압기</t>
+        </is>
+      </c>
+      <c r="F751" t="inlineStr">
+        <is>
+          <t>언제 어디서나 손쉽게 지압, 휴대성이 뛰어나 바쁜 일상에 딱 맞는 아이템입니다.</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>휴대용 다용도 지압기 추천, 손쉬운 지압과 휴대성 겸비</t>
+        </is>
+      </c>
+      <c r="H751" t="inlineStr">
+        <is>
+          <t>언제 어디서나 간편하게 사용하는 휴대용 다용도 지압기로 바쁜 일상 속 긴장을 풀어줍니다.</t>
+        </is>
+      </c>
+      <c r="I751" t="inlineStr">
+        <is>
+          <t>휴대용 지압기, 다용도 지압기, 손 마사지, 휴대성 좋은 지압기, 일상 스트레스 해소</t>
+        </is>
+      </c>
+      <c r="J751" t="inlineStr">
+        <is>
+          <t>건강</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="n">
+        <v>751</v>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>유리막코팅제로 빗길에도 안전한 운전 환경 만들기</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://naver.me/FQyvsiWl</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230404_151/1680572342593peXH5_JPEG/81708176401642250_467553252.jpg</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>빗길 안전 유리막코팅</t>
+        </is>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>비 오는 날 시야 확보 어렵죠? 유리막코팅제로 빗길도 안심 운전하세요.</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>유리막코팅제 추천 빗길 운전 시야 확보로 안전운전</t>
+        </is>
+      </c>
+      <c r="H752" t="inlineStr">
+        <is>
+          <t>비 오는 날 시야 확보가 어려운 분들을 위한 유리막코팅제입니다. 빗길에도 뚜렷한 시야로 안전한 운전을 도와줍니다.</t>
+        </is>
+      </c>
+      <c r="I752" t="inlineStr">
+        <is>
+          <t>유리막코팅제,빗길운전,안전운전,차유리코팅,시야확보</t>
+        </is>
+      </c>
+      <c r="J752" t="inlineStr">
+        <is>
+          <t>자동차/용품</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="n">
+        <v>752</v>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>출퇴근 준비에 딱, CM-6820 캡슐커피머신 활용법</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://naver.me/GgBlo2GZ</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>https://shop-phinf.pstatic.net/20230224_63/1677214255480n6nR0_JPEG/78350039177691536_1887752395.jpg</t>
+        </is>
+      </c>
+      <c r="E753" t="inlineStr">
+        <is>
+          <t>간편 출퇴근 캡슐커피머신</t>
+        </is>
+      </c>
+      <c r="F753" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 신속하게 신선한 커피를 즐기고 싶은 당신을 위한 완벽한 선택입니다.</t>
+        </is>
+      </c>
+      <c r="G753" t="inlineStr">
+        <is>
+          <t>출퇴근 준비에 좋은 CM-6820 캡슐커피머신 추천</t>
+        </is>
+      </c>
+      <c r="H753" t="inlineStr">
+        <is>
+          <t>바쁜 출퇴근길에도 신속하게 신선한 커피를 즐길 수 있는 CM-6820 캡슐커피머신으로 편리한 커피 타임을 경험하세요.</t>
+        </is>
+      </c>
+      <c r="I753" t="inlineStr">
+        <is>
+          <t>캡슐커피머신,출퇴근커피,CM-6820,신속커피,신선커피,편리한커피,홈카페</t>
+        </is>
+      </c>
+      <c r="J753" t="inlineStr">
+        <is>
+          <t>가전,주방</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9" copies="3000"/>
 </worksheet>
 </file>
</xml_diff>